<commit_message>
Updated 96 cases for Assignment 2
</commit_message>
<xml_diff>
--- a/Middle Assignment/TestDesignTechique1_PhamHongAnh.xlsx
+++ b/Middle Assignment/TestDesignTechique1_PhamHongAnh.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NashTech\Rookies\NashTech_Homework\Middle Assignment 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NashTech\Rookies\NashTech_Homework\Middle Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B745C8B-334D-4CA4-9B83-68AFB934DBBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F01F91-6927-4CDE-82F7-8EA0C7CF8B43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="10400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -827,7 +827,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="205">
   <si>
     <t>ID</t>
   </si>
@@ -1213,18 +1213,12 @@
 2. Photo 2-15 is in the photo list</t>
   </si>
   <si>
-    <t>1.  Sign up with phone number</t>
-  </si>
-  <si>
     <t>Check if the button can slide</t>
   </si>
   <si>
     <t>SMS Verification code</t>
   </si>
   <si>
-    <t>Phone number text field and 'Slide to get SMS code' button</t>
-  </si>
-  <si>
     <t>When copying a phone number and pasting it in the text field</t>
   </si>
   <si>
@@ -1276,9 +1270,6 @@
     <t>When entering less than 10 numeric characters in the text field</t>
   </si>
   <si>
-    <t>When entering no numeric characters in the text field</t>
-  </si>
-  <si>
     <t>When entering fewer than 6 numeric characters</t>
   </si>
   <si>
@@ -1288,9 +1279,6 @@
     <t>When entering exactly 6 numeric characters</t>
   </si>
   <si>
-    <t>When entering no numeric character</t>
-  </si>
-  <si>
     <t>When entering between 6 and 50 blank spaces</t>
   </si>
   <si>
@@ -1300,9 +1288,6 @@
     <t>When clicking on the Eye icon</t>
   </si>
   <si>
-    <t>When entering a valid phone number</t>
-  </si>
-  <si>
     <t xml:space="preserve">When clicking on the close (x) button </t>
   </si>
   <si>
@@ -1366,28 +1351,118 @@
     <t>Check default - Check if the button is clickable</t>
   </si>
   <si>
-    <t xml:space="preserve">After entering all mandatory (*) information </t>
-  </si>
-  <si>
-    <t xml:space="preserve">When users don't enter phone numbers </t>
-  </si>
-  <si>
-    <t>When users don't enter SMS verification code</t>
-  </si>
-  <si>
-    <t>When users don't enter Full name</t>
-  </si>
-  <si>
-    <t>When users don't enter Password</t>
-  </si>
-  <si>
-    <t>When all required fields are empty</t>
-  </si>
-  <si>
-    <t>When the field is empty</t>
-  </si>
-  <si>
-    <t>2.  Sign up with phone number</t>
+    <t>1.  Testing fields</t>
+  </si>
+  <si>
+    <t>2.  Testing functions</t>
+  </si>
+  <si>
+    <t>When entering an email without a domain</t>
+  </si>
+  <si>
+    <t>When entering an email without the character @</t>
+  </si>
+  <si>
+    <t>When entering an email without the (.) character</t>
+  </si>
+  <si>
+    <t>When entering an email without the characters before the @</t>
+  </si>
+  <si>
+    <t>When entering blank spaces</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sign up with phone number </t>
+  </si>
+  <si>
+    <t>When entering only alphabetic values</t>
+  </si>
+  <si>
+    <t>When entering only numerical values</t>
+  </si>
+  <si>
+    <t>Slide to get SMS code' button</t>
+  </si>
+  <si>
+    <t>When users enter a valid phone number and then slide the button</t>
+  </si>
+  <si>
+    <t>When users enter an already existing phone number and then slide the button</t>
+  </si>
+  <si>
+    <t>(Precondition)</t>
+  </si>
+  <si>
+    <t>Check default - Check the initial position</t>
+  </si>
+  <si>
+    <t>When users enter no phone number and then slide the button</t>
+  </si>
+  <si>
+    <t>After entering all mandatory (*) information valid</t>
+  </si>
+  <si>
+    <t>When signing up with no SMS verification code</t>
+  </si>
+  <si>
+    <t>When signing up with no Full name</t>
+  </si>
+  <si>
+    <t>When signing up with no Password</t>
+  </si>
+  <si>
+    <t>Check default - Check if the 'Sign up with Email' button is available</t>
+  </si>
+  <si>
+    <t>Check default - Check if the 'Sign up with Phone number' button is available</t>
+  </si>
+  <si>
+    <t>When users enter a valid email and then slide the button</t>
+  </si>
+  <si>
+    <t>When users enter no email and then slide the button</t>
+  </si>
+  <si>
+    <t>When users enter an already existing email and then slide the button</t>
+  </si>
+  <si>
+    <t>Check the button's position after users enter an invalid value and slide</t>
+  </si>
+  <si>
+    <t>'Facebook' button</t>
+  </si>
+  <si>
+    <t>When signing up after entering all mandatory (*) information valid</t>
+  </si>
+  <si>
+    <t>When signing up with a Facebook account</t>
+  </si>
+  <si>
+    <t>When signing up with a Google account</t>
+  </si>
+  <si>
+    <t>'Google' button</t>
+  </si>
+  <si>
+    <t>Sign up with Facebook</t>
+  </si>
+  <si>
+    <t>Sign up with Google</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phone number </t>
+  </si>
+  <si>
+    <t>Check đầu số +84 hoặc 0</t>
+  </si>
+  <si>
+    <t>When signing up with all required fields empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sign up with Email </t>
   </si>
 </sst>
 </file>
@@ -1609,7 +1684,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1723,11 +1798,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -14252,17 +14339,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{861DB058-9ABC-4928-81FB-0309C7B8DB85}">
-  <dimension ref="A1:Z102"/>
+  <dimension ref="A1:Z212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="28" customWidth="1"/>
     <col min="2" max="2" width="33" style="31" customWidth="1"/>
-    <col min="3" max="3" width="29" style="28" customWidth="1"/>
+    <col min="3" max="3" width="29" style="48" customWidth="1"/>
     <col min="4" max="4" width="27.6328125" style="28" customWidth="1"/>
     <col min="5" max="5" width="12.1796875" style="28" customWidth="1"/>
     <col min="6" max="6" width="17" style="28" customWidth="1"/>
@@ -14278,7 +14365,7 @@
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="45" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
@@ -14319,7 +14406,7 @@
     </row>
     <row r="2" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="35" t="s">
-        <v>121</v>
+        <v>167</v>
       </c>
       <c r="B2" s="42"/>
       <c r="C2" s="42"/>
@@ -14349,16 +14436,16 @@
     </row>
     <row r="3" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="37" t="s">
-        <v>124</v>
-      </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
+        <v>201</v>
+      </c>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
       <c r="J3" s="26"/>
       <c r="K3" s="26"/>
       <c r="L3" s="26"/>
@@ -14382,9 +14469,9 @@
         <v>1</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="C4" s="13"/>
+        <v>121</v>
+      </c>
+      <c r="C4" s="46"/>
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
@@ -14398,9 +14485,9 @@
         <v>2</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="C5" s="13"/>
+        <v>147</v>
+      </c>
+      <c r="C5" s="46"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
@@ -14414,9 +14501,9 @@
         <v>3</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="C6" s="13"/>
+        <v>135</v>
+      </c>
+      <c r="C6" s="46"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
@@ -14430,9 +14517,9 @@
         <v>4</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>140</v>
-      </c>
-      <c r="C7" s="13"/>
+        <v>138</v>
+      </c>
+      <c r="C7" s="46"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
@@ -14442,13 +14529,13 @@
     </row>
     <row r="8" spans="1:26" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="27">
-        <f t="shared" ref="A8:A71" ca="1" si="0">IF(OFFSET(A8,-1,0) ="",OFFSET(A8,-2,0)+1,OFFSET(A8,-1,0)+1 )</f>
+        <f t="shared" ref="A8:A75" ca="1" si="0">IF(OFFSET(A8,-1,0) ="",OFFSET(A8,-2,0)+1,OFFSET(A8,-1,0)+1 )</f>
         <v>5</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="C8" s="13"/>
+        <v>139</v>
+      </c>
+      <c r="C8" s="46"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
@@ -14456,15 +14543,15 @@
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
     </row>
-    <row r="9" spans="1:26" s="10" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
-      <c r="B9" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="C9" s="13"/>
+      <c r="B9" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" s="46"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
@@ -14478,9 +14565,9 @@
         <v>7</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="C10" s="13"/>
+        <v>124</v>
+      </c>
+      <c r="C10" s="46"/>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
@@ -14488,15 +14575,15 @@
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="1:26" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" s="10" customFormat="1" ht="20.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>8</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="C11" s="13"/>
+        <v>125</v>
+      </c>
+      <c r="C11" s="46"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
@@ -14504,15 +14591,15 @@
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
     </row>
-    <row r="12" spans="1:26" s="10" customFormat="1" ht="20.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" s="10" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>9</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="C12" s="13"/>
+        <v>126</v>
+      </c>
+      <c r="C12" s="46"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
@@ -14520,15 +14607,15 @@
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
     </row>
-    <row r="13" spans="1:26" s="10" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>10</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="C13" s="13"/>
+        <v>137</v>
+      </c>
+      <c r="C13" s="46"/>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
@@ -14536,15 +14623,17 @@
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
     </row>
-    <row r="14" spans="1:26" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" s="10" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>11</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="C14" s="13"/>
+        <v>127</v>
+      </c>
+      <c r="C14" s="46" t="s">
+        <v>202</v>
+      </c>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
@@ -14552,15 +14641,15 @@
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
     </row>
-    <row r="15" spans="1:26" s="10" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" s="10" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>12</v>
       </c>
-      <c r="B15" s="29" t="s">
-        <v>129</v>
-      </c>
-      <c r="C15" s="13"/>
+      <c r="B15" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C15" s="46"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
@@ -14568,30 +14657,45 @@
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
     </row>
-    <row r="16" spans="1:26" s="10" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="27">
-        <f t="shared" ca="1" si="0"/>
+    <row r="16" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="43" t="s">
+        <v>122</v>
+      </c>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="44"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="26"/>
+      <c r="O16" s="26"/>
+      <c r="P16" s="26"/>
+      <c r="Q16" s="26"/>
+      <c r="R16" s="26"/>
+      <c r="S16" s="26"/>
+      <c r="T16" s="26"/>
+      <c r="U16" s="26"/>
+      <c r="V16" s="26"/>
+      <c r="W16" s="26"/>
+      <c r="X16" s="26"/>
+      <c r="Y16" s="26"/>
+      <c r="Z16" s="26"/>
+    </row>
+    <row r="17" spans="1:26" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="27">
+        <f ca="1">IF(OFFSET(A17,-2,0) ="",OFFSET(A17,-2,0)+1,OFFSET(A17,-2,0)+1 )</f>
         <v>13</v>
       </c>
-      <c r="B16" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-    </row>
-    <row r="17" spans="1:26" s="10" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="27">
-        <f t="shared" ca="1" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B17" s="29" t="s">
-        <v>178</v>
-      </c>
+      <c r="B17" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="C17" s="46"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
@@ -14599,15 +14703,15 @@
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
     </row>
-    <row r="18" spans="1:26" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" s="10" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="27">
-        <f t="shared" ca="1" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="C18" s="13"/>
+        <f ca="1">IF(OFFSET(A18,-1,0) ="",OFFSET(A18,-2,0)+1,OFFSET(A18,-1,0)+1 )</f>
+        <v>14</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="C18" s="46"/>
       <c r="D18" s="13"/>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
@@ -14615,44 +14719,31 @@
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
     </row>
-    <row r="19" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="B19" s="43"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="26"/>
-      <c r="O19" s="26"/>
-      <c r="P19" s="26"/>
-      <c r="Q19" s="26"/>
-      <c r="R19" s="26"/>
-      <c r="S19" s="26"/>
-      <c r="T19" s="26"/>
-      <c r="U19" s="26"/>
-      <c r="V19" s="26"/>
-      <c r="W19" s="26"/>
-      <c r="X19" s="26"/>
-      <c r="Y19" s="26"/>
-      <c r="Z19" s="26"/>
-    </row>
-    <row r="20" spans="1:26" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="C19" s="46"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+    </row>
+    <row r="20" spans="1:26" s="10" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="27">
+        <f t="shared" ca="1" si="0"/>
         <v>16</v>
       </c>
-      <c r="B20" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="C20" s="13"/>
+      <c r="B20" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="C20" s="46"/>
       <c r="D20" s="13"/>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
@@ -14660,15 +14751,15 @@
       <c r="H20" s="13"/>
       <c r="I20" s="13"/>
     </row>
-    <row r="21" spans="1:26" s="10" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" s="10" customFormat="1" ht="24.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="27">
-        <f ca="1">IF(OFFSET(A21,-1,0) ="",OFFSET(A21,-2,0)+1,OFFSET(A21,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="0"/>
         <v>17</v>
       </c>
-      <c r="B21" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="C21" s="13"/>
+      <c r="B21" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="C21" s="46"/>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
@@ -14676,15 +14767,15 @@
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
     </row>
-    <row r="22" spans="1:26" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" s="10" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>18</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>143</v>
-      </c>
-      <c r="C22" s="13"/>
+        <v>128</v>
+      </c>
+      <c r="C22" s="46"/>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
@@ -14692,15 +14783,15 @@
       <c r="H22" s="13"/>
       <c r="I22" s="13"/>
     </row>
-    <row r="23" spans="1:26" s="10" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>19</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="C23" s="13"/>
+        <v>129</v>
+      </c>
+      <c r="C23" s="46"/>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
@@ -14708,15 +14799,15 @@
       <c r="H23" s="13"/>
       <c r="I23" s="13"/>
     </row>
-    <row r="24" spans="1:26" s="10" customFormat="1" ht="24.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>20</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>145</v>
-      </c>
-      <c r="C24" s="13"/>
+        <v>130</v>
+      </c>
+      <c r="C24" s="46"/>
       <c r="D24" s="13"/>
       <c r="E24" s="13"/>
       <c r="F24" s="13"/>
@@ -14724,15 +14815,15 @@
       <c r="H24" s="13"/>
       <c r="I24" s="13"/>
     </row>
-    <row r="25" spans="1:26" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" s="10" customFormat="1" ht="20.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>21</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="C25" s="13"/>
+        <v>126</v>
+      </c>
+      <c r="C25" s="46"/>
       <c r="D25" s="13"/>
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
@@ -14740,15 +14831,15 @@
       <c r="H25" s="13"/>
       <c r="I25" s="13"/>
     </row>
-    <row r="26" spans="1:26" s="10" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" s="10" customFormat="1" ht="20.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>22</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="C26" s="13"/>
+        <v>137</v>
+      </c>
+      <c r="C26" s="47"/>
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
@@ -14756,78 +14847,90 @@
       <c r="H26" s="13"/>
       <c r="I26" s="13"/>
     </row>
-    <row r="27" spans="1:26" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">IF(OFFSET(A27,-1,0) ="",OFFSET(A27,-2,0)+1,OFFSET(A27,-1,0)+1 )</f>
         <v>23</v>
       </c>
-      <c r="B27" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
+      <c r="B27" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C27" s="47"/>
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
       <c r="H27" s="13"/>
       <c r="I27" s="13"/>
     </row>
-    <row r="28" spans="1:26" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="27">
-        <f t="shared" ca="1" si="0"/>
+    <row r="28" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="B28" s="44"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="26"/>
+      <c r="M28" s="26"/>
+      <c r="N28" s="26"/>
+      <c r="O28" s="26"/>
+      <c r="P28" s="26"/>
+      <c r="Q28" s="26"/>
+      <c r="R28" s="26"/>
+      <c r="S28" s="26"/>
+      <c r="T28" s="26"/>
+      <c r="U28" s="26"/>
+      <c r="V28" s="26"/>
+      <c r="W28" s="26"/>
+      <c r="X28" s="26"/>
+      <c r="Y28" s="26"/>
+      <c r="Z28" s="26"/>
+    </row>
+    <row r="29" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="27">
+        <f ca="1">IF(OFFSET(A29,-2,0) ="",OFFSET(A29,-2,0)+1,OFFSET(A29,-2,0)+1 )</f>
         <v>24</v>
       </c>
-      <c r="B28" s="29" t="s">
-        <v>132</v>
-      </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-    </row>
-    <row r="29" spans="1:26" s="10" customFormat="1" ht="20.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="27">
-        <f t="shared" ca="1" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B29" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
+      <c r="B29" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="C29" s="47"/>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
       <c r="H29" s="13"/>
       <c r="I29" s="13"/>
     </row>
-    <row r="30" spans="1:26" s="10" customFormat="1" ht="20.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="27">
-        <f t="shared" ca="1" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="B30" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="D30" s="13"/>
+        <f ca="1">IF(OFFSET(A30,-1,0) ="",OFFSET(A30,-2,0)+1,OFFSET(A30,-1,0)+1 )</f>
+        <v>25</v>
+      </c>
+      <c r="B30" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="C30" s="47"/>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
       <c r="G30" s="13"/>
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
     </row>
-    <row r="31" spans="1:26" s="10" customFormat="1" ht="21.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="27">
-        <f t="shared" ca="1" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="B31" s="29" t="s">
-        <v>178</v>
-      </c>
-      <c r="D31" s="30"/>
+        <f t="shared" ref="A31:A36" ca="1" si="1">IF(OFFSET(A31,-1,0) ="",OFFSET(A31,-2,0)+1,OFFSET(A31,-1,0)+1 )</f>
+        <v>26</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="C31" s="47"/>
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
       <c r="G31" s="13"/>
@@ -14836,120 +14939,118 @@
     </row>
     <row r="32" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="27">
-        <f ca="1">IF(OFFSET(A32,-1,0) ="",OFFSET(A32,-2,0)+1,OFFSET(A32,-1,0)+1 )</f>
-        <v>28</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>27</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>151</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="C32" s="47"/>
       <c r="E32" s="13"/>
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
       <c r="I32" s="13"/>
     </row>
-    <row r="33" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="44" t="s">
-        <v>133</v>
-      </c>
-      <c r="B33" s="43"/>
-      <c r="C33" s="43"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="43"/>
-      <c r="H33" s="43"/>
-      <c r="I33" s="43"/>
-      <c r="J33" s="26"/>
-      <c r="K33" s="26"/>
-      <c r="L33" s="26"/>
-      <c r="M33" s="26"/>
-      <c r="N33" s="26"/>
-      <c r="O33" s="26"/>
-      <c r="P33" s="26"/>
-      <c r="Q33" s="26"/>
-      <c r="R33" s="26"/>
-      <c r="S33" s="26"/>
-      <c r="T33" s="26"/>
-      <c r="U33" s="26"/>
-      <c r="V33" s="26"/>
-      <c r="W33" s="26"/>
-      <c r="X33" s="26"/>
-      <c r="Y33" s="26"/>
-      <c r="Z33" s="26"/>
-    </row>
-    <row r="34" spans="1:26" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="C33" s="47"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+    </row>
+    <row r="34" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="27">
+        <f t="shared" ca="1" si="1"/>
         <v>29</v>
       </c>
-      <c r="B34" s="29" t="s">
-        <v>134</v>
-      </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
+      <c r="B34" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C34" s="47"/>
       <c r="E34" s="13"/>
       <c r="F34" s="13"/>
       <c r="G34" s="13"/>
       <c r="H34" s="13"/>
       <c r="I34" s="13"/>
     </row>
-    <row r="35" spans="1:26" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="27">
         <f ca="1">IF(OFFSET(A35,-1,0) ="",OFFSET(A35,-2,0)+1,OFFSET(A35,-1,0)+1 )</f>
         <v>30</v>
       </c>
-      <c r="B35" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
+      <c r="B35" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="C35" s="47"/>
       <c r="E35" s="13"/>
       <c r="F35" s="13"/>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
       <c r="I35" s="13"/>
     </row>
-    <row r="36" spans="1:26" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="27">
-        <f ca="1">IF(OFFSET(A36,-1,0) ="",OFFSET(A36,-2,0)+1,OFFSET(A36,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="1"/>
         <v>31</v>
       </c>
-      <c r="B36" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
+      <c r="B36" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C36" s="47"/>
       <c r="E36" s="13"/>
       <c r="F36" s="13"/>
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
       <c r="I36" s="13"/>
     </row>
-    <row r="37" spans="1:26" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="27">
-        <f t="shared" ca="1" si="0"/>
+    <row r="37" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="B37" s="44"/>
+      <c r="C37" s="44"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="44"/>
+      <c r="G37" s="44"/>
+      <c r="H37" s="44"/>
+      <c r="I37" s="44"/>
+      <c r="J37" s="26"/>
+      <c r="K37" s="26"/>
+      <c r="L37" s="26"/>
+      <c r="M37" s="26"/>
+      <c r="N37" s="26"/>
+      <c r="O37" s="26"/>
+      <c r="P37" s="26"/>
+      <c r="Q37" s="26"/>
+      <c r="R37" s="26"/>
+      <c r="S37" s="26"/>
+      <c r="T37" s="26"/>
+      <c r="U37" s="26"/>
+      <c r="V37" s="26"/>
+      <c r="W37" s="26"/>
+      <c r="X37" s="26"/>
+      <c r="Y37" s="26"/>
+      <c r="Z37" s="26"/>
+    </row>
+    <row r="38" spans="1:26" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="27">
+        <f ca="1">IF(OFFSET(A38,-2,0) ="",OFFSET(A38,-2,0)+1,OFFSET(A38,-2,0)+1 )</f>
         <v>32</v>
       </c>
-      <c r="B37" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-    </row>
-    <row r="38" spans="1:26" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="27">
-        <f t="shared" ca="1" si="0"/>
-        <v>33</v>
-      </c>
       <c r="B38" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="C38" s="13"/>
+        <v>132</v>
+      </c>
+      <c r="C38" s="46"/>
       <c r="D38" s="13"/>
       <c r="E38" s="13"/>
       <c r="F38" s="13"/>
@@ -14957,15 +15058,15 @@
       <c r="H38" s="13"/>
       <c r="I38" s="13"/>
     </row>
-    <row r="39" spans="1:26" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="27">
-        <f t="shared" ca="1" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="B39" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="C39" s="13"/>
+        <f ca="1">IF(OFFSET(A39,-1,0) ="",OFFSET(A39,-2,0)+1,OFFSET(A39,-1,0)+1 )</f>
+        <v>33</v>
+      </c>
+      <c r="B39" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="C39" s="46"/>
       <c r="D39" s="13"/>
       <c r="E39" s="13"/>
       <c r="F39" s="13"/>
@@ -14973,15 +15074,15 @@
       <c r="H39" s="13"/>
       <c r="I39" s="13"/>
     </row>
-    <row r="40" spans="1:26" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="27">
-        <f t="shared" ca="1" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="B40" s="29" t="s">
-        <v>132</v>
-      </c>
-      <c r="C40" s="13"/>
+        <f ca="1">IF(OFFSET(A40,-1,0) ="",OFFSET(A40,-2,0)+1,OFFSET(A40,-1,0)+1 )</f>
+        <v>34</v>
+      </c>
+      <c r="B40" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="C40" s="46"/>
       <c r="D40" s="13"/>
       <c r="E40" s="13"/>
       <c r="F40" s="13"/>
@@ -14989,15 +15090,15 @@
       <c r="H40" s="13"/>
       <c r="I40" s="13"/>
     </row>
-    <row r="41" spans="1:26" s="10" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B41" s="29" t="s">
-        <v>147</v>
-      </c>
-      <c r="C41" s="13"/>
+        <v>133</v>
+      </c>
+      <c r="C41" s="46"/>
       <c r="D41" s="13"/>
       <c r="E41" s="13"/>
       <c r="F41" s="13"/>
@@ -15005,15 +15106,15 @@
       <c r="H41" s="13"/>
       <c r="I41" s="13"/>
     </row>
-    <row r="42" spans="1:26" s="10" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B42" s="29" t="s">
-        <v>148</v>
-      </c>
-      <c r="C42" s="13"/>
+        <v>134</v>
+      </c>
+      <c r="C42" s="46"/>
       <c r="D42" s="13"/>
       <c r="E42" s="13"/>
       <c r="F42" s="13"/>
@@ -15021,15 +15122,15 @@
       <c r="H42" s="13"/>
       <c r="I42" s="13"/>
     </row>
-    <row r="43" spans="1:26" s="10" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B43" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="C43" s="13"/>
+        <v>136</v>
+      </c>
+      <c r="C43" s="46"/>
       <c r="D43" s="13"/>
       <c r="E43" s="13"/>
       <c r="F43" s="13"/>
@@ -15037,15 +15138,15 @@
       <c r="H43" s="13"/>
       <c r="I43" s="13"/>
     </row>
-    <row r="44" spans="1:26" s="10" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B44" s="29" t="s">
-        <v>178</v>
-      </c>
-      <c r="C44" s="13"/>
+        <v>130</v>
+      </c>
+      <c r="C44" s="46"/>
       <c r="D44" s="13"/>
       <c r="E44" s="13"/>
       <c r="F44" s="13"/>
@@ -15053,15 +15154,15 @@
       <c r="H44" s="13"/>
       <c r="I44" s="13"/>
     </row>
-    <row r="45" spans="1:26" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" s="10" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="B45" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="C45" s="13"/>
+        <v>39</v>
+      </c>
+      <c r="B45" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="C45" s="46"/>
       <c r="D45" s="13"/>
       <c r="E45" s="13"/>
       <c r="F45" s="13"/>
@@ -15069,15 +15170,15 @@
       <c r="H45" s="13"/>
       <c r="I45" s="13"/>
     </row>
-    <row r="46" spans="1:26" s="10" customFormat="1" ht="25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" s="10" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="B46" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="C46" s="13"/>
+        <v>40</v>
+      </c>
+      <c r="B46" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="C46" s="46"/>
       <c r="D46" s="13"/>
       <c r="E46" s="13"/>
       <c r="F46" s="13"/>
@@ -15085,41 +15186,47 @@
       <c r="H46" s="13"/>
       <c r="I46" s="13"/>
     </row>
-    <row r="47" spans="1:26" s="10" customFormat="1" ht="21.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="44" t="s">
-        <v>153</v>
-      </c>
-      <c r="B47" s="43"/>
-      <c r="C47" s="43"/>
-      <c r="D47" s="43"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="43"/>
-      <c r="G47" s="43"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="43"/>
-    </row>
-    <row r="48" spans="1:26" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" s="10" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B47" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="C47" s="46"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="13"/>
+    </row>
+    <row r="48" spans="1:26" s="10" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="27">
+        <f t="shared" ca="1" si="0"/>
         <v>42</v>
       </c>
-      <c r="B48" s="30" t="s">
-        <v>152</v>
-      </c>
+      <c r="B48" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="C48" s="46"/>
+      <c r="D48" s="13"/>
       <c r="E48" s="13"/>
       <c r="F48" s="13"/>
       <c r="G48" s="13"/>
       <c r="H48" s="13"/>
       <c r="I48" s="13"/>
     </row>
-    <row r="49" spans="1:9" s="10" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" s="10" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>43</v>
       </c>
-      <c r="B49" s="30" t="s">
-        <v>154</v>
-      </c>
-      <c r="C49" s="13"/>
+      <c r="B49" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="C49" s="46"/>
       <c r="D49" s="13"/>
       <c r="E49" s="13"/>
       <c r="F49" s="13"/>
@@ -15127,15 +15234,15 @@
       <c r="H49" s="13"/>
       <c r="I49" s="13"/>
     </row>
-    <row r="50" spans="1:9" s="10" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>44</v>
       </c>
       <c r="B50" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="C50" s="13"/>
+        <v>145</v>
+      </c>
+      <c r="C50" s="46"/>
       <c r="D50" s="13"/>
       <c r="E50" s="13"/>
       <c r="F50" s="13"/>
@@ -15143,15 +15250,15 @@
       <c r="H50" s="13"/>
       <c r="I50" s="13"/>
     </row>
-    <row r="51" spans="1:9" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" s="10" customFormat="1" ht="24.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>45</v>
       </c>
-      <c r="B51" s="30" t="s">
-        <v>156</v>
-      </c>
-      <c r="C51" s="13"/>
+      <c r="B51" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C51" s="46"/>
       <c r="D51" s="13"/>
       <c r="E51" s="13"/>
       <c r="F51" s="13"/>
@@ -15159,43 +15266,43 @@
       <c r="H51" s="13"/>
       <c r="I51" s="13"/>
     </row>
-    <row r="52" spans="1:9" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="27">
+    <row r="52" spans="1:9" s="10" customFormat="1" ht="21.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="43" t="s">
+        <v>148</v>
+      </c>
+      <c r="B52" s="44"/>
+      <c r="C52" s="44"/>
+      <c r="D52" s="44"/>
+      <c r="E52" s="44"/>
+      <c r="F52" s="44"/>
+      <c r="G52" s="44"/>
+      <c r="H52" s="44"/>
+      <c r="I52" s="44"/>
+    </row>
+    <row r="53" spans="1:9" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="27">
+        <f ca="1">IF(OFFSET(A53,-2,0) ="",OFFSET(A53,-2,0)+1,OFFSET(A53,-2,0)+1 )</f>
+        <v>46</v>
+      </c>
+      <c r="B53" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="C53" s="47"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="13"/>
+    </row>
+    <row r="54" spans="1:9" s="10" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="B52" s="30" t="s">
-        <v>157</v>
-      </c>
-      <c r="C52" s="13"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="13"/>
-      <c r="F52" s="13"/>
-      <c r="G52" s="13"/>
-      <c r="H52" s="13"/>
-      <c r="I52" s="13"/>
-    </row>
-    <row r="53" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="44" t="s">
-        <v>160</v>
-      </c>
-      <c r="B53" s="43"/>
-      <c r="C53" s="43"/>
-      <c r="D53" s="43"/>
-      <c r="E53" s="43"/>
-      <c r="F53" s="43"/>
-      <c r="G53" s="43"/>
-      <c r="H53" s="43"/>
-      <c r="I53" s="43"/>
-    </row>
-    <row r="54" spans="1:9" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="27">
         <v>47</v>
       </c>
       <c r="B54" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="C54" s="13"/>
+        <v>149</v>
+      </c>
+      <c r="C54" s="46"/>
       <c r="D54" s="13"/>
       <c r="E54" s="13"/>
       <c r="F54" s="13"/>
@@ -15203,15 +15310,15 @@
       <c r="H54" s="13"/>
       <c r="I54" s="13"/>
     </row>
-    <row r="55" spans="1:9" s="10" customFormat="1" ht="25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" s="10" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>48</v>
       </c>
       <c r="B55" s="30" t="s">
-        <v>154</v>
-      </c>
-      <c r="C55" s="13"/>
+        <v>150</v>
+      </c>
+      <c r="C55" s="46"/>
       <c r="D55" s="13"/>
       <c r="E55" s="13"/>
       <c r="F55" s="13"/>
@@ -15219,15 +15326,15 @@
       <c r="H55" s="13"/>
       <c r="I55" s="13"/>
     </row>
-    <row r="56" spans="1:9" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>49</v>
       </c>
       <c r="B56" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="C56" s="13"/>
+        <v>151</v>
+      </c>
+      <c r="C56" s="46"/>
       <c r="D56" s="13"/>
       <c r="E56" s="13"/>
       <c r="F56" s="13"/>
@@ -15235,15 +15342,15 @@
       <c r="H56" s="13"/>
       <c r="I56" s="13"/>
     </row>
-    <row r="57" spans="1:9" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>50</v>
       </c>
       <c r="B57" s="30" t="s">
-        <v>159</v>
-      </c>
-      <c r="C57" s="13"/>
+        <v>152</v>
+      </c>
+      <c r="C57" s="46"/>
       <c r="D57" s="13"/>
       <c r="E57" s="13"/>
       <c r="F57" s="13"/>
@@ -15252,26 +15359,28 @@
       <c r="I57" s="13"/>
     </row>
     <row r="58" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="B58" s="43"/>
-      <c r="C58" s="43"/>
-      <c r="D58" s="43"/>
-      <c r="E58" s="43"/>
-      <c r="F58" s="43"/>
-      <c r="G58" s="43"/>
-      <c r="H58" s="43"/>
-      <c r="I58" s="43"/>
-    </row>
-    <row r="59" spans="1:9" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="B58" s="44"/>
+      <c r="C58" s="44"/>
+      <c r="D58" s="44"/>
+      <c r="E58" s="44"/>
+      <c r="F58" s="44"/>
+      <c r="G58" s="44"/>
+      <c r="H58" s="44"/>
+      <c r="I58" s="44"/>
+    </row>
+    <row r="59" spans="1:9" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="27">
+        <f ca="1">IF(OFFSET(A59,-2,0) ="",OFFSET(A59,-2,0)+1,OFFSET(A59,-2,0)+1 )</f>
         <v>51</v>
       </c>
       <c r="B59" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="C59" s="13"/>
+        <v>147</v>
+      </c>
+      <c r="C59" s="46"/>
+      <c r="D59" s="13"/>
       <c r="E59" s="13"/>
       <c r="F59" s="13"/>
       <c r="G59" s="13"/>
@@ -15284,40 +15393,41 @@
         <v>52</v>
       </c>
       <c r="B60" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="C60" s="13"/>
+        <v>149</v>
+      </c>
+      <c r="C60" s="46"/>
+      <c r="D60" s="13"/>
       <c r="E60" s="13"/>
       <c r="F60" s="13"/>
       <c r="G60" s="13"/>
       <c r="H60" s="13"/>
       <c r="I60" s="13"/>
     </row>
-    <row r="61" spans="1:9" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>53</v>
       </c>
-      <c r="B61" s="29" t="s">
-        <v>162</v>
-      </c>
-      <c r="C61" s="13"/>
-      <c r="D61" s="30"/>
+      <c r="B61" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="C61" s="46"/>
+      <c r="D61" s="13"/>
       <c r="E61" s="13"/>
       <c r="F61" s="13"/>
       <c r="G61" s="13"/>
       <c r="H61" s="13"/>
       <c r="I61" s="13"/>
     </row>
-    <row r="62" spans="1:9" s="10" customFormat="1" ht="25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>54</v>
       </c>
-      <c r="B62" s="29" t="s">
-        <v>164</v>
-      </c>
-      <c r="C62" s="13"/>
+      <c r="B62" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="C62" s="46"/>
       <c r="D62" s="13"/>
       <c r="E62" s="13"/>
       <c r="F62" s="13"/>
@@ -15325,79 +15435,74 @@
       <c r="H62" s="13"/>
       <c r="I62" s="13"/>
     </row>
-    <row r="63" spans="1:9" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="27">
-        <f t="shared" ca="1" si="0"/>
+    <row r="63" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="43" t="s">
+        <v>156</v>
+      </c>
+      <c r="B63" s="44"/>
+      <c r="C63" s="44"/>
+      <c r="D63" s="44"/>
+      <c r="E63" s="44"/>
+      <c r="F63" s="44"/>
+      <c r="G63" s="44"/>
+      <c r="H63" s="44"/>
+      <c r="I63" s="44"/>
+    </row>
+    <row r="64" spans="1:9" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="27">
+        <f ca="1">IF(OFFSET(A64,-2,0) ="",OFFSET(A64,-2,0)+1,OFFSET(A64,-2,0)+1 )</f>
         <v>55</v>
       </c>
-      <c r="B63" s="29" t="s">
-        <v>163</v>
-      </c>
-      <c r="C63" s="13"/>
-      <c r="D63" s="13"/>
-      <c r="E63" s="13"/>
-      <c r="F63" s="13"/>
-      <c r="G63" s="13"/>
-      <c r="H63" s="13"/>
-      <c r="I63" s="13"/>
-    </row>
-    <row r="64" spans="1:9" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="27">
-        <f t="shared" ca="1" si="0"/>
-        <v>56</v>
-      </c>
-      <c r="B64" s="29" t="s">
-        <v>132</v>
-      </c>
-      <c r="C64" s="13"/>
-      <c r="D64" s="13"/>
+      <c r="B64" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="C64" s="46"/>
       <c r="E64" s="13"/>
       <c r="F64" s="13"/>
       <c r="G64" s="13"/>
       <c r="H64" s="13"/>
       <c r="I64" s="13"/>
     </row>
-    <row r="65" spans="1:9" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" s="10" customFormat="1" ht="25" x14ac:dyDescent="0.25">
       <c r="A65" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="B65" s="29" t="s">
-        <v>147</v>
-      </c>
-      <c r="C65" s="13"/>
-      <c r="D65" s="13"/>
+        <v>56</v>
+      </c>
+      <c r="B65" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="C65" s="46"/>
       <c r="E65" s="13"/>
       <c r="F65" s="13"/>
       <c r="G65" s="13"/>
       <c r="H65" s="13"/>
       <c r="I65" s="13"/>
     </row>
-    <row r="66" spans="1:9" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B66" s="29" t="s">
-        <v>148</v>
-      </c>
-      <c r="C66" s="13"/>
-      <c r="D66" s="13"/>
+        <v>157</v>
+      </c>
+      <c r="C66" s="46"/>
+      <c r="D66" s="30"/>
       <c r="E66" s="13"/>
       <c r="F66" s="13"/>
       <c r="G66" s="13"/>
       <c r="H66" s="13"/>
       <c r="I66" s="13"/>
     </row>
-    <row r="67" spans="1:9" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" s="10" customFormat="1" ht="25" x14ac:dyDescent="0.25">
       <c r="A67" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B67" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="C67" s="13"/>
+        <v>159</v>
+      </c>
+      <c r="C67" s="46"/>
       <c r="D67" s="13"/>
       <c r="E67" s="13"/>
       <c r="F67" s="13"/>
@@ -15405,15 +15510,15 @@
       <c r="H67" s="13"/>
       <c r="I67" s="13"/>
     </row>
-    <row r="68" spans="1:9" s="10" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="B68" s="30" t="s">
-        <v>165</v>
-      </c>
-      <c r="C68" s="13"/>
+        <v>59</v>
+      </c>
+      <c r="B68" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="C68" s="46"/>
       <c r="D68" s="13"/>
       <c r="E68" s="13"/>
       <c r="F68" s="13"/>
@@ -15421,15 +15526,15 @@
       <c r="H68" s="13"/>
       <c r="I68" s="13"/>
     </row>
-    <row r="69" spans="1:9" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
-      </c>
-      <c r="B69" s="30" t="s">
-        <v>166</v>
-      </c>
-      <c r="C69" s="13"/>
+        <v>60</v>
+      </c>
+      <c r="B69" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="C69" s="46"/>
       <c r="D69" s="13"/>
       <c r="E69" s="13"/>
       <c r="F69" s="13"/>
@@ -15437,15 +15542,15 @@
       <c r="H69" s="13"/>
       <c r="I69" s="13"/>
     </row>
-    <row r="70" spans="1:9" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B70" s="29" t="s">
-        <v>178</v>
-      </c>
-      <c r="C70" s="13"/>
+        <v>143</v>
+      </c>
+      <c r="C70" s="46"/>
       <c r="D70" s="13"/>
       <c r="E70" s="13"/>
       <c r="F70" s="13"/>
@@ -15453,15 +15558,15 @@
       <c r="H70" s="13"/>
       <c r="I70" s="13"/>
     </row>
-    <row r="71" spans="1:9" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
-      </c>
-      <c r="B71" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="C71" s="13"/>
+        <v>62</v>
+      </c>
+      <c r="B71" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="C71" s="46"/>
       <c r="D71" s="13"/>
       <c r="E71" s="13"/>
       <c r="F71" s="13"/>
@@ -15469,27 +15574,31 @@
       <c r="H71" s="13"/>
       <c r="I71" s="13"/>
     </row>
-    <row r="72" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="44" t="s">
-        <v>167</v>
-      </c>
-      <c r="B72" s="43"/>
-      <c r="C72" s="43"/>
-      <c r="D72" s="43"/>
-      <c r="E72" s="43"/>
-      <c r="F72" s="43"/>
-      <c r="G72" s="43"/>
-      <c r="H72" s="43"/>
-      <c r="I72" s="43"/>
-    </row>
-    <row r="73" spans="1:9" s="10" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="B72" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="C72" s="46"/>
+      <c r="D72" s="13"/>
+      <c r="E72" s="13"/>
+      <c r="F72" s="13"/>
+      <c r="G72" s="13"/>
+      <c r="H72" s="13"/>
+      <c r="I72" s="13"/>
+    </row>
+    <row r="73" spans="1:26" s="10" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="27">
-        <v>63</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>64</v>
       </c>
       <c r="B73" s="30" t="s">
-        <v>168</v>
-      </c>
-      <c r="C73" s="13"/>
+        <v>160</v>
+      </c>
+      <c r="C73" s="46"/>
       <c r="D73" s="13"/>
       <c r="E73" s="13"/>
       <c r="F73" s="13"/>
@@ -15497,15 +15606,15 @@
       <c r="H73" s="13"/>
       <c r="I73" s="13"/>
     </row>
-    <row r="74" spans="1:9" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="27">
-        <f t="shared" ref="A74:A98" ca="1" si="1">IF(OFFSET(A74,-1,0) ="",OFFSET(A74,-2,0)+1,OFFSET(A74,-1,0)+1 )</f>
-        <v>64</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>65</v>
       </c>
       <c r="B74" s="30" t="s">
-        <v>169</v>
-      </c>
-      <c r="C74" s="13"/>
+        <v>161</v>
+      </c>
+      <c r="C74" s="46"/>
       <c r="D74" s="13"/>
       <c r="E74" s="13"/>
       <c r="F74" s="13"/>
@@ -15513,59 +15622,74 @@
       <c r="H74" s="13"/>
       <c r="I74" s="13"/>
     </row>
-    <row r="75" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="44" t="s">
-        <v>170</v>
-      </c>
-      <c r="B75" s="43"/>
-      <c r="C75" s="43"/>
-      <c r="D75" s="43"/>
-      <c r="E75" s="43"/>
-      <c r="F75" s="43"/>
-      <c r="G75" s="43"/>
-      <c r="H75" s="43"/>
-      <c r="I75" s="43"/>
-    </row>
-    <row r="76" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="27">
-        <v>65</v>
-      </c>
-      <c r="B76" s="30" t="s">
-        <v>171</v>
-      </c>
-      <c r="C76" s="13"/>
-      <c r="D76" s="13"/>
-      <c r="E76" s="13"/>
-      <c r="F76" s="13"/>
-      <c r="G76" s="13"/>
-      <c r="H76" s="13"/>
-      <c r="I76" s="13"/>
-    </row>
-    <row r="77" spans="1:9" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="27">
-        <f t="shared" ca="1" si="1"/>
+    <row r="75" spans="1:26" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="27">
+        <f t="shared" ca="1" si="0"/>
         <v>66</v>
       </c>
-      <c r="B77" s="30" t="s">
-        <v>172</v>
-      </c>
-      <c r="C77" s="13"/>
-      <c r="D77" s="13"/>
-      <c r="E77" s="13"/>
-      <c r="F77" s="13"/>
-      <c r="G77" s="13"/>
-      <c r="H77" s="13"/>
-      <c r="I77" s="13"/>
-    </row>
-    <row r="78" spans="1:9" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C75" s="46"/>
+      <c r="D75" s="13"/>
+      <c r="E75" s="13"/>
+      <c r="F75" s="13"/>
+      <c r="G75" s="13"/>
+      <c r="H75" s="13"/>
+      <c r="I75" s="13"/>
+    </row>
+    <row r="76" spans="1:26" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="B76" s="42"/>
+      <c r="C76" s="42"/>
+      <c r="D76" s="42"/>
+      <c r="E76" s="42"/>
+      <c r="F76" s="42"/>
+      <c r="G76" s="42"/>
+      <c r="H76" s="42"/>
+      <c r="I76" s="42"/>
+    </row>
+    <row r="77" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="43" t="s">
+        <v>178</v>
+      </c>
+      <c r="B77" s="44"/>
+      <c r="C77" s="44"/>
+      <c r="D77" s="44"/>
+      <c r="E77" s="44"/>
+      <c r="F77" s="44"/>
+      <c r="G77" s="44"/>
+      <c r="H77" s="44"/>
+      <c r="I77" s="44"/>
+      <c r="J77" s="26"/>
+      <c r="K77" s="26"/>
+      <c r="L77" s="26"/>
+      <c r="M77" s="26"/>
+      <c r="N77" s="26"/>
+      <c r="O77" s="26"/>
+      <c r="P77" s="26"/>
+      <c r="Q77" s="26"/>
+      <c r="R77" s="26"/>
+      <c r="S77" s="26"/>
+      <c r="T77" s="26"/>
+      <c r="U77" s="26"/>
+      <c r="V77" s="26"/>
+      <c r="W77" s="26"/>
+      <c r="X77" s="26"/>
+      <c r="Y77" s="26"/>
+      <c r="Z77" s="26"/>
+    </row>
+    <row r="78" spans="1:26" s="10" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="27">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">IF(OFFSET(A78,-3,0) ="",OFFSET(A78,-3,0)+1,OFFSET(A78,-3,0)+1 )</f>
         <v>67</v>
       </c>
       <c r="B78" s="30" t="s">
-        <v>173</v>
-      </c>
-      <c r="C78" s="13"/>
+        <v>121</v>
+      </c>
+      <c r="C78" s="47"/>
       <c r="D78" s="13"/>
       <c r="E78" s="13"/>
       <c r="F78" s="13"/>
@@ -15573,15 +15697,15 @@
       <c r="H78" s="13"/>
       <c r="I78" s="13"/>
     </row>
-    <row r="79" spans="1:9" s="10" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="27">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">IF(OFFSET(A79,-1,0) ="",OFFSET(A79,-2,0)+1,OFFSET(A79,-1,0)+1 )</f>
         <v>68</v>
       </c>
-      <c r="B79" s="30" t="s">
-        <v>174</v>
-      </c>
-      <c r="C79" s="13"/>
+      <c r="B79" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="C79" s="46"/>
       <c r="D79" s="13"/>
       <c r="E79" s="13"/>
       <c r="F79" s="13"/>
@@ -15589,15 +15713,15 @@
       <c r="H79" s="13"/>
       <c r="I79" s="13"/>
     </row>
-    <row r="80" spans="1:9" s="10" customFormat="1" ht="21.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:26" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="27">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">IF(OFFSET(A80,-1,0) ="",OFFSET(A80,-2,0)+1,OFFSET(A80,-1,0)+1 )</f>
         <v>69</v>
       </c>
-      <c r="B80" s="30" t="s">
-        <v>175</v>
-      </c>
-      <c r="C80" s="13"/>
+      <c r="B80" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="C80" s="46"/>
       <c r="D80" s="13"/>
       <c r="E80" s="13"/>
       <c r="F80" s="13"/>
@@ -15605,31 +15729,28 @@
       <c r="H80" s="13"/>
       <c r="I80" s="13"/>
     </row>
-    <row r="81" spans="1:9" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="27">
-        <f t="shared" ca="1" si="1"/>
+    <row r="81" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="43" t="s">
+        <v>162</v>
+      </c>
+      <c r="B81" s="44"/>
+      <c r="C81" s="44"/>
+      <c r="D81" s="44"/>
+      <c r="E81" s="44"/>
+      <c r="F81" s="44"/>
+      <c r="G81" s="44"/>
+      <c r="H81" s="44"/>
+      <c r="I81" s="44"/>
+    </row>
+    <row r="82" spans="1:9" s="10" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="27">
+        <f ca="1">IF(OFFSET(A82,-2,0) ="",OFFSET(A82,-2,0)+1,OFFSET(A82,-2,0)+1 )</f>
         <v>70</v>
       </c>
-      <c r="B81" s="30" t="s">
-        <v>176</v>
-      </c>
-      <c r="C81" s="13"/>
-      <c r="D81" s="13"/>
-      <c r="E81" s="13"/>
-      <c r="F81" s="13"/>
-      <c r="G81" s="13"/>
-      <c r="H81" s="13"/>
-      <c r="I81" s="13"/>
-    </row>
-    <row r="82" spans="1:9" s="10" customFormat="1" ht="24.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>71</v>
-      </c>
       <c r="B82" s="30" t="s">
-        <v>177</v>
-      </c>
-      <c r="C82" s="13"/>
+        <v>163</v>
+      </c>
+      <c r="C82" s="46"/>
       <c r="D82" s="13"/>
       <c r="E82" s="13"/>
       <c r="F82" s="13"/>
@@ -15637,39 +15758,44 @@
       <c r="H82" s="13"/>
       <c r="I82" s="13"/>
     </row>
-    <row r="83" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="35" t="s">
-        <v>179</v>
-      </c>
-      <c r="B83" s="42"/>
-      <c r="C83" s="42"/>
-      <c r="D83" s="42"/>
-      <c r="E83" s="42"/>
-      <c r="F83" s="42"/>
-      <c r="G83" s="42"/>
-      <c r="H83" s="42"/>
-      <c r="I83" s="42"/>
-    </row>
-    <row r="84" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="27">
+    <row r="83" spans="1:9" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="27">
+        <f t="shared" ref="A83" ca="1" si="2">IF(OFFSET(A83,-1,0) ="",OFFSET(A83,-2,0)+1,OFFSET(A83,-1,0)+1 )</f>
+        <v>71</v>
+      </c>
+      <c r="B83" s="30" t="s">
+        <v>164</v>
+      </c>
+      <c r="C83" s="46"/>
+      <c r="D83" s="13"/>
+      <c r="E83" s="13"/>
+      <c r="F83" s="13"/>
+      <c r="G83" s="13"/>
+      <c r="H83" s="13"/>
+      <c r="I83" s="13"/>
+    </row>
+    <row r="84" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="43" t="s">
+        <v>165</v>
+      </c>
+      <c r="B84" s="44"/>
+      <c r="C84" s="44"/>
+      <c r="D84" s="44"/>
+      <c r="E84" s="44"/>
+      <c r="F84" s="44"/>
+      <c r="G84" s="44"/>
+      <c r="H84" s="44"/>
+      <c r="I84" s="44"/>
+    </row>
+    <row r="85" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="27">
+        <f ca="1">IF(OFFSET(A85,-2,0) ="",OFFSET(A85,-2,0)+1,OFFSET(A85,-2,0)+1 )</f>
         <v>72</v>
       </c>
-      <c r="B84" s="30"/>
-      <c r="C84" s="13"/>
-      <c r="D84" s="13"/>
-      <c r="E84" s="13"/>
-      <c r="F84" s="13"/>
-      <c r="G84" s="13"/>
-      <c r="H84" s="13"/>
-      <c r="I84" s="13"/>
-    </row>
-    <row r="85" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>73</v>
-      </c>
-      <c r="B85" s="30"/>
-      <c r="C85" s="13"/>
+      <c r="B85" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="C85" s="46"/>
       <c r="D85" s="13"/>
       <c r="E85" s="13"/>
       <c r="F85" s="13"/>
@@ -15677,27 +15803,28 @@
       <c r="H85" s="13"/>
       <c r="I85" s="13"/>
     </row>
-    <row r="86" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>74</v>
-      </c>
-      <c r="B86" s="30"/>
-      <c r="C86" s="13"/>
-      <c r="D86" s="13"/>
-      <c r="E86" s="13"/>
-      <c r="F86" s="13"/>
-      <c r="G86" s="13"/>
-      <c r="H86" s="13"/>
-      <c r="I86" s="13"/>
-    </row>
-    <row r="87" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="43" t="s">
+        <v>194</v>
+      </c>
+      <c r="B86" s="44"/>
+      <c r="C86" s="44"/>
+      <c r="D86" s="44"/>
+      <c r="E86" s="44"/>
+      <c r="F86" s="44"/>
+      <c r="G86" s="44"/>
+      <c r="H86" s="44"/>
+      <c r="I86" s="44"/>
+    </row>
+    <row r="87" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>75</v>
-      </c>
-      <c r="B87" s="30"/>
-      <c r="C87" s="13"/>
+        <f ca="1">IF(OFFSET(A87,-2,0) ="",OFFSET(A87,-2,0)+1,OFFSET(A87,-2,0)+1 )</f>
+        <v>73</v>
+      </c>
+      <c r="B87" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="C87" s="46"/>
       <c r="D87" s="13"/>
       <c r="E87" s="13"/>
       <c r="F87" s="13"/>
@@ -15705,27 +15832,28 @@
       <c r="H87" s="13"/>
       <c r="I87" s="13"/>
     </row>
-    <row r="88" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>76</v>
-      </c>
-      <c r="B88" s="30"/>
-      <c r="C88" s="13"/>
-      <c r="D88" s="13"/>
-      <c r="E88" s="13"/>
-      <c r="F88" s="13"/>
-      <c r="G88" s="13"/>
-      <c r="H88" s="13"/>
-      <c r="I88" s="13"/>
-    </row>
-    <row r="89" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="43" t="s">
+        <v>198</v>
+      </c>
+      <c r="B88" s="44"/>
+      <c r="C88" s="44"/>
+      <c r="D88" s="44"/>
+      <c r="E88" s="44"/>
+      <c r="F88" s="44"/>
+      <c r="G88" s="44"/>
+      <c r="H88" s="44"/>
+      <c r="I88" s="44"/>
+    </row>
+    <row r="89" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>77</v>
-      </c>
-      <c r="B89" s="30"/>
-      <c r="C89" s="13"/>
+        <f ca="1">IF(OFFSET(A89,-2,0) ="",OFFSET(A89,-2,0)+1,OFFSET(A89,-2,0)+1 )</f>
+        <v>74</v>
+      </c>
+      <c r="B89" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="C89" s="46"/>
       <c r="D89" s="13"/>
       <c r="E89" s="13"/>
       <c r="F89" s="13"/>
@@ -15733,27 +15861,28 @@
       <c r="H89" s="13"/>
       <c r="I89" s="13"/>
     </row>
-    <row r="90" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>78</v>
-      </c>
-      <c r="B90" s="30"/>
-      <c r="C90" s="13"/>
-      <c r="D90" s="13"/>
-      <c r="E90" s="13"/>
-      <c r="F90" s="13"/>
-      <c r="G90" s="13"/>
-      <c r="H90" s="13"/>
-      <c r="I90" s="13"/>
-    </row>
-    <row r="91" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="43" t="s">
+        <v>175</v>
+      </c>
+      <c r="B90" s="44"/>
+      <c r="C90" s="44"/>
+      <c r="D90" s="44"/>
+      <c r="E90" s="44"/>
+      <c r="F90" s="44"/>
+      <c r="G90" s="44"/>
+      <c r="H90" s="44"/>
+      <c r="I90" s="44"/>
+    </row>
+    <row r="91" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>79</v>
-      </c>
-      <c r="B91" s="30"/>
-      <c r="C91" s="13"/>
+        <f ca="1">IF(OFFSET(A91,-2,0) ="",OFFSET(A91,-2,0)+1,OFFSET(A91,-2,0)+1 )</f>
+        <v>75</v>
+      </c>
+      <c r="B91" s="30" t="s">
+        <v>179</v>
+      </c>
+      <c r="C91" s="46"/>
       <c r="D91" s="13"/>
       <c r="E91" s="13"/>
       <c r="F91" s="13"/>
@@ -15761,13 +15890,15 @@
       <c r="H91" s="13"/>
       <c r="I91" s="13"/>
     </row>
-    <row r="92" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>80</v>
-      </c>
-      <c r="B92" s="30"/>
-      <c r="C92" s="13"/>
+        <f ca="1">IF(OFFSET(A92,-1,0) ="",OFFSET(A92,-2,0)+1,OFFSET(A92,-1,0)+1 )</f>
+        <v>76</v>
+      </c>
+      <c r="B92" s="30" t="s">
+        <v>183</v>
+      </c>
+      <c r="C92" s="46"/>
       <c r="D92" s="13"/>
       <c r="E92" s="13"/>
       <c r="F92" s="13"/>
@@ -15775,13 +15906,15 @@
       <c r="H92" s="13"/>
       <c r="I92" s="13"/>
     </row>
-    <row r="93" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>81</v>
-      </c>
-      <c r="B93" s="30"/>
-      <c r="C93" s="13"/>
+        <f ca="1">IF(OFFSET(A93,-1,0) ="",OFFSET(A93,-2,0)+1,OFFSET(A93,-1,0)+1 )</f>
+        <v>77</v>
+      </c>
+      <c r="B93" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="C93" s="46"/>
       <c r="D93" s="13"/>
       <c r="E93" s="13"/>
       <c r="F93" s="13"/>
@@ -15789,55 +15922,65 @@
       <c r="H93" s="13"/>
       <c r="I93" s="13"/>
     </row>
-    <row r="94" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>82</v>
-      </c>
-      <c r="B94" s="30"/>
-      <c r="C94" s="13"/>
-      <c r="D94" s="13"/>
+        <f ca="1">IF(OFFSET(A94,-1,0) ="",OFFSET(A94,-2,0)+1,OFFSET(A94,-1,0)+1 )</f>
+        <v>78</v>
+      </c>
+      <c r="B94" s="30" t="s">
+        <v>184</v>
+      </c>
+      <c r="C94" s="46" t="s">
+        <v>181</v>
+      </c>
+      <c r="D94" s="30"/>
       <c r="E94" s="13"/>
       <c r="F94" s="13"/>
       <c r="G94" s="13"/>
       <c r="H94" s="13"/>
       <c r="I94" s="13"/>
     </row>
-    <row r="95" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" s="10" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>83</v>
-      </c>
-      <c r="B95" s="30"/>
-      <c r="C95" s="13"/>
-      <c r="D95" s="13"/>
+        <f ca="1">IF(OFFSET(A95,-1,0) ="",OFFSET(A95,-2,0)+1,OFFSET(A95,-1,0)+1 )</f>
+        <v>79</v>
+      </c>
+      <c r="B95" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="C95" s="46"/>
+      <c r="D95" s="30"/>
       <c r="E95" s="13"/>
       <c r="F95" s="13"/>
       <c r="G95" s="13"/>
       <c r="H95" s="13"/>
       <c r="I95" s="13"/>
     </row>
-    <row r="96" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>84</v>
-      </c>
-      <c r="B96" s="30"/>
-      <c r="C96" s="13"/>
-      <c r="D96" s="13"/>
+        <f ca="1">IF(OFFSET(A96,-1,0) ="",OFFSET(A96,-2,0)+1,OFFSET(A96,-1,0)+1 )</f>
+        <v>80</v>
+      </c>
+      <c r="B96" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="C96" s="46"/>
+      <c r="D96" s="30"/>
       <c r="E96" s="13"/>
       <c r="F96" s="13"/>
       <c r="G96" s="13"/>
       <c r="H96" s="13"/>
       <c r="I96" s="13"/>
     </row>
-    <row r="97" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>85</v>
-      </c>
-      <c r="B97" s="30"/>
-      <c r="C97" s="13"/>
+        <f ca="1">IF(OFFSET(A97,-1,0) ="",OFFSET(A97,-2,0)+1,OFFSET(A97,-1,0)+1 )</f>
+        <v>81</v>
+      </c>
+      <c r="B97" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="C97" s="46"/>
       <c r="D97" s="13"/>
       <c r="E97" s="13"/>
       <c r="F97" s="13"/>
@@ -15845,13 +15988,15 @@
       <c r="H97" s="13"/>
       <c r="I97" s="13"/>
     </row>
-    <row r="98" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>86</v>
-      </c>
-      <c r="B98" s="30"/>
-      <c r="C98" s="13"/>
+        <f ca="1">IF(OFFSET(A98,-1,0) ="",OFFSET(A98,-2,0)+1,OFFSET(A98,-1,0)+1 )</f>
+        <v>82</v>
+      </c>
+      <c r="B98" s="30" t="s">
+        <v>203</v>
+      </c>
+      <c r="C98" s="46"/>
       <c r="D98" s="13"/>
       <c r="E98" s="13"/>
       <c r="F98" s="13"/>
@@ -15859,10 +16004,15 @@
       <c r="H98" s="13"/>
       <c r="I98" s="13"/>
     </row>
-    <row r="99" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="13"/>
-      <c r="B99" s="30"/>
-      <c r="C99" s="13"/>
+    <row r="99" spans="1:9" s="10" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="27">
+        <f ca="1">IF(OFFSET(A99,-1,0) ="",OFFSET(A99,-2,0)+1,OFFSET(A99,-1,0)+1 )</f>
+        <v>83</v>
+      </c>
+      <c r="B99" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="C99" s="46"/>
       <c r="D99" s="13"/>
       <c r="E99" s="13"/>
       <c r="F99" s="13"/>
@@ -15870,21 +16020,28 @@
       <c r="H99" s="13"/>
       <c r="I99" s="13"/>
     </row>
-    <row r="100" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="13"/>
-      <c r="B100" s="30"/>
-      <c r="C100" s="13"/>
-      <c r="D100" s="13"/>
-      <c r="E100" s="13"/>
-      <c r="F100" s="13"/>
-      <c r="G100" s="13"/>
-      <c r="H100" s="13"/>
-      <c r="I100" s="13"/>
-    </row>
-    <row r="101" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="13"/>
-      <c r="B101" s="30"/>
-      <c r="C101" s="13"/>
+    <row r="100" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="43" t="s">
+        <v>204</v>
+      </c>
+      <c r="B100" s="44"/>
+      <c r="C100" s="44"/>
+      <c r="D100" s="44"/>
+      <c r="E100" s="44"/>
+      <c r="F100" s="44"/>
+      <c r="G100" s="44"/>
+      <c r="H100" s="44"/>
+      <c r="I100" s="44"/>
+    </row>
+    <row r="101" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="27">
+        <f ca="1">IF(OFFSET(A101,-2,0) ="",OFFSET(A101,-2,0)+1,OFFSET(A101,-2,0)+1 )</f>
+        <v>84</v>
+      </c>
+      <c r="B101" s="30" t="s">
+        <v>190</v>
+      </c>
+      <c r="C101" s="46"/>
       <c r="D101" s="13"/>
       <c r="E101" s="13"/>
       <c r="F101" s="13"/>
@@ -15892,10 +16049,15 @@
       <c r="H101" s="13"/>
       <c r="I101" s="13"/>
     </row>
-    <row r="102" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="13"/>
-      <c r="B102" s="30"/>
-      <c r="C102" s="13"/>
+    <row r="102" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="27">
+        <f ca="1">IF(OFFSET(A102,-1,0) ="",OFFSET(A102,-2,0)+1,OFFSET(A102,-1,0)+1 )</f>
+        <v>85</v>
+      </c>
+      <c r="B102" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="C102" s="46"/>
       <c r="D102" s="13"/>
       <c r="E102" s="13"/>
       <c r="F102" s="13"/>
@@ -15903,18 +16065,1287 @@
       <c r="H102" s="13"/>
       <c r="I102" s="13"/>
     </row>
+    <row r="103" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="27">
+        <f ca="1">IF(OFFSET(A103,-1,0) ="",OFFSET(A103,-2,0)+1,OFFSET(A103,-1,0)+1 )</f>
+        <v>86</v>
+      </c>
+      <c r="B103" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="C103" s="46"/>
+      <c r="D103" s="13"/>
+      <c r="E103" s="13"/>
+      <c r="F103" s="13"/>
+      <c r="G103" s="13"/>
+      <c r="H103" s="13"/>
+      <c r="I103" s="13"/>
+    </row>
+    <row r="104" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="27">
+        <f ca="1">IF(OFFSET(A104,-1,0) ="",OFFSET(A104,-2,0)+1,OFFSET(A104,-1,0)+1 )</f>
+        <v>87</v>
+      </c>
+      <c r="B104" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="C104" s="46" t="s">
+        <v>181</v>
+      </c>
+      <c r="D104" s="30"/>
+      <c r="E104" s="13"/>
+      <c r="F104" s="13"/>
+      <c r="G104" s="13"/>
+      <c r="H104" s="13"/>
+      <c r="I104" s="13"/>
+    </row>
+    <row r="105" spans="1:9" s="10" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="27">
+        <f ca="1">IF(OFFSET(A105,-1,0) ="",OFFSET(A105,-2,0)+1,OFFSET(A105,-1,0)+1 )</f>
+        <v>88</v>
+      </c>
+      <c r="B105" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="C105" s="46"/>
+      <c r="D105" s="30"/>
+      <c r="E105" s="13"/>
+      <c r="F105" s="13"/>
+      <c r="G105" s="13"/>
+      <c r="H105" s="13"/>
+      <c r="I105" s="13"/>
+    </row>
+    <row r="106" spans="1:9" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="27">
+        <f ca="1">IF(OFFSET(A106,-1,0) ="",OFFSET(A106,-2,0)+1,OFFSET(A106,-1,0)+1 )</f>
+        <v>89</v>
+      </c>
+      <c r="B106" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="C106" s="46"/>
+      <c r="D106" s="30"/>
+      <c r="E106" s="13"/>
+      <c r="F106" s="13"/>
+      <c r="G106" s="13"/>
+      <c r="H106" s="13"/>
+      <c r="I106" s="13"/>
+    </row>
+    <row r="107" spans="1:9" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="27">
+        <f ca="1">IF(OFFSET(A107,-1,0) ="",OFFSET(A107,-2,0)+1,OFFSET(A107,-1,0)+1 )</f>
+        <v>90</v>
+      </c>
+      <c r="B107" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="C107" s="46"/>
+      <c r="D107" s="13"/>
+      <c r="E107" s="13"/>
+      <c r="F107" s="13"/>
+      <c r="G107" s="13"/>
+      <c r="H107" s="13"/>
+      <c r="I107" s="13"/>
+    </row>
+    <row r="108" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="27">
+        <f ca="1">IF(OFFSET(A108,-1,0) ="",OFFSET(A108,-2,0)+1,OFFSET(A108,-1,0)+1 )</f>
+        <v>91</v>
+      </c>
+      <c r="B108" s="30" t="s">
+        <v>203</v>
+      </c>
+      <c r="C108" s="46"/>
+      <c r="D108" s="13"/>
+      <c r="E108" s="13"/>
+      <c r="F108" s="13"/>
+      <c r="G108" s="13"/>
+      <c r="H108" s="13"/>
+      <c r="I108" s="13"/>
+    </row>
+    <row r="109" spans="1:9" s="10" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="27">
+        <f ca="1">IF(OFFSET(A109,-1,0) ="",OFFSET(A109,-2,0)+1,OFFSET(A109,-1,0)+1 )</f>
+        <v>92</v>
+      </c>
+      <c r="B109" s="30" t="s">
+        <v>189</v>
+      </c>
+      <c r="C109" s="46"/>
+      <c r="D109" s="13"/>
+      <c r="E109" s="13"/>
+      <c r="F109" s="13"/>
+      <c r="G109" s="13"/>
+      <c r="H109" s="13"/>
+      <c r="I109" s="13"/>
+    </row>
+    <row r="110" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="43" t="s">
+        <v>199</v>
+      </c>
+      <c r="B110" s="44"/>
+      <c r="C110" s="44"/>
+      <c r="D110" s="44"/>
+      <c r="E110" s="44"/>
+      <c r="F110" s="44"/>
+      <c r="G110" s="44"/>
+      <c r="H110" s="44"/>
+      <c r="I110" s="44"/>
+    </row>
+    <row r="111" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="27">
+        <f ca="1">IF(OFFSET(A111,-2,0) ="",OFFSET(A111,-2,0)+1,OFFSET(A111,-2,0)+1 )</f>
+        <v>93</v>
+      </c>
+      <c r="B111" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="C111" s="46"/>
+      <c r="D111" s="13"/>
+      <c r="E111" s="13"/>
+      <c r="F111" s="13"/>
+      <c r="G111" s="13"/>
+      <c r="H111" s="13"/>
+      <c r="I111" s="13"/>
+    </row>
+    <row r="112" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="43" t="s">
+        <v>200</v>
+      </c>
+      <c r="B112" s="44"/>
+      <c r="C112" s="44"/>
+      <c r="D112" s="44"/>
+      <c r="E112" s="44"/>
+      <c r="F112" s="44"/>
+      <c r="G112" s="44"/>
+      <c r="H112" s="44"/>
+      <c r="I112" s="44"/>
+    </row>
+    <row r="113" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="27">
+        <f ca="1">IF(OFFSET(A113,-2,0) ="",OFFSET(A113,-2,0)+1,OFFSET(A113,-2,0)+1 )</f>
+        <v>94</v>
+      </c>
+      <c r="B113" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="C113" s="46"/>
+      <c r="D113" s="13"/>
+      <c r="E113" s="13"/>
+      <c r="F113" s="13"/>
+      <c r="G113" s="13"/>
+      <c r="H113" s="13"/>
+      <c r="I113" s="13"/>
+    </row>
+    <row r="114" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="27"/>
+      <c r="B114" s="30"/>
+      <c r="C114" s="46"/>
+      <c r="D114" s="13"/>
+      <c r="E114" s="13"/>
+      <c r="F114" s="13"/>
+      <c r="G114" s="13"/>
+      <c r="H114" s="13"/>
+      <c r="I114" s="13"/>
+    </row>
+    <row r="115" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="27"/>
+      <c r="B115" s="30"/>
+      <c r="C115" s="46"/>
+      <c r="D115" s="13"/>
+      <c r="E115" s="13"/>
+      <c r="F115" s="13"/>
+      <c r="G115" s="13"/>
+      <c r="H115" s="13"/>
+      <c r="I115" s="13"/>
+    </row>
+    <row r="116" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="27"/>
+      <c r="B116" s="30"/>
+      <c r="C116" s="46"/>
+      <c r="D116" s="13"/>
+      <c r="E116" s="13"/>
+      <c r="F116" s="13"/>
+      <c r="G116" s="13"/>
+      <c r="H116" s="13"/>
+      <c r="I116" s="13"/>
+    </row>
+    <row r="117" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="27"/>
+      <c r="B117" s="30"/>
+      <c r="C117" s="46"/>
+      <c r="D117" s="13"/>
+      <c r="E117" s="13"/>
+      <c r="F117" s="13"/>
+      <c r="G117" s="13"/>
+      <c r="H117" s="13"/>
+      <c r="I117" s="13"/>
+    </row>
+    <row r="118" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="27"/>
+      <c r="B118" s="30"/>
+      <c r="C118" s="46"/>
+      <c r="D118" s="13"/>
+      <c r="E118" s="13"/>
+      <c r="F118" s="13"/>
+      <c r="G118" s="13"/>
+      <c r="H118" s="13"/>
+      <c r="I118" s="13"/>
+    </row>
+    <row r="119" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="27"/>
+      <c r="B119" s="30"/>
+      <c r="C119" s="46"/>
+      <c r="D119" s="13"/>
+      <c r="E119" s="13"/>
+      <c r="F119" s="13"/>
+      <c r="G119" s="13"/>
+      <c r="H119" s="13"/>
+      <c r="I119" s="13"/>
+    </row>
+    <row r="120" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="27"/>
+      <c r="B120" s="30"/>
+      <c r="C120" s="46"/>
+      <c r="D120" s="13"/>
+      <c r="E120" s="13"/>
+      <c r="F120" s="13"/>
+      <c r="G120" s="13"/>
+      <c r="H120" s="13"/>
+      <c r="I120" s="13"/>
+    </row>
+    <row r="121" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="27"/>
+      <c r="B121" s="30"/>
+      <c r="C121" s="46"/>
+      <c r="D121" s="13"/>
+      <c r="E121" s="13"/>
+      <c r="F121" s="13"/>
+      <c r="G121" s="13"/>
+      <c r="H121" s="13"/>
+      <c r="I121" s="13"/>
+    </row>
+    <row r="122" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="27"/>
+      <c r="B122" s="30"/>
+      <c r="C122" s="46"/>
+      <c r="D122" s="13"/>
+      <c r="E122" s="13"/>
+      <c r="F122" s="13"/>
+      <c r="G122" s="13"/>
+      <c r="H122" s="13"/>
+      <c r="I122" s="13"/>
+    </row>
+    <row r="123" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="27"/>
+      <c r="B123" s="30"/>
+      <c r="C123" s="46"/>
+      <c r="D123" s="13"/>
+      <c r="E123" s="13"/>
+      <c r="F123" s="13"/>
+      <c r="G123" s="13"/>
+      <c r="H123" s="13"/>
+      <c r="I123" s="13"/>
+    </row>
+    <row r="124" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="27"/>
+      <c r="B124" s="30"/>
+      <c r="C124" s="46"/>
+      <c r="D124" s="13"/>
+      <c r="E124" s="13"/>
+      <c r="F124" s="13"/>
+      <c r="G124" s="13"/>
+      <c r="H124" s="13"/>
+      <c r="I124" s="13"/>
+    </row>
+    <row r="125" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="27"/>
+      <c r="B125" s="30"/>
+      <c r="C125" s="46"/>
+      <c r="D125" s="13"/>
+      <c r="E125" s="13"/>
+      <c r="F125" s="13"/>
+      <c r="G125" s="13"/>
+      <c r="H125" s="13"/>
+      <c r="I125" s="13"/>
+    </row>
+    <row r="126" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="27"/>
+      <c r="B126" s="30"/>
+      <c r="C126" s="46"/>
+      <c r="D126" s="13"/>
+      <c r="E126" s="13"/>
+      <c r="F126" s="13"/>
+      <c r="G126" s="13"/>
+      <c r="H126" s="13"/>
+      <c r="I126" s="13"/>
+    </row>
+    <row r="127" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="27"/>
+      <c r="B127" s="30"/>
+      <c r="C127" s="46"/>
+      <c r="D127" s="13"/>
+      <c r="E127" s="13"/>
+      <c r="F127" s="13"/>
+      <c r="G127" s="13"/>
+      <c r="H127" s="13"/>
+      <c r="I127" s="13"/>
+    </row>
+    <row r="128" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="27"/>
+      <c r="B128" s="30"/>
+      <c r="C128" s="46"/>
+      <c r="D128" s="13"/>
+      <c r="E128" s="13"/>
+      <c r="F128" s="13"/>
+      <c r="G128" s="13"/>
+      <c r="H128" s="13"/>
+      <c r="I128" s="13"/>
+    </row>
+    <row r="129" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="27"/>
+      <c r="B129" s="30"/>
+      <c r="C129" s="46"/>
+      <c r="D129" s="13"/>
+      <c r="E129" s="13"/>
+      <c r="F129" s="13"/>
+      <c r="G129" s="13"/>
+      <c r="H129" s="13"/>
+      <c r="I129" s="13"/>
+    </row>
+    <row r="130" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="27"/>
+      <c r="B130" s="30"/>
+      <c r="C130" s="46"/>
+      <c r="D130" s="13"/>
+      <c r="E130" s="13"/>
+      <c r="F130" s="13"/>
+      <c r="G130" s="13"/>
+      <c r="H130" s="13"/>
+      <c r="I130" s="13"/>
+    </row>
+    <row r="131" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="27"/>
+      <c r="B131" s="30"/>
+      <c r="C131" s="46"/>
+      <c r="D131" s="13"/>
+      <c r="E131" s="13"/>
+      <c r="F131" s="13"/>
+      <c r="G131" s="13"/>
+      <c r="H131" s="13"/>
+      <c r="I131" s="13"/>
+    </row>
+    <row r="132" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="27"/>
+      <c r="B132" s="30"/>
+      <c r="C132" s="46"/>
+      <c r="D132" s="13"/>
+      <c r="E132" s="13"/>
+      <c r="F132" s="13"/>
+      <c r="G132" s="13"/>
+      <c r="H132" s="13"/>
+      <c r="I132" s="13"/>
+    </row>
+    <row r="133" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="27"/>
+      <c r="B133" s="30"/>
+      <c r="C133" s="46"/>
+      <c r="D133" s="13"/>
+      <c r="E133" s="13"/>
+      <c r="F133" s="13"/>
+      <c r="G133" s="13"/>
+      <c r="H133" s="13"/>
+      <c r="I133" s="13"/>
+    </row>
+    <row r="134" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="27"/>
+      <c r="B134" s="30"/>
+      <c r="C134" s="46"/>
+      <c r="D134" s="13"/>
+      <c r="E134" s="13"/>
+      <c r="F134" s="13"/>
+      <c r="G134" s="13"/>
+      <c r="H134" s="13"/>
+      <c r="I134" s="13"/>
+    </row>
+    <row r="135" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="27"/>
+      <c r="B135" s="30"/>
+      <c r="C135" s="46"/>
+      <c r="D135" s="13"/>
+      <c r="E135" s="13"/>
+      <c r="F135" s="13"/>
+      <c r="G135" s="13"/>
+      <c r="H135" s="13"/>
+      <c r="I135" s="13"/>
+    </row>
+    <row r="136" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="27"/>
+      <c r="B136" s="30"/>
+      <c r="C136" s="46"/>
+      <c r="D136" s="13"/>
+      <c r="E136" s="13"/>
+      <c r="F136" s="13"/>
+      <c r="G136" s="13"/>
+      <c r="H136" s="13"/>
+      <c r="I136" s="13"/>
+    </row>
+    <row r="137" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="27"/>
+      <c r="B137" s="30"/>
+      <c r="C137" s="46"/>
+      <c r="D137" s="13"/>
+      <c r="E137" s="13"/>
+      <c r="F137" s="13"/>
+      <c r="G137" s="13"/>
+      <c r="H137" s="13"/>
+      <c r="I137" s="13"/>
+    </row>
+    <row r="138" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="27"/>
+      <c r="B138" s="30"/>
+      <c r="C138" s="46"/>
+      <c r="D138" s="13"/>
+      <c r="E138" s="13"/>
+      <c r="F138" s="13"/>
+      <c r="G138" s="13"/>
+      <c r="H138" s="13"/>
+      <c r="I138" s="13"/>
+    </row>
+    <row r="139" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="27"/>
+      <c r="B139" s="30"/>
+      <c r="C139" s="46"/>
+      <c r="D139" s="13"/>
+      <c r="E139" s="13"/>
+      <c r="F139" s="13"/>
+      <c r="G139" s="13"/>
+      <c r="H139" s="13"/>
+      <c r="I139" s="13"/>
+    </row>
+    <row r="140" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="27"/>
+      <c r="B140" s="30"/>
+      <c r="C140" s="46"/>
+      <c r="D140" s="13"/>
+      <c r="E140" s="13"/>
+      <c r="F140" s="13"/>
+      <c r="G140" s="13"/>
+      <c r="H140" s="13"/>
+      <c r="I140" s="13"/>
+    </row>
+    <row r="141" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="27"/>
+      <c r="B141" s="30"/>
+      <c r="C141" s="46"/>
+      <c r="D141" s="13"/>
+      <c r="E141" s="13"/>
+      <c r="F141" s="13"/>
+      <c r="G141" s="13"/>
+      <c r="H141" s="13"/>
+      <c r="I141" s="13"/>
+    </row>
+    <row r="142" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="27"/>
+      <c r="B142" s="30"/>
+      <c r="C142" s="46"/>
+      <c r="D142" s="13"/>
+      <c r="E142" s="13"/>
+      <c r="F142" s="13"/>
+      <c r="G142" s="13"/>
+      <c r="H142" s="13"/>
+      <c r="I142" s="13"/>
+    </row>
+    <row r="143" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="27"/>
+      <c r="B143" s="30"/>
+      <c r="C143" s="46"/>
+      <c r="D143" s="13"/>
+      <c r="E143" s="13"/>
+      <c r="F143" s="13"/>
+      <c r="G143" s="13"/>
+      <c r="H143" s="13"/>
+      <c r="I143" s="13"/>
+    </row>
+    <row r="144" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="27"/>
+      <c r="B144" s="30"/>
+      <c r="C144" s="46"/>
+      <c r="D144" s="13"/>
+      <c r="E144" s="13"/>
+      <c r="F144" s="13"/>
+      <c r="G144" s="13"/>
+      <c r="H144" s="13"/>
+      <c r="I144" s="13"/>
+    </row>
+    <row r="145" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="27"/>
+      <c r="B145" s="30"/>
+      <c r="C145" s="46"/>
+      <c r="D145" s="13"/>
+      <c r="E145" s="13"/>
+      <c r="F145" s="13"/>
+      <c r="G145" s="13"/>
+      <c r="H145" s="13"/>
+      <c r="I145" s="13"/>
+    </row>
+    <row r="146" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="27"/>
+      <c r="B146" s="30"/>
+      <c r="C146" s="46"/>
+      <c r="D146" s="13"/>
+      <c r="E146" s="13"/>
+      <c r="F146" s="13"/>
+      <c r="G146" s="13"/>
+      <c r="H146" s="13"/>
+      <c r="I146" s="13"/>
+    </row>
+    <row r="147" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="27"/>
+      <c r="B147" s="30"/>
+      <c r="C147" s="46"/>
+      <c r="D147" s="13"/>
+      <c r="E147" s="13"/>
+      <c r="F147" s="13"/>
+      <c r="G147" s="13"/>
+      <c r="H147" s="13"/>
+      <c r="I147" s="13"/>
+    </row>
+    <row r="148" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="27"/>
+      <c r="B148" s="30"/>
+      <c r="C148" s="46"/>
+      <c r="D148" s="13"/>
+      <c r="E148" s="13"/>
+      <c r="F148" s="13"/>
+      <c r="G148" s="13"/>
+      <c r="H148" s="13"/>
+      <c r="I148" s="13"/>
+    </row>
+    <row r="149" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="27"/>
+      <c r="B149" s="30"/>
+      <c r="C149" s="46"/>
+      <c r="D149" s="13"/>
+      <c r="E149" s="13"/>
+      <c r="F149" s="13"/>
+      <c r="G149" s="13"/>
+      <c r="H149" s="13"/>
+      <c r="I149" s="13"/>
+    </row>
+    <row r="150" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="27"/>
+      <c r="B150" s="30"/>
+      <c r="C150" s="46"/>
+      <c r="D150" s="13"/>
+      <c r="E150" s="13"/>
+      <c r="F150" s="13"/>
+      <c r="G150" s="13"/>
+      <c r="H150" s="13"/>
+      <c r="I150" s="13"/>
+    </row>
+    <row r="151" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="27"/>
+      <c r="B151" s="30"/>
+      <c r="C151" s="46"/>
+      <c r="D151" s="13"/>
+      <c r="E151" s="13"/>
+      <c r="F151" s="13"/>
+      <c r="G151" s="13"/>
+      <c r="H151" s="13"/>
+      <c r="I151" s="13"/>
+    </row>
+    <row r="152" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="27"/>
+      <c r="B152" s="30"/>
+      <c r="C152" s="46"/>
+      <c r="D152" s="13"/>
+      <c r="E152" s="13"/>
+      <c r="F152" s="13"/>
+      <c r="G152" s="13"/>
+      <c r="H152" s="13"/>
+      <c r="I152" s="13"/>
+    </row>
+    <row r="153" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="27"/>
+      <c r="B153" s="30"/>
+      <c r="C153" s="46"/>
+      <c r="D153" s="13"/>
+      <c r="E153" s="13"/>
+      <c r="F153" s="13"/>
+      <c r="G153" s="13"/>
+      <c r="H153" s="13"/>
+      <c r="I153" s="13"/>
+    </row>
+    <row r="154" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="27"/>
+      <c r="B154" s="30"/>
+      <c r="C154" s="46"/>
+      <c r="D154" s="13"/>
+      <c r="E154" s="13"/>
+      <c r="F154" s="13"/>
+      <c r="G154" s="13"/>
+      <c r="H154" s="13"/>
+      <c r="I154" s="13"/>
+    </row>
+    <row r="155" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="27"/>
+      <c r="B155" s="30"/>
+      <c r="C155" s="46"/>
+      <c r="D155" s="13"/>
+      <c r="E155" s="13"/>
+      <c r="F155" s="13"/>
+      <c r="G155" s="13"/>
+      <c r="H155" s="13"/>
+      <c r="I155" s="13"/>
+    </row>
+    <row r="156" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="27"/>
+      <c r="B156" s="30"/>
+      <c r="C156" s="46"/>
+      <c r="D156" s="13"/>
+      <c r="E156" s="13"/>
+      <c r="F156" s="13"/>
+      <c r="G156" s="13"/>
+      <c r="H156" s="13"/>
+      <c r="I156" s="13"/>
+    </row>
+    <row r="157" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="27"/>
+      <c r="B157" s="30"/>
+      <c r="C157" s="46"/>
+      <c r="D157" s="13"/>
+      <c r="E157" s="13"/>
+      <c r="F157" s="13"/>
+      <c r="G157" s="13"/>
+      <c r="H157" s="13"/>
+      <c r="I157" s="13"/>
+    </row>
+    <row r="158" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="27"/>
+      <c r="B158" s="30"/>
+      <c r="C158" s="46"/>
+      <c r="D158" s="13"/>
+      <c r="E158" s="13"/>
+      <c r="F158" s="13"/>
+      <c r="G158" s="13"/>
+      <c r="H158" s="13"/>
+      <c r="I158" s="13"/>
+    </row>
+    <row r="159" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="27"/>
+      <c r="B159" s="30"/>
+      <c r="C159" s="46"/>
+      <c r="D159" s="13"/>
+      <c r="E159" s="13"/>
+      <c r="F159" s="13"/>
+      <c r="G159" s="13"/>
+      <c r="H159" s="13"/>
+      <c r="I159" s="13"/>
+    </row>
+    <row r="160" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="27"/>
+      <c r="B160" s="30"/>
+      <c r="C160" s="46"/>
+      <c r="D160" s="13"/>
+      <c r="E160" s="13"/>
+      <c r="F160" s="13"/>
+      <c r="G160" s="13"/>
+      <c r="H160" s="13"/>
+      <c r="I160" s="13"/>
+    </row>
+    <row r="161" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="27"/>
+      <c r="B161" s="30"/>
+      <c r="C161" s="46"/>
+      <c r="D161" s="13"/>
+      <c r="E161" s="13"/>
+      <c r="F161" s="13"/>
+      <c r="G161" s="13"/>
+      <c r="H161" s="13"/>
+      <c r="I161" s="13"/>
+    </row>
+    <row r="162" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="27"/>
+      <c r="B162" s="30"/>
+      <c r="C162" s="46"/>
+      <c r="D162" s="13"/>
+      <c r="E162" s="13"/>
+      <c r="F162" s="13"/>
+      <c r="G162" s="13"/>
+      <c r="H162" s="13"/>
+      <c r="I162" s="13"/>
+    </row>
+    <row r="163" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="27"/>
+      <c r="B163" s="30"/>
+      <c r="C163" s="46"/>
+      <c r="D163" s="13"/>
+      <c r="E163" s="13"/>
+      <c r="F163" s="13"/>
+      <c r="G163" s="13"/>
+      <c r="H163" s="13"/>
+      <c r="I163" s="13"/>
+    </row>
+    <row r="164" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="27"/>
+      <c r="B164" s="30"/>
+      <c r="C164" s="46"/>
+      <c r="D164" s="13"/>
+      <c r="E164" s="13"/>
+      <c r="F164" s="13"/>
+      <c r="G164" s="13"/>
+      <c r="H164" s="13"/>
+      <c r="I164" s="13"/>
+    </row>
+    <row r="165" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="27"/>
+      <c r="B165" s="30"/>
+      <c r="C165" s="46"/>
+      <c r="D165" s="13"/>
+      <c r="E165" s="13"/>
+      <c r="F165" s="13"/>
+      <c r="G165" s="13"/>
+      <c r="H165" s="13"/>
+      <c r="I165" s="13"/>
+    </row>
+    <row r="166" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="27"/>
+      <c r="B166" s="30"/>
+      <c r="C166" s="46"/>
+      <c r="D166" s="13"/>
+      <c r="E166" s="13"/>
+      <c r="F166" s="13"/>
+      <c r="G166" s="13"/>
+      <c r="H166" s="13"/>
+      <c r="I166" s="13"/>
+    </row>
+    <row r="167" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="27"/>
+      <c r="B167" s="30"/>
+      <c r="C167" s="46"/>
+      <c r="D167" s="13"/>
+      <c r="E167" s="13"/>
+      <c r="F167" s="13"/>
+      <c r="G167" s="13"/>
+      <c r="H167" s="13"/>
+      <c r="I167" s="13"/>
+    </row>
+    <row r="168" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="27"/>
+      <c r="B168" s="30"/>
+      <c r="C168" s="46"/>
+      <c r="D168" s="13"/>
+      <c r="E168" s="13"/>
+      <c r="F168" s="13"/>
+      <c r="G168" s="13"/>
+      <c r="H168" s="13"/>
+      <c r="I168" s="13"/>
+    </row>
+    <row r="169" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="27"/>
+      <c r="B169" s="30"/>
+      <c r="C169" s="46"/>
+      <c r="D169" s="13"/>
+      <c r="E169" s="13"/>
+      <c r="F169" s="13"/>
+      <c r="G169" s="13"/>
+      <c r="H169" s="13"/>
+      <c r="I169" s="13"/>
+    </row>
+    <row r="170" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="27"/>
+      <c r="B170" s="30"/>
+      <c r="C170" s="46"/>
+      <c r="D170" s="13"/>
+      <c r="E170" s="13"/>
+      <c r="F170" s="13"/>
+      <c r="G170" s="13"/>
+      <c r="H170" s="13"/>
+      <c r="I170" s="13"/>
+    </row>
+    <row r="171" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A171" s="27"/>
+      <c r="B171" s="30"/>
+      <c r="C171" s="46"/>
+      <c r="D171" s="13"/>
+      <c r="E171" s="13"/>
+      <c r="F171" s="13"/>
+      <c r="G171" s="13"/>
+      <c r="H171" s="13"/>
+      <c r="I171" s="13"/>
+    </row>
+    <row r="172" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="27"/>
+      <c r="B172" s="30"/>
+      <c r="C172" s="46"/>
+      <c r="D172" s="13"/>
+      <c r="E172" s="13"/>
+      <c r="F172" s="13"/>
+      <c r="G172" s="13"/>
+      <c r="H172" s="13"/>
+      <c r="I172" s="13"/>
+    </row>
+    <row r="173" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="27"/>
+      <c r="B173" s="30"/>
+      <c r="C173" s="46"/>
+      <c r="D173" s="13"/>
+      <c r="E173" s="13"/>
+      <c r="F173" s="13"/>
+      <c r="G173" s="13"/>
+      <c r="H173" s="13"/>
+      <c r="I173" s="13"/>
+    </row>
+    <row r="174" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="27"/>
+      <c r="B174" s="30"/>
+      <c r="C174" s="46"/>
+      <c r="D174" s="13"/>
+      <c r="E174" s="13"/>
+      <c r="F174" s="13"/>
+      <c r="G174" s="13"/>
+      <c r="H174" s="13"/>
+      <c r="I174" s="13"/>
+    </row>
+    <row r="175" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="27"/>
+      <c r="B175" s="30"/>
+      <c r="C175" s="46"/>
+      <c r="D175" s="13"/>
+      <c r="E175" s="13"/>
+      <c r="F175" s="13"/>
+      <c r="G175" s="13"/>
+      <c r="H175" s="13"/>
+      <c r="I175" s="13"/>
+    </row>
+    <row r="176" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="27"/>
+      <c r="B176" s="30"/>
+      <c r="C176" s="46"/>
+      <c r="D176" s="13"/>
+      <c r="E176" s="13"/>
+      <c r="F176" s="13"/>
+      <c r="G176" s="13"/>
+      <c r="H176" s="13"/>
+      <c r="I176" s="13"/>
+    </row>
+    <row r="177" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A177" s="27"/>
+      <c r="B177" s="30"/>
+      <c r="C177" s="46"/>
+      <c r="D177" s="13"/>
+      <c r="E177" s="13"/>
+      <c r="F177" s="13"/>
+      <c r="G177" s="13"/>
+      <c r="H177" s="13"/>
+      <c r="I177" s="13"/>
+    </row>
+    <row r="178" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="27"/>
+      <c r="B178" s="30"/>
+      <c r="C178" s="46"/>
+      <c r="D178" s="13"/>
+      <c r="E178" s="13"/>
+      <c r="F178" s="13"/>
+      <c r="G178" s="13"/>
+      <c r="H178" s="13"/>
+      <c r="I178" s="13"/>
+    </row>
+    <row r="179" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A179" s="27"/>
+      <c r="B179" s="30"/>
+      <c r="C179" s="46"/>
+      <c r="D179" s="13"/>
+      <c r="E179" s="13"/>
+      <c r="F179" s="13"/>
+      <c r="G179" s="13"/>
+      <c r="H179" s="13"/>
+      <c r="I179" s="13"/>
+    </row>
+    <row r="180" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A180" s="27"/>
+      <c r="B180" s="30"/>
+      <c r="C180" s="46"/>
+      <c r="D180" s="13"/>
+      <c r="E180" s="13"/>
+      <c r="F180" s="13"/>
+      <c r="G180" s="13"/>
+      <c r="H180" s="13"/>
+      <c r="I180" s="13"/>
+    </row>
+    <row r="181" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A181" s="27"/>
+      <c r="B181" s="30"/>
+      <c r="C181" s="46"/>
+      <c r="D181" s="13"/>
+      <c r="E181" s="13"/>
+      <c r="F181" s="13"/>
+      <c r="G181" s="13"/>
+      <c r="H181" s="13"/>
+      <c r="I181" s="13"/>
+    </row>
+    <row r="182" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A182" s="27"/>
+      <c r="B182" s="30"/>
+      <c r="C182" s="46"/>
+      <c r="D182" s="13"/>
+      <c r="E182" s="13"/>
+      <c r="F182" s="13"/>
+      <c r="G182" s="13"/>
+      <c r="H182" s="13"/>
+      <c r="I182" s="13"/>
+    </row>
+    <row r="183" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A183" s="27"/>
+      <c r="B183" s="30"/>
+      <c r="C183" s="46"/>
+      <c r="D183" s="13"/>
+      <c r="E183" s="13"/>
+      <c r="F183" s="13"/>
+      <c r="G183" s="13"/>
+      <c r="H183" s="13"/>
+      <c r="I183" s="13"/>
+    </row>
+    <row r="184" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="27"/>
+      <c r="B184" s="30"/>
+      <c r="C184" s="46"/>
+      <c r="D184" s="13"/>
+      <c r="E184" s="13"/>
+      <c r="F184" s="13"/>
+      <c r="G184" s="13"/>
+      <c r="H184" s="13"/>
+      <c r="I184" s="13"/>
+    </row>
+    <row r="185" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A185" s="27"/>
+      <c r="B185" s="30"/>
+      <c r="C185" s="46"/>
+      <c r="D185" s="13"/>
+      <c r="E185" s="13"/>
+      <c r="F185" s="13"/>
+      <c r="G185" s="13"/>
+      <c r="H185" s="13"/>
+      <c r="I185" s="13"/>
+    </row>
+    <row r="186" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A186" s="27"/>
+      <c r="B186" s="30"/>
+      <c r="C186" s="46"/>
+      <c r="D186" s="13"/>
+      <c r="E186" s="13"/>
+      <c r="F186" s="13"/>
+      <c r="G186" s="13"/>
+      <c r="H186" s="13"/>
+      <c r="I186" s="13"/>
+    </row>
+    <row r="187" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A187" s="27"/>
+      <c r="B187" s="30"/>
+      <c r="C187" s="46"/>
+      <c r="D187" s="13"/>
+      <c r="E187" s="13"/>
+      <c r="F187" s="13"/>
+      <c r="G187" s="13"/>
+      <c r="H187" s="13"/>
+      <c r="I187" s="13"/>
+    </row>
+    <row r="188" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="27"/>
+      <c r="B188" s="30"/>
+      <c r="C188" s="46"/>
+      <c r="D188" s="13"/>
+      <c r="E188" s="13"/>
+      <c r="F188" s="13"/>
+      <c r="G188" s="13"/>
+      <c r="H188" s="13"/>
+      <c r="I188" s="13"/>
+    </row>
+    <row r="189" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A189" s="27"/>
+      <c r="B189" s="30"/>
+      <c r="C189" s="46"/>
+      <c r="D189" s="13"/>
+      <c r="E189" s="13"/>
+      <c r="F189" s="13"/>
+      <c r="G189" s="13"/>
+      <c r="H189" s="13"/>
+      <c r="I189" s="13"/>
+    </row>
+    <row r="190" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A190" s="27"/>
+      <c r="B190" s="30"/>
+      <c r="C190" s="46"/>
+      <c r="D190" s="13"/>
+      <c r="E190" s="13"/>
+      <c r="F190" s="13"/>
+      <c r="G190" s="13"/>
+      <c r="H190" s="13"/>
+      <c r="I190" s="13"/>
+    </row>
+    <row r="191" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="27"/>
+      <c r="B191" s="30"/>
+      <c r="C191" s="46"/>
+      <c r="D191" s="13"/>
+      <c r="E191" s="13"/>
+      <c r="F191" s="13"/>
+      <c r="G191" s="13"/>
+      <c r="H191" s="13"/>
+      <c r="I191" s="13"/>
+    </row>
+    <row r="192" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A192" s="27"/>
+      <c r="B192" s="30"/>
+      <c r="C192" s="46"/>
+      <c r="D192" s="13"/>
+      <c r="E192" s="13"/>
+      <c r="F192" s="13"/>
+      <c r="G192" s="13"/>
+      <c r="H192" s="13"/>
+      <c r="I192" s="13"/>
+    </row>
+    <row r="193" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="27"/>
+      <c r="B193" s="30"/>
+      <c r="C193" s="46"/>
+      <c r="D193" s="13"/>
+      <c r="E193" s="13"/>
+      <c r="F193" s="13"/>
+      <c r="G193" s="13"/>
+      <c r="H193" s="13"/>
+      <c r="I193" s="13"/>
+    </row>
+    <row r="194" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="27"/>
+      <c r="B194" s="30"/>
+      <c r="C194" s="46"/>
+      <c r="D194" s="13"/>
+      <c r="E194" s="13"/>
+      <c r="F194" s="13"/>
+      <c r="G194" s="13"/>
+      <c r="H194" s="13"/>
+      <c r="I194" s="13"/>
+    </row>
+    <row r="195" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A195" s="27"/>
+      <c r="B195" s="30"/>
+      <c r="C195" s="46"/>
+      <c r="D195" s="13"/>
+      <c r="E195" s="13"/>
+      <c r="F195" s="13"/>
+      <c r="G195" s="13"/>
+      <c r="H195" s="13"/>
+      <c r="I195" s="13"/>
+    </row>
+    <row r="196" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A196" s="27"/>
+      <c r="B196" s="30"/>
+      <c r="C196" s="46"/>
+      <c r="D196" s="13"/>
+      <c r="E196" s="13"/>
+      <c r="F196" s="13"/>
+      <c r="G196" s="13"/>
+      <c r="H196" s="13"/>
+      <c r="I196" s="13"/>
+    </row>
+    <row r="197" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A197" s="27"/>
+      <c r="B197" s="30"/>
+      <c r="C197" s="46"/>
+      <c r="D197" s="13"/>
+      <c r="E197" s="13"/>
+      <c r="F197" s="13"/>
+      <c r="G197" s="13"/>
+      <c r="H197" s="13"/>
+      <c r="I197" s="13"/>
+    </row>
+    <row r="198" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A198" s="27"/>
+      <c r="B198" s="30"/>
+      <c r="C198" s="46"/>
+      <c r="D198" s="13"/>
+      <c r="E198" s="13"/>
+      <c r="F198" s="13"/>
+      <c r="G198" s="13"/>
+      <c r="H198" s="13"/>
+      <c r="I198" s="13"/>
+    </row>
+    <row r="199" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A199" s="27"/>
+      <c r="B199" s="30"/>
+      <c r="C199" s="46"/>
+      <c r="D199" s="13"/>
+      <c r="E199" s="13"/>
+      <c r="F199" s="13"/>
+      <c r="G199" s="13"/>
+      <c r="H199" s="13"/>
+      <c r="I199" s="13"/>
+    </row>
+    <row r="200" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A200" s="27"/>
+      <c r="B200" s="30"/>
+      <c r="C200" s="46"/>
+      <c r="D200" s="13"/>
+      <c r="E200" s="13"/>
+      <c r="F200" s="13"/>
+      <c r="G200" s="13"/>
+      <c r="H200" s="13"/>
+      <c r="I200" s="13"/>
+    </row>
+    <row r="201" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A201" s="27"/>
+      <c r="B201" s="30"/>
+      <c r="C201" s="46"/>
+      <c r="D201" s="13"/>
+      <c r="E201" s="13"/>
+      <c r="F201" s="13"/>
+      <c r="G201" s="13"/>
+      <c r="H201" s="13"/>
+      <c r="I201" s="13"/>
+    </row>
+    <row r="202" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A202" s="27"/>
+      <c r="B202" s="30"/>
+      <c r="C202" s="46"/>
+      <c r="D202" s="13"/>
+      <c r="E202" s="13"/>
+      <c r="F202" s="13"/>
+      <c r="G202" s="13"/>
+      <c r="H202" s="13"/>
+      <c r="I202" s="13"/>
+    </row>
+    <row r="203" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A203" s="27"/>
+      <c r="B203" s="30"/>
+      <c r="C203" s="46"/>
+      <c r="D203" s="13"/>
+      <c r="E203" s="13"/>
+      <c r="F203" s="13"/>
+      <c r="G203" s="13"/>
+      <c r="H203" s="13"/>
+      <c r="I203" s="13"/>
+    </row>
+    <row r="204" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A204" s="27"/>
+      <c r="B204" s="30"/>
+      <c r="C204" s="46"/>
+      <c r="D204" s="13"/>
+      <c r="E204" s="13"/>
+      <c r="F204" s="13"/>
+      <c r="G204" s="13"/>
+      <c r="H204" s="13"/>
+      <c r="I204" s="13"/>
+    </row>
+    <row r="205" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A205" s="27"/>
+      <c r="B205" s="30"/>
+      <c r="C205" s="46"/>
+      <c r="D205" s="13"/>
+      <c r="E205" s="13"/>
+      <c r="F205" s="13"/>
+      <c r="G205" s="13"/>
+      <c r="H205" s="13"/>
+      <c r="I205" s="13"/>
+    </row>
+    <row r="206" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A206" s="27"/>
+      <c r="B206" s="30"/>
+      <c r="C206" s="46"/>
+      <c r="D206" s="13"/>
+      <c r="E206" s="13"/>
+      <c r="F206" s="13"/>
+      <c r="G206" s="13"/>
+      <c r="H206" s="13"/>
+      <c r="I206" s="13"/>
+    </row>
+    <row r="207" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A207" s="27"/>
+      <c r="B207" s="30"/>
+      <c r="C207" s="46"/>
+      <c r="D207" s="13"/>
+      <c r="E207" s="13"/>
+      <c r="F207" s="13"/>
+      <c r="G207" s="13"/>
+      <c r="H207" s="13"/>
+      <c r="I207" s="13"/>
+    </row>
+    <row r="208" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A208" s="27"/>
+      <c r="B208" s="30"/>
+      <c r="C208" s="46"/>
+      <c r="D208" s="13"/>
+      <c r="E208" s="13"/>
+      <c r="F208" s="13"/>
+      <c r="G208" s="13"/>
+      <c r="H208" s="13"/>
+      <c r="I208" s="13"/>
+    </row>
+    <row r="209" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A209" s="27"/>
+      <c r="B209" s="30"/>
+      <c r="C209" s="46"/>
+      <c r="D209" s="13"/>
+      <c r="E209" s="13"/>
+      <c r="F209" s="13"/>
+      <c r="G209" s="13"/>
+      <c r="H209" s="13"/>
+      <c r="I209" s="13"/>
+    </row>
+    <row r="210" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A210" s="27"/>
+      <c r="B210" s="30"/>
+      <c r="C210" s="46"/>
+      <c r="D210" s="13"/>
+      <c r="E210" s="13"/>
+      <c r="F210" s="13"/>
+      <c r="G210" s="13"/>
+      <c r="H210" s="13"/>
+      <c r="I210" s="13"/>
+    </row>
+    <row r="211" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A211" s="27"/>
+      <c r="B211" s="30"/>
+      <c r="C211" s="46"/>
+      <c r="D211" s="13"/>
+      <c r="E211" s="13"/>
+      <c r="F211" s="13"/>
+      <c r="G211" s="13"/>
+      <c r="H211" s="13"/>
+      <c r="I211" s="13"/>
+    </row>
+    <row r="212" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A212" s="27"/>
+      <c r="B212" s="30"/>
+      <c r="C212" s="46"/>
+      <c r="D212" s="13"/>
+      <c r="E212" s="13"/>
+      <c r="F212" s="13"/>
+      <c r="G212" s="13"/>
+      <c r="H212" s="13"/>
+      <c r="I212" s="13"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A83:I83"/>
-    <mergeCell ref="A47:I47"/>
-    <mergeCell ref="A53:I53"/>
-    <mergeCell ref="A58:I58"/>
-    <mergeCell ref="A72:I72"/>
-    <mergeCell ref="A75:I75"/>
+  <mergeCells count="18">
+    <mergeCell ref="A84:I84"/>
+    <mergeCell ref="A86:I86"/>
+    <mergeCell ref="A88:I88"/>
+    <mergeCell ref="A110:I110"/>
+    <mergeCell ref="A112:I112"/>
+    <mergeCell ref="A90:I90"/>
+    <mergeCell ref="A77:I77"/>
+    <mergeCell ref="A100:I100"/>
+    <mergeCell ref="A81:I81"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A19:I19"/>
-    <mergeCell ref="A33:I33"/>
+    <mergeCell ref="A16:I16"/>
+    <mergeCell ref="A28:I28"/>
+    <mergeCell ref="A37:I37"/>
+    <mergeCell ref="A76:I76"/>
+    <mergeCell ref="A52:I52"/>
+    <mergeCell ref="A58:I58"/>
+    <mergeCell ref="A63:I63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added bound value for phone num
</commit_message>
<xml_diff>
--- a/Middle Assignment/TestDesignTechique1_PhamHongAnh.xlsx
+++ b/Middle Assignment/TestDesignTechique1_PhamHongAnh.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NashTech\Rookies\NashTech_Homework\Middle Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F92185E-3783-4B1D-94E7-D8C752A33D39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71D15E3-6CCE-40D1-87DF-4E3F03E09153}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="10400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment 1" sheetId="1" r:id="rId1"/>
@@ -822,12 +822,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{A18BB002-197E-4D45-89D4-C7B92B686A20}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>ADMIN:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="209">
   <si>
     <t>ID</t>
   </si>
@@ -1234,9 +1258,6 @@
     <t>When entering 0 at the initial</t>
   </si>
   <si>
-    <t>When copying a 6-digit code and pasting it in the text field</t>
-  </si>
-  <si>
     <t>When entering a blank space between the numbers</t>
   </si>
   <si>
@@ -1463,6 +1484,21 @@
   </si>
   <si>
     <t xml:space="preserve">Sign up with Email </t>
+  </si>
+  <si>
+    <t>When entering 10 numeric characters</t>
+  </si>
+  <si>
+    <t>Check all drop down values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thêm decision table </t>
+  </si>
+  <si>
+    <t>Check boundary value của phone number (Done)</t>
+  </si>
+  <si>
+    <t>3.  Test flow</t>
   </si>
 </sst>
 </file>
@@ -1684,7 +1720,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1815,6 +1851,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -14339,10 +14381,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{861DB058-9ABC-4928-81FB-0309C7B8DB85}">
-  <dimension ref="A1:Z212"/>
+  <dimension ref="A1:Z200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="C109" sqref="C109"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -14355,7 +14397,7 @@
     <col min="6" max="6" width="17" style="28" customWidth="1"/>
     <col min="7" max="7" width="14.54296875" style="28" customWidth="1"/>
     <col min="8" max="8" width="17.08984375" style="28" customWidth="1"/>
-    <col min="9" max="9" width="15.1796875" style="28" customWidth="1"/>
+    <col min="9" max="9" width="15.1796875" style="50" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="10" customFormat="1" ht="26" x14ac:dyDescent="0.35">
@@ -14406,7 +14448,7 @@
     </row>
     <row r="2" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="39" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B2" s="48"/>
       <c r="C2" s="48"/>
@@ -14436,7 +14478,7 @@
     </row>
     <row r="3" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="41" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B3" s="47"/>
       <c r="C3" s="47"/>
@@ -14464,20 +14506,22 @@
       <c r="Y3" s="26"/>
       <c r="Z3" s="26"/>
     </row>
-    <row r="4" spans="1:26" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" s="10" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>1</v>
       </c>
       <c r="B4" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="C4" s="33"/>
+      <c r="C4" s="49" t="s">
+        <v>207</v>
+      </c>
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
+      <c r="I4" s="49"/>
     </row>
     <row r="5" spans="1:26" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="27">
@@ -14485,7 +14529,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C5" s="33"/>
       <c r="D5" s="13"/>
@@ -14493,7 +14537,7 @@
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
+      <c r="I5" s="49"/>
     </row>
     <row r="6" spans="1:26" s="10" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27">
@@ -14501,7 +14545,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C6" s="33"/>
       <c r="D6" s="13"/>
@@ -14509,15 +14553,15 @@
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-    </row>
-    <row r="7" spans="1:26" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="49"/>
+    </row>
+    <row r="7" spans="1:26" s="10" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="27">
         <f ca="1">IF(OFFSET(A7,-1,0) ="",OFFSET(A7,-2,0)+1,OFFSET(A7,-1,0)+1 )</f>
         <v>4</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>138</v>
+        <v>204</v>
       </c>
       <c r="C7" s="33"/>
       <c r="D7" s="13"/>
@@ -14525,15 +14569,15 @@
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
+      <c r="I7" s="49"/>
     </row>
     <row r="8" spans="1:26" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="27">
-        <f t="shared" ref="A8:A75" ca="1" si="0">IF(OFFSET(A8,-1,0) ="",OFFSET(A8,-2,0)+1,OFFSET(A8,-1,0)+1 )</f>
+        <f ca="1">IF(OFFSET(A8,-1,0) ="",OFFSET(A8,-2,0)+1,OFFSET(A8,-1,0)+1 )</f>
         <v>5</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C8" s="33"/>
       <c r="D8" s="13"/>
@@ -14541,15 +14585,15 @@
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-    </row>
-    <row r="9" spans="1:26" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="49"/>
+    </row>
+    <row r="9" spans="1:26" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="A9:A76" ca="1" si="0">IF(OFFSET(A9,-1,0) ="",OFFSET(A9,-2,0)+1,OFFSET(A9,-1,0)+1 )</f>
         <v>6</v>
       </c>
-      <c r="B9" s="29" t="s">
-        <v>123</v>
+      <c r="B9" s="30" t="s">
+        <v>138</v>
       </c>
       <c r="C9" s="33"/>
       <c r="D9" s="13"/>
@@ -14557,7 +14601,7 @@
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
+      <c r="I9" s="49"/>
     </row>
     <row r="10" spans="1:26" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27">
@@ -14565,7 +14609,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C10" s="33"/>
       <c r="D10" s="13"/>
@@ -14573,15 +14617,15 @@
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-    </row>
-    <row r="11" spans="1:26" s="10" customFormat="1" ht="20.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="49"/>
+    </row>
+    <row r="11" spans="1:26" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>8</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C11" s="33"/>
       <c r="D11" s="13"/>
@@ -14589,15 +14633,15 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-    </row>
-    <row r="12" spans="1:26" s="10" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I11" s="49"/>
+    </row>
+    <row r="12" spans="1:26" s="10" customFormat="1" ht="20.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>9</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C12" s="33"/>
       <c r="D12" s="13"/>
@@ -14605,15 +14649,15 @@
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-    </row>
-    <row r="13" spans="1:26" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I12" s="49"/>
+    </row>
+    <row r="13" spans="1:26" s="10" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>10</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="C13" s="33"/>
       <c r="D13" s="13"/>
@@ -14621,95 +14665,95 @@
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-    </row>
-    <row r="14" spans="1:26" s="10" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I13" s="49"/>
+    </row>
+    <row r="14" spans="1:26" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>11</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="C14" s="33" t="s">
-        <v>202</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="C14" s="33"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-    </row>
-    <row r="15" spans="1:26" s="10" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I14" s="49"/>
+    </row>
+    <row r="15" spans="1:26" s="10" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>12</v>
       </c>
-      <c r="B15" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="C15" s="33"/>
+      <c r="B15" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>201</v>
+      </c>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-    </row>
-    <row r="16" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="46" t="s">
+      <c r="I15" s="49"/>
+    </row>
+    <row r="16" spans="1:26" s="10" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="C16" s="33"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="49"/>
+    </row>
+    <row r="17" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="B16" s="47"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26"/>
-      <c r="O16" s="26"/>
-      <c r="P16" s="26"/>
-      <c r="Q16" s="26"/>
-      <c r="R16" s="26"/>
-      <c r="S16" s="26"/>
-      <c r="T16" s="26"/>
-      <c r="U16" s="26"/>
-      <c r="V16" s="26"/>
-      <c r="W16" s="26"/>
-      <c r="X16" s="26"/>
-      <c r="Y16" s="26"/>
-      <c r="Z16" s="26"/>
-    </row>
-    <row r="17" spans="1:26" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="27">
-        <f ca="1">IF(OFFSET(A17,-2,0) ="",OFFSET(A17,-2,0)+1,OFFSET(A17,-2,0)+1 )</f>
-        <v>13</v>
-      </c>
-      <c r="B17" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-    </row>
-    <row r="18" spans="1:26" s="10" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="47"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="26"/>
+      <c r="Q17" s="26"/>
+      <c r="R17" s="26"/>
+      <c r="S17" s="26"/>
+      <c r="T17" s="26"/>
+      <c r="U17" s="26"/>
+      <c r="V17" s="26"/>
+      <c r="W17" s="26"/>
+      <c r="X17" s="26"/>
+      <c r="Y17" s="26"/>
+      <c r="Z17" s="26"/>
+    </row>
+    <row r="18" spans="1:26" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="27">
-        <f ca="1">IF(OFFSET(A18,-1,0) ="",OFFSET(A18,-2,0)+1,OFFSET(A18,-1,0)+1 )</f>
+        <f ca="1">IF(OFFSET(A18,-2,0) ="",OFFSET(A18,-2,0)+1,OFFSET(A18,-2,0)+1 )</f>
         <v>14</v>
       </c>
       <c r="B18" s="30" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="C18" s="33"/>
       <c r="D18" s="13"/>
@@ -14717,15 +14761,15 @@
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
       <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-    </row>
-    <row r="19" spans="1:26" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I18" s="49"/>
+    </row>
+    <row r="19" spans="1:26" s="10" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">IF(OFFSET(A19,-1,0) ="",OFFSET(A19,-2,0)+1,OFFSET(A19,-1,0)+1 )</f>
         <v>15</v>
       </c>
-      <c r="B19" s="29" t="s">
-        <v>140</v>
+      <c r="B19" s="30" t="s">
+        <v>134</v>
       </c>
       <c r="C19" s="33"/>
       <c r="D19" s="13"/>
@@ -14733,15 +14777,15 @@
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-    </row>
-    <row r="20" spans="1:26" s="10" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I19" s="49"/>
+    </row>
+    <row r="20" spans="1:26" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>16</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C20" s="33"/>
       <c r="D20" s="13"/>
@@ -14749,15 +14793,15 @@
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-    </row>
-    <row r="21" spans="1:26" s="10" customFormat="1" ht="24.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I20" s="49"/>
+    </row>
+    <row r="21" spans="1:26" s="10" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>17</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C21" s="33"/>
       <c r="D21" s="13"/>
@@ -14765,15 +14809,15 @@
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-    </row>
-    <row r="22" spans="1:26" s="10" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I21" s="49"/>
+    </row>
+    <row r="22" spans="1:26" s="10" customFormat="1" ht="24.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>18</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="C22" s="33"/>
       <c r="D22" s="13"/>
@@ -14781,7 +14825,7 @@
       <c r="F22" s="13"/>
       <c r="G22" s="13"/>
       <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
+      <c r="I22" s="49"/>
     </row>
     <row r="23" spans="1:26" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="27">
@@ -14789,7 +14833,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C23" s="33"/>
       <c r="D23" s="13"/>
@@ -14797,7 +14841,7 @@
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
+      <c r="I23" s="49"/>
     </row>
     <row r="24" spans="1:26" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="27">
@@ -14805,7 +14849,7 @@
         <v>20</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C24" s="33"/>
       <c r="D24" s="13"/>
@@ -14813,7 +14857,7 @@
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
+      <c r="I24" s="49"/>
     </row>
     <row r="25" spans="1:26" s="10" customFormat="1" ht="20.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="27">
@@ -14829,7 +14873,7 @@
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
       <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
+      <c r="I25" s="49"/>
     </row>
     <row r="26" spans="1:26" s="10" customFormat="1" ht="20.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="27">
@@ -14837,7 +14881,7 @@
         <v>22</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C26" s="34"/>
       <c r="D26" s="13"/>
@@ -14845,7 +14889,7 @@
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
+      <c r="I26" s="49"/>
     </row>
     <row r="27" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="27">
@@ -14853,18 +14897,18 @@
         <v>23</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C27" s="34"/>
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
       <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
+      <c r="I27" s="49"/>
     </row>
     <row r="28" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="46" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B28" s="47"/>
       <c r="C28" s="47"/>
@@ -14898,14 +14942,14 @@
         <v>24</v>
       </c>
       <c r="B29" s="30" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C29" s="34"/>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
       <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
+      <c r="I29" s="49"/>
     </row>
     <row r="30" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="27">
@@ -14913,14 +14957,14 @@
         <v>25</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C30" s="34"/>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
       <c r="G30" s="13"/>
       <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
+      <c r="I30" s="49"/>
     </row>
     <row r="31" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="27">
@@ -14928,14 +14972,14 @@
         <v>26</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C31" s="34"/>
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
       <c r="G31" s="13"/>
       <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
+      <c r="I31" s="49"/>
     </row>
     <row r="32" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="27">
@@ -14943,14 +14987,14 @@
         <v>27</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C32" s="34"/>
       <c r="E32" s="13"/>
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
+      <c r="I32" s="49"/>
     </row>
     <row r="33" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="27">
@@ -14958,14 +15002,14 @@
         <v>28</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C33" s="34"/>
       <c r="E33" s="13"/>
       <c r="F33" s="13"/>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
+      <c r="I33" s="49"/>
     </row>
     <row r="34" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="27">
@@ -14973,14 +15017,14 @@
         <v>29</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C34" s="34"/>
       <c r="E34" s="13"/>
       <c r="F34" s="13"/>
       <c r="G34" s="13"/>
       <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
+      <c r="I34" s="49"/>
     </row>
     <row r="35" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="27">
@@ -14988,14 +15032,14 @@
         <v>30</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C35" s="34"/>
       <c r="E35" s="13"/>
       <c r="F35" s="13"/>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
+      <c r="I35" s="49"/>
     </row>
     <row r="36" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="27">
@@ -15003,18 +15047,18 @@
         <v>31</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C36" s="34"/>
       <c r="E36" s="13"/>
       <c r="F36" s="13"/>
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
+      <c r="I36" s="49"/>
     </row>
     <row r="37" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="46" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B37" s="47"/>
       <c r="C37" s="47"/>
@@ -15048,15 +15092,17 @@
         <v>32</v>
       </c>
       <c r="B38" s="29" t="s">
-        <v>132</v>
-      </c>
-      <c r="C38" s="33"/>
+        <v>131</v>
+      </c>
+      <c r="C38" s="33" t="s">
+        <v>206</v>
+      </c>
       <c r="D38" s="13"/>
       <c r="E38" s="13"/>
       <c r="F38" s="13"/>
       <c r="G38" s="13"/>
       <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
+      <c r="I38" s="49"/>
     </row>
     <row r="39" spans="1:26" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="27">
@@ -15064,7 +15110,7 @@
         <v>33</v>
       </c>
       <c r="B39" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C39" s="33"/>
       <c r="D39" s="13"/>
@@ -15072,7 +15118,7 @@
       <c r="F39" s="13"/>
       <c r="G39" s="13"/>
       <c r="H39" s="13"/>
-      <c r="I39" s="13"/>
+      <c r="I39" s="49"/>
     </row>
     <row r="40" spans="1:26" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="27">
@@ -15080,7 +15126,7 @@
         <v>34</v>
       </c>
       <c r="B40" s="30" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C40" s="33"/>
       <c r="D40" s="13"/>
@@ -15088,7 +15134,7 @@
       <c r="F40" s="13"/>
       <c r="G40" s="13"/>
       <c r="H40" s="13"/>
-      <c r="I40" s="13"/>
+      <c r="I40" s="49"/>
     </row>
     <row r="41" spans="1:26" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="27">
@@ -15096,7 +15142,7 @@
         <v>35</v>
       </c>
       <c r="B41" s="29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C41" s="33"/>
       <c r="D41" s="13"/>
@@ -15104,7 +15150,7 @@
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
       <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
+      <c r="I41" s="49"/>
     </row>
     <row r="42" spans="1:26" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="27">
@@ -15112,7 +15158,7 @@
         <v>36</v>
       </c>
       <c r="B42" s="29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C42" s="33"/>
       <c r="D42" s="13"/>
@@ -15120,7 +15166,7 @@
       <c r="F42" s="13"/>
       <c r="G42" s="13"/>
       <c r="H42" s="13"/>
-      <c r="I42" s="13"/>
+      <c r="I42" s="49"/>
     </row>
     <row r="43" spans="1:26" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="27">
@@ -15128,7 +15174,7 @@
         <v>37</v>
       </c>
       <c r="B43" s="29" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C43" s="33"/>
       <c r="D43" s="13"/>
@@ -15136,7 +15182,7 @@
       <c r="F43" s="13"/>
       <c r="G43" s="13"/>
       <c r="H43" s="13"/>
-      <c r="I43" s="13"/>
+      <c r="I43" s="49"/>
     </row>
     <row r="44" spans="1:26" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="27">
@@ -15144,7 +15190,7 @@
         <v>38</v>
       </c>
       <c r="B44" s="29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C44" s="33"/>
       <c r="D44" s="13"/>
@@ -15152,7 +15198,7 @@
       <c r="F44" s="13"/>
       <c r="G44" s="13"/>
       <c r="H44" s="13"/>
-      <c r="I44" s="13"/>
+      <c r="I44" s="49"/>
     </row>
     <row r="45" spans="1:26" s="10" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="27">
@@ -15160,7 +15206,7 @@
         <v>39</v>
       </c>
       <c r="B45" s="29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C45" s="33"/>
       <c r="D45" s="13"/>
@@ -15168,7 +15214,7 @@
       <c r="F45" s="13"/>
       <c r="G45" s="13"/>
       <c r="H45" s="13"/>
-      <c r="I45" s="13"/>
+      <c r="I45" s="49"/>
     </row>
     <row r="46" spans="1:26" s="10" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="27">
@@ -15176,7 +15222,7 @@
         <v>40</v>
       </c>
       <c r="B46" s="29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C46" s="33"/>
       <c r="D46" s="13"/>
@@ -15184,7 +15230,7 @@
       <c r="F46" s="13"/>
       <c r="G46" s="13"/>
       <c r="H46" s="13"/>
-      <c r="I46" s="13"/>
+      <c r="I46" s="49"/>
     </row>
     <row r="47" spans="1:26" s="10" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="27">
@@ -15200,7 +15246,7 @@
       <c r="F47" s="13"/>
       <c r="G47" s="13"/>
       <c r="H47" s="13"/>
-      <c r="I47" s="13"/>
+      <c r="I47" s="49"/>
     </row>
     <row r="48" spans="1:26" s="10" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="27">
@@ -15208,7 +15254,7 @@
         <v>42</v>
       </c>
       <c r="B48" s="29" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C48" s="33"/>
       <c r="D48" s="13"/>
@@ -15216,7 +15262,7 @@
       <c r="F48" s="13"/>
       <c r="G48" s="13"/>
       <c r="H48" s="13"/>
-      <c r="I48" s="13"/>
+      <c r="I48" s="49"/>
     </row>
     <row r="49" spans="1:9" s="10" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="27">
@@ -15224,7 +15270,7 @@
         <v>43</v>
       </c>
       <c r="B49" s="29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C49" s="33"/>
       <c r="D49" s="13"/>
@@ -15232,7 +15278,7 @@
       <c r="F49" s="13"/>
       <c r="G49" s="13"/>
       <c r="H49" s="13"/>
-      <c r="I49" s="13"/>
+      <c r="I49" s="49"/>
     </row>
     <row r="50" spans="1:9" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="27">
@@ -15240,7 +15286,7 @@
         <v>44</v>
       </c>
       <c r="B50" s="30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C50" s="33"/>
       <c r="D50" s="13"/>
@@ -15248,7 +15294,7 @@
       <c r="F50" s="13"/>
       <c r="G50" s="13"/>
       <c r="H50" s="13"/>
-      <c r="I50" s="13"/>
+      <c r="I50" s="49"/>
     </row>
     <row r="51" spans="1:9" s="10" customFormat="1" ht="24.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="27">
@@ -15256,7 +15302,7 @@
         <v>45</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C51" s="33"/>
       <c r="D51" s="13"/>
@@ -15264,11 +15310,11 @@
       <c r="F51" s="13"/>
       <c r="G51" s="13"/>
       <c r="H51" s="13"/>
-      <c r="I51" s="13"/>
+      <c r="I51" s="49"/>
     </row>
     <row r="52" spans="1:9" s="10" customFormat="1" ht="21.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="46" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B52" s="47"/>
       <c r="C52" s="47"/>
@@ -15285,14 +15331,14 @@
         <v>46</v>
       </c>
       <c r="B53" s="30" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C53" s="34"/>
       <c r="E53" s="13"/>
       <c r="F53" s="13"/>
       <c r="G53" s="13"/>
       <c r="H53" s="13"/>
-      <c r="I53" s="13"/>
+      <c r="I53" s="49"/>
     </row>
     <row r="54" spans="1:9" s="10" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="27">
@@ -15300,7 +15346,7 @@
         <v>47</v>
       </c>
       <c r="B54" s="30" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C54" s="33"/>
       <c r="D54" s="13"/>
@@ -15308,15 +15354,15 @@
       <c r="F54" s="13"/>
       <c r="G54" s="13"/>
       <c r="H54" s="13"/>
-      <c r="I54" s="13"/>
-    </row>
-    <row r="55" spans="1:9" s="10" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I54" s="49"/>
+    </row>
+    <row r="55" spans="1:9" s="10" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>48</v>
       </c>
       <c r="B55" s="30" t="s">
-        <v>150</v>
+        <v>205</v>
       </c>
       <c r="C55" s="33"/>
       <c r="D55" s="13"/>
@@ -15324,15 +15370,15 @@
       <c r="F55" s="13"/>
       <c r="G55" s="13"/>
       <c r="H55" s="13"/>
-      <c r="I55" s="13"/>
-    </row>
-    <row r="56" spans="1:9" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I55" s="49"/>
+    </row>
+    <row r="56" spans="1:9" s="10" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>49</v>
       </c>
       <c r="B56" s="30" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C56" s="33"/>
       <c r="D56" s="13"/>
@@ -15340,15 +15386,15 @@
       <c r="F56" s="13"/>
       <c r="G56" s="13"/>
       <c r="H56" s="13"/>
-      <c r="I56" s="13"/>
-    </row>
-    <row r="57" spans="1:9" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I56" s="49"/>
+    </row>
+    <row r="57" spans="1:9" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>50</v>
       </c>
       <c r="B57" s="30" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C57" s="33"/>
       <c r="D57" s="13"/>
@@ -15356,44 +15402,44 @@
       <c r="F57" s="13"/>
       <c r="G57" s="13"/>
       <c r="H57" s="13"/>
-      <c r="I57" s="13"/>
-    </row>
-    <row r="58" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="46" t="s">
-        <v>155</v>
-      </c>
-      <c r="B58" s="47"/>
-      <c r="C58" s="47"/>
-      <c r="D58" s="47"/>
-      <c r="E58" s="47"/>
-      <c r="F58" s="47"/>
-      <c r="G58" s="47"/>
-      <c r="H58" s="47"/>
-      <c r="I58" s="47"/>
-    </row>
-    <row r="59" spans="1:9" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="27">
-        <f ca="1">IF(OFFSET(A59,-2,0) ="",OFFSET(A59,-2,0)+1,OFFSET(A59,-2,0)+1 )</f>
+      <c r="I57" s="49"/>
+    </row>
+    <row r="58" spans="1:9" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="27">
+        <f t="shared" ca="1" si="0"/>
         <v>51</v>
       </c>
-      <c r="B59" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="C59" s="33"/>
-      <c r="D59" s="13"/>
-      <c r="E59" s="13"/>
-      <c r="F59" s="13"/>
-      <c r="G59" s="13"/>
-      <c r="H59" s="13"/>
-      <c r="I59" s="13"/>
-    </row>
-    <row r="60" spans="1:9" s="10" customFormat="1" ht="25" x14ac:dyDescent="0.25">
+      <c r="B58" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="C58" s="33"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="49"/>
+    </row>
+    <row r="59" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="46" t="s">
+        <v>154</v>
+      </c>
+      <c r="B59" s="47"/>
+      <c r="C59" s="47"/>
+      <c r="D59" s="47"/>
+      <c r="E59" s="47"/>
+      <c r="F59" s="47"/>
+      <c r="G59" s="47"/>
+      <c r="H59" s="47"/>
+      <c r="I59" s="47"/>
+    </row>
+    <row r="60" spans="1:9" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">IF(OFFSET(A60,-2,0) ="",OFFSET(A60,-2,0)+1,OFFSET(A60,-2,0)+1 )</f>
         <v>52</v>
       </c>
       <c r="B60" s="30" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C60" s="33"/>
       <c r="D60" s="13"/>
@@ -15401,15 +15447,15 @@
       <c r="F60" s="13"/>
       <c r="G60" s="13"/>
       <c r="H60" s="13"/>
-      <c r="I60" s="13"/>
-    </row>
-    <row r="61" spans="1:9" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I60" s="49"/>
+    </row>
+    <row r="61" spans="1:9" s="10" customFormat="1" ht="25" x14ac:dyDescent="0.25">
       <c r="A61" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>53</v>
       </c>
       <c r="B61" s="30" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C61" s="33"/>
       <c r="D61" s="13"/>
@@ -15417,7 +15463,7 @@
       <c r="F61" s="13"/>
       <c r="G61" s="13"/>
       <c r="H61" s="13"/>
-      <c r="I61" s="13"/>
+      <c r="I61" s="49"/>
     </row>
     <row r="62" spans="1:9" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="27">
@@ -15425,7 +15471,7 @@
         <v>54</v>
       </c>
       <c r="B62" s="30" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C62" s="33"/>
       <c r="D62" s="13"/>
@@ -15433,84 +15479,84 @@
       <c r="F62" s="13"/>
       <c r="G62" s="13"/>
       <c r="H62" s="13"/>
-      <c r="I62" s="13"/>
-    </row>
-    <row r="63" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="46" t="s">
-        <v>156</v>
-      </c>
-      <c r="B63" s="47"/>
-      <c r="C63" s="47"/>
-      <c r="D63" s="47"/>
-      <c r="E63" s="47"/>
-      <c r="F63" s="47"/>
-      <c r="G63" s="47"/>
-      <c r="H63" s="47"/>
-      <c r="I63" s="47"/>
-    </row>
-    <row r="64" spans="1:9" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="27">
-        <f ca="1">IF(OFFSET(A64,-2,0) ="",OFFSET(A64,-2,0)+1,OFFSET(A64,-2,0)+1 )</f>
+      <c r="I62" s="49"/>
+    </row>
+    <row r="63" spans="1:9" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="27">
+        <f t="shared" ca="1" si="0"/>
         <v>55</v>
       </c>
-      <c r="B64" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="C64" s="33"/>
-      <c r="E64" s="13"/>
-      <c r="F64" s="13"/>
-      <c r="G64" s="13"/>
-      <c r="H64" s="13"/>
-      <c r="I64" s="13"/>
-    </row>
-    <row r="65" spans="1:26" s="10" customFormat="1" ht="25" x14ac:dyDescent="0.25">
+      <c r="B63" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="C63" s="33"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="13"/>
+      <c r="I63" s="49"/>
+    </row>
+    <row r="64" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="46" t="s">
+        <v>155</v>
+      </c>
+      <c r="B64" s="47"/>
+      <c r="C64" s="47"/>
+      <c r="D64" s="47"/>
+      <c r="E64" s="47"/>
+      <c r="F64" s="47"/>
+      <c r="G64" s="47"/>
+      <c r="H64" s="47"/>
+      <c r="I64" s="47"/>
+    </row>
+    <row r="65" spans="1:9" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">IF(OFFSET(A65,-2,0) ="",OFFSET(A65,-2,0)+1,OFFSET(A65,-2,0)+1 )</f>
         <v>56</v>
       </c>
       <c r="B65" s="30" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="C65" s="33"/>
       <c r="E65" s="13"/>
       <c r="F65" s="13"/>
       <c r="G65" s="13"/>
       <c r="H65" s="13"/>
-      <c r="I65" s="13"/>
-    </row>
-    <row r="66" spans="1:26" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I65" s="49"/>
+    </row>
+    <row r="66" spans="1:9" s="10" customFormat="1" ht="25" x14ac:dyDescent="0.25">
       <c r="A66" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>57</v>
       </c>
-      <c r="B66" s="29" t="s">
-        <v>157</v>
+      <c r="B66" s="30" t="s">
+        <v>134</v>
       </c>
       <c r="C66" s="33"/>
-      <c r="D66" s="30"/>
       <c r="E66" s="13"/>
       <c r="F66" s="13"/>
       <c r="G66" s="13"/>
       <c r="H66" s="13"/>
-      <c r="I66" s="13"/>
-    </row>
-    <row r="67" spans="1:26" s="10" customFormat="1" ht="25" x14ac:dyDescent="0.25">
+      <c r="I66" s="49"/>
+    </row>
+    <row r="67" spans="1:9" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>58</v>
       </c>
       <c r="B67" s="29" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C67" s="33"/>
-      <c r="D67" s="13"/>
+      <c r="D67" s="30"/>
       <c r="E67" s="13"/>
       <c r="F67" s="13"/>
       <c r="G67" s="13"/>
       <c r="H67" s="13"/>
-      <c r="I67" s="13"/>
-    </row>
-    <row r="68" spans="1:26" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I67" s="49"/>
+    </row>
+    <row r="68" spans="1:9" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>59</v>
@@ -15524,15 +15570,15 @@
       <c r="F68" s="13"/>
       <c r="G68" s="13"/>
       <c r="H68" s="13"/>
-      <c r="I68" s="13"/>
-    </row>
-    <row r="69" spans="1:26" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I68" s="49"/>
+    </row>
+    <row r="69" spans="1:9" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>60</v>
       </c>
       <c r="B69" s="29" t="s">
-        <v>130</v>
+        <v>157</v>
       </c>
       <c r="C69" s="33"/>
       <c r="D69" s="13"/>
@@ -15540,15 +15586,15 @@
       <c r="F69" s="13"/>
       <c r="G69" s="13"/>
       <c r="H69" s="13"/>
-      <c r="I69" s="13"/>
-    </row>
-    <row r="70" spans="1:26" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I69" s="49"/>
+    </row>
+    <row r="70" spans="1:9" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>61</v>
       </c>
       <c r="B70" s="29" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="C70" s="33"/>
       <c r="D70" s="13"/>
@@ -15556,15 +15602,15 @@
       <c r="F70" s="13"/>
       <c r="G70" s="13"/>
       <c r="H70" s="13"/>
-      <c r="I70" s="13"/>
-    </row>
-    <row r="71" spans="1:26" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I70" s="49"/>
+    </row>
+    <row r="71" spans="1:9" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>62</v>
       </c>
       <c r="B71" s="29" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C71" s="33"/>
       <c r="D71" s="13"/>
@@ -15572,15 +15618,15 @@
       <c r="F71" s="13"/>
       <c r="G71" s="13"/>
       <c r="H71" s="13"/>
-      <c r="I71" s="13"/>
-    </row>
-    <row r="72" spans="1:26" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I71" s="49"/>
+    </row>
+    <row r="72" spans="1:9" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>63</v>
       </c>
       <c r="B72" s="29" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="C72" s="33"/>
       <c r="D72" s="13"/>
@@ -15588,15 +15634,15 @@
       <c r="F72" s="13"/>
       <c r="G72" s="13"/>
       <c r="H72" s="13"/>
-      <c r="I72" s="13"/>
-    </row>
-    <row r="73" spans="1:26" s="10" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I72" s="49"/>
+    </row>
+    <row r="73" spans="1:9" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>64</v>
       </c>
-      <c r="B73" s="30" t="s">
-        <v>160</v>
+      <c r="B73" s="29" t="s">
+        <v>126</v>
       </c>
       <c r="C73" s="33"/>
       <c r="D73" s="13"/>
@@ -15604,15 +15650,15 @@
       <c r="F73" s="13"/>
       <c r="G73" s="13"/>
       <c r="H73" s="13"/>
-      <c r="I73" s="13"/>
-    </row>
-    <row r="74" spans="1:26" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I73" s="49"/>
+    </row>
+    <row r="74" spans="1:9" s="10" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>65</v>
       </c>
       <c r="B74" s="30" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C74" s="33"/>
       <c r="D74" s="13"/>
@@ -15620,15 +15666,15 @@
       <c r="F74" s="13"/>
       <c r="G74" s="13"/>
       <c r="H74" s="13"/>
-      <c r="I74" s="13"/>
-    </row>
-    <row r="75" spans="1:26" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I74" s="49"/>
+    </row>
+    <row r="75" spans="1:9" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>66</v>
       </c>
-      <c r="B75" s="15" t="s">
-        <v>146</v>
+      <c r="B75" s="30" t="s">
+        <v>160</v>
       </c>
       <c r="C75" s="33"/>
       <c r="D75" s="13"/>
@@ -15636,74 +15682,57 @@
       <c r="F75" s="13"/>
       <c r="G75" s="13"/>
       <c r="H75" s="13"/>
-      <c r="I75" s="13"/>
-    </row>
-    <row r="76" spans="1:26" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="39" t="s">
-        <v>168</v>
-      </c>
-      <c r="B76" s="48"/>
-      <c r="C76" s="48"/>
-      <c r="D76" s="48"/>
-      <c r="E76" s="48"/>
-      <c r="F76" s="48"/>
-      <c r="G76" s="48"/>
-      <c r="H76" s="48"/>
-      <c r="I76" s="48"/>
-    </row>
-    <row r="77" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="46" t="s">
+      <c r="I75" s="49"/>
+    </row>
+    <row r="76" spans="1:9" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="B76" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="C76" s="33"/>
+      <c r="D76" s="13"/>
+      <c r="E76" s="13"/>
+      <c r="F76" s="13"/>
+      <c r="G76" s="13"/>
+      <c r="H76" s="13"/>
+      <c r="I76" s="49"/>
+    </row>
+    <row r="77" spans="1:9" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="B77" s="48"/>
+      <c r="C77" s="48"/>
+      <c r="D77" s="48"/>
+      <c r="E77" s="48"/>
+      <c r="F77" s="48"/>
+      <c r="G77" s="48"/>
+      <c r="H77" s="48"/>
+      <c r="I77" s="48"/>
+    </row>
+    <row r="78" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="46" t="s">
+        <v>174</v>
+      </c>
+      <c r="B78" s="47"/>
+      <c r="C78" s="47"/>
+      <c r="D78" s="47"/>
+      <c r="E78" s="47"/>
+      <c r="F78" s="47"/>
+      <c r="G78" s="47"/>
+      <c r="H78" s="47"/>
+      <c r="I78" s="47"/>
+    </row>
+    <row r="79" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="27">
+        <f ca="1">IF(OFFSET(A79,-3,0) ="",OFFSET(A79,-3,0)+1,OFFSET(A79,-3,0)+1 )</f>
+        <v>68</v>
+      </c>
+      <c r="B79" s="30" t="s">
         <v>178</v>
-      </c>
-      <c r="B77" s="47"/>
-      <c r="C77" s="47"/>
-      <c r="D77" s="47"/>
-      <c r="E77" s="47"/>
-      <c r="F77" s="47"/>
-      <c r="G77" s="47"/>
-      <c r="H77" s="47"/>
-      <c r="I77" s="47"/>
-      <c r="J77" s="26"/>
-      <c r="K77" s="26"/>
-      <c r="L77" s="26"/>
-      <c r="M77" s="26"/>
-      <c r="N77" s="26"/>
-      <c r="O77" s="26"/>
-      <c r="P77" s="26"/>
-      <c r="Q77" s="26"/>
-      <c r="R77" s="26"/>
-      <c r="S77" s="26"/>
-      <c r="T77" s="26"/>
-      <c r="U77" s="26"/>
-      <c r="V77" s="26"/>
-      <c r="W77" s="26"/>
-      <c r="X77" s="26"/>
-      <c r="Y77" s="26"/>
-      <c r="Z77" s="26"/>
-    </row>
-    <row r="78" spans="1:26" s="10" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="27">
-        <f ca="1">IF(OFFSET(A78,-3,0) ="",OFFSET(A78,-3,0)+1,OFFSET(A78,-3,0)+1 )</f>
-        <v>67</v>
-      </c>
-      <c r="B78" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="C78" s="34"/>
-      <c r="D78" s="13"/>
-      <c r="E78" s="13"/>
-      <c r="F78" s="13"/>
-      <c r="G78" s="13"/>
-      <c r="H78" s="13"/>
-      <c r="I78" s="13"/>
-    </row>
-    <row r="79" spans="1:26" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="27">
-        <f ca="1">IF(OFFSET(A79,-1,0) ="",OFFSET(A79,-2,0)+1,OFFSET(A79,-1,0)+1 )</f>
-        <v>68</v>
-      </c>
-      <c r="B79" s="12" t="s">
-        <v>182</v>
       </c>
       <c r="C79" s="33"/>
       <c r="D79" s="13"/>
@@ -15711,15 +15740,15 @@
       <c r="F79" s="13"/>
       <c r="G79" s="13"/>
       <c r="H79" s="13"/>
-      <c r="I79" s="13"/>
-    </row>
-    <row r="80" spans="1:26" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I79" s="49"/>
+    </row>
+    <row r="80" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="27">
-        <f ca="1">IF(OFFSET(A80,-1,0) ="",OFFSET(A80,-2,0)+1,OFFSET(A80,-1,0)+1 )</f>
+        <f t="shared" ref="A80:A87" ca="1" si="2">IF(OFFSET(A80,-1,0) ="",OFFSET(A80,-2,0)+1,OFFSET(A80,-1,0)+1 )</f>
         <v>69</v>
       </c>
-      <c r="B80" s="15" t="s">
-        <v>193</v>
+      <c r="B80" s="30" t="s">
+        <v>182</v>
       </c>
       <c r="C80" s="33"/>
       <c r="D80" s="13"/>
@@ -15727,73 +15756,81 @@
       <c r="F80" s="13"/>
       <c r="G80" s="13"/>
       <c r="H80" s="13"/>
-      <c r="I80" s="13"/>
-    </row>
-    <row r="81" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="46" t="s">
-        <v>162</v>
-      </c>
-      <c r="B81" s="47"/>
-      <c r="C81" s="47"/>
-      <c r="D81" s="47"/>
-      <c r="E81" s="47"/>
-      <c r="F81" s="47"/>
-      <c r="G81" s="47"/>
-      <c r="H81" s="47"/>
-      <c r="I81" s="47"/>
-    </row>
-    <row r="82" spans="1:9" s="10" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I80" s="49"/>
+    </row>
+    <row r="81" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="B81" s="30" t="s">
+        <v>179</v>
+      </c>
+      <c r="C81" s="33"/>
+      <c r="D81" s="13"/>
+      <c r="E81" s="13"/>
+      <c r="F81" s="13"/>
+      <c r="G81" s="13"/>
+      <c r="H81" s="13"/>
+      <c r="I81" s="49"/>
+    </row>
+    <row r="82" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="27">
-        <f ca="1">IF(OFFSET(A82,-2,0) ="",OFFSET(A82,-2,0)+1,OFFSET(A82,-2,0)+1 )</f>
-        <v>70</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>71</v>
       </c>
       <c r="B82" s="30" t="s">
-        <v>163</v>
-      </c>
-      <c r="C82" s="33"/>
-      <c r="D82" s="13"/>
+        <v>183</v>
+      </c>
+      <c r="C82" s="33" t="s">
+        <v>180</v>
+      </c>
+      <c r="D82" s="30"/>
       <c r="E82" s="13"/>
       <c r="F82" s="13"/>
       <c r="G82" s="13"/>
       <c r="H82" s="13"/>
-      <c r="I82" s="13"/>
-    </row>
-    <row r="83" spans="1:9" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I82" s="49"/>
+    </row>
+    <row r="83" spans="1:9" s="10" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="27">
-        <f t="shared" ref="A83" ca="1" si="2">IF(OFFSET(A83,-1,0) ="",OFFSET(A83,-2,0)+1,OFFSET(A83,-1,0)+1 )</f>
-        <v>71</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>72</v>
       </c>
       <c r="B83" s="30" t="s">
-        <v>164</v>
+        <v>184</v>
       </c>
       <c r="C83" s="33"/>
-      <c r="D83" s="13"/>
+      <c r="D83" s="30"/>
       <c r="E83" s="13"/>
       <c r="F83" s="13"/>
       <c r="G83" s="13"/>
       <c r="H83" s="13"/>
-      <c r="I83" s="13"/>
-    </row>
-    <row r="84" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="46" t="s">
-        <v>165</v>
-      </c>
-      <c r="B84" s="47"/>
-      <c r="C84" s="47"/>
-      <c r="D84" s="47"/>
-      <c r="E84" s="47"/>
-      <c r="F84" s="47"/>
-      <c r="G84" s="47"/>
-      <c r="H84" s="47"/>
-      <c r="I84" s="47"/>
-    </row>
-    <row r="85" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I83" s="49"/>
+    </row>
+    <row r="84" spans="1:9" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>73</v>
+      </c>
+      <c r="B84" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="C84" s="33"/>
+      <c r="D84" s="30"/>
+      <c r="E84" s="13"/>
+      <c r="F84" s="13"/>
+      <c r="G84" s="13"/>
+      <c r="H84" s="13"/>
+      <c r="I84" s="49"/>
+    </row>
+    <row r="85" spans="1:9" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="27">
-        <f ca="1">IF(OFFSET(A85,-2,0) ="",OFFSET(A85,-2,0)+1,OFFSET(A85,-2,0)+1 )</f>
-        <v>72</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>74</v>
       </c>
       <c r="B85" s="30" t="s">
-        <v>166</v>
+        <v>186</v>
       </c>
       <c r="C85" s="33"/>
       <c r="D85" s="13"/>
@@ -15801,28 +15838,31 @@
       <c r="F85" s="13"/>
       <c r="G85" s="13"/>
       <c r="H85" s="13"/>
-      <c r="I85" s="13"/>
-    </row>
-    <row r="86" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="B86" s="47"/>
-      <c r="C86" s="47"/>
-      <c r="D86" s="47"/>
-      <c r="E86" s="47"/>
-      <c r="F86" s="47"/>
-      <c r="G86" s="47"/>
-      <c r="H86" s="47"/>
-      <c r="I86" s="47"/>
-    </row>
-    <row r="87" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I85" s="49"/>
+    </row>
+    <row r="86" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>75</v>
+      </c>
+      <c r="B86" s="30" t="s">
+        <v>202</v>
+      </c>
+      <c r="C86" s="33"/>
+      <c r="D86" s="13"/>
+      <c r="E86" s="13"/>
+      <c r="F86" s="13"/>
+      <c r="G86" s="13"/>
+      <c r="H86" s="13"/>
+      <c r="I86" s="49"/>
+    </row>
+    <row r="87" spans="1:9" s="10" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="27">
-        <f ca="1">IF(OFFSET(A87,-2,0) ="",OFFSET(A87,-2,0)+1,OFFSET(A87,-2,0)+1 )</f>
-        <v>73</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>76</v>
       </c>
       <c r="B87" s="30" t="s">
-        <v>166</v>
+        <v>187</v>
       </c>
       <c r="C87" s="33"/>
       <c r="D87" s="13"/>
@@ -15830,11 +15870,11 @@
       <c r="F87" s="13"/>
       <c r="G87" s="13"/>
       <c r="H87" s="13"/>
-      <c r="I87" s="13"/>
-    </row>
-    <row r="88" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I87" s="49"/>
+    </row>
+    <row r="88" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="46" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="B88" s="47"/>
       <c r="C88" s="47"/>
@@ -15845,13 +15885,13 @@
       <c r="H88" s="47"/>
       <c r="I88" s="47"/>
     </row>
-    <row r="89" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="27">
         <f ca="1">IF(OFFSET(A89,-2,0) ="",OFFSET(A89,-2,0)+1,OFFSET(A89,-2,0)+1 )</f>
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B89" s="30" t="s">
-        <v>166</v>
+        <v>189</v>
       </c>
       <c r="C89" s="33"/>
       <c r="D89" s="13"/>
@@ -15859,28 +15899,31 @@
       <c r="F89" s="13"/>
       <c r="G89" s="13"/>
       <c r="H89" s="13"/>
-      <c r="I89" s="13"/>
-    </row>
-    <row r="90" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="46" t="s">
-        <v>175</v>
-      </c>
-      <c r="B90" s="47"/>
-      <c r="C90" s="47"/>
-      <c r="D90" s="47"/>
-      <c r="E90" s="47"/>
-      <c r="F90" s="47"/>
-      <c r="G90" s="47"/>
-      <c r="H90" s="47"/>
-      <c r="I90" s="47"/>
-    </row>
-    <row r="91" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I89" s="49"/>
+    </row>
+    <row r="90" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="27">
+        <f t="shared" ref="A90:A97" ca="1" si="3">IF(OFFSET(A90,-1,0) ="",OFFSET(A90,-2,0)+1,OFFSET(A90,-1,0)+1 )</f>
+        <v>78</v>
+      </c>
+      <c r="B90" s="30" t="s">
+        <v>190</v>
+      </c>
+      <c r="C90" s="33"/>
+      <c r="D90" s="13"/>
+      <c r="E90" s="13"/>
+      <c r="F90" s="13"/>
+      <c r="G90" s="13"/>
+      <c r="H90" s="13"/>
+      <c r="I90" s="49"/>
+    </row>
+    <row r="91" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="27">
-        <f ca="1">IF(OFFSET(A91,-2,0) ="",OFFSET(A91,-2,0)+1,OFFSET(A91,-2,0)+1 )</f>
-        <v>75</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>79</v>
       </c>
       <c r="B91" s="30" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="C91" s="33"/>
       <c r="D91" s="13"/>
@@ -15888,97 +15931,97 @@
       <c r="F91" s="13"/>
       <c r="G91" s="13"/>
       <c r="H91" s="13"/>
-      <c r="I91" s="13"/>
-    </row>
-    <row r="92" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I91" s="49"/>
+    </row>
+    <row r="92" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="27">
-        <f t="shared" ref="A92:A99" ca="1" si="3">IF(OFFSET(A92,-1,0) ="",OFFSET(A92,-2,0)+1,OFFSET(A92,-1,0)+1 )</f>
-        <v>76</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>80</v>
       </c>
       <c r="B92" s="30" t="s">
-        <v>183</v>
-      </c>
-      <c r="C92" s="33"/>
-      <c r="D92" s="13"/>
+        <v>194</v>
+      </c>
+      <c r="C92" s="33" t="s">
+        <v>180</v>
+      </c>
+      <c r="D92" s="30"/>
       <c r="E92" s="13"/>
       <c r="F92" s="13"/>
       <c r="G92" s="13"/>
       <c r="H92" s="13"/>
-      <c r="I92" s="13"/>
-    </row>
-    <row r="93" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I92" s="49"/>
+    </row>
+    <row r="93" spans="1:9" s="10" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B93" s="30" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C93" s="33"/>
-      <c r="D93" s="13"/>
+      <c r="D93" s="30"/>
       <c r="E93" s="13"/>
       <c r="F93" s="13"/>
       <c r="G93" s="13"/>
       <c r="H93" s="13"/>
-      <c r="I93" s="13"/>
-    </row>
-    <row r="94" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I93" s="49"/>
+    </row>
+    <row r="94" spans="1:9" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B94" s="30" t="s">
-        <v>184</v>
-      </c>
-      <c r="C94" s="33" t="s">
-        <v>181</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="C94" s="33"/>
       <c r="D94" s="30"/>
       <c r="E94" s="13"/>
       <c r="F94" s="13"/>
       <c r="G94" s="13"/>
       <c r="H94" s="13"/>
-      <c r="I94" s="13"/>
-    </row>
-    <row r="95" spans="1:9" s="10" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I94" s="49"/>
+    </row>
+    <row r="95" spans="1:9" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B95" s="30" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C95" s="33"/>
-      <c r="D95" s="30"/>
+      <c r="D95" s="13"/>
       <c r="E95" s="13"/>
       <c r="F95" s="13"/>
       <c r="G95" s="13"/>
       <c r="H95" s="13"/>
-      <c r="I95" s="13"/>
-    </row>
-    <row r="96" spans="1:9" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I95" s="49"/>
+    </row>
+    <row r="96" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B96" s="30" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
       <c r="C96" s="33"/>
-      <c r="D96" s="30"/>
+      <c r="D96" s="13"/>
       <c r="E96" s="13"/>
       <c r="F96" s="13"/>
       <c r="G96" s="13"/>
       <c r="H96" s="13"/>
-      <c r="I96" s="13"/>
-    </row>
-    <row r="97" spans="1:9" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I96" s="49"/>
+    </row>
+    <row r="97" spans="1:26" s="10" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="27">
         <f t="shared" ca="1" si="3"/>
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B97" s="30" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C97" s="33"/>
       <c r="D97" s="13"/>
@@ -15986,31 +16029,28 @@
       <c r="F97" s="13"/>
       <c r="G97" s="13"/>
       <c r="H97" s="13"/>
-      <c r="I97" s="13"/>
-    </row>
-    <row r="98" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="27">
-        <f t="shared" ca="1" si="3"/>
-        <v>82</v>
-      </c>
-      <c r="B98" s="30" t="s">
-        <v>203</v>
-      </c>
-      <c r="C98" s="33"/>
-      <c r="D98" s="13"/>
-      <c r="E98" s="13"/>
-      <c r="F98" s="13"/>
-      <c r="G98" s="13"/>
-      <c r="H98" s="13"/>
-      <c r="I98" s="13"/>
-    </row>
-    <row r="99" spans="1:9" s="10" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I97" s="49"/>
+    </row>
+    <row r="98" spans="1:26" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="46" t="s">
+        <v>198</v>
+      </c>
+      <c r="B98" s="47"/>
+      <c r="C98" s="47"/>
+      <c r="D98" s="47"/>
+      <c r="E98" s="47"/>
+      <c r="F98" s="47"/>
+      <c r="G98" s="47"/>
+      <c r="H98" s="47"/>
+      <c r="I98" s="47"/>
+    </row>
+    <row r="99" spans="1:26" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="27">
-        <f t="shared" ca="1" si="3"/>
-        <v>83</v>
+        <f ca="1">IF(OFFSET(A99,-2,0) ="",OFFSET(A99,-2,0)+1,OFFSET(A99,-2,0)+1 )</f>
+        <v>86</v>
       </c>
       <c r="B99" s="30" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="C99" s="33"/>
       <c r="D99" s="13"/>
@@ -16018,11 +16058,11 @@
       <c r="F99" s="13"/>
       <c r="G99" s="13"/>
       <c r="H99" s="13"/>
-      <c r="I99" s="13"/>
-    </row>
-    <row r="100" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I99" s="49"/>
+    </row>
+    <row r="100" spans="1:26" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="46" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B100" s="47"/>
       <c r="C100" s="47"/>
@@ -16033,13 +16073,13 @@
       <c r="H100" s="47"/>
       <c r="I100" s="47"/>
     </row>
-    <row r="101" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:26" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="27">
         <f ca="1">IF(OFFSET(A101,-2,0) ="",OFFSET(A101,-2,0)+1,OFFSET(A101,-2,0)+1 )</f>
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B101" s="30" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="C101" s="33"/>
       <c r="D101" s="13"/>
@@ -16047,97 +16087,101 @@
       <c r="F101" s="13"/>
       <c r="G101" s="13"/>
       <c r="H101" s="13"/>
-      <c r="I101" s="13"/>
-    </row>
-    <row r="102" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="27">
-        <f t="shared" ref="A102:A109" ca="1" si="4">IF(OFFSET(A102,-1,0) ="",OFFSET(A102,-2,0)+1,OFFSET(A102,-1,0)+1 )</f>
-        <v>85</v>
-      </c>
-      <c r="B102" s="30" t="s">
-        <v>191</v>
-      </c>
+      <c r="I101" s="49"/>
+    </row>
+    <row r="102" spans="1:26" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="27"/>
+      <c r="B102" s="30"/>
       <c r="C102" s="33"/>
       <c r="D102" s="13"/>
       <c r="E102" s="13"/>
       <c r="F102" s="13"/>
       <c r="G102" s="13"/>
       <c r="H102" s="13"/>
-      <c r="I102" s="13"/>
-    </row>
-    <row r="103" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="27">
-        <f t="shared" ca="1" si="4"/>
-        <v>86</v>
-      </c>
-      <c r="B103" s="30" t="s">
-        <v>192</v>
-      </c>
-      <c r="C103" s="33"/>
-      <c r="D103" s="13"/>
-      <c r="E103" s="13"/>
-      <c r="F103" s="13"/>
-      <c r="G103" s="13"/>
-      <c r="H103" s="13"/>
-      <c r="I103" s="13"/>
-    </row>
-    <row r="104" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="27">
-        <f t="shared" ca="1" si="4"/>
-        <v>87</v>
-      </c>
-      <c r="B104" s="30" t="s">
-        <v>195</v>
-      </c>
-      <c r="C104" s="33" t="s">
-        <v>181</v>
-      </c>
-      <c r="D104" s="30"/>
-      <c r="E104" s="13"/>
-      <c r="F104" s="13"/>
-      <c r="G104" s="13"/>
-      <c r="H104" s="13"/>
-      <c r="I104" s="13"/>
-    </row>
-    <row r="105" spans="1:9" s="10" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I102" s="49"/>
+    </row>
+    <row r="103" spans="1:26" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="39" t="s">
+        <v>208</v>
+      </c>
+      <c r="B103" s="48"/>
+      <c r="C103" s="48"/>
+      <c r="D103" s="48"/>
+      <c r="E103" s="48"/>
+      <c r="F103" s="48"/>
+      <c r="G103" s="48"/>
+      <c r="H103" s="48"/>
+      <c r="I103" s="48"/>
+    </row>
+    <row r="104" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A104" s="46" t="s">
+        <v>177</v>
+      </c>
+      <c r="B104" s="47"/>
+      <c r="C104" s="47"/>
+      <c r="D104" s="47"/>
+      <c r="E104" s="47"/>
+      <c r="F104" s="47"/>
+      <c r="G104" s="47"/>
+      <c r="H104" s="47"/>
+      <c r="I104" s="47"/>
+      <c r="J104" s="26"/>
+      <c r="K104" s="26"/>
+      <c r="L104" s="26"/>
+      <c r="M104" s="26"/>
+      <c r="N104" s="26"/>
+      <c r="O104" s="26"/>
+      <c r="P104" s="26"/>
+      <c r="Q104" s="26"/>
+      <c r="R104" s="26"/>
+      <c r="S104" s="26"/>
+      <c r="T104" s="26"/>
+      <c r="U104" s="26"/>
+      <c r="V104" s="26"/>
+      <c r="W104" s="26"/>
+      <c r="X104" s="26"/>
+      <c r="Y104" s="26"/>
+      <c r="Z104" s="26"/>
+    </row>
+    <row r="105" spans="1:26" s="10" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="27">
-        <f t="shared" ca="1" si="4"/>
-        <v>88</v>
+        <f ca="1">IF(OFFSET(A105,-3,0) ="",OFFSET(A105,-3,0)+1,OFFSET(A105,-3,0)+1 )</f>
+        <v>1</v>
       </c>
       <c r="B105" s="30" t="s">
-        <v>185</v>
-      </c>
-      <c r="C105" s="33"/>
-      <c r="D105" s="30"/>
+        <v>121</v>
+      </c>
+      <c r="C105" s="34"/>
+      <c r="D105" s="13"/>
       <c r="E105" s="13"/>
       <c r="F105" s="13"/>
       <c r="G105" s="13"/>
       <c r="H105" s="13"/>
-      <c r="I105" s="13"/>
-    </row>
-    <row r="106" spans="1:9" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I105" s="49"/>
+    </row>
+    <row r="106" spans="1:26" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="27">
-        <f t="shared" ca="1" si="4"/>
-        <v>89</v>
-      </c>
-      <c r="B106" s="30" t="s">
-        <v>186</v>
+        <f ca="1">IF(OFFSET(A106,-1,0) ="",OFFSET(A106,-2,0)+1,OFFSET(A106,-1,0)+1 )</f>
+        <v>2</v>
+      </c>
+      <c r="B106" s="12" t="s">
+        <v>181</v>
       </c>
       <c r="C106" s="33"/>
-      <c r="D106" s="30"/>
+      <c r="D106" s="13"/>
       <c r="E106" s="13"/>
       <c r="F106" s="13"/>
       <c r="G106" s="13"/>
       <c r="H106" s="13"/>
-      <c r="I106" s="13"/>
-    </row>
-    <row r="107" spans="1:9" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I106" s="49"/>
+    </row>
+    <row r="107" spans="1:26" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="27">
-        <f t="shared" ca="1" si="4"/>
-        <v>90</v>
-      </c>
-      <c r="B107" s="30" t="s">
-        <v>187</v>
+        <f ca="1">IF(OFFSET(A107,-1,0) ="",OFFSET(A107,-2,0)+1,OFFSET(A107,-1,0)+1 )</f>
+        <v>3</v>
+      </c>
+      <c r="B107" s="15" t="s">
+        <v>192</v>
       </c>
       <c r="C107" s="33"/>
       <c r="D107" s="13"/>
@@ -16145,31 +16189,28 @@
       <c r="F107" s="13"/>
       <c r="G107" s="13"/>
       <c r="H107" s="13"/>
-      <c r="I107" s="13"/>
-    </row>
-    <row r="108" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="27">
-        <f t="shared" ca="1" si="4"/>
-        <v>91</v>
-      </c>
-      <c r="B108" s="30" t="s">
-        <v>203</v>
-      </c>
-      <c r="C108" s="33"/>
-      <c r="D108" s="13"/>
-      <c r="E108" s="13"/>
-      <c r="F108" s="13"/>
-      <c r="G108" s="13"/>
-      <c r="H108" s="13"/>
-      <c r="I108" s="13"/>
-    </row>
-    <row r="109" spans="1:9" s="10" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I107" s="49"/>
+    </row>
+    <row r="108" spans="1:26" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="46" t="s">
+        <v>161</v>
+      </c>
+      <c r="B108" s="47"/>
+      <c r="C108" s="47"/>
+      <c r="D108" s="47"/>
+      <c r="E108" s="47"/>
+      <c r="F108" s="47"/>
+      <c r="G108" s="47"/>
+      <c r="H108" s="47"/>
+      <c r="I108" s="47"/>
+    </row>
+    <row r="109" spans="1:26" s="10" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="27">
-        <f t="shared" ca="1" si="4"/>
-        <v>92</v>
+        <f ca="1">IF(OFFSET(A109,-2,0) ="",OFFSET(A109,-2,0)+1,OFFSET(A109,-2,0)+1 )</f>
+        <v>4</v>
       </c>
       <c r="B109" s="30" t="s">
-        <v>189</v>
+        <v>162</v>
       </c>
       <c r="C109" s="33"/>
       <c r="D109" s="13"/>
@@ -16177,98 +16218,110 @@
       <c r="F109" s="13"/>
       <c r="G109" s="13"/>
       <c r="H109" s="13"/>
-      <c r="I109" s="13"/>
-    </row>
-    <row r="110" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="46" t="s">
-        <v>199</v>
-      </c>
-      <c r="B110" s="47"/>
-      <c r="C110" s="47"/>
-      <c r="D110" s="47"/>
-      <c r="E110" s="47"/>
-      <c r="F110" s="47"/>
-      <c r="G110" s="47"/>
-      <c r="H110" s="47"/>
-      <c r="I110" s="47"/>
-    </row>
-    <row r="111" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="27">
-        <f ca="1">IF(OFFSET(A111,-2,0) ="",OFFSET(A111,-2,0)+1,OFFSET(A111,-2,0)+1 )</f>
-        <v>93</v>
-      </c>
-      <c r="B111" s="30" t="s">
-        <v>196</v>
-      </c>
-      <c r="C111" s="33"/>
-      <c r="D111" s="13"/>
-      <c r="E111" s="13"/>
-      <c r="F111" s="13"/>
-      <c r="G111" s="13"/>
-      <c r="H111" s="13"/>
-      <c r="I111" s="13"/>
-    </row>
-    <row r="112" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="46" t="s">
-        <v>200</v>
-      </c>
-      <c r="B112" s="47"/>
-      <c r="C112" s="47"/>
-      <c r="D112" s="47"/>
-      <c r="E112" s="47"/>
-      <c r="F112" s="47"/>
-      <c r="G112" s="47"/>
-      <c r="H112" s="47"/>
-      <c r="I112" s="47"/>
-    </row>
-    <row r="113" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="27">
-        <f ca="1">IF(OFFSET(A113,-2,0) ="",OFFSET(A113,-2,0)+1,OFFSET(A113,-2,0)+1 )</f>
-        <v>94</v>
-      </c>
-      <c r="B113" s="30" t="s">
-        <v>197</v>
-      </c>
-      <c r="C113" s="33"/>
-      <c r="D113" s="13"/>
-      <c r="E113" s="13"/>
-      <c r="F113" s="13"/>
-      <c r="G113" s="13"/>
-      <c r="H113" s="13"/>
-      <c r="I113" s="13"/>
+      <c r="I109" s="49"/>
+    </row>
+    <row r="110" spans="1:26" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="27">
+        <f t="shared" ref="A110" ca="1" si="4">IF(OFFSET(A110,-1,0) ="",OFFSET(A110,-2,0)+1,OFFSET(A110,-1,0)+1 )</f>
+        <v>5</v>
+      </c>
+      <c r="B110" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="C110" s="33"/>
+      <c r="D110" s="13"/>
+      <c r="E110" s="13"/>
+      <c r="F110" s="13"/>
+      <c r="G110" s="13"/>
+      <c r="H110" s="13"/>
+      <c r="I110" s="49"/>
+    </row>
+    <row r="111" spans="1:26" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="46" t="s">
+        <v>164</v>
+      </c>
+      <c r="B111" s="47"/>
+      <c r="C111" s="47"/>
+      <c r="D111" s="47"/>
+      <c r="E111" s="47"/>
+      <c r="F111" s="47"/>
+      <c r="G111" s="47"/>
+      <c r="H111" s="47"/>
+      <c r="I111" s="47"/>
+    </row>
+    <row r="112" spans="1:26" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="27">
+        <f ca="1">IF(OFFSET(A112,-2,0) ="",OFFSET(A112,-2,0)+1,OFFSET(A112,-2,0)+1 )</f>
+        <v>6</v>
+      </c>
+      <c r="B112" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="C112" s="33"/>
+      <c r="D112" s="13"/>
+      <c r="E112" s="13"/>
+      <c r="F112" s="13"/>
+      <c r="G112" s="13"/>
+      <c r="H112" s="13"/>
+      <c r="I112" s="49"/>
+    </row>
+    <row r="113" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="46" t="s">
+        <v>193</v>
+      </c>
+      <c r="B113" s="47"/>
+      <c r="C113" s="47"/>
+      <c r="D113" s="47"/>
+      <c r="E113" s="47"/>
+      <c r="F113" s="47"/>
+      <c r="G113" s="47"/>
+      <c r="H113" s="47"/>
+      <c r="I113" s="47"/>
     </row>
     <row r="114" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="27"/>
-      <c r="B114" s="30"/>
+      <c r="A114" s="27">
+        <f ca="1">IF(OFFSET(A114,-2,0) ="",OFFSET(A114,-2,0)+1,OFFSET(A114,-2,0)+1 )</f>
+        <v>7</v>
+      </c>
+      <c r="B114" s="30" t="s">
+        <v>165</v>
+      </c>
       <c r="C114" s="33"/>
       <c r="D114" s="13"/>
       <c r="E114" s="13"/>
       <c r="F114" s="13"/>
       <c r="G114" s="13"/>
       <c r="H114" s="13"/>
-      <c r="I114" s="13"/>
-    </row>
-    <row r="115" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="27"/>
-      <c r="B115" s="30"/>
-      <c r="C115" s="33"/>
-      <c r="D115" s="13"/>
-      <c r="E115" s="13"/>
-      <c r="F115" s="13"/>
-      <c r="G115" s="13"/>
-      <c r="H115" s="13"/>
-      <c r="I115" s="13"/>
+      <c r="I114" s="49"/>
+    </row>
+    <row r="115" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="46" t="s">
+        <v>197</v>
+      </c>
+      <c r="B115" s="47"/>
+      <c r="C115" s="47"/>
+      <c r="D115" s="47"/>
+      <c r="E115" s="47"/>
+      <c r="F115" s="47"/>
+      <c r="G115" s="47"/>
+      <c r="H115" s="47"/>
+      <c r="I115" s="47"/>
     </row>
     <row r="116" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="27"/>
-      <c r="B116" s="30"/>
+      <c r="A116" s="27">
+        <f ca="1">IF(OFFSET(A116,-2,0) ="",OFFSET(A116,-2,0)+1,OFFSET(A116,-2,0)+1 )</f>
+        <v>8</v>
+      </c>
+      <c r="B116" s="30" t="s">
+        <v>165</v>
+      </c>
       <c r="C116" s="33"/>
       <c r="D116" s="13"/>
       <c r="E116" s="13"/>
       <c r="F116" s="13"/>
       <c r="G116" s="13"/>
       <c r="H116" s="13"/>
-      <c r="I116" s="13"/>
+      <c r="I116" s="49"/>
     </row>
     <row r="117" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="27"/>
@@ -16279,7 +16332,7 @@
       <c r="F117" s="13"/>
       <c r="G117" s="13"/>
       <c r="H117" s="13"/>
-      <c r="I117" s="13"/>
+      <c r="I117" s="49"/>
     </row>
     <row r="118" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="27"/>
@@ -16290,7 +16343,7 @@
       <c r="F118" s="13"/>
       <c r="G118" s="13"/>
       <c r="H118" s="13"/>
-      <c r="I118" s="13"/>
+      <c r="I118" s="49"/>
     </row>
     <row r="119" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="27"/>
@@ -16301,7 +16354,7 @@
       <c r="F119" s="13"/>
       <c r="G119" s="13"/>
       <c r="H119" s="13"/>
-      <c r="I119" s="13"/>
+      <c r="I119" s="49"/>
     </row>
     <row r="120" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="27"/>
@@ -16312,7 +16365,7 @@
       <c r="F120" s="13"/>
       <c r="G120" s="13"/>
       <c r="H120" s="13"/>
-      <c r="I120" s="13"/>
+      <c r="I120" s="49"/>
     </row>
     <row r="121" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="27"/>
@@ -16323,7 +16376,7 @@
       <c r="F121" s="13"/>
       <c r="G121" s="13"/>
       <c r="H121" s="13"/>
-      <c r="I121" s="13"/>
+      <c r="I121" s="49"/>
     </row>
     <row r="122" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="27"/>
@@ -16334,7 +16387,7 @@
       <c r="F122" s="13"/>
       <c r="G122" s="13"/>
       <c r="H122" s="13"/>
-      <c r="I122" s="13"/>
+      <c r="I122" s="49"/>
     </row>
     <row r="123" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="27"/>
@@ -16345,7 +16398,7 @@
       <c r="F123" s="13"/>
       <c r="G123" s="13"/>
       <c r="H123" s="13"/>
-      <c r="I123" s="13"/>
+      <c r="I123" s="49"/>
     </row>
     <row r="124" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="27"/>
@@ -16356,7 +16409,7 @@
       <c r="F124" s="13"/>
       <c r="G124" s="13"/>
       <c r="H124" s="13"/>
-      <c r="I124" s="13"/>
+      <c r="I124" s="49"/>
     </row>
     <row r="125" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="27"/>
@@ -16367,7 +16420,7 @@
       <c r="F125" s="13"/>
       <c r="G125" s="13"/>
       <c r="H125" s="13"/>
-      <c r="I125" s="13"/>
+      <c r="I125" s="49"/>
     </row>
     <row r="126" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="27"/>
@@ -16378,7 +16431,7 @@
       <c r="F126" s="13"/>
       <c r="G126" s="13"/>
       <c r="H126" s="13"/>
-      <c r="I126" s="13"/>
+      <c r="I126" s="49"/>
     </row>
     <row r="127" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="27"/>
@@ -16389,7 +16442,7 @@
       <c r="F127" s="13"/>
       <c r="G127" s="13"/>
       <c r="H127" s="13"/>
-      <c r="I127" s="13"/>
+      <c r="I127" s="49"/>
     </row>
     <row r="128" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="27"/>
@@ -16400,7 +16453,7 @@
       <c r="F128" s="13"/>
       <c r="G128" s="13"/>
       <c r="H128" s="13"/>
-      <c r="I128" s="13"/>
+      <c r="I128" s="49"/>
     </row>
     <row r="129" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="27"/>
@@ -16411,7 +16464,7 @@
       <c r="F129" s="13"/>
       <c r="G129" s="13"/>
       <c r="H129" s="13"/>
-      <c r="I129" s="13"/>
+      <c r="I129" s="49"/>
     </row>
     <row r="130" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="27"/>
@@ -16422,7 +16475,7 @@
       <c r="F130" s="13"/>
       <c r="G130" s="13"/>
       <c r="H130" s="13"/>
-      <c r="I130" s="13"/>
+      <c r="I130" s="49"/>
     </row>
     <row r="131" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="27"/>
@@ -16433,7 +16486,7 @@
       <c r="F131" s="13"/>
       <c r="G131" s="13"/>
       <c r="H131" s="13"/>
-      <c r="I131" s="13"/>
+      <c r="I131" s="49"/>
     </row>
     <row r="132" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="27"/>
@@ -16444,7 +16497,7 @@
       <c r="F132" s="13"/>
       <c r="G132" s="13"/>
       <c r="H132" s="13"/>
-      <c r="I132" s="13"/>
+      <c r="I132" s="49"/>
     </row>
     <row r="133" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="27"/>
@@ -16455,7 +16508,7 @@
       <c r="F133" s="13"/>
       <c r="G133" s="13"/>
       <c r="H133" s="13"/>
-      <c r="I133" s="13"/>
+      <c r="I133" s="49"/>
     </row>
     <row r="134" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="27"/>
@@ -16466,7 +16519,7 @@
       <c r="F134" s="13"/>
       <c r="G134" s="13"/>
       <c r="H134" s="13"/>
-      <c r="I134" s="13"/>
+      <c r="I134" s="49"/>
     </row>
     <row r="135" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="27"/>
@@ -16477,7 +16530,7 @@
       <c r="F135" s="13"/>
       <c r="G135" s="13"/>
       <c r="H135" s="13"/>
-      <c r="I135" s="13"/>
+      <c r="I135" s="49"/>
     </row>
     <row r="136" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="27"/>
@@ -16488,7 +16541,7 @@
       <c r="F136" s="13"/>
       <c r="G136" s="13"/>
       <c r="H136" s="13"/>
-      <c r="I136" s="13"/>
+      <c r="I136" s="49"/>
     </row>
     <row r="137" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="27"/>
@@ -16499,7 +16552,7 @@
       <c r="F137" s="13"/>
       <c r="G137" s="13"/>
       <c r="H137" s="13"/>
-      <c r="I137" s="13"/>
+      <c r="I137" s="49"/>
     </row>
     <row r="138" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="27"/>
@@ -16510,7 +16563,7 @@
       <c r="F138" s="13"/>
       <c r="G138" s="13"/>
       <c r="H138" s="13"/>
-      <c r="I138" s="13"/>
+      <c r="I138" s="49"/>
     </row>
     <row r="139" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="27"/>
@@ -16521,7 +16574,7 @@
       <c r="F139" s="13"/>
       <c r="G139" s="13"/>
       <c r="H139" s="13"/>
-      <c r="I139" s="13"/>
+      <c r="I139" s="49"/>
     </row>
     <row r="140" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="27"/>
@@ -16532,7 +16585,7 @@
       <c r="F140" s="13"/>
       <c r="G140" s="13"/>
       <c r="H140" s="13"/>
-      <c r="I140" s="13"/>
+      <c r="I140" s="49"/>
     </row>
     <row r="141" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="27"/>
@@ -16543,7 +16596,7 @@
       <c r="F141" s="13"/>
       <c r="G141" s="13"/>
       <c r="H141" s="13"/>
-      <c r="I141" s="13"/>
+      <c r="I141" s="49"/>
     </row>
     <row r="142" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="27"/>
@@ -16554,7 +16607,7 @@
       <c r="F142" s="13"/>
       <c r="G142" s="13"/>
       <c r="H142" s="13"/>
-      <c r="I142" s="13"/>
+      <c r="I142" s="49"/>
     </row>
     <row r="143" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="27"/>
@@ -16565,7 +16618,7 @@
       <c r="F143" s="13"/>
       <c r="G143" s="13"/>
       <c r="H143" s="13"/>
-      <c r="I143" s="13"/>
+      <c r="I143" s="49"/>
     </row>
     <row r="144" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="27"/>
@@ -16576,7 +16629,7 @@
       <c r="F144" s="13"/>
       <c r="G144" s="13"/>
       <c r="H144" s="13"/>
-      <c r="I144" s="13"/>
+      <c r="I144" s="49"/>
     </row>
     <row r="145" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="27"/>
@@ -16587,7 +16640,7 @@
       <c r="F145" s="13"/>
       <c r="G145" s="13"/>
       <c r="H145" s="13"/>
-      <c r="I145" s="13"/>
+      <c r="I145" s="49"/>
     </row>
     <row r="146" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="27"/>
@@ -16598,7 +16651,7 @@
       <c r="F146" s="13"/>
       <c r="G146" s="13"/>
       <c r="H146" s="13"/>
-      <c r="I146" s="13"/>
+      <c r="I146" s="49"/>
     </row>
     <row r="147" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="27"/>
@@ -16609,7 +16662,7 @@
       <c r="F147" s="13"/>
       <c r="G147" s="13"/>
       <c r="H147" s="13"/>
-      <c r="I147" s="13"/>
+      <c r="I147" s="49"/>
     </row>
     <row r="148" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="27"/>
@@ -16620,7 +16673,7 @@
       <c r="F148" s="13"/>
       <c r="G148" s="13"/>
       <c r="H148" s="13"/>
-      <c r="I148" s="13"/>
+      <c r="I148" s="49"/>
     </row>
     <row r="149" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="27"/>
@@ -16631,7 +16684,7 @@
       <c r="F149" s="13"/>
       <c r="G149" s="13"/>
       <c r="H149" s="13"/>
-      <c r="I149" s="13"/>
+      <c r="I149" s="49"/>
     </row>
     <row r="150" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="27"/>
@@ -16642,7 +16695,7 @@
       <c r="F150" s="13"/>
       <c r="G150" s="13"/>
       <c r="H150" s="13"/>
-      <c r="I150" s="13"/>
+      <c r="I150" s="49"/>
     </row>
     <row r="151" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="27"/>
@@ -16653,7 +16706,7 @@
       <c r="F151" s="13"/>
       <c r="G151" s="13"/>
       <c r="H151" s="13"/>
-      <c r="I151" s="13"/>
+      <c r="I151" s="49"/>
     </row>
     <row r="152" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="27"/>
@@ -16664,7 +16717,7 @@
       <c r="F152" s="13"/>
       <c r="G152" s="13"/>
       <c r="H152" s="13"/>
-      <c r="I152" s="13"/>
+      <c r="I152" s="49"/>
     </row>
     <row r="153" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="27"/>
@@ -16675,7 +16728,7 @@
       <c r="F153" s="13"/>
       <c r="G153" s="13"/>
       <c r="H153" s="13"/>
-      <c r="I153" s="13"/>
+      <c r="I153" s="49"/>
     </row>
     <row r="154" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="27"/>
@@ -16686,7 +16739,7 @@
       <c r="F154" s="13"/>
       <c r="G154" s="13"/>
       <c r="H154" s="13"/>
-      <c r="I154" s="13"/>
+      <c r="I154" s="49"/>
     </row>
     <row r="155" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="27"/>
@@ -16697,7 +16750,7 @@
       <c r="F155" s="13"/>
       <c r="G155" s="13"/>
       <c r="H155" s="13"/>
-      <c r="I155" s="13"/>
+      <c r="I155" s="49"/>
     </row>
     <row r="156" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="27"/>
@@ -16708,7 +16761,7 @@
       <c r="F156" s="13"/>
       <c r="G156" s="13"/>
       <c r="H156" s="13"/>
-      <c r="I156" s="13"/>
+      <c r="I156" s="49"/>
     </row>
     <row r="157" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="27"/>
@@ -16719,7 +16772,7 @@
       <c r="F157" s="13"/>
       <c r="G157" s="13"/>
       <c r="H157" s="13"/>
-      <c r="I157" s="13"/>
+      <c r="I157" s="49"/>
     </row>
     <row r="158" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="27"/>
@@ -16730,7 +16783,7 @@
       <c r="F158" s="13"/>
       <c r="G158" s="13"/>
       <c r="H158" s="13"/>
-      <c r="I158" s="13"/>
+      <c r="I158" s="49"/>
     </row>
     <row r="159" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="27"/>
@@ -16741,7 +16794,7 @@
       <c r="F159" s="13"/>
       <c r="G159" s="13"/>
       <c r="H159" s="13"/>
-      <c r="I159" s="13"/>
+      <c r="I159" s="49"/>
     </row>
     <row r="160" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="27"/>
@@ -16752,7 +16805,7 @@
       <c r="F160" s="13"/>
       <c r="G160" s="13"/>
       <c r="H160" s="13"/>
-      <c r="I160" s="13"/>
+      <c r="I160" s="49"/>
     </row>
     <row r="161" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="27"/>
@@ -16763,7 +16816,7 @@
       <c r="F161" s="13"/>
       <c r="G161" s="13"/>
       <c r="H161" s="13"/>
-      <c r="I161" s="13"/>
+      <c r="I161" s="49"/>
     </row>
     <row r="162" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="27"/>
@@ -16774,7 +16827,7 @@
       <c r="F162" s="13"/>
       <c r="G162" s="13"/>
       <c r="H162" s="13"/>
-      <c r="I162" s="13"/>
+      <c r="I162" s="49"/>
     </row>
     <row r="163" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="27"/>
@@ -16785,7 +16838,7 @@
       <c r="F163" s="13"/>
       <c r="G163" s="13"/>
       <c r="H163" s="13"/>
-      <c r="I163" s="13"/>
+      <c r="I163" s="49"/>
     </row>
     <row r="164" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="27"/>
@@ -16796,7 +16849,7 @@
       <c r="F164" s="13"/>
       <c r="G164" s="13"/>
       <c r="H164" s="13"/>
-      <c r="I164" s="13"/>
+      <c r="I164" s="49"/>
     </row>
     <row r="165" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="27"/>
@@ -16807,7 +16860,7 @@
       <c r="F165" s="13"/>
       <c r="G165" s="13"/>
       <c r="H165" s="13"/>
-      <c r="I165" s="13"/>
+      <c r="I165" s="49"/>
     </row>
     <row r="166" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="27"/>
@@ -16818,7 +16871,7 @@
       <c r="F166" s="13"/>
       <c r="G166" s="13"/>
       <c r="H166" s="13"/>
-      <c r="I166" s="13"/>
+      <c r="I166" s="49"/>
     </row>
     <row r="167" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="27"/>
@@ -16829,7 +16882,7 @@
       <c r="F167" s="13"/>
       <c r="G167" s="13"/>
       <c r="H167" s="13"/>
-      <c r="I167" s="13"/>
+      <c r="I167" s="49"/>
     </row>
     <row r="168" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="27"/>
@@ -16840,7 +16893,7 @@
       <c r="F168" s="13"/>
       <c r="G168" s="13"/>
       <c r="H168" s="13"/>
-      <c r="I168" s="13"/>
+      <c r="I168" s="49"/>
     </row>
     <row r="169" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="27"/>
@@ -16851,7 +16904,7 @@
       <c r="F169" s="13"/>
       <c r="G169" s="13"/>
       <c r="H169" s="13"/>
-      <c r="I169" s="13"/>
+      <c r="I169" s="49"/>
     </row>
     <row r="170" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="27"/>
@@ -16862,7 +16915,7 @@
       <c r="F170" s="13"/>
       <c r="G170" s="13"/>
       <c r="H170" s="13"/>
-      <c r="I170" s="13"/>
+      <c r="I170" s="49"/>
     </row>
     <row r="171" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="27"/>
@@ -16873,7 +16926,7 @@
       <c r="F171" s="13"/>
       <c r="G171" s="13"/>
       <c r="H171" s="13"/>
-      <c r="I171" s="13"/>
+      <c r="I171" s="49"/>
     </row>
     <row r="172" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="27"/>
@@ -16884,7 +16937,7 @@
       <c r="F172" s="13"/>
       <c r="G172" s="13"/>
       <c r="H172" s="13"/>
-      <c r="I172" s="13"/>
+      <c r="I172" s="49"/>
     </row>
     <row r="173" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="27"/>
@@ -16895,7 +16948,7 @@
       <c r="F173" s="13"/>
       <c r="G173" s="13"/>
       <c r="H173" s="13"/>
-      <c r="I173" s="13"/>
+      <c r="I173" s="49"/>
     </row>
     <row r="174" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="27"/>
@@ -16906,7 +16959,7 @@
       <c r="F174" s="13"/>
       <c r="G174" s="13"/>
       <c r="H174" s="13"/>
-      <c r="I174" s="13"/>
+      <c r="I174" s="49"/>
     </row>
     <row r="175" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="27"/>
@@ -16917,7 +16970,7 @@
       <c r="F175" s="13"/>
       <c r="G175" s="13"/>
       <c r="H175" s="13"/>
-      <c r="I175" s="13"/>
+      <c r="I175" s="49"/>
     </row>
     <row r="176" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="27"/>
@@ -16928,7 +16981,7 @@
       <c r="F176" s="13"/>
       <c r="G176" s="13"/>
       <c r="H176" s="13"/>
-      <c r="I176" s="13"/>
+      <c r="I176" s="49"/>
     </row>
     <row r="177" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="27"/>
@@ -16939,7 +16992,7 @@
       <c r="F177" s="13"/>
       <c r="G177" s="13"/>
       <c r="H177" s="13"/>
-      <c r="I177" s="13"/>
+      <c r="I177" s="49"/>
     </row>
     <row r="178" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="27"/>
@@ -16950,7 +17003,7 @@
       <c r="F178" s="13"/>
       <c r="G178" s="13"/>
       <c r="H178" s="13"/>
-      <c r="I178" s="13"/>
+      <c r="I178" s="49"/>
     </row>
     <row r="179" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="27"/>
@@ -16961,7 +17014,7 @@
       <c r="F179" s="13"/>
       <c r="G179" s="13"/>
       <c r="H179" s="13"/>
-      <c r="I179" s="13"/>
+      <c r="I179" s="49"/>
     </row>
     <row r="180" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="27"/>
@@ -16972,7 +17025,7 @@
       <c r="F180" s="13"/>
       <c r="G180" s="13"/>
       <c r="H180" s="13"/>
-      <c r="I180" s="13"/>
+      <c r="I180" s="49"/>
     </row>
     <row r="181" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="27"/>
@@ -16983,7 +17036,7 @@
       <c r="F181" s="13"/>
       <c r="G181" s="13"/>
       <c r="H181" s="13"/>
-      <c r="I181" s="13"/>
+      <c r="I181" s="49"/>
     </row>
     <row r="182" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="27"/>
@@ -16994,7 +17047,7 @@
       <c r="F182" s="13"/>
       <c r="G182" s="13"/>
       <c r="H182" s="13"/>
-      <c r="I182" s="13"/>
+      <c r="I182" s="49"/>
     </row>
     <row r="183" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="27"/>
@@ -17005,7 +17058,7 @@
       <c r="F183" s="13"/>
       <c r="G183" s="13"/>
       <c r="H183" s="13"/>
-      <c r="I183" s="13"/>
+      <c r="I183" s="49"/>
     </row>
     <row r="184" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="27"/>
@@ -17016,7 +17069,7 @@
       <c r="F184" s="13"/>
       <c r="G184" s="13"/>
       <c r="H184" s="13"/>
-      <c r="I184" s="13"/>
+      <c r="I184" s="49"/>
     </row>
     <row r="185" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="27"/>
@@ -17027,7 +17080,7 @@
       <c r="F185" s="13"/>
       <c r="G185" s="13"/>
       <c r="H185" s="13"/>
-      <c r="I185" s="13"/>
+      <c r="I185" s="49"/>
     </row>
     <row r="186" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="27"/>
@@ -17038,7 +17091,7 @@
       <c r="F186" s="13"/>
       <c r="G186" s="13"/>
       <c r="H186" s="13"/>
-      <c r="I186" s="13"/>
+      <c r="I186" s="49"/>
     </row>
     <row r="187" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="27"/>
@@ -17049,7 +17102,7 @@
       <c r="F187" s="13"/>
       <c r="G187" s="13"/>
       <c r="H187" s="13"/>
-      <c r="I187" s="13"/>
+      <c r="I187" s="49"/>
     </row>
     <row r="188" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="27"/>
@@ -17060,7 +17113,7 @@
       <c r="F188" s="13"/>
       <c r="G188" s="13"/>
       <c r="H188" s="13"/>
-      <c r="I188" s="13"/>
+      <c r="I188" s="49"/>
     </row>
     <row r="189" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="27"/>
@@ -17071,7 +17124,7 @@
       <c r="F189" s="13"/>
       <c r="G189" s="13"/>
       <c r="H189" s="13"/>
-      <c r="I189" s="13"/>
+      <c r="I189" s="49"/>
     </row>
     <row r="190" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="27"/>
@@ -17082,7 +17135,7 @@
       <c r="F190" s="13"/>
       <c r="G190" s="13"/>
       <c r="H190" s="13"/>
-      <c r="I190" s="13"/>
+      <c r="I190" s="49"/>
     </row>
     <row r="191" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="27"/>
@@ -17093,7 +17146,7 @@
       <c r="F191" s="13"/>
       <c r="G191" s="13"/>
       <c r="H191" s="13"/>
-      <c r="I191" s="13"/>
+      <c r="I191" s="49"/>
     </row>
     <row r="192" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="27"/>
@@ -17104,7 +17157,7 @@
       <c r="F192" s="13"/>
       <c r="G192" s="13"/>
       <c r="H192" s="13"/>
-      <c r="I192" s="13"/>
+      <c r="I192" s="49"/>
     </row>
     <row r="193" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="27"/>
@@ -17115,7 +17168,7 @@
       <c r="F193" s="13"/>
       <c r="G193" s="13"/>
       <c r="H193" s="13"/>
-      <c r="I193" s="13"/>
+      <c r="I193" s="49"/>
     </row>
     <row r="194" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="27"/>
@@ -17126,7 +17179,7 @@
       <c r="F194" s="13"/>
       <c r="G194" s="13"/>
       <c r="H194" s="13"/>
-      <c r="I194" s="13"/>
+      <c r="I194" s="49"/>
     </row>
     <row r="195" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="27"/>
@@ -17137,7 +17190,7 @@
       <c r="F195" s="13"/>
       <c r="G195" s="13"/>
       <c r="H195" s="13"/>
-      <c r="I195" s="13"/>
+      <c r="I195" s="49"/>
     </row>
     <row r="196" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="27"/>
@@ -17148,7 +17201,7 @@
       <c r="F196" s="13"/>
       <c r="G196" s="13"/>
       <c r="H196" s="13"/>
-      <c r="I196" s="13"/>
+      <c r="I196" s="49"/>
     </row>
     <row r="197" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="27"/>
@@ -17159,7 +17212,7 @@
       <c r="F197" s="13"/>
       <c r="G197" s="13"/>
       <c r="H197" s="13"/>
-      <c r="I197" s="13"/>
+      <c r="I197" s="49"/>
     </row>
     <row r="198" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="27"/>
@@ -17170,7 +17223,7 @@
       <c r="F198" s="13"/>
       <c r="G198" s="13"/>
       <c r="H198" s="13"/>
-      <c r="I198" s="13"/>
+      <c r="I198" s="49"/>
     </row>
     <row r="199" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="27"/>
@@ -17181,7 +17234,7 @@
       <c r="F199" s="13"/>
       <c r="G199" s="13"/>
       <c r="H199" s="13"/>
-      <c r="I199" s="13"/>
+      <c r="I199" s="49"/>
     </row>
     <row r="200" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="27"/>
@@ -17192,160 +17245,29 @@
       <c r="F200" s="13"/>
       <c r="G200" s="13"/>
       <c r="H200" s="13"/>
-      <c r="I200" s="13"/>
-    </row>
-    <row r="201" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A201" s="27"/>
-      <c r="B201" s="30"/>
-      <c r="C201" s="33"/>
-      <c r="D201" s="13"/>
-      <c r="E201" s="13"/>
-      <c r="F201" s="13"/>
-      <c r="G201" s="13"/>
-      <c r="H201" s="13"/>
-      <c r="I201" s="13"/>
-    </row>
-    <row r="202" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A202" s="27"/>
-      <c r="B202" s="30"/>
-      <c r="C202" s="33"/>
-      <c r="D202" s="13"/>
-      <c r="E202" s="13"/>
-      <c r="F202" s="13"/>
-      <c r="G202" s="13"/>
-      <c r="H202" s="13"/>
-      <c r="I202" s="13"/>
-    </row>
-    <row r="203" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A203" s="27"/>
-      <c r="B203" s="30"/>
-      <c r="C203" s="33"/>
-      <c r="D203" s="13"/>
-      <c r="E203" s="13"/>
-      <c r="F203" s="13"/>
-      <c r="G203" s="13"/>
-      <c r="H203" s="13"/>
-      <c r="I203" s="13"/>
-    </row>
-    <row r="204" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A204" s="27"/>
-      <c r="B204" s="30"/>
-      <c r="C204" s="33"/>
-      <c r="D204" s="13"/>
-      <c r="E204" s="13"/>
-      <c r="F204" s="13"/>
-      <c r="G204" s="13"/>
-      <c r="H204" s="13"/>
-      <c r="I204" s="13"/>
-    </row>
-    <row r="205" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A205" s="27"/>
-      <c r="B205" s="30"/>
-      <c r="C205" s="33"/>
-      <c r="D205" s="13"/>
-      <c r="E205" s="13"/>
-      <c r="F205" s="13"/>
-      <c r="G205" s="13"/>
-      <c r="H205" s="13"/>
-      <c r="I205" s="13"/>
-    </row>
-    <row r="206" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A206" s="27"/>
-      <c r="B206" s="30"/>
-      <c r="C206" s="33"/>
-      <c r="D206" s="13"/>
-      <c r="E206" s="13"/>
-      <c r="F206" s="13"/>
-      <c r="G206" s="13"/>
-      <c r="H206" s="13"/>
-      <c r="I206" s="13"/>
-    </row>
-    <row r="207" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A207" s="27"/>
-      <c r="B207" s="30"/>
-      <c r="C207" s="33"/>
-      <c r="D207" s="13"/>
-      <c r="E207" s="13"/>
-      <c r="F207" s="13"/>
-      <c r="G207" s="13"/>
-      <c r="H207" s="13"/>
-      <c r="I207" s="13"/>
-    </row>
-    <row r="208" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A208" s="27"/>
-      <c r="B208" s="30"/>
-      <c r="C208" s="33"/>
-      <c r="D208" s="13"/>
-      <c r="E208" s="13"/>
-      <c r="F208" s="13"/>
-      <c r="G208" s="13"/>
-      <c r="H208" s="13"/>
-      <c r="I208" s="13"/>
-    </row>
-    <row r="209" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A209" s="27"/>
-      <c r="B209" s="30"/>
-      <c r="C209" s="33"/>
-      <c r="D209" s="13"/>
-      <c r="E209" s="13"/>
-      <c r="F209" s="13"/>
-      <c r="G209" s="13"/>
-      <c r="H209" s="13"/>
-      <c r="I209" s="13"/>
-    </row>
-    <row r="210" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A210" s="27"/>
-      <c r="B210" s="30"/>
-      <c r="C210" s="33"/>
-      <c r="D210" s="13"/>
-      <c r="E210" s="13"/>
-      <c r="F210" s="13"/>
-      <c r="G210" s="13"/>
-      <c r="H210" s="13"/>
-      <c r="I210" s="13"/>
-    </row>
-    <row r="211" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A211" s="27"/>
-      <c r="B211" s="30"/>
-      <c r="C211" s="33"/>
-      <c r="D211" s="13"/>
-      <c r="E211" s="13"/>
-      <c r="F211" s="13"/>
-      <c r="G211" s="13"/>
-      <c r="H211" s="13"/>
-      <c r="I211" s="13"/>
-    </row>
-    <row r="212" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A212" s="27"/>
-      <c r="B212" s="30"/>
-      <c r="C212" s="33"/>
-      <c r="D212" s="13"/>
-      <c r="E212" s="13"/>
-      <c r="F212" s="13"/>
-      <c r="G212" s="13"/>
-      <c r="H212" s="13"/>
-      <c r="I212" s="13"/>
+      <c r="I200" s="49"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="A77:I77"/>
+  <mergeCells count="19">
+    <mergeCell ref="A98:I98"/>
     <mergeCell ref="A100:I100"/>
-    <mergeCell ref="A81:I81"/>
+    <mergeCell ref="A78:I78"/>
+    <mergeCell ref="A103:I103"/>
+    <mergeCell ref="A104:I104"/>
+    <mergeCell ref="A88:I88"/>
+    <mergeCell ref="A108:I108"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A16:I16"/>
+    <mergeCell ref="A17:I17"/>
     <mergeCell ref="A28:I28"/>
     <mergeCell ref="A37:I37"/>
-    <mergeCell ref="A76:I76"/>
+    <mergeCell ref="A77:I77"/>
     <mergeCell ref="A52:I52"/>
-    <mergeCell ref="A58:I58"/>
-    <mergeCell ref="A63:I63"/>
-    <mergeCell ref="A84:I84"/>
-    <mergeCell ref="A86:I86"/>
-    <mergeCell ref="A88:I88"/>
-    <mergeCell ref="A110:I110"/>
-    <mergeCell ref="A112:I112"/>
-    <mergeCell ref="A90:I90"/>
+    <mergeCell ref="A59:I59"/>
+    <mergeCell ref="A64:I64"/>
+    <mergeCell ref="A111:I111"/>
+    <mergeCell ref="A113:I113"/>
+    <mergeCell ref="A115:I115"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added folders for Sele HW Day 2
</commit_message>
<xml_diff>
--- a/Middle Assignment/TestDesignTechique1_PhamHongAnh.xlsx
+++ b/Middle Assignment/TestDesignTechique1_PhamHongAnh.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NashTech\Rookies\NashTech_Homework\Middle Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71D15E3-6CCE-40D1-87DF-4E3F03E09153}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124897DF-C24E-4976-AAE7-ADDD4AE16624}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment 1" sheetId="1" r:id="rId1"/>
@@ -851,7 +851,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="208">
   <si>
     <t>ID</t>
   </si>
@@ -1421,9 +1421,6 @@
   </si>
   <si>
     <t>When users enter no phone number and then slide the button</t>
-  </si>
-  <si>
-    <t>After entering all mandatory (*) information valid</t>
   </si>
   <si>
     <t>When signing up with no SMS verification code</t>
@@ -1817,6 +1814,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1851,12 +1854,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2138,17 +2135,17 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -2168,17 +2165,17 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -2567,17 +2564,17 @@
       <c r="Z13" s="2"/>
     </row>
     <row r="14" spans="1:26" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="42"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -2965,17 +2962,17 @@
       <c r="Z24" s="2"/>
     </row>
     <row r="25" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="43" t="s">
+      <c r="A25" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="44"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="45"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="47"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
@@ -3067,17 +3064,17 @@
       <c r="Z27" s="2"/>
     </row>
     <row r="28" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="44"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="45"/>
+      <c r="B28" s="46"/>
+      <c r="C28" s="46"/>
+      <c r="D28" s="46"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="46"/>
+      <c r="H28" s="46"/>
+      <c r="I28" s="47"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
@@ -3170,17 +3167,17 @@
       <c r="Z30" s="2"/>
     </row>
     <row r="31" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="39" t="s">
+      <c r="A31" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="42"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -3200,17 +3197,17 @@
       <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="36" t="s">
+      <c r="A32" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="37"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="37"/>
-      <c r="G32" s="37"/>
-      <c r="H32" s="37"/>
-      <c r="I32" s="38"/>
+      <c r="B32" s="39"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="40"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
@@ -3404,17 +3401,17 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="36" t="s">
+      <c r="A42" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B42" s="37"/>
-      <c r="C42" s="37"/>
-      <c r="D42" s="37"/>
-      <c r="E42" s="37"/>
-      <c r="F42" s="37"/>
-      <c r="G42" s="37"/>
-      <c r="H42" s="37"/>
-      <c r="I42" s="38"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="39"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="39"/>
+      <c r="H42" s="39"/>
+      <c r="I42" s="40"/>
     </row>
     <row r="43" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
@@ -14381,10 +14378,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{861DB058-9ABC-4928-81FB-0309C7B8DB85}">
-  <dimension ref="A1:Z200"/>
+  <dimension ref="A1:Z196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94:I94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -14397,7 +14394,7 @@
     <col min="6" max="6" width="17" style="28" customWidth="1"/>
     <col min="7" max="7" width="14.54296875" style="28" customWidth="1"/>
     <col min="8" max="8" width="17.08984375" style="28" customWidth="1"/>
-    <col min="9" max="9" width="15.1796875" style="50" customWidth="1"/>
+    <col min="9" max="9" width="15.1796875" style="37" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="10" customFormat="1" ht="26" x14ac:dyDescent="0.35">
@@ -14447,17 +14444,17 @@
       <c r="Z1" s="26"/>
     </row>
     <row r="2" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="41" t="s">
         <v>166</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
       <c r="J2" s="26"/>
       <c r="K2" s="26"/>
       <c r="L2" s="26"/>
@@ -14477,17 +14474,17 @@
       <c r="Z2" s="26"/>
     </row>
     <row r="3" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="41" t="s">
-        <v>200</v>
-      </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
+      <c r="A3" s="43" t="s">
+        <v>199</v>
+      </c>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
       <c r="J3" s="26"/>
       <c r="K3" s="26"/>
       <c r="L3" s="26"/>
@@ -14513,15 +14510,15 @@
       <c r="B4" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="C4" s="49" t="s">
-        <v>207</v>
+      <c r="C4" s="36" t="s">
+        <v>206</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
-      <c r="I4" s="49"/>
+      <c r="I4" s="36"/>
     </row>
     <row r="5" spans="1:26" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="27">
@@ -14537,7 +14534,7 @@
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
-      <c r="I5" s="49"/>
+      <c r="I5" s="36"/>
     </row>
     <row r="6" spans="1:26" s="10" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27">
@@ -14553,7 +14550,7 @@
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
-      <c r="I6" s="49"/>
+      <c r="I6" s="36"/>
     </row>
     <row r="7" spans="1:26" s="10" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="27">
@@ -14561,7 +14558,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C7" s="33"/>
       <c r="D7" s="13"/>
@@ -14569,7 +14566,7 @@
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
-      <c r="I7" s="49"/>
+      <c r="I7" s="36"/>
     </row>
     <row r="8" spans="1:26" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="27">
@@ -14585,11 +14582,11 @@
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
-      <c r="I8" s="49"/>
+      <c r="I8" s="36"/>
     </row>
     <row r="9" spans="1:26" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27">
-        <f t="shared" ref="A9:A76" ca="1" si="0">IF(OFFSET(A9,-1,0) ="",OFFSET(A9,-2,0)+1,OFFSET(A9,-1,0)+1 )</f>
+        <f t="shared" ref="A9:A79" ca="1" si="0">IF(OFFSET(A9,-1,0) ="",OFFSET(A9,-2,0)+1,OFFSET(A9,-1,0)+1 )</f>
         <v>6</v>
       </c>
       <c r="B9" s="30" t="s">
@@ -14601,7 +14598,7 @@
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
-      <c r="I9" s="49"/>
+      <c r="I9" s="36"/>
     </row>
     <row r="10" spans="1:26" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27">
@@ -14617,7 +14614,7 @@
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
-      <c r="I10" s="49"/>
+      <c r="I10" s="36"/>
     </row>
     <row r="11" spans="1:26" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="27">
@@ -14633,7 +14630,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
-      <c r="I11" s="49"/>
+      <c r="I11" s="36"/>
     </row>
     <row r="12" spans="1:26" s="10" customFormat="1" ht="20.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="27">
@@ -14649,7 +14646,7 @@
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
-      <c r="I12" s="49"/>
+      <c r="I12" s="36"/>
     </row>
     <row r="13" spans="1:26" s="10" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="27">
@@ -14665,7 +14662,7 @@
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
-      <c r="I13" s="49"/>
+      <c r="I13" s="36"/>
     </row>
     <row r="14" spans="1:26" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="27">
@@ -14681,7 +14678,7 @@
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
-      <c r="I14" s="49"/>
+      <c r="I14" s="36"/>
     </row>
     <row r="15" spans="1:26" s="10" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="27">
@@ -14692,14 +14689,14 @@
         <v>127</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
-      <c r="I15" s="49"/>
+      <c r="I15" s="36"/>
     </row>
     <row r="16" spans="1:26" s="10" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="27">
@@ -14715,20 +14712,20 @@
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
-      <c r="I16" s="49"/>
+      <c r="I16" s="36"/>
     </row>
     <row r="17" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="46" t="s">
+      <c r="A17" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="B17" s="47"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
       <c r="J17" s="26"/>
       <c r="K17" s="26"/>
       <c r="L17" s="26"/>
@@ -14761,7 +14758,7 @@
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
       <c r="H18" s="13"/>
-      <c r="I18" s="49"/>
+      <c r="I18" s="36"/>
     </row>
     <row r="19" spans="1:26" s="10" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="27">
@@ -14777,7 +14774,7 @@
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
-      <c r="I19" s="49"/>
+      <c r="I19" s="36"/>
     </row>
     <row r="20" spans="1:26" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="27">
@@ -14793,7 +14790,7 @@
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
-      <c r="I20" s="49"/>
+      <c r="I20" s="36"/>
     </row>
     <row r="21" spans="1:26" s="10" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="27">
@@ -14809,7 +14806,7 @@
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
-      <c r="I21" s="49"/>
+      <c r="I21" s="36"/>
     </row>
     <row r="22" spans="1:26" s="10" customFormat="1" ht="24.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="27">
@@ -14825,7 +14822,7 @@
       <c r="F22" s="13"/>
       <c r="G22" s="13"/>
       <c r="H22" s="13"/>
-      <c r="I22" s="49"/>
+      <c r="I22" s="36"/>
     </row>
     <row r="23" spans="1:26" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="27">
@@ -14841,7 +14838,7 @@
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
-      <c r="I23" s="49"/>
+      <c r="I23" s="36"/>
     </row>
     <row r="24" spans="1:26" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="27">
@@ -14857,7 +14854,7 @@
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
-      <c r="I24" s="49"/>
+      <c r="I24" s="36"/>
     </row>
     <row r="25" spans="1:26" s="10" customFormat="1" ht="20.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="27">
@@ -14873,7 +14870,7 @@
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
       <c r="H25" s="13"/>
-      <c r="I25" s="49"/>
+      <c r="I25" s="36"/>
     </row>
     <row r="26" spans="1:26" s="10" customFormat="1" ht="20.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="27">
@@ -14889,112 +14886,113 @@
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
-      <c r="I26" s="49"/>
-    </row>
-    <row r="27" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I26" s="36"/>
+    </row>
+    <row r="27" spans="1:26" s="10" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="27">
         <f ca="1">IF(OFFSET(A27,-1,0) ="",OFFSET(A27,-2,0)+1,OFFSET(A27,-1,0)+1 )</f>
         <v>23</v>
       </c>
-      <c r="B27" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="C27" s="34"/>
+      <c r="B27" s="30" t="s">
+        <v>183</v>
+      </c>
+      <c r="C27" s="33"/>
+      <c r="D27" s="30"/>
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
       <c r="H27" s="13"/>
-      <c r="I27" s="49"/>
-    </row>
-    <row r="28" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="46" t="s">
+      <c r="I27" s="36"/>
+    </row>
+    <row r="28" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="27">
+        <f ca="1">IF(OFFSET(A28,-1,0) ="",OFFSET(A28,-2,0)+1,OFFSET(A28,-1,0)+1 )</f>
+        <v>24</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="C28" s="34"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="36"/>
+    </row>
+    <row r="29" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="48" t="s">
         <v>173</v>
       </c>
-      <c r="B28" s="47"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="47"/>
-      <c r="H28" s="47"/>
-      <c r="I28" s="47"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="26"/>
-      <c r="M28" s="26"/>
-      <c r="N28" s="26"/>
-      <c r="O28" s="26"/>
-      <c r="P28" s="26"/>
-      <c r="Q28" s="26"/>
-      <c r="R28" s="26"/>
-      <c r="S28" s="26"/>
-      <c r="T28" s="26"/>
-      <c r="U28" s="26"/>
-      <c r="V28" s="26"/>
-      <c r="W28" s="26"/>
-      <c r="X28" s="26"/>
-      <c r="Y28" s="26"/>
-      <c r="Z28" s="26"/>
-    </row>
-    <row r="29" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="27">
-        <f ca="1">IF(OFFSET(A29,-2,0) ="",OFFSET(A29,-2,0)+1,OFFSET(A29,-2,0)+1 )</f>
-        <v>24</v>
-      </c>
-      <c r="B29" s="30" t="s">
-        <v>146</v>
-      </c>
-      <c r="C29" s="34"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
       <c r="I29" s="49"/>
+      <c r="J29" s="26"/>
+      <c r="K29" s="26"/>
+      <c r="L29" s="26"/>
+      <c r="M29" s="26"/>
+      <c r="N29" s="26"/>
+      <c r="O29" s="26"/>
+      <c r="P29" s="26"/>
+      <c r="Q29" s="26"/>
+      <c r="R29" s="26"/>
+      <c r="S29" s="26"/>
+      <c r="T29" s="26"/>
+      <c r="U29" s="26"/>
+      <c r="V29" s="26"/>
+      <c r="W29" s="26"/>
+      <c r="X29" s="26"/>
+      <c r="Y29" s="26"/>
+      <c r="Z29" s="26"/>
     </row>
     <row r="30" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="27">
-        <f ca="1">IF(OFFSET(A30,-1,0) ="",OFFSET(A30,-2,0)+1,OFFSET(A30,-1,0)+1 )</f>
+        <f ca="1">IF(OFFSET(A30,-2,0) ="",OFFSET(A30,-2,0)+1,OFFSET(A30,-2,0)+1 )</f>
         <v>25</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="C30" s="34"/>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
       <c r="G30" s="13"/>
       <c r="H30" s="13"/>
-      <c r="I30" s="49"/>
+      <c r="I30" s="36"/>
     </row>
     <row r="31" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="27">
-        <f t="shared" ref="A31:A36" ca="1" si="1">IF(OFFSET(A31,-1,0) ="",OFFSET(A31,-2,0)+1,OFFSET(A31,-1,0)+1 )</f>
+        <f ca="1">IF(OFFSET(A31,-1,0) ="",OFFSET(A31,-2,0)+1,OFFSET(A31,-1,0)+1 )</f>
         <v>26</v>
       </c>
-      <c r="B31" s="15" t="s">
-        <v>168</v>
+      <c r="B31" s="30" t="s">
+        <v>134</v>
       </c>
       <c r="C31" s="34"/>
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
       <c r="G31" s="13"/>
       <c r="H31" s="13"/>
-      <c r="I31" s="49"/>
+      <c r="I31" s="36"/>
     </row>
     <row r="32" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="27">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ref="A32:A37" ca="1" si="1">IF(OFFSET(A32,-1,0) ="",OFFSET(A32,-2,0)+1,OFFSET(A32,-1,0)+1 )</f>
         <v>27</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C32" s="34"/>
       <c r="E32" s="13"/>
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
-      <c r="I32" s="49"/>
+      <c r="I32" s="36"/>
     </row>
     <row r="33" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="27">
@@ -15002,14 +15000,14 @@
         <v>28</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C33" s="34"/>
       <c r="E33" s="13"/>
       <c r="F33" s="13"/>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
-      <c r="I33" s="49"/>
+      <c r="I33" s="36"/>
     </row>
     <row r="34" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="27">
@@ -15017,108 +15015,107 @@
         <v>29</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C34" s="34"/>
       <c r="E34" s="13"/>
       <c r="F34" s="13"/>
       <c r="G34" s="13"/>
       <c r="H34" s="13"/>
-      <c r="I34" s="49"/>
+      <c r="I34" s="36"/>
     </row>
     <row r="35" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="27">
-        <f ca="1">IF(OFFSET(A35,-1,0) ="",OFFSET(A35,-2,0)+1,OFFSET(A35,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="1"/>
         <v>30</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C35" s="34"/>
       <c r="E35" s="13"/>
       <c r="F35" s="13"/>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
-      <c r="I35" s="49"/>
+      <c r="I35" s="36"/>
     </row>
     <row r="36" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="27">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">IF(OFFSET(A36,-1,0) ="",OFFSET(A36,-2,0)+1,OFFSET(A36,-1,0)+1 )</f>
         <v>31</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="C36" s="34"/>
       <c r="E36" s="13"/>
       <c r="F36" s="13"/>
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
-      <c r="I36" s="49"/>
-    </row>
-    <row r="37" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="46" t="s">
+      <c r="I36" s="36"/>
+    </row>
+    <row r="37" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="C37" s="34"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="36"/>
+    </row>
+    <row r="38" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="48" t="s">
         <v>130</v>
       </c>
-      <c r="B37" s="47"/>
-      <c r="C37" s="47"/>
-      <c r="D37" s="47"/>
-      <c r="E37" s="47"/>
-      <c r="F37" s="47"/>
-      <c r="G37" s="47"/>
-      <c r="H37" s="47"/>
-      <c r="I37" s="47"/>
-      <c r="J37" s="26"/>
-      <c r="K37" s="26"/>
-      <c r="L37" s="26"/>
-      <c r="M37" s="26"/>
-      <c r="N37" s="26"/>
-      <c r="O37" s="26"/>
-      <c r="P37" s="26"/>
-      <c r="Q37" s="26"/>
-      <c r="R37" s="26"/>
-      <c r="S37" s="26"/>
-      <c r="T37" s="26"/>
-      <c r="U37" s="26"/>
-      <c r="V37" s="26"/>
-      <c r="W37" s="26"/>
-      <c r="X37" s="26"/>
-      <c r="Y37" s="26"/>
-      <c r="Z37" s="26"/>
-    </row>
-    <row r="38" spans="1:26" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="27">
-        <f ca="1">IF(OFFSET(A38,-2,0) ="",OFFSET(A38,-2,0)+1,OFFSET(A38,-2,0)+1 )</f>
-        <v>32</v>
-      </c>
-      <c r="B38" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="C38" s="33" t="s">
-        <v>206</v>
-      </c>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="49"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="49"/>
       <c r="I38" s="49"/>
+      <c r="J38" s="26"/>
+      <c r="K38" s="26"/>
+      <c r="L38" s="26"/>
+      <c r="M38" s="26"/>
+      <c r="N38" s="26"/>
+      <c r="O38" s="26"/>
+      <c r="P38" s="26"/>
+      <c r="Q38" s="26"/>
+      <c r="R38" s="26"/>
+      <c r="S38" s="26"/>
+      <c r="T38" s="26"/>
+      <c r="U38" s="26"/>
+      <c r="V38" s="26"/>
+      <c r="W38" s="26"/>
+      <c r="X38" s="26"/>
+      <c r="Y38" s="26"/>
+      <c r="Z38" s="26"/>
     </row>
     <row r="39" spans="1:26" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="27">
-        <f ca="1">IF(OFFSET(A39,-1,0) ="",OFFSET(A39,-2,0)+1,OFFSET(A39,-1,0)+1 )</f>
+        <f ca="1">IF(OFFSET(A39,-2,0) ="",OFFSET(A39,-2,0)+1,OFFSET(A39,-2,0)+1 )</f>
         <v>33</v>
       </c>
-      <c r="B39" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="C39" s="33"/>
+      <c r="B39" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="C39" s="33" t="s">
+        <v>205</v>
+      </c>
       <c r="D39" s="13"/>
       <c r="E39" s="13"/>
       <c r="F39" s="13"/>
       <c r="G39" s="13"/>
       <c r="H39" s="13"/>
-      <c r="I39" s="49"/>
+      <c r="I39" s="36"/>
     </row>
     <row r="40" spans="1:26" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="27">
@@ -15126,7 +15123,7 @@
         <v>34</v>
       </c>
       <c r="B40" s="30" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="C40" s="33"/>
       <c r="D40" s="13"/>
@@ -15134,15 +15131,15 @@
       <c r="F40" s="13"/>
       <c r="G40" s="13"/>
       <c r="H40" s="13"/>
-      <c r="I40" s="49"/>
-    </row>
-    <row r="41" spans="1:26" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I40" s="36"/>
+    </row>
+    <row r="41" spans="1:26" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">IF(OFFSET(A41,-1,0) ="",OFFSET(A41,-2,0)+1,OFFSET(A41,-1,0)+1 )</f>
         <v>35</v>
       </c>
-      <c r="B41" s="29" t="s">
-        <v>132</v>
+      <c r="B41" s="30" t="s">
+        <v>146</v>
       </c>
       <c r="C41" s="33"/>
       <c r="D41" s="13"/>
@@ -15150,15 +15147,15 @@
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
       <c r="H41" s="13"/>
-      <c r="I41" s="49"/>
-    </row>
-    <row r="42" spans="1:26" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I41" s="36"/>
+    </row>
+    <row r="42" spans="1:26" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>36</v>
       </c>
       <c r="B42" s="29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C42" s="33"/>
       <c r="D42" s="13"/>
@@ -15166,15 +15163,15 @@
       <c r="F42" s="13"/>
       <c r="G42" s="13"/>
       <c r="H42" s="13"/>
-      <c r="I42" s="49"/>
-    </row>
-    <row r="43" spans="1:26" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I42" s="36"/>
+    </row>
+    <row r="43" spans="1:26" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>37</v>
       </c>
       <c r="B43" s="29" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C43" s="33"/>
       <c r="D43" s="13"/>
@@ -15182,15 +15179,15 @@
       <c r="F43" s="13"/>
       <c r="G43" s="13"/>
       <c r="H43" s="13"/>
-      <c r="I43" s="49"/>
-    </row>
-    <row r="44" spans="1:26" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I43" s="36"/>
+    </row>
+    <row r="44" spans="1:26" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>38</v>
       </c>
       <c r="B44" s="29" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="C44" s="33"/>
       <c r="D44" s="13"/>
@@ -15198,15 +15195,15 @@
       <c r="F44" s="13"/>
       <c r="G44" s="13"/>
       <c r="H44" s="13"/>
-      <c r="I44" s="49"/>
-    </row>
-    <row r="45" spans="1:26" s="10" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I44" s="36"/>
+    </row>
+    <row r="45" spans="1:26" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>39</v>
       </c>
       <c r="B45" s="29" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="C45" s="33"/>
       <c r="D45" s="13"/>
@@ -15214,15 +15211,15 @@
       <c r="F45" s="13"/>
       <c r="G45" s="13"/>
       <c r="H45" s="13"/>
-      <c r="I45" s="49"/>
-    </row>
-    <row r="46" spans="1:26" s="10" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I45" s="36"/>
+    </row>
+    <row r="46" spans="1:26" s="10" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>40</v>
       </c>
       <c r="B46" s="29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C46" s="33"/>
       <c r="D46" s="13"/>
@@ -15230,15 +15227,15 @@
       <c r="F46" s="13"/>
       <c r="G46" s="13"/>
       <c r="H46" s="13"/>
-      <c r="I46" s="49"/>
-    </row>
-    <row r="47" spans="1:26" s="10" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I46" s="36"/>
+    </row>
+    <row r="47" spans="1:26" s="10" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>41</v>
       </c>
       <c r="B47" s="29" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="C47" s="33"/>
       <c r="D47" s="13"/>
@@ -15246,7 +15243,7 @@
       <c r="F47" s="13"/>
       <c r="G47" s="13"/>
       <c r="H47" s="13"/>
-      <c r="I47" s="49"/>
+      <c r="I47" s="36"/>
     </row>
     <row r="48" spans="1:26" s="10" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="27">
@@ -15254,7 +15251,7 @@
         <v>42</v>
       </c>
       <c r="B48" s="29" t="s">
-        <v>175</v>
+        <v>126</v>
       </c>
       <c r="C48" s="33"/>
       <c r="D48" s="13"/>
@@ -15262,7 +15259,7 @@
       <c r="F48" s="13"/>
       <c r="G48" s="13"/>
       <c r="H48" s="13"/>
-      <c r="I48" s="49"/>
+      <c r="I48" s="36"/>
     </row>
     <row r="49" spans="1:9" s="10" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="27">
@@ -15270,7 +15267,7 @@
         <v>43</v>
       </c>
       <c r="B49" s="29" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C49" s="33"/>
       <c r="D49" s="13"/>
@@ -15278,15 +15275,15 @@
       <c r="F49" s="13"/>
       <c r="G49" s="13"/>
       <c r="H49" s="13"/>
-      <c r="I49" s="49"/>
-    </row>
-    <row r="50" spans="1:9" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I49" s="36"/>
+    </row>
+    <row r="50" spans="1:9" s="10" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>44</v>
       </c>
-      <c r="B50" s="30" t="s">
-        <v>144</v>
+      <c r="B50" s="29" t="s">
+        <v>176</v>
       </c>
       <c r="C50" s="33"/>
       <c r="D50" s="13"/>
@@ -15294,15 +15291,15 @@
       <c r="F50" s="13"/>
       <c r="G50" s="13"/>
       <c r="H50" s="13"/>
-      <c r="I50" s="49"/>
-    </row>
-    <row r="51" spans="1:9" s="10" customFormat="1" ht="24.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I50" s="36"/>
+    </row>
+    <row r="51" spans="1:9" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>45</v>
       </c>
-      <c r="B51" s="15" t="s">
-        <v>145</v>
+      <c r="B51" s="30" t="s">
+        <v>144</v>
       </c>
       <c r="C51" s="33"/>
       <c r="D51" s="13"/>
@@ -15310,75 +15307,75 @@
       <c r="F51" s="13"/>
       <c r="G51" s="13"/>
       <c r="H51" s="13"/>
-      <c r="I51" s="49"/>
-    </row>
-    <row r="52" spans="1:9" s="10" customFormat="1" ht="21.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="46" t="s">
-        <v>147</v>
-      </c>
-      <c r="B52" s="47"/>
-      <c r="C52" s="47"/>
-      <c r="D52" s="47"/>
-      <c r="E52" s="47"/>
-      <c r="F52" s="47"/>
-      <c r="G52" s="47"/>
-      <c r="H52" s="47"/>
-      <c r="I52" s="47"/>
-    </row>
-    <row r="53" spans="1:9" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I51" s="36"/>
+    </row>
+    <row r="52" spans="1:9" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="27">
+        <f ca="1">IF(OFFSET(A52,-1,0) ="",OFFSET(A52,-2,0)+1,OFFSET(A52,-1,0)+1 )</f>
+        <v>46</v>
+      </c>
+      <c r="B52" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="C52" s="33"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="36"/>
+    </row>
+    <row r="53" spans="1:9" s="10" customFormat="1" ht="24.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="27">
-        <f ca="1">IF(OFFSET(A53,-2,0) ="",OFFSET(A53,-2,0)+1,OFFSET(A53,-2,0)+1 )</f>
-        <v>46</v>
-      </c>
-      <c r="B53" s="30" t="s">
-        <v>146</v>
-      </c>
-      <c r="C53" s="34"/>
+        <f t="shared" ca="1" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B53" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="C53" s="33"/>
+      <c r="D53" s="13"/>
       <c r="E53" s="13"/>
       <c r="F53" s="13"/>
       <c r="G53" s="13"/>
       <c r="H53" s="13"/>
-      <c r="I53" s="49"/>
-    </row>
-    <row r="54" spans="1:9" s="10" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="27">
-        <f t="shared" ca="1" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="B54" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="C54" s="33"/>
-      <c r="D54" s="13"/>
-      <c r="E54" s="13"/>
-      <c r="F54" s="13"/>
-      <c r="G54" s="13"/>
-      <c r="H54" s="13"/>
+      <c r="I53" s="36"/>
+    </row>
+    <row r="54" spans="1:9" s="10" customFormat="1" ht="21.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="B54" s="49"/>
+      <c r="C54" s="49"/>
+      <c r="D54" s="49"/>
+      <c r="E54" s="49"/>
+      <c r="F54" s="49"/>
+      <c r="G54" s="49"/>
+      <c r="H54" s="49"/>
       <c r="I54" s="49"/>
     </row>
-    <row r="55" spans="1:9" s="10" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">IF(OFFSET(A55,-2,0) ="",OFFSET(A55,-2,0)+1,OFFSET(A55,-2,0)+1 )</f>
         <v>48</v>
       </c>
       <c r="B55" s="30" t="s">
-        <v>205</v>
-      </c>
-      <c r="C55" s="33"/>
-      <c r="D55" s="13"/>
+        <v>146</v>
+      </c>
+      <c r="C55" s="34"/>
       <c r="E55" s="13"/>
       <c r="F55" s="13"/>
       <c r="G55" s="13"/>
       <c r="H55" s="13"/>
-      <c r="I55" s="49"/>
-    </row>
-    <row r="56" spans="1:9" s="10" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I55" s="36"/>
+    </row>
+    <row r="56" spans="1:9" s="10" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>49</v>
       </c>
       <c r="B56" s="30" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C56" s="33"/>
       <c r="D56" s="13"/>
@@ -15386,15 +15383,15 @@
       <c r="F56" s="13"/>
       <c r="G56" s="13"/>
       <c r="H56" s="13"/>
-      <c r="I56" s="49"/>
-    </row>
-    <row r="57" spans="1:9" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I56" s="36"/>
+    </row>
+    <row r="57" spans="1:9" s="10" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>50</v>
       </c>
       <c r="B57" s="30" t="s">
-        <v>150</v>
+        <v>204</v>
       </c>
       <c r="C57" s="33"/>
       <c r="D57" s="13"/>
@@ -15402,15 +15399,15 @@
       <c r="F57" s="13"/>
       <c r="G57" s="13"/>
       <c r="H57" s="13"/>
-      <c r="I57" s="49"/>
-    </row>
-    <row r="58" spans="1:9" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I57" s="36"/>
+    </row>
+    <row r="58" spans="1:9" s="10" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>51</v>
       </c>
       <c r="B58" s="30" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C58" s="33"/>
       <c r="D58" s="13"/>
@@ -15418,28 +15415,31 @@
       <c r="F58" s="13"/>
       <c r="G58" s="13"/>
       <c r="H58" s="13"/>
-      <c r="I58" s="49"/>
-    </row>
-    <row r="59" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="46" t="s">
-        <v>154</v>
-      </c>
-      <c r="B59" s="47"/>
-      <c r="C59" s="47"/>
-      <c r="D59" s="47"/>
-      <c r="E59" s="47"/>
-      <c r="F59" s="47"/>
-      <c r="G59" s="47"/>
-      <c r="H59" s="47"/>
-      <c r="I59" s="47"/>
-    </row>
-    <row r="60" spans="1:9" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I58" s="36"/>
+    </row>
+    <row r="59" spans="1:9" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B59" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="C59" s="33"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="36"/>
+    </row>
+    <row r="60" spans="1:9" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="27">
-        <f ca="1">IF(OFFSET(A60,-2,0) ="",OFFSET(A60,-2,0)+1,OFFSET(A60,-2,0)+1 )</f>
-        <v>52</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>53</v>
       </c>
       <c r="B60" s="30" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="C60" s="33"/>
       <c r="D60" s="13"/>
@@ -15447,31 +15447,28 @@
       <c r="F60" s="13"/>
       <c r="G60" s="13"/>
       <c r="H60" s="13"/>
-      <c r="I60" s="49"/>
-    </row>
-    <row r="61" spans="1:9" s="10" customFormat="1" ht="25" x14ac:dyDescent="0.25">
-      <c r="A61" s="27">
-        <f t="shared" ca="1" si="0"/>
-        <v>53</v>
-      </c>
-      <c r="B61" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="C61" s="33"/>
-      <c r="D61" s="13"/>
-      <c r="E61" s="13"/>
-      <c r="F61" s="13"/>
-      <c r="G61" s="13"/>
-      <c r="H61" s="13"/>
+      <c r="I60" s="36"/>
+    </row>
+    <row r="61" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="48" t="s">
+        <v>154</v>
+      </c>
+      <c r="B61" s="49"/>
+      <c r="C61" s="49"/>
+      <c r="D61" s="49"/>
+      <c r="E61" s="49"/>
+      <c r="F61" s="49"/>
+      <c r="G61" s="49"/>
+      <c r="H61" s="49"/>
       <c r="I61" s="49"/>
     </row>
-    <row r="62" spans="1:9" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">IF(OFFSET(A62,-2,0) ="",OFFSET(A62,-2,0)+1,OFFSET(A62,-2,0)+1 )</f>
         <v>54</v>
       </c>
       <c r="B62" s="30" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C62" s="33"/>
       <c r="D62" s="13"/>
@@ -15479,15 +15476,15 @@
       <c r="F62" s="13"/>
       <c r="G62" s="13"/>
       <c r="H62" s="13"/>
-      <c r="I62" s="49"/>
-    </row>
-    <row r="63" spans="1:9" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I62" s="36"/>
+    </row>
+    <row r="63" spans="1:9" s="10" customFormat="1" ht="25" x14ac:dyDescent="0.25">
       <c r="A63" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>55</v>
       </c>
       <c r="B63" s="30" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C63" s="33"/>
       <c r="D63" s="13"/>
@@ -15495,106 +15492,106 @@
       <c r="F63" s="13"/>
       <c r="G63" s="13"/>
       <c r="H63" s="13"/>
-      <c r="I63" s="49"/>
-    </row>
-    <row r="64" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="46" t="s">
-        <v>155</v>
-      </c>
-      <c r="B64" s="47"/>
-      <c r="C64" s="47"/>
-      <c r="D64" s="47"/>
-      <c r="E64" s="47"/>
-      <c r="F64" s="47"/>
-      <c r="G64" s="47"/>
-      <c r="H64" s="47"/>
-      <c r="I64" s="47"/>
-    </row>
-    <row r="65" spans="1:9" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I63" s="36"/>
+    </row>
+    <row r="64" spans="1:9" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B64" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="C64" s="33"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="13"/>
+      <c r="H64" s="13"/>
+      <c r="I64" s="36"/>
+    </row>
+    <row r="65" spans="1:9" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="27">
-        <f ca="1">IF(OFFSET(A65,-2,0) ="",OFFSET(A65,-2,0)+1,OFFSET(A65,-2,0)+1 )</f>
-        <v>56</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>57</v>
       </c>
       <c r="B65" s="30" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="C65" s="33"/>
+      <c r="D65" s="13"/>
       <c r="E65" s="13"/>
       <c r="F65" s="13"/>
       <c r="G65" s="13"/>
       <c r="H65" s="13"/>
-      <c r="I65" s="49"/>
-    </row>
-    <row r="66" spans="1:9" s="10" customFormat="1" ht="25" x14ac:dyDescent="0.25">
-      <c r="A66" s="27">
-        <f t="shared" ca="1" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="B66" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="C66" s="33"/>
-      <c r="E66" s="13"/>
-      <c r="F66" s="13"/>
-      <c r="G66" s="13"/>
-      <c r="H66" s="13"/>
+      <c r="I65" s="36"/>
+    </row>
+    <row r="66" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="48" t="s">
+        <v>155</v>
+      </c>
+      <c r="B66" s="49"/>
+      <c r="C66" s="49"/>
+      <c r="D66" s="49"/>
+      <c r="E66" s="49"/>
+      <c r="F66" s="49"/>
+      <c r="G66" s="49"/>
+      <c r="H66" s="49"/>
       <c r="I66" s="49"/>
     </row>
-    <row r="67" spans="1:9" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">IF(OFFSET(A67,-2,0) ="",OFFSET(A67,-2,0)+1,OFFSET(A67,-2,0)+1 )</f>
         <v>58</v>
       </c>
-      <c r="B67" s="29" t="s">
-        <v>156</v>
+      <c r="B67" s="30" t="s">
+        <v>146</v>
       </c>
       <c r="C67" s="33"/>
-      <c r="D67" s="30"/>
       <c r="E67" s="13"/>
       <c r="F67" s="13"/>
       <c r="G67" s="13"/>
       <c r="H67" s="13"/>
-      <c r="I67" s="49"/>
-    </row>
-    <row r="68" spans="1:9" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I67" s="36"/>
+    </row>
+    <row r="68" spans="1:9" s="10" customFormat="1" ht="25" x14ac:dyDescent="0.25">
       <c r="A68" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>59</v>
       </c>
-      <c r="B68" s="29" t="s">
-        <v>158</v>
+      <c r="B68" s="30" t="s">
+        <v>134</v>
       </c>
       <c r="C68" s="33"/>
-      <c r="D68" s="13"/>
       <c r="E68" s="13"/>
       <c r="F68" s="13"/>
       <c r="G68" s="13"/>
       <c r="H68" s="13"/>
-      <c r="I68" s="49"/>
-    </row>
-    <row r="69" spans="1:9" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I68" s="36"/>
+    </row>
+    <row r="69" spans="1:9" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>60</v>
       </c>
       <c r="B69" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C69" s="33"/>
-      <c r="D69" s="13"/>
+      <c r="D69" s="30"/>
       <c r="E69" s="13"/>
       <c r="F69" s="13"/>
       <c r="G69" s="13"/>
       <c r="H69" s="13"/>
-      <c r="I69" s="49"/>
-    </row>
-    <row r="70" spans="1:9" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I69" s="36"/>
+    </row>
+    <row r="70" spans="1:9" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>61</v>
       </c>
       <c r="B70" s="29" t="s">
-        <v>129</v>
+        <v>158</v>
       </c>
       <c r="C70" s="33"/>
       <c r="D70" s="13"/>
@@ -15602,15 +15599,15 @@
       <c r="F70" s="13"/>
       <c r="G70" s="13"/>
       <c r="H70" s="13"/>
-      <c r="I70" s="49"/>
-    </row>
-    <row r="71" spans="1:9" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I70" s="36"/>
+    </row>
+    <row r="71" spans="1:9" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>62</v>
       </c>
       <c r="B71" s="29" t="s">
-        <v>142</v>
+        <v>157</v>
       </c>
       <c r="C71" s="33"/>
       <c r="D71" s="13"/>
@@ -15618,15 +15615,15 @@
       <c r="F71" s="13"/>
       <c r="G71" s="13"/>
       <c r="H71" s="13"/>
-      <c r="I71" s="49"/>
-    </row>
-    <row r="72" spans="1:9" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I71" s="36"/>
+    </row>
+    <row r="72" spans="1:9" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>63</v>
       </c>
       <c r="B72" s="29" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="C72" s="33"/>
       <c r="D72" s="13"/>
@@ -15634,15 +15631,15 @@
       <c r="F72" s="13"/>
       <c r="G72" s="13"/>
       <c r="H72" s="13"/>
-      <c r="I72" s="49"/>
-    </row>
-    <row r="73" spans="1:9" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I72" s="36"/>
+    </row>
+    <row r="73" spans="1:9" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>64</v>
       </c>
       <c r="B73" s="29" t="s">
-        <v>126</v>
+        <v>142</v>
       </c>
       <c r="C73" s="33"/>
       <c r="D73" s="13"/>
@@ -15650,15 +15647,15 @@
       <c r="F73" s="13"/>
       <c r="G73" s="13"/>
       <c r="H73" s="13"/>
-      <c r="I73" s="49"/>
-    </row>
-    <row r="74" spans="1:9" s="10" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I73" s="36"/>
+    </row>
+    <row r="74" spans="1:9" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>65</v>
       </c>
-      <c r="B74" s="30" t="s">
-        <v>159</v>
+      <c r="B74" s="29" t="s">
+        <v>143</v>
       </c>
       <c r="C74" s="33"/>
       <c r="D74" s="13"/>
@@ -15666,15 +15663,15 @@
       <c r="F74" s="13"/>
       <c r="G74" s="13"/>
       <c r="H74" s="13"/>
-      <c r="I74" s="49"/>
-    </row>
-    <row r="75" spans="1:9" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I74" s="36"/>
+    </row>
+    <row r="75" spans="1:9" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>66</v>
       </c>
-      <c r="B75" s="30" t="s">
-        <v>160</v>
+      <c r="B75" s="29" t="s">
+        <v>126</v>
       </c>
       <c r="C75" s="33"/>
       <c r="D75" s="13"/>
@@ -15682,15 +15679,15 @@
       <c r="F75" s="13"/>
       <c r="G75" s="13"/>
       <c r="H75" s="13"/>
-      <c r="I75" s="49"/>
-    </row>
-    <row r="76" spans="1:9" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I75" s="36"/>
+    </row>
+    <row r="76" spans="1:9" s="10" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>67</v>
       </c>
-      <c r="B76" s="15" t="s">
-        <v>145</v>
+      <c r="B76" s="30" t="s">
+        <v>159</v>
       </c>
       <c r="C76" s="33"/>
       <c r="D76" s="13"/>
@@ -15698,41 +15695,47 @@
       <c r="F76" s="13"/>
       <c r="G76" s="13"/>
       <c r="H76" s="13"/>
-      <c r="I76" s="49"/>
-    </row>
-    <row r="77" spans="1:9" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="39" t="s">
-        <v>167</v>
-      </c>
-      <c r="B77" s="48"/>
-      <c r="C77" s="48"/>
-      <c r="D77" s="48"/>
-      <c r="E77" s="48"/>
-      <c r="F77" s="48"/>
-      <c r="G77" s="48"/>
-      <c r="H77" s="48"/>
-      <c r="I77" s="48"/>
-    </row>
-    <row r="78" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="46" t="s">
-        <v>174</v>
-      </c>
-      <c r="B78" s="47"/>
-      <c r="C78" s="47"/>
-      <c r="D78" s="47"/>
-      <c r="E78" s="47"/>
-      <c r="F78" s="47"/>
-      <c r="G78" s="47"/>
-      <c r="H78" s="47"/>
-      <c r="I78" s="47"/>
-    </row>
-    <row r="79" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I76" s="36"/>
+    </row>
+    <row r="77" spans="1:9" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="B77" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="C77" s="33"/>
+      <c r="D77" s="13"/>
+      <c r="E77" s="13"/>
+      <c r="F77" s="13"/>
+      <c r="G77" s="13"/>
+      <c r="H77" s="13"/>
+      <c r="I77" s="36"/>
+    </row>
+    <row r="78" spans="1:9" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="27">
+        <f ca="1">IF(OFFSET(A78,-1,0) ="",OFFSET(A78,-2,0)+1,OFFSET(A78,-1,0)+1 )</f>
+        <v>69</v>
+      </c>
+      <c r="B78" s="30" t="s">
+        <v>184</v>
+      </c>
+      <c r="C78" s="33"/>
+      <c r="D78" s="30"/>
+      <c r="E78" s="13"/>
+      <c r="F78" s="13"/>
+      <c r="G78" s="13"/>
+      <c r="H78" s="13"/>
+      <c r="I78" s="36"/>
+    </row>
+    <row r="79" spans="1:9" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="27">
-        <f ca="1">IF(OFFSET(A79,-3,0) ="",OFFSET(A79,-3,0)+1,OFFSET(A79,-3,0)+1 )</f>
-        <v>68</v>
-      </c>
-      <c r="B79" s="30" t="s">
-        <v>178</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="B79" s="15" t="s">
+        <v>145</v>
       </c>
       <c r="C79" s="33"/>
       <c r="D79" s="13"/>
@@ -15740,113 +15743,107 @@
       <c r="F79" s="13"/>
       <c r="G79" s="13"/>
       <c r="H79" s="13"/>
-      <c r="I79" s="49"/>
-    </row>
-    <row r="80" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="27">
-        <f t="shared" ref="A80:A87" ca="1" si="2">IF(OFFSET(A80,-1,0) ="",OFFSET(A80,-2,0)+1,OFFSET(A80,-1,0)+1 )</f>
-        <v>69</v>
-      </c>
-      <c r="B80" s="30" t="s">
-        <v>182</v>
-      </c>
-      <c r="C80" s="33"/>
-      <c r="D80" s="13"/>
-      <c r="E80" s="13"/>
-      <c r="F80" s="13"/>
-      <c r="G80" s="13"/>
-      <c r="H80" s="13"/>
-      <c r="I80" s="49"/>
-    </row>
-    <row r="81" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="27">
-        <f t="shared" ca="1" si="2"/>
-        <v>70</v>
-      </c>
-      <c r="B81" s="30" t="s">
-        <v>179</v>
-      </c>
-      <c r="C81" s="33"/>
-      <c r="D81" s="13"/>
-      <c r="E81" s="13"/>
-      <c r="F81" s="13"/>
-      <c r="G81" s="13"/>
-      <c r="H81" s="13"/>
+      <c r="I79" s="36"/>
+    </row>
+    <row r="80" spans="1:9" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="41" t="s">
+        <v>167</v>
+      </c>
+      <c r="B80" s="50"/>
+      <c r="C80" s="50"/>
+      <c r="D80" s="50"/>
+      <c r="E80" s="50"/>
+      <c r="F80" s="50"/>
+      <c r="G80" s="50"/>
+      <c r="H80" s="50"/>
+      <c r="I80" s="50"/>
+    </row>
+    <row r="81" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="48" t="s">
+        <v>174</v>
+      </c>
+      <c r="B81" s="49"/>
+      <c r="C81" s="49"/>
+      <c r="D81" s="49"/>
+      <c r="E81" s="49"/>
+      <c r="F81" s="49"/>
+      <c r="G81" s="49"/>
+      <c r="H81" s="49"/>
       <c r="I81" s="49"/>
     </row>
-    <row r="82" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="27">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">IF(OFFSET(A82,-3,0) ="",OFFSET(A82,-3,0)+1,OFFSET(A82,-3,0)+1 )</f>
         <v>71</v>
       </c>
       <c r="B82" s="30" t="s">
-        <v>183</v>
-      </c>
-      <c r="C82" s="33" t="s">
-        <v>180</v>
-      </c>
-      <c r="D82" s="30"/>
+        <v>178</v>
+      </c>
+      <c r="C82" s="33"/>
+      <c r="D82" s="13"/>
       <c r="E82" s="13"/>
       <c r="F82" s="13"/>
       <c r="G82" s="13"/>
       <c r="H82" s="13"/>
-      <c r="I82" s="49"/>
-    </row>
-    <row r="83" spans="1:9" s="10" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I82" s="36"/>
+    </row>
+    <row r="83" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="27">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ref="A83:A86" ca="1" si="2">IF(OFFSET(A83,-1,0) ="",OFFSET(A83,-2,0)+1,OFFSET(A83,-1,0)+1 )</f>
         <v>72</v>
       </c>
       <c r="B83" s="30" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C83" s="33"/>
-      <c r="D83" s="30"/>
+      <c r="D83" s="13"/>
       <c r="E83" s="13"/>
       <c r="F83" s="13"/>
       <c r="G83" s="13"/>
       <c r="H83" s="13"/>
-      <c r="I83" s="49"/>
-    </row>
-    <row r="84" spans="1:9" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I83" s="36"/>
+    </row>
+    <row r="84" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="27">
         <f t="shared" ca="1" si="2"/>
         <v>73</v>
       </c>
       <c r="B84" s="30" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C84" s="33"/>
-      <c r="D84" s="30"/>
+      <c r="D84" s="13"/>
       <c r="E84" s="13"/>
       <c r="F84" s="13"/>
       <c r="G84" s="13"/>
       <c r="H84" s="13"/>
-      <c r="I84" s="49"/>
-    </row>
-    <row r="85" spans="1:9" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I84" s="36"/>
+    </row>
+    <row r="85" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="27">
         <f t="shared" ca="1" si="2"/>
         <v>74</v>
       </c>
       <c r="B85" s="30" t="s">
-        <v>186</v>
-      </c>
-      <c r="C85" s="33"/>
-      <c r="D85" s="13"/>
+        <v>193</v>
+      </c>
+      <c r="C85" s="33" t="s">
+        <v>180</v>
+      </c>
+      <c r="D85" s="30"/>
       <c r="E85" s="13"/>
       <c r="F85" s="13"/>
       <c r="G85" s="13"/>
       <c r="H85" s="13"/>
-      <c r="I85" s="49"/>
-    </row>
-    <row r="86" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I85" s="36"/>
+    </row>
+    <row r="86" spans="1:9" s="10" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="27">
         <f t="shared" ca="1" si="2"/>
         <v>75</v>
       </c>
       <c r="B86" s="30" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="C86" s="33"/>
       <c r="D86" s="13"/>
@@ -15854,40 +15851,40 @@
       <c r="F86" s="13"/>
       <c r="G86" s="13"/>
       <c r="H86" s="13"/>
-      <c r="I86" s="49"/>
-    </row>
-    <row r="87" spans="1:9" s="10" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="27">
-        <f t="shared" ca="1" si="2"/>
+      <c r="I86" s="36"/>
+    </row>
+    <row r="87" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="48" t="s">
+        <v>202</v>
+      </c>
+      <c r="B87" s="49"/>
+      <c r="C87" s="49"/>
+      <c r="D87" s="49"/>
+      <c r="E87" s="49"/>
+      <c r="F87" s="49"/>
+      <c r="G87" s="49"/>
+      <c r="H87" s="49"/>
+      <c r="I87" s="49"/>
+    </row>
+    <row r="88" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="27">
+        <f ca="1">IF(OFFSET(A88,-2,0) ="",OFFSET(A88,-2,0)+1,OFFSET(A88,-2,0)+1 )</f>
         <v>76</v>
       </c>
-      <c r="B87" s="30" t="s">
-        <v>187</v>
-      </c>
-      <c r="C87" s="33"/>
-      <c r="D87" s="13"/>
-      <c r="E87" s="13"/>
-      <c r="F87" s="13"/>
-      <c r="G87" s="13"/>
-      <c r="H87" s="13"/>
-      <c r="I87" s="49"/>
-    </row>
-    <row r="88" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="46" t="s">
-        <v>203</v>
-      </c>
-      <c r="B88" s="47"/>
-      <c r="C88" s="47"/>
-      <c r="D88" s="47"/>
-      <c r="E88" s="47"/>
-      <c r="F88" s="47"/>
-      <c r="G88" s="47"/>
-      <c r="H88" s="47"/>
-      <c r="I88" s="47"/>
+      <c r="B88" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="C88" s="33"/>
+      <c r="D88" s="13"/>
+      <c r="E88" s="13"/>
+      <c r="F88" s="13"/>
+      <c r="G88" s="13"/>
+      <c r="H88" s="13"/>
+      <c r="I88" s="36"/>
     </row>
     <row r="89" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="27">
-        <f ca="1">IF(OFFSET(A89,-2,0) ="",OFFSET(A89,-2,0)+1,OFFSET(A89,-2,0)+1 )</f>
+        <f t="shared" ref="A89:A93" ca="1" si="3">IF(OFFSET(A89,-1,0) ="",OFFSET(A89,-2,0)+1,OFFSET(A89,-1,0)+1 )</f>
         <v>77</v>
       </c>
       <c r="B89" s="30" t="s">
@@ -15899,11 +15896,11 @@
       <c r="F89" s="13"/>
       <c r="G89" s="13"/>
       <c r="H89" s="13"/>
-      <c r="I89" s="49"/>
-    </row>
-    <row r="90" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I89" s="36"/>
+    </row>
+    <row r="90" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="27">
-        <f t="shared" ref="A90:A97" ca="1" si="3">IF(OFFSET(A90,-1,0) ="",OFFSET(A90,-2,0)+1,OFFSET(A90,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="3"/>
         <v>78</v>
       </c>
       <c r="B90" s="30" t="s">
@@ -15915,23 +15912,25 @@
       <c r="F90" s="13"/>
       <c r="G90" s="13"/>
       <c r="H90" s="13"/>
-      <c r="I90" s="49"/>
-    </row>
-    <row r="91" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I90" s="36"/>
+    </row>
+    <row r="91" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="27">
         <f t="shared" ca="1" si="3"/>
         <v>79</v>
       </c>
       <c r="B91" s="30" t="s">
-        <v>191</v>
-      </c>
-      <c r="C91" s="33"/>
-      <c r="D91" s="13"/>
+        <v>193</v>
+      </c>
+      <c r="C91" s="33" t="s">
+        <v>180</v>
+      </c>
+      <c r="D91" s="30"/>
       <c r="E91" s="13"/>
       <c r="F91" s="13"/>
       <c r="G91" s="13"/>
       <c r="H91" s="13"/>
-      <c r="I91" s="49"/>
+      <c r="I91" s="36"/>
     </row>
     <row r="92" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="27">
@@ -15939,57 +15938,52 @@
         <v>80</v>
       </c>
       <c r="B92" s="30" t="s">
-        <v>194</v>
-      </c>
-      <c r="C92" s="33" t="s">
-        <v>180</v>
-      </c>
-      <c r="D92" s="30"/>
+        <v>201</v>
+      </c>
+      <c r="C92" s="33"/>
+      <c r="D92" s="13"/>
       <c r="E92" s="13"/>
       <c r="F92" s="13"/>
       <c r="G92" s="13"/>
       <c r="H92" s="13"/>
-      <c r="I92" s="49"/>
-    </row>
-    <row r="93" spans="1:9" s="10" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I92" s="36"/>
+    </row>
+    <row r="93" spans="1:9" s="10" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="27">
         <f t="shared" ca="1" si="3"/>
         <v>81</v>
       </c>
       <c r="B93" s="30" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C93" s="33"/>
-      <c r="D93" s="30"/>
+      <c r="D93" s="13"/>
       <c r="E93" s="13"/>
       <c r="F93" s="13"/>
       <c r="G93" s="13"/>
       <c r="H93" s="13"/>
-      <c r="I93" s="49"/>
-    </row>
-    <row r="94" spans="1:9" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="27">
-        <f t="shared" ca="1" si="3"/>
+      <c r="I93" s="36"/>
+    </row>
+    <row r="94" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="48" t="s">
+        <v>197</v>
+      </c>
+      <c r="B94" s="49"/>
+      <c r="C94" s="49"/>
+      <c r="D94" s="49"/>
+      <c r="E94" s="49"/>
+      <c r="F94" s="49"/>
+      <c r="G94" s="49"/>
+      <c r="H94" s="49"/>
+      <c r="I94" s="49"/>
+    </row>
+    <row r="95" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="27">
+        <f ca="1">IF(OFFSET(A95,-2,0) ="",OFFSET(A95,-2,0)+1,OFFSET(A95,-2,0)+1 )</f>
         <v>82</v>
       </c>
-      <c r="B94" s="30" t="s">
-        <v>185</v>
-      </c>
-      <c r="C94" s="33"/>
-      <c r="D94" s="30"/>
-      <c r="E94" s="13"/>
-      <c r="F94" s="13"/>
-      <c r="G94" s="13"/>
-      <c r="H94" s="13"/>
-      <c r="I94" s="49"/>
-    </row>
-    <row r="95" spans="1:9" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="27">
-        <f t="shared" ca="1" si="3"/>
-        <v>83</v>
-      </c>
       <c r="B95" s="30" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="C95" s="33"/>
       <c r="D95" s="13"/>
@@ -15997,31 +15991,28 @@
       <c r="F95" s="13"/>
       <c r="G95" s="13"/>
       <c r="H95" s="13"/>
-      <c r="I95" s="49"/>
-    </row>
-    <row r="96" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="27">
-        <f t="shared" ca="1" si="3"/>
-        <v>84</v>
-      </c>
-      <c r="B96" s="30" t="s">
-        <v>202</v>
-      </c>
-      <c r="C96" s="33"/>
-      <c r="D96" s="13"/>
-      <c r="E96" s="13"/>
-      <c r="F96" s="13"/>
-      <c r="G96" s="13"/>
-      <c r="H96" s="13"/>
+      <c r="I95" s="36"/>
+    </row>
+    <row r="96" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="48" t="s">
+        <v>198</v>
+      </c>
+      <c r="B96" s="49"/>
+      <c r="C96" s="49"/>
+      <c r="D96" s="49"/>
+      <c r="E96" s="49"/>
+      <c r="F96" s="49"/>
+      <c r="G96" s="49"/>
+      <c r="H96" s="49"/>
       <c r="I96" s="49"/>
     </row>
-    <row r="97" spans="1:26" s="10" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:26" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="27">
-        <f t="shared" ca="1" si="3"/>
-        <v>85</v>
+        <f ca="1">IF(OFFSET(A97,-2,0) ="",OFFSET(A97,-2,0)+1,OFFSET(A97,-2,0)+1 )</f>
+        <v>83</v>
       </c>
       <c r="B97" s="30" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="C97" s="33"/>
       <c r="D97" s="13"/>
@@ -16029,143 +16020,146 @@
       <c r="F97" s="13"/>
       <c r="G97" s="13"/>
       <c r="H97" s="13"/>
-      <c r="I97" s="49"/>
-    </row>
-    <row r="98" spans="1:26" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="46" t="s">
-        <v>198</v>
-      </c>
-      <c r="B98" s="47"/>
-      <c r="C98" s="47"/>
-      <c r="D98" s="47"/>
-      <c r="E98" s="47"/>
-      <c r="F98" s="47"/>
-      <c r="G98" s="47"/>
-      <c r="H98" s="47"/>
-      <c r="I98" s="47"/>
-    </row>
-    <row r="99" spans="1:26" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="27">
-        <f ca="1">IF(OFFSET(A99,-2,0) ="",OFFSET(A99,-2,0)+1,OFFSET(A99,-2,0)+1 )</f>
-        <v>86</v>
-      </c>
-      <c r="B99" s="30" t="s">
-        <v>195</v>
-      </c>
-      <c r="C99" s="33"/>
-      <c r="D99" s="13"/>
-      <c r="E99" s="13"/>
-      <c r="F99" s="13"/>
-      <c r="G99" s="13"/>
-      <c r="H99" s="13"/>
-      <c r="I99" s="49"/>
-    </row>
-    <row r="100" spans="1:26" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="46" t="s">
-        <v>199</v>
-      </c>
-      <c r="B100" s="47"/>
-      <c r="C100" s="47"/>
-      <c r="D100" s="47"/>
-      <c r="E100" s="47"/>
-      <c r="F100" s="47"/>
-      <c r="G100" s="47"/>
-      <c r="H100" s="47"/>
-      <c r="I100" s="47"/>
-    </row>
-    <row r="101" spans="1:26" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I97" s="36"/>
+    </row>
+    <row r="98" spans="1:26" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="27"/>
+      <c r="B98" s="30"/>
+      <c r="C98" s="33"/>
+      <c r="D98" s="13"/>
+      <c r="E98" s="13"/>
+      <c r="F98" s="13"/>
+      <c r="G98" s="13"/>
+      <c r="H98" s="13"/>
+      <c r="I98" s="36"/>
+    </row>
+    <row r="99" spans="1:26" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="41" t="s">
+        <v>207</v>
+      </c>
+      <c r="B99" s="50"/>
+      <c r="C99" s="50"/>
+      <c r="D99" s="50"/>
+      <c r="E99" s="50"/>
+      <c r="F99" s="50"/>
+      <c r="G99" s="50"/>
+      <c r="H99" s="50"/>
+      <c r="I99" s="50"/>
+    </row>
+    <row r="100" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="48" t="s">
+        <v>177</v>
+      </c>
+      <c r="B100" s="49"/>
+      <c r="C100" s="49"/>
+      <c r="D100" s="49"/>
+      <c r="E100" s="49"/>
+      <c r="F100" s="49"/>
+      <c r="G100" s="49"/>
+      <c r="H100" s="49"/>
+      <c r="I100" s="49"/>
+      <c r="J100" s="26"/>
+      <c r="K100" s="26"/>
+      <c r="L100" s="26"/>
+      <c r="M100" s="26"/>
+      <c r="N100" s="26"/>
+      <c r="O100" s="26"/>
+      <c r="P100" s="26"/>
+      <c r="Q100" s="26"/>
+      <c r="R100" s="26"/>
+      <c r="S100" s="26"/>
+      <c r="T100" s="26"/>
+      <c r="U100" s="26"/>
+      <c r="V100" s="26"/>
+      <c r="W100" s="26"/>
+      <c r="X100" s="26"/>
+      <c r="Y100" s="26"/>
+      <c r="Z100" s="26"/>
+    </row>
+    <row r="101" spans="1:26" s="10" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="27">
-        <f ca="1">IF(OFFSET(A101,-2,0) ="",OFFSET(A101,-2,0)+1,OFFSET(A101,-2,0)+1 )</f>
-        <v>87</v>
+        <f ca="1">IF(OFFSET(A101,-3,0) ="",OFFSET(A101,-3,0)+1,OFFSET(A101,-3,0)+1 )</f>
+        <v>1</v>
       </c>
       <c r="B101" s="30" t="s">
-        <v>196</v>
-      </c>
-      <c r="C101" s="33"/>
+        <v>121</v>
+      </c>
+      <c r="C101" s="34"/>
       <c r="D101" s="13"/>
       <c r="E101" s="13"/>
       <c r="F101" s="13"/>
       <c r="G101" s="13"/>
       <c r="H101" s="13"/>
-      <c r="I101" s="49"/>
-    </row>
-    <row r="102" spans="1:26" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="27"/>
-      <c r="B102" s="30"/>
+      <c r="I101" s="36"/>
+    </row>
+    <row r="102" spans="1:26" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="27">
+        <f ca="1">IF(OFFSET(A102,-1,0) ="",OFFSET(A102,-2,0)+1,OFFSET(A102,-1,0)+1 )</f>
+        <v>2</v>
+      </c>
+      <c r="B102" s="12" t="s">
+        <v>181</v>
+      </c>
       <c r="C102" s="33"/>
       <c r="D102" s="13"/>
       <c r="E102" s="13"/>
       <c r="F102" s="13"/>
       <c r="G102" s="13"/>
       <c r="H102" s="13"/>
-      <c r="I102" s="49"/>
-    </row>
-    <row r="103" spans="1:26" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="39" t="s">
-        <v>208</v>
-      </c>
-      <c r="B103" s="48"/>
-      <c r="C103" s="48"/>
-      <c r="D103" s="48"/>
-      <c r="E103" s="48"/>
-      <c r="F103" s="48"/>
-      <c r="G103" s="48"/>
-      <c r="H103" s="48"/>
-      <c r="I103" s="48"/>
-    </row>
-    <row r="104" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A104" s="46" t="s">
-        <v>177</v>
-      </c>
-      <c r="B104" s="47"/>
-      <c r="C104" s="47"/>
-      <c r="D104" s="47"/>
-      <c r="E104" s="47"/>
-      <c r="F104" s="47"/>
-      <c r="G104" s="47"/>
-      <c r="H104" s="47"/>
-      <c r="I104" s="47"/>
-      <c r="J104" s="26"/>
-      <c r="K104" s="26"/>
-      <c r="L104" s="26"/>
-      <c r="M104" s="26"/>
-      <c r="N104" s="26"/>
-      <c r="O104" s="26"/>
-      <c r="P104" s="26"/>
-      <c r="Q104" s="26"/>
-      <c r="R104" s="26"/>
-      <c r="S104" s="26"/>
-      <c r="T104" s="26"/>
-      <c r="U104" s="26"/>
-      <c r="V104" s="26"/>
-      <c r="W104" s="26"/>
-      <c r="X104" s="26"/>
-      <c r="Y104" s="26"/>
-      <c r="Z104" s="26"/>
-    </row>
-    <row r="105" spans="1:26" s="10" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I102" s="36"/>
+    </row>
+    <row r="103" spans="1:26" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="27">
+        <f ca="1">IF(OFFSET(A103,-1,0) ="",OFFSET(A103,-2,0)+1,OFFSET(A103,-1,0)+1 )</f>
+        <v>3</v>
+      </c>
+      <c r="B103" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="C103" s="33"/>
+      <c r="D103" s="13"/>
+      <c r="E103" s="13"/>
+      <c r="F103" s="13"/>
+      <c r="G103" s="13"/>
+      <c r="H103" s="13"/>
+      <c r="I103" s="36"/>
+    </row>
+    <row r="104" spans="1:26" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="48" t="s">
+        <v>161</v>
+      </c>
+      <c r="B104" s="49"/>
+      <c r="C104" s="49"/>
+      <c r="D104" s="49"/>
+      <c r="E104" s="49"/>
+      <c r="F104" s="49"/>
+      <c r="G104" s="49"/>
+      <c r="H104" s="49"/>
+      <c r="I104" s="49"/>
+    </row>
+    <row r="105" spans="1:26" s="10" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="27">
-        <f ca="1">IF(OFFSET(A105,-3,0) ="",OFFSET(A105,-3,0)+1,OFFSET(A105,-3,0)+1 )</f>
-        <v>1</v>
+        <f ca="1">IF(OFFSET(A105,-2,0) ="",OFFSET(A105,-2,0)+1,OFFSET(A105,-2,0)+1 )</f>
+        <v>4</v>
       </c>
       <c r="B105" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="C105" s="34"/>
+        <v>162</v>
+      </c>
+      <c r="C105" s="33"/>
       <c r="D105" s="13"/>
       <c r="E105" s="13"/>
       <c r="F105" s="13"/>
       <c r="G105" s="13"/>
       <c r="H105" s="13"/>
-      <c r="I105" s="49"/>
-    </row>
-    <row r="106" spans="1:26" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I105" s="36"/>
+    </row>
+    <row r="106" spans="1:26" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="27">
-        <f ca="1">IF(OFFSET(A106,-1,0) ="",OFFSET(A106,-2,0)+1,OFFSET(A106,-1,0)+1 )</f>
-        <v>2</v>
-      </c>
-      <c r="B106" s="12" t="s">
-        <v>181</v>
+        <f t="shared" ref="A106" ca="1" si="4">IF(OFFSET(A106,-1,0) ="",OFFSET(A106,-2,0)+1,OFFSET(A106,-1,0)+1 )</f>
+        <v>5</v>
+      </c>
+      <c r="B106" s="30" t="s">
+        <v>163</v>
       </c>
       <c r="C106" s="33"/>
       <c r="D106" s="13"/>
@@ -16173,60 +16167,57 @@
       <c r="F106" s="13"/>
       <c r="G106" s="13"/>
       <c r="H106" s="13"/>
-      <c r="I106" s="49"/>
-    </row>
-    <row r="107" spans="1:26" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="27">
-        <f ca="1">IF(OFFSET(A107,-1,0) ="",OFFSET(A107,-2,0)+1,OFFSET(A107,-1,0)+1 )</f>
-        <v>3</v>
-      </c>
-      <c r="B107" s="15" t="s">
+      <c r="I106" s="36"/>
+    </row>
+    <row r="107" spans="1:26" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="B107" s="49"/>
+      <c r="C107" s="49"/>
+      <c r="D107" s="49"/>
+      <c r="E107" s="49"/>
+      <c r="F107" s="49"/>
+      <c r="G107" s="49"/>
+      <c r="H107" s="49"/>
+      <c r="I107" s="49"/>
+    </row>
+    <row r="108" spans="1:26" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="27">
+        <f ca="1">IF(OFFSET(A108,-2,0) ="",OFFSET(A108,-2,0)+1,OFFSET(A108,-2,0)+1 )</f>
+        <v>6</v>
+      </c>
+      <c r="B108" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="C108" s="33"/>
+      <c r="D108" s="13"/>
+      <c r="E108" s="13"/>
+      <c r="F108" s="13"/>
+      <c r="G108" s="13"/>
+      <c r="H108" s="13"/>
+      <c r="I108" s="36"/>
+    </row>
+    <row r="109" spans="1:26" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="48" t="s">
         <v>192</v>
       </c>
-      <c r="C107" s="33"/>
-      <c r="D107" s="13"/>
-      <c r="E107" s="13"/>
-      <c r="F107" s="13"/>
-      <c r="G107" s="13"/>
-      <c r="H107" s="13"/>
-      <c r="I107" s="49"/>
-    </row>
-    <row r="108" spans="1:26" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="46" t="s">
-        <v>161</v>
-      </c>
-      <c r="B108" s="47"/>
-      <c r="C108" s="47"/>
-      <c r="D108" s="47"/>
-      <c r="E108" s="47"/>
-      <c r="F108" s="47"/>
-      <c r="G108" s="47"/>
-      <c r="H108" s="47"/>
-      <c r="I108" s="47"/>
-    </row>
-    <row r="109" spans="1:26" s="10" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="27">
-        <f ca="1">IF(OFFSET(A109,-2,0) ="",OFFSET(A109,-2,0)+1,OFFSET(A109,-2,0)+1 )</f>
-        <v>4</v>
-      </c>
-      <c r="B109" s="30" t="s">
-        <v>162</v>
-      </c>
-      <c r="C109" s="33"/>
-      <c r="D109" s="13"/>
-      <c r="E109" s="13"/>
-      <c r="F109" s="13"/>
-      <c r="G109" s="13"/>
-      <c r="H109" s="13"/>
+      <c r="B109" s="49"/>
+      <c r="C109" s="49"/>
+      <c r="D109" s="49"/>
+      <c r="E109" s="49"/>
+      <c r="F109" s="49"/>
+      <c r="G109" s="49"/>
+      <c r="H109" s="49"/>
       <c r="I109" s="49"/>
     </row>
-    <row r="110" spans="1:26" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:26" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="27">
-        <f t="shared" ref="A110" ca="1" si="4">IF(OFFSET(A110,-1,0) ="",OFFSET(A110,-2,0)+1,OFFSET(A110,-1,0)+1 )</f>
-        <v>5</v>
+        <f ca="1">IF(OFFSET(A110,-2,0) ="",OFFSET(A110,-2,0)+1,OFFSET(A110,-2,0)+1 )</f>
+        <v>7</v>
       </c>
       <c r="B110" s="30" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C110" s="33"/>
       <c r="D110" s="13"/>
@@ -16234,25 +16225,25 @@
       <c r="F110" s="13"/>
       <c r="G110" s="13"/>
       <c r="H110" s="13"/>
-      <c r="I110" s="49"/>
+      <c r="I110" s="36"/>
     </row>
     <row r="111" spans="1:26" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="46" t="s">
-        <v>164</v>
-      </c>
-      <c r="B111" s="47"/>
-      <c r="C111" s="47"/>
-      <c r="D111" s="47"/>
-      <c r="E111" s="47"/>
-      <c r="F111" s="47"/>
-      <c r="G111" s="47"/>
-      <c r="H111" s="47"/>
-      <c r="I111" s="47"/>
+      <c r="A111" s="48" t="s">
+        <v>196</v>
+      </c>
+      <c r="B111" s="49"/>
+      <c r="C111" s="49"/>
+      <c r="D111" s="49"/>
+      <c r="E111" s="49"/>
+      <c r="F111" s="49"/>
+      <c r="G111" s="49"/>
+      <c r="H111" s="49"/>
+      <c r="I111" s="49"/>
     </row>
     <row r="112" spans="1:26" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="27">
         <f ca="1">IF(OFFSET(A112,-2,0) ="",OFFSET(A112,-2,0)+1,OFFSET(A112,-2,0)+1 )</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B112" s="30" t="s">
         <v>165</v>
@@ -16263,65 +16254,51 @@
       <c r="F112" s="13"/>
       <c r="G112" s="13"/>
       <c r="H112" s="13"/>
-      <c r="I112" s="49"/>
-    </row>
-    <row r="113" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="46" t="s">
-        <v>193</v>
-      </c>
-      <c r="B113" s="47"/>
-      <c r="C113" s="47"/>
-      <c r="D113" s="47"/>
-      <c r="E113" s="47"/>
-      <c r="F113" s="47"/>
-      <c r="G113" s="47"/>
-      <c r="H113" s="47"/>
-      <c r="I113" s="47"/>
+      <c r="I112" s="36"/>
+    </row>
+    <row r="113" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="27"/>
+      <c r="B113" s="30"/>
+      <c r="C113" s="33"/>
+      <c r="D113" s="13"/>
+      <c r="E113" s="13"/>
+      <c r="F113" s="13"/>
+      <c r="G113" s="13"/>
+      <c r="H113" s="13"/>
+      <c r="I113" s="36"/>
     </row>
     <row r="114" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="27">
-        <f ca="1">IF(OFFSET(A114,-2,0) ="",OFFSET(A114,-2,0)+1,OFFSET(A114,-2,0)+1 )</f>
-        <v>7</v>
-      </c>
-      <c r="B114" s="30" t="s">
-        <v>165</v>
-      </c>
+      <c r="A114" s="27"/>
+      <c r="B114" s="30"/>
       <c r="C114" s="33"/>
       <c r="D114" s="13"/>
       <c r="E114" s="13"/>
       <c r="F114" s="13"/>
       <c r="G114" s="13"/>
       <c r="H114" s="13"/>
-      <c r="I114" s="49"/>
-    </row>
-    <row r="115" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="46" t="s">
-        <v>197</v>
-      </c>
-      <c r="B115" s="47"/>
-      <c r="C115" s="47"/>
-      <c r="D115" s="47"/>
-      <c r="E115" s="47"/>
-      <c r="F115" s="47"/>
-      <c r="G115" s="47"/>
-      <c r="H115" s="47"/>
-      <c r="I115" s="47"/>
+      <c r="I114" s="36"/>
+    </row>
+    <row r="115" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="27"/>
+      <c r="B115" s="30"/>
+      <c r="C115" s="33"/>
+      <c r="D115" s="13"/>
+      <c r="E115" s="13"/>
+      <c r="F115" s="13"/>
+      <c r="G115" s="13"/>
+      <c r="H115" s="13"/>
+      <c r="I115" s="36"/>
     </row>
     <row r="116" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="27">
-        <f ca="1">IF(OFFSET(A116,-2,0) ="",OFFSET(A116,-2,0)+1,OFFSET(A116,-2,0)+1 )</f>
-        <v>8</v>
-      </c>
-      <c r="B116" s="30" t="s">
-        <v>165</v>
-      </c>
+      <c r="A116" s="27"/>
+      <c r="B116" s="30"/>
       <c r="C116" s="33"/>
       <c r="D116" s="13"/>
       <c r="E116" s="13"/>
       <c r="F116" s="13"/>
       <c r="G116" s="13"/>
       <c r="H116" s="13"/>
-      <c r="I116" s="49"/>
+      <c r="I116" s="36"/>
     </row>
     <row r="117" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="27"/>
@@ -16332,7 +16309,7 @@
       <c r="F117" s="13"/>
       <c r="G117" s="13"/>
       <c r="H117" s="13"/>
-      <c r="I117" s="49"/>
+      <c r="I117" s="36"/>
     </row>
     <row r="118" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="27"/>
@@ -16343,7 +16320,7 @@
       <c r="F118" s="13"/>
       <c r="G118" s="13"/>
       <c r="H118" s="13"/>
-      <c r="I118" s="49"/>
+      <c r="I118" s="36"/>
     </row>
     <row r="119" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="27"/>
@@ -16354,7 +16331,7 @@
       <c r="F119" s="13"/>
       <c r="G119" s="13"/>
       <c r="H119" s="13"/>
-      <c r="I119" s="49"/>
+      <c r="I119" s="36"/>
     </row>
     <row r="120" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="27"/>
@@ -16365,7 +16342,7 @@
       <c r="F120" s="13"/>
       <c r="G120" s="13"/>
       <c r="H120" s="13"/>
-      <c r="I120" s="49"/>
+      <c r="I120" s="36"/>
     </row>
     <row r="121" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="27"/>
@@ -16376,7 +16353,7 @@
       <c r="F121" s="13"/>
       <c r="G121" s="13"/>
       <c r="H121" s="13"/>
-      <c r="I121" s="49"/>
+      <c r="I121" s="36"/>
     </row>
     <row r="122" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="27"/>
@@ -16387,7 +16364,7 @@
       <c r="F122" s="13"/>
       <c r="G122" s="13"/>
       <c r="H122" s="13"/>
-      <c r="I122" s="49"/>
+      <c r="I122" s="36"/>
     </row>
     <row r="123" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="27"/>
@@ -16398,7 +16375,7 @@
       <c r="F123" s="13"/>
       <c r="G123" s="13"/>
       <c r="H123" s="13"/>
-      <c r="I123" s="49"/>
+      <c r="I123" s="36"/>
     </row>
     <row r="124" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="27"/>
@@ -16409,7 +16386,7 @@
       <c r="F124" s="13"/>
       <c r="G124" s="13"/>
       <c r="H124" s="13"/>
-      <c r="I124" s="49"/>
+      <c r="I124" s="36"/>
     </row>
     <row r="125" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="27"/>
@@ -16420,7 +16397,7 @@
       <c r="F125" s="13"/>
       <c r="G125" s="13"/>
       <c r="H125" s="13"/>
-      <c r="I125" s="49"/>
+      <c r="I125" s="36"/>
     </row>
     <row r="126" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="27"/>
@@ -16431,7 +16408,7 @@
       <c r="F126" s="13"/>
       <c r="G126" s="13"/>
       <c r="H126" s="13"/>
-      <c r="I126" s="49"/>
+      <c r="I126" s="36"/>
     </row>
     <row r="127" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="27"/>
@@ -16442,7 +16419,7 @@
       <c r="F127" s="13"/>
       <c r="G127" s="13"/>
       <c r="H127" s="13"/>
-      <c r="I127" s="49"/>
+      <c r="I127" s="36"/>
     </row>
     <row r="128" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="27"/>
@@ -16453,7 +16430,7 @@
       <c r="F128" s="13"/>
       <c r="G128" s="13"/>
       <c r="H128" s="13"/>
-      <c r="I128" s="49"/>
+      <c r="I128" s="36"/>
     </row>
     <row r="129" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="27"/>
@@ -16464,7 +16441,7 @@
       <c r="F129" s="13"/>
       <c r="G129" s="13"/>
       <c r="H129" s="13"/>
-      <c r="I129" s="49"/>
+      <c r="I129" s="36"/>
     </row>
     <row r="130" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="27"/>
@@ -16475,7 +16452,7 @@
       <c r="F130" s="13"/>
       <c r="G130" s="13"/>
       <c r="H130" s="13"/>
-      <c r="I130" s="49"/>
+      <c r="I130" s="36"/>
     </row>
     <row r="131" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="27"/>
@@ -16486,7 +16463,7 @@
       <c r="F131" s="13"/>
       <c r="G131" s="13"/>
       <c r="H131" s="13"/>
-      <c r="I131" s="49"/>
+      <c r="I131" s="36"/>
     </row>
     <row r="132" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="27"/>
@@ -16497,7 +16474,7 @@
       <c r="F132" s="13"/>
       <c r="G132" s="13"/>
       <c r="H132" s="13"/>
-      <c r="I132" s="49"/>
+      <c r="I132" s="36"/>
     </row>
     <row r="133" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="27"/>
@@ -16508,7 +16485,7 @@
       <c r="F133" s="13"/>
       <c r="G133" s="13"/>
       <c r="H133" s="13"/>
-      <c r="I133" s="49"/>
+      <c r="I133" s="36"/>
     </row>
     <row r="134" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="27"/>
@@ -16519,7 +16496,7 @@
       <c r="F134" s="13"/>
       <c r="G134" s="13"/>
       <c r="H134" s="13"/>
-      <c r="I134" s="49"/>
+      <c r="I134" s="36"/>
     </row>
     <row r="135" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="27"/>
@@ -16530,7 +16507,7 @@
       <c r="F135" s="13"/>
       <c r="G135" s="13"/>
       <c r="H135" s="13"/>
-      <c r="I135" s="49"/>
+      <c r="I135" s="36"/>
     </row>
     <row r="136" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="27"/>
@@ -16541,7 +16518,7 @@
       <c r="F136" s="13"/>
       <c r="G136" s="13"/>
       <c r="H136" s="13"/>
-      <c r="I136" s="49"/>
+      <c r="I136" s="36"/>
     </row>
     <row r="137" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="27"/>
@@ -16552,7 +16529,7 @@
       <c r="F137" s="13"/>
       <c r="G137" s="13"/>
       <c r="H137" s="13"/>
-      <c r="I137" s="49"/>
+      <c r="I137" s="36"/>
     </row>
     <row r="138" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="27"/>
@@ -16563,7 +16540,7 @@
       <c r="F138" s="13"/>
       <c r="G138" s="13"/>
       <c r="H138" s="13"/>
-      <c r="I138" s="49"/>
+      <c r="I138" s="36"/>
     </row>
     <row r="139" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="27"/>
@@ -16574,7 +16551,7 @@
       <c r="F139" s="13"/>
       <c r="G139" s="13"/>
       <c r="H139" s="13"/>
-      <c r="I139" s="49"/>
+      <c r="I139" s="36"/>
     </row>
     <row r="140" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="27"/>
@@ -16585,7 +16562,7 @@
       <c r="F140" s="13"/>
       <c r="G140" s="13"/>
       <c r="H140" s="13"/>
-      <c r="I140" s="49"/>
+      <c r="I140" s="36"/>
     </row>
     <row r="141" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="27"/>
@@ -16596,7 +16573,7 @@
       <c r="F141" s="13"/>
       <c r="G141" s="13"/>
       <c r="H141" s="13"/>
-      <c r="I141" s="49"/>
+      <c r="I141" s="36"/>
     </row>
     <row r="142" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="27"/>
@@ -16607,7 +16584,7 @@
       <c r="F142" s="13"/>
       <c r="G142" s="13"/>
       <c r="H142" s="13"/>
-      <c r="I142" s="49"/>
+      <c r="I142" s="36"/>
     </row>
     <row r="143" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="27"/>
@@ -16618,7 +16595,7 @@
       <c r="F143" s="13"/>
       <c r="G143" s="13"/>
       <c r="H143" s="13"/>
-      <c r="I143" s="49"/>
+      <c r="I143" s="36"/>
     </row>
     <row r="144" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="27"/>
@@ -16629,7 +16606,7 @@
       <c r="F144" s="13"/>
       <c r="G144" s="13"/>
       <c r="H144" s="13"/>
-      <c r="I144" s="49"/>
+      <c r="I144" s="36"/>
     </row>
     <row r="145" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="27"/>
@@ -16640,7 +16617,7 @@
       <c r="F145" s="13"/>
       <c r="G145" s="13"/>
       <c r="H145" s="13"/>
-      <c r="I145" s="49"/>
+      <c r="I145" s="36"/>
     </row>
     <row r="146" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="27"/>
@@ -16651,7 +16628,7 @@
       <c r="F146" s="13"/>
       <c r="G146" s="13"/>
       <c r="H146" s="13"/>
-      <c r="I146" s="49"/>
+      <c r="I146" s="36"/>
     </row>
     <row r="147" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="27"/>
@@ -16662,7 +16639,7 @@
       <c r="F147" s="13"/>
       <c r="G147" s="13"/>
       <c r="H147" s="13"/>
-      <c r="I147" s="49"/>
+      <c r="I147" s="36"/>
     </row>
     <row r="148" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="27"/>
@@ -16673,7 +16650,7 @@
       <c r="F148" s="13"/>
       <c r="G148" s="13"/>
       <c r="H148" s="13"/>
-      <c r="I148" s="49"/>
+      <c r="I148" s="36"/>
     </row>
     <row r="149" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="27"/>
@@ -16684,7 +16661,7 @@
       <c r="F149" s="13"/>
       <c r="G149" s="13"/>
       <c r="H149" s="13"/>
-      <c r="I149" s="49"/>
+      <c r="I149" s="36"/>
     </row>
     <row r="150" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="27"/>
@@ -16695,7 +16672,7 @@
       <c r="F150" s="13"/>
       <c r="G150" s="13"/>
       <c r="H150" s="13"/>
-      <c r="I150" s="49"/>
+      <c r="I150" s="36"/>
     </row>
     <row r="151" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="27"/>
@@ -16706,7 +16683,7 @@
       <c r="F151" s="13"/>
       <c r="G151" s="13"/>
       <c r="H151" s="13"/>
-      <c r="I151" s="49"/>
+      <c r="I151" s="36"/>
     </row>
     <row r="152" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="27"/>
@@ -16717,7 +16694,7 @@
       <c r="F152" s="13"/>
       <c r="G152" s="13"/>
       <c r="H152" s="13"/>
-      <c r="I152" s="49"/>
+      <c r="I152" s="36"/>
     </row>
     <row r="153" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="27"/>
@@ -16728,7 +16705,7 @@
       <c r="F153" s="13"/>
       <c r="G153" s="13"/>
       <c r="H153" s="13"/>
-      <c r="I153" s="49"/>
+      <c r="I153" s="36"/>
     </row>
     <row r="154" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="27"/>
@@ -16739,7 +16716,7 @@
       <c r="F154" s="13"/>
       <c r="G154" s="13"/>
       <c r="H154" s="13"/>
-      <c r="I154" s="49"/>
+      <c r="I154" s="36"/>
     </row>
     <row r="155" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="27"/>
@@ -16750,7 +16727,7 @@
       <c r="F155" s="13"/>
       <c r="G155" s="13"/>
       <c r="H155" s="13"/>
-      <c r="I155" s="49"/>
+      <c r="I155" s="36"/>
     </row>
     <row r="156" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="27"/>
@@ -16761,7 +16738,7 @@
       <c r="F156" s="13"/>
       <c r="G156" s="13"/>
       <c r="H156" s="13"/>
-      <c r="I156" s="49"/>
+      <c r="I156" s="36"/>
     </row>
     <row r="157" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="27"/>
@@ -16772,7 +16749,7 @@
       <c r="F157" s="13"/>
       <c r="G157" s="13"/>
       <c r="H157" s="13"/>
-      <c r="I157" s="49"/>
+      <c r="I157" s="36"/>
     </row>
     <row r="158" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="27"/>
@@ -16783,7 +16760,7 @@
       <c r="F158" s="13"/>
       <c r="G158" s="13"/>
       <c r="H158" s="13"/>
-      <c r="I158" s="49"/>
+      <c r="I158" s="36"/>
     </row>
     <row r="159" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="27"/>
@@ -16794,7 +16771,7 @@
       <c r="F159" s="13"/>
       <c r="G159" s="13"/>
       <c r="H159" s="13"/>
-      <c r="I159" s="49"/>
+      <c r="I159" s="36"/>
     </row>
     <row r="160" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="27"/>
@@ -16805,7 +16782,7 @@
       <c r="F160" s="13"/>
       <c r="G160" s="13"/>
       <c r="H160" s="13"/>
-      <c r="I160" s="49"/>
+      <c r="I160" s="36"/>
     </row>
     <row r="161" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="27"/>
@@ -16816,7 +16793,7 @@
       <c r="F161" s="13"/>
       <c r="G161" s="13"/>
       <c r="H161" s="13"/>
-      <c r="I161" s="49"/>
+      <c r="I161" s="36"/>
     </row>
     <row r="162" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="27"/>
@@ -16827,7 +16804,7 @@
       <c r="F162" s="13"/>
       <c r="G162" s="13"/>
       <c r="H162" s="13"/>
-      <c r="I162" s="49"/>
+      <c r="I162" s="36"/>
     </row>
     <row r="163" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="27"/>
@@ -16838,7 +16815,7 @@
       <c r="F163" s="13"/>
       <c r="G163" s="13"/>
       <c r="H163" s="13"/>
-      <c r="I163" s="49"/>
+      <c r="I163" s="36"/>
     </row>
     <row r="164" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="27"/>
@@ -16849,7 +16826,7 @@
       <c r="F164" s="13"/>
       <c r="G164" s="13"/>
       <c r="H164" s="13"/>
-      <c r="I164" s="49"/>
+      <c r="I164" s="36"/>
     </row>
     <row r="165" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="27"/>
@@ -16860,7 +16837,7 @@
       <c r="F165" s="13"/>
       <c r="G165" s="13"/>
       <c r="H165" s="13"/>
-      <c r="I165" s="49"/>
+      <c r="I165" s="36"/>
     </row>
     <row r="166" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="27"/>
@@ -16871,7 +16848,7 @@
       <c r="F166" s="13"/>
       <c r="G166" s="13"/>
       <c r="H166" s="13"/>
-      <c r="I166" s="49"/>
+      <c r="I166" s="36"/>
     </row>
     <row r="167" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="27"/>
@@ -16882,7 +16859,7 @@
       <c r="F167" s="13"/>
       <c r="G167" s="13"/>
       <c r="H167" s="13"/>
-      <c r="I167" s="49"/>
+      <c r="I167" s="36"/>
     </row>
     <row r="168" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="27"/>
@@ -16893,7 +16870,7 @@
       <c r="F168" s="13"/>
       <c r="G168" s="13"/>
       <c r="H168" s="13"/>
-      <c r="I168" s="49"/>
+      <c r="I168" s="36"/>
     </row>
     <row r="169" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="27"/>
@@ -16904,7 +16881,7 @@
       <c r="F169" s="13"/>
       <c r="G169" s="13"/>
       <c r="H169" s="13"/>
-      <c r="I169" s="49"/>
+      <c r="I169" s="36"/>
     </row>
     <row r="170" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="27"/>
@@ -16915,7 +16892,7 @@
       <c r="F170" s="13"/>
       <c r="G170" s="13"/>
       <c r="H170" s="13"/>
-      <c r="I170" s="49"/>
+      <c r="I170" s="36"/>
     </row>
     <row r="171" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="27"/>
@@ -16926,7 +16903,7 @@
       <c r="F171" s="13"/>
       <c r="G171" s="13"/>
       <c r="H171" s="13"/>
-      <c r="I171" s="49"/>
+      <c r="I171" s="36"/>
     </row>
     <row r="172" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="27"/>
@@ -16937,7 +16914,7 @@
       <c r="F172" s="13"/>
       <c r="G172" s="13"/>
       <c r="H172" s="13"/>
-      <c r="I172" s="49"/>
+      <c r="I172" s="36"/>
     </row>
     <row r="173" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="27"/>
@@ -16948,7 +16925,7 @@
       <c r="F173" s="13"/>
       <c r="G173" s="13"/>
       <c r="H173" s="13"/>
-      <c r="I173" s="49"/>
+      <c r="I173" s="36"/>
     </row>
     <row r="174" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="27"/>
@@ -16959,7 +16936,7 @@
       <c r="F174" s="13"/>
       <c r="G174" s="13"/>
       <c r="H174" s="13"/>
-      <c r="I174" s="49"/>
+      <c r="I174" s="36"/>
     </row>
     <row r="175" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="27"/>
@@ -16970,7 +16947,7 @@
       <c r="F175" s="13"/>
       <c r="G175" s="13"/>
       <c r="H175" s="13"/>
-      <c r="I175" s="49"/>
+      <c r="I175" s="36"/>
     </row>
     <row r="176" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="27"/>
@@ -16981,7 +16958,7 @@
       <c r="F176" s="13"/>
       <c r="G176" s="13"/>
       <c r="H176" s="13"/>
-      <c r="I176" s="49"/>
+      <c r="I176" s="36"/>
     </row>
     <row r="177" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="27"/>
@@ -16992,7 +16969,7 @@
       <c r="F177" s="13"/>
       <c r="G177" s="13"/>
       <c r="H177" s="13"/>
-      <c r="I177" s="49"/>
+      <c r="I177" s="36"/>
     </row>
     <row r="178" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="27"/>
@@ -17003,7 +16980,7 @@
       <c r="F178" s="13"/>
       <c r="G178" s="13"/>
       <c r="H178" s="13"/>
-      <c r="I178" s="49"/>
+      <c r="I178" s="36"/>
     </row>
     <row r="179" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="27"/>
@@ -17014,7 +16991,7 @@
       <c r="F179" s="13"/>
       <c r="G179" s="13"/>
       <c r="H179" s="13"/>
-      <c r="I179" s="49"/>
+      <c r="I179" s="36"/>
     </row>
     <row r="180" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="27"/>
@@ -17025,7 +17002,7 @@
       <c r="F180" s="13"/>
       <c r="G180" s="13"/>
       <c r="H180" s="13"/>
-      <c r="I180" s="49"/>
+      <c r="I180" s="36"/>
     </row>
     <row r="181" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="27"/>
@@ -17036,7 +17013,7 @@
       <c r="F181" s="13"/>
       <c r="G181" s="13"/>
       <c r="H181" s="13"/>
-      <c r="I181" s="49"/>
+      <c r="I181" s="36"/>
     </row>
     <row r="182" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="27"/>
@@ -17047,7 +17024,7 @@
       <c r="F182" s="13"/>
       <c r="G182" s="13"/>
       <c r="H182" s="13"/>
-      <c r="I182" s="49"/>
+      <c r="I182" s="36"/>
     </row>
     <row r="183" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="27"/>
@@ -17058,7 +17035,7 @@
       <c r="F183" s="13"/>
       <c r="G183" s="13"/>
       <c r="H183" s="13"/>
-      <c r="I183" s="49"/>
+      <c r="I183" s="36"/>
     </row>
     <row r="184" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="27"/>
@@ -17069,7 +17046,7 @@
       <c r="F184" s="13"/>
       <c r="G184" s="13"/>
       <c r="H184" s="13"/>
-      <c r="I184" s="49"/>
+      <c r="I184" s="36"/>
     </row>
     <row r="185" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="27"/>
@@ -17080,7 +17057,7 @@
       <c r="F185" s="13"/>
       <c r="G185" s="13"/>
       <c r="H185" s="13"/>
-      <c r="I185" s="49"/>
+      <c r="I185" s="36"/>
     </row>
     <row r="186" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="27"/>
@@ -17091,7 +17068,7 @@
       <c r="F186" s="13"/>
       <c r="G186" s="13"/>
       <c r="H186" s="13"/>
-      <c r="I186" s="49"/>
+      <c r="I186" s="36"/>
     </row>
     <row r="187" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="27"/>
@@ -17102,7 +17079,7 @@
       <c r="F187" s="13"/>
       <c r="G187" s="13"/>
       <c r="H187" s="13"/>
-      <c r="I187" s="49"/>
+      <c r="I187" s="36"/>
     </row>
     <row r="188" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="27"/>
@@ -17113,7 +17090,7 @@
       <c r="F188" s="13"/>
       <c r="G188" s="13"/>
       <c r="H188" s="13"/>
-      <c r="I188" s="49"/>
+      <c r="I188" s="36"/>
     </row>
     <row r="189" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="27"/>
@@ -17124,7 +17101,7 @@
       <c r="F189" s="13"/>
       <c r="G189" s="13"/>
       <c r="H189" s="13"/>
-      <c r="I189" s="49"/>
+      <c r="I189" s="36"/>
     </row>
     <row r="190" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="27"/>
@@ -17135,7 +17112,7 @@
       <c r="F190" s="13"/>
       <c r="G190" s="13"/>
       <c r="H190" s="13"/>
-      <c r="I190" s="49"/>
+      <c r="I190" s="36"/>
     </row>
     <row r="191" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="27"/>
@@ -17146,7 +17123,7 @@
       <c r="F191" s="13"/>
       <c r="G191" s="13"/>
       <c r="H191" s="13"/>
-      <c r="I191" s="49"/>
+      <c r="I191" s="36"/>
     </row>
     <row r="192" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="27"/>
@@ -17157,7 +17134,7 @@
       <c r="F192" s="13"/>
       <c r="G192" s="13"/>
       <c r="H192" s="13"/>
-      <c r="I192" s="49"/>
+      <c r="I192" s="36"/>
     </row>
     <row r="193" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="27"/>
@@ -17168,7 +17145,7 @@
       <c r="F193" s="13"/>
       <c r="G193" s="13"/>
       <c r="H193" s="13"/>
-      <c r="I193" s="49"/>
+      <c r="I193" s="36"/>
     </row>
     <row r="194" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="27"/>
@@ -17179,7 +17156,7 @@
       <c r="F194" s="13"/>
       <c r="G194" s="13"/>
       <c r="H194" s="13"/>
-      <c r="I194" s="49"/>
+      <c r="I194" s="36"/>
     </row>
     <row r="195" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="27"/>
@@ -17190,7 +17167,7 @@
       <c r="F195" s="13"/>
       <c r="G195" s="13"/>
       <c r="H195" s="13"/>
-      <c r="I195" s="49"/>
+      <c r="I195" s="36"/>
     </row>
     <row r="196" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="27"/>
@@ -17201,73 +17178,29 @@
       <c r="F196" s="13"/>
       <c r="G196" s="13"/>
       <c r="H196" s="13"/>
-      <c r="I196" s="49"/>
-    </row>
-    <row r="197" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A197" s="27"/>
-      <c r="B197" s="30"/>
-      <c r="C197" s="33"/>
-      <c r="D197" s="13"/>
-      <c r="E197" s="13"/>
-      <c r="F197" s="13"/>
-      <c r="G197" s="13"/>
-      <c r="H197" s="13"/>
-      <c r="I197" s="49"/>
-    </row>
-    <row r="198" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A198" s="27"/>
-      <c r="B198" s="30"/>
-      <c r="C198" s="33"/>
-      <c r="D198" s="13"/>
-      <c r="E198" s="13"/>
-      <c r="F198" s="13"/>
-      <c r="G198" s="13"/>
-      <c r="H198" s="13"/>
-      <c r="I198" s="49"/>
-    </row>
-    <row r="199" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A199" s="27"/>
-      <c r="B199" s="30"/>
-      <c r="C199" s="33"/>
-      <c r="D199" s="13"/>
-      <c r="E199" s="13"/>
-      <c r="F199" s="13"/>
-      <c r="G199" s="13"/>
-      <c r="H199" s="13"/>
-      <c r="I199" s="49"/>
-    </row>
-    <row r="200" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A200" s="27"/>
-      <c r="B200" s="30"/>
-      <c r="C200" s="33"/>
-      <c r="D200" s="13"/>
-      <c r="E200" s="13"/>
-      <c r="F200" s="13"/>
-      <c r="G200" s="13"/>
-      <c r="H200" s="13"/>
-      <c r="I200" s="49"/>
+      <c r="I196" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A98:I98"/>
-    <mergeCell ref="A100:I100"/>
-    <mergeCell ref="A78:I78"/>
-    <mergeCell ref="A103:I103"/>
+    <mergeCell ref="A107:I107"/>
+    <mergeCell ref="A109:I109"/>
+    <mergeCell ref="A111:I111"/>
     <mergeCell ref="A104:I104"/>
-    <mergeCell ref="A88:I88"/>
-    <mergeCell ref="A108:I108"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A17:I17"/>
-    <mergeCell ref="A28:I28"/>
-    <mergeCell ref="A37:I37"/>
-    <mergeCell ref="A77:I77"/>
-    <mergeCell ref="A52:I52"/>
-    <mergeCell ref="A59:I59"/>
-    <mergeCell ref="A64:I64"/>
-    <mergeCell ref="A111:I111"/>
-    <mergeCell ref="A113:I113"/>
-    <mergeCell ref="A115:I115"/>
+    <mergeCell ref="A29:I29"/>
+    <mergeCell ref="A38:I38"/>
+    <mergeCell ref="A80:I80"/>
+    <mergeCell ref="A54:I54"/>
+    <mergeCell ref="A61:I61"/>
+    <mergeCell ref="A66:I66"/>
+    <mergeCell ref="A94:I94"/>
+    <mergeCell ref="A96:I96"/>
+    <mergeCell ref="A81:I81"/>
+    <mergeCell ref="A99:I99"/>
+    <mergeCell ref="A100:I100"/>
+    <mergeCell ref="A87:I87"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Moved "no sms/name/pass"  + Only phone
- Moved "no sms/name/pass" to corresponding fields
- Only  sign up with phone
</commit_message>
<xml_diff>
--- a/Middle Assignment/TestDesignTechique1_PhamHongAnh.xlsx
+++ b/Middle Assignment/TestDesignTechique1_PhamHongAnh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NashTech\Rookies\NashTech_Homework\Middle Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124897DF-C24E-4976-AAE7-ADDD4AE16624}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F211A0-F8CC-4C66-9A19-982B7E54F47B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -851,7 +851,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="215">
   <si>
     <t>ID</t>
   </si>
@@ -1453,9 +1453,6 @@
     <t>'Facebook' button</t>
   </si>
   <si>
-    <t>When signing up after entering all mandatory (*) information valid</t>
-  </si>
-  <si>
     <t>When signing up with a Facebook account</t>
   </si>
   <si>
@@ -1477,9 +1474,6 @@
     <t>Check đầu số +84 hoặc 0</t>
   </si>
   <si>
-    <t>When signing up with all required fields empty</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sign up with Email </t>
   </si>
   <si>
@@ -1489,20 +1483,47 @@
     <t>Check all drop down values</t>
   </si>
   <si>
-    <t xml:space="preserve">Thêm decision table </t>
-  </si>
-  <si>
     <t>Check boundary value của phone number (Done)</t>
   </si>
   <si>
     <t>3.  Test flow</t>
+  </si>
+  <si>
+    <t>(NOTE: Các cases check button cho vào test flow)</t>
+  </si>
+  <si>
+    <t>When signing up fail after entering all mandatory (*) information valid</t>
+  </si>
+  <si>
+    <t>ĐỂ SAU</t>
+  </si>
+  <si>
+    <t>When entering only special characters</t>
+  </si>
+  <si>
+    <t>When entering alphabetic and numerical values only</t>
+  </si>
+  <si>
+    <t>When entering alphabetic and special values only</t>
+  </si>
+  <si>
+    <t>When entering numerical and special values only</t>
+  </si>
+  <si>
+    <t>When clicking on the "Sign up with email" button</t>
+  </si>
+  <si>
+    <t>Thêm decision table (Done)</t>
+  </si>
+  <si>
+    <t>Chuyển vào từng field tương ứng (Done)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1580,8 +1601,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1627,6 +1656,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1717,7 +1752,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1806,15 +1841,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1846,14 +1872,26 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2135,17 +2173,17 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -2165,17 +2203,17 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -2564,17 +2602,17 @@
       <c r="Z13" s="2"/>
     </row>
     <row r="14" spans="1:26" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="44"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -2962,17 +3000,17 @@
       <c r="Z24" s="2"/>
     </row>
     <row r="25" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="45" t="s">
+      <c r="A25" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="46"/>
-      <c r="C25" s="46"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="46"/>
-      <c r="G25" s="46"/>
-      <c r="H25" s="46"/>
-      <c r="I25" s="47"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="43"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="44"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
@@ -3064,17 +3102,17 @@
       <c r="Z27" s="2"/>
     </row>
     <row r="28" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="46"/>
-      <c r="C28" s="46"/>
-      <c r="D28" s="46"/>
-      <c r="E28" s="46"/>
-      <c r="F28" s="46"/>
-      <c r="G28" s="46"/>
-      <c r="H28" s="46"/>
-      <c r="I28" s="47"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="44"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
@@ -3167,17 +3205,17 @@
       <c r="Z30" s="2"/>
     </row>
     <row r="31" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="41" t="s">
+      <c r="A31" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="42"/>
-      <c r="C31" s="42"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="42"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="39"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -3197,17 +3235,17 @@
       <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="38" t="s">
+      <c r="A32" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="39"/>
-      <c r="C32" s="39"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="39"/>
-      <c r="I32" s="40"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="37"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
@@ -3401,17 +3439,17 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="38" t="s">
+      <c r="A42" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B42" s="39"/>
-      <c r="C42" s="39"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="39"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="39"/>
-      <c r="H42" s="39"/>
-      <c r="I42" s="40"/>
+      <c r="B42" s="36"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="36"/>
+      <c r="G42" s="36"/>
+      <c r="H42" s="36"/>
+      <c r="I42" s="37"/>
     </row>
     <row r="43" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
@@ -14378,23 +14416,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{861DB058-9ABC-4928-81FB-0309C7B8DB85}">
-  <dimension ref="A1:Z196"/>
+  <dimension ref="A1:Z198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94:I94"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="28" customWidth="1"/>
     <col min="2" max="2" width="33" style="31" customWidth="1"/>
-    <col min="3" max="3" width="29" style="35" customWidth="1"/>
+    <col min="3" max="3" width="29" style="31" customWidth="1"/>
     <col min="4" max="4" width="27.6328125" style="28" customWidth="1"/>
     <col min="5" max="5" width="12.1796875" style="28" customWidth="1"/>
     <col min="6" max="6" width="17" style="28" customWidth="1"/>
     <col min="7" max="7" width="14.54296875" style="28" customWidth="1"/>
     <col min="8" max="8" width="17.08984375" style="28" customWidth="1"/>
-    <col min="9" max="9" width="15.1796875" style="37" customWidth="1"/>
+    <col min="9" max="9" width="15.1796875" style="34" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="10" customFormat="1" ht="26" x14ac:dyDescent="0.35">
@@ -14444,17 +14482,17 @@
       <c r="Z1" s="26"/>
     </row>
     <row r="2" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="38" t="s">
         <v>166</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
       <c r="J2" s="26"/>
       <c r="K2" s="26"/>
       <c r="L2" s="26"/>
@@ -14474,17 +14512,17 @@
       <c r="Z2" s="26"/>
     </row>
     <row r="3" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="43" t="s">
-        <v>199</v>
-      </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
+      <c r="A3" s="40" t="s">
+        <v>198</v>
+      </c>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
       <c r="J3" s="26"/>
       <c r="K3" s="26"/>
       <c r="L3" s="26"/>
@@ -14510,15 +14548,15 @@
       <c r="B4" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="C4" s="36" t="s">
-        <v>206</v>
+      <c r="C4" s="33" t="s">
+        <v>203</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
-      <c r="I4" s="36"/>
+      <c r="I4" s="33"/>
     </row>
     <row r="5" spans="1:26" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="27">
@@ -14528,13 +14566,13 @@
       <c r="B5" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="C5" s="33"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
-      <c r="I5" s="36"/>
+      <c r="I5" s="33"/>
     </row>
     <row r="6" spans="1:26" s="10" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27">
@@ -14544,13 +14582,13 @@
       <c r="B6" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="C6" s="33"/>
+      <c r="C6" s="30"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
-      <c r="I6" s="36"/>
+      <c r="I6" s="33"/>
     </row>
     <row r="7" spans="1:26" s="10" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="27">
@@ -14558,15 +14596,15 @@
         <v>4</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>203</v>
-      </c>
-      <c r="C7" s="33"/>
+        <v>201</v>
+      </c>
+      <c r="C7" s="30"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
-      <c r="I7" s="36"/>
+      <c r="I7" s="33"/>
     </row>
     <row r="8" spans="1:26" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="27">
@@ -14576,29 +14614,29 @@
       <c r="B8" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="C8" s="33"/>
+      <c r="C8" s="30"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
-      <c r="I8" s="36"/>
+      <c r="I8" s="33"/>
     </row>
     <row r="9" spans="1:26" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27">
-        <f t="shared" ref="A9:A79" ca="1" si="0">IF(OFFSET(A9,-1,0) ="",OFFSET(A9,-2,0)+1,OFFSET(A9,-1,0)+1 )</f>
+        <f t="shared" ref="A9:A81" ca="1" si="0">IF(OFFSET(A9,-1,0) ="",OFFSET(A9,-2,0)+1,OFFSET(A9,-1,0)+1 )</f>
         <v>6</v>
       </c>
       <c r="B9" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="C9" s="33"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
-      <c r="I9" s="36"/>
+      <c r="I9" s="33"/>
     </row>
     <row r="10" spans="1:26" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27">
@@ -14608,13 +14646,13 @@
       <c r="B10" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="C10" s="33"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
-      <c r="I10" s="36"/>
+      <c r="I10" s="33"/>
     </row>
     <row r="11" spans="1:26" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="27">
@@ -14624,13 +14662,13 @@
       <c r="B11" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="C11" s="33"/>
+      <c r="C11" s="30"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
-      <c r="I11" s="36"/>
+      <c r="I11" s="33"/>
     </row>
     <row r="12" spans="1:26" s="10" customFormat="1" ht="20.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="27">
@@ -14640,13 +14678,13 @@
       <c r="B12" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="C12" s="33"/>
+      <c r="C12" s="30"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
-      <c r="I12" s="36"/>
+      <c r="I12" s="33"/>
     </row>
     <row r="13" spans="1:26" s="10" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="27">
@@ -14656,13 +14694,13 @@
       <c r="B13" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="C13" s="33"/>
+      <c r="C13" s="30"/>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
-      <c r="I13" s="36"/>
+      <c r="I13" s="33"/>
     </row>
     <row r="14" spans="1:26" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="27">
@@ -14672,13 +14710,13 @@
       <c r="B14" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="C14" s="33"/>
+      <c r="C14" s="30"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
-      <c r="I14" s="36"/>
+      <c r="I14" s="33"/>
     </row>
     <row r="15" spans="1:26" s="10" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="27">
@@ -14688,15 +14726,15 @@
       <c r="B15" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="C15" s="33" t="s">
-        <v>200</v>
+      <c r="C15" s="30" t="s">
+        <v>199</v>
       </c>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
-      <c r="I15" s="36"/>
+      <c r="I15" s="33"/>
     </row>
     <row r="16" spans="1:26" s="10" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="27">
@@ -14706,26 +14744,26 @@
       <c r="B16" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="C16" s="33"/>
+      <c r="C16" s="30"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
-      <c r="I16" s="36"/>
+      <c r="I16" s="33"/>
     </row>
     <row r="17" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="B17" s="49"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
       <c r="J17" s="26"/>
       <c r="K17" s="26"/>
       <c r="L17" s="26"/>
@@ -14752,13 +14790,13 @@
       <c r="B18" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="C18" s="33"/>
+      <c r="C18" s="30"/>
       <c r="D18" s="13"/>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
       <c r="H18" s="13"/>
-      <c r="I18" s="36"/>
+      <c r="I18" s="33"/>
     </row>
     <row r="19" spans="1:26" s="10" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="27">
@@ -14768,13 +14806,13 @@
       <c r="B19" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="C19" s="33"/>
+      <c r="C19" s="30"/>
       <c r="D19" s="13"/>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
-      <c r="I19" s="36"/>
+      <c r="I19" s="33"/>
     </row>
     <row r="20" spans="1:26" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="27">
@@ -14784,13 +14822,13 @@
       <c r="B20" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="C20" s="33"/>
+      <c r="C20" s="30"/>
       <c r="D20" s="13"/>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
-      <c r="I20" s="36"/>
+      <c r="I20" s="33"/>
     </row>
     <row r="21" spans="1:26" s="10" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="27">
@@ -14800,13 +14838,13 @@
       <c r="B21" s="29" t="s">
         <v>140</v>
       </c>
-      <c r="C21" s="33"/>
+      <c r="C21" s="30"/>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
-      <c r="I21" s="36"/>
+      <c r="I21" s="33"/>
     </row>
     <row r="22" spans="1:26" s="10" customFormat="1" ht="24.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="27">
@@ -14816,13 +14854,13 @@
       <c r="B22" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="C22" s="33"/>
+      <c r="C22" s="30"/>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
       <c r="G22" s="13"/>
       <c r="H22" s="13"/>
-      <c r="I22" s="36"/>
+      <c r="I22" s="33"/>
     </row>
     <row r="23" spans="1:26" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="27">
@@ -14832,13 +14870,13 @@
       <c r="B23" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="C23" s="33"/>
+      <c r="C23" s="30"/>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
-      <c r="I23" s="36"/>
+      <c r="I23" s="33"/>
     </row>
     <row r="24" spans="1:26" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="27">
@@ -14848,13 +14886,13 @@
       <c r="B24" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="C24" s="33"/>
+      <c r="C24" s="30"/>
       <c r="D24" s="13"/>
       <c r="E24" s="13"/>
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
-      <c r="I24" s="36"/>
+      <c r="I24" s="33"/>
     </row>
     <row r="25" spans="1:26" s="10" customFormat="1" ht="20.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="27">
@@ -14864,13 +14902,13 @@
       <c r="B25" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="C25" s="33"/>
+      <c r="C25" s="30"/>
       <c r="D25" s="13"/>
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
       <c r="H25" s="13"/>
-      <c r="I25" s="36"/>
+      <c r="I25" s="33"/>
     </row>
     <row r="26" spans="1:26" s="10" customFormat="1" ht="20.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="27">
@@ -14880,13 +14918,13 @@
       <c r="B26" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="C26" s="34"/>
+      <c r="C26" s="51"/>
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
-      <c r="I26" s="36"/>
+      <c r="I26" s="33"/>
     </row>
     <row r="27" spans="1:26" s="10" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="27">
@@ -14896,13 +14934,15 @@
       <c r="B27" s="30" t="s">
         <v>183</v>
       </c>
-      <c r="C27" s="33"/>
+      <c r="C27" s="29" t="s">
+        <v>214</v>
+      </c>
       <c r="D27" s="30"/>
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
       <c r="H27" s="13"/>
-      <c r="I27" s="36"/>
+      <c r="I27" s="33"/>
     </row>
     <row r="28" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="27">
@@ -14912,25 +14952,25 @@
       <c r="B28" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="C28" s="34"/>
+      <c r="C28" s="51"/>
       <c r="E28" s="13"/>
       <c r="F28" s="13"/>
       <c r="G28" s="13"/>
       <c r="H28" s="13"/>
-      <c r="I28" s="36"/>
+      <c r="I28" s="33"/>
     </row>
     <row r="29" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="48" t="s">
+      <c r="A29" s="46" t="s">
         <v>173</v>
       </c>
-      <c r="B29" s="49"/>
-      <c r="C29" s="49"/>
-      <c r="D29" s="49"/>
-      <c r="E29" s="49"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="49"/>
-      <c r="H29" s="49"/>
-      <c r="I29" s="49"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="47"/>
       <c r="J29" s="26"/>
       <c r="K29" s="26"/>
       <c r="L29" s="26"/>
@@ -14957,12 +14997,12 @@
       <c r="B30" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="C30" s="34"/>
+      <c r="C30" s="51"/>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
       <c r="G30" s="13"/>
       <c r="H30" s="13"/>
-      <c r="I30" s="36"/>
+      <c r="I30" s="33"/>
     </row>
     <row r="31" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="27">
@@ -14972,12 +15012,12 @@
       <c r="B31" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="C31" s="34"/>
+      <c r="C31" s="51"/>
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
       <c r="G31" s="13"/>
       <c r="H31" s="13"/>
-      <c r="I31" s="36"/>
+      <c r="I31" s="33"/>
     </row>
     <row r="32" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="27">
@@ -14987,12 +15027,12 @@
       <c r="B32" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="C32" s="34"/>
+      <c r="C32" s="51"/>
       <c r="E32" s="13"/>
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
-      <c r="I32" s="36"/>
+      <c r="I32" s="33"/>
     </row>
     <row r="33" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="27">
@@ -15002,12 +15042,12 @@
       <c r="B33" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="C33" s="34"/>
+      <c r="C33" s="51"/>
       <c r="E33" s="13"/>
       <c r="F33" s="13"/>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
-      <c r="I33" s="36"/>
+      <c r="I33" s="33"/>
     </row>
     <row r="34" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="27">
@@ -15017,12 +15057,12 @@
       <c r="B34" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C34" s="34"/>
+      <c r="C34" s="51"/>
       <c r="E34" s="13"/>
       <c r="F34" s="13"/>
       <c r="G34" s="13"/>
       <c r="H34" s="13"/>
-      <c r="I34" s="36"/>
+      <c r="I34" s="33"/>
     </row>
     <row r="35" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="27">
@@ -15032,12 +15072,12 @@
       <c r="B35" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="C35" s="34"/>
+      <c r="C35" s="51"/>
       <c r="E35" s="13"/>
       <c r="F35" s="13"/>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
-      <c r="I35" s="36"/>
+      <c r="I35" s="33"/>
     </row>
     <row r="36" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="27">
@@ -15047,12 +15087,12 @@
       <c r="B36" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="C36" s="34"/>
+      <c r="C36" s="51"/>
       <c r="E36" s="13"/>
       <c r="F36" s="13"/>
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
-      <c r="I36" s="36"/>
+      <c r="I36" s="33"/>
     </row>
     <row r="37" spans="1:26" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="27">
@@ -15062,25 +15102,25 @@
       <c r="B37" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="C37" s="34"/>
+      <c r="C37" s="51"/>
       <c r="E37" s="13"/>
       <c r="F37" s="13"/>
       <c r="G37" s="13"/>
       <c r="H37" s="13"/>
-      <c r="I37" s="36"/>
+      <c r="I37" s="33"/>
     </row>
     <row r="38" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="48" t="s">
+      <c r="A38" s="46" t="s">
         <v>130</v>
       </c>
-      <c r="B38" s="49"/>
-      <c r="C38" s="49"/>
-      <c r="D38" s="49"/>
-      <c r="E38" s="49"/>
-      <c r="F38" s="49"/>
-      <c r="G38" s="49"/>
-      <c r="H38" s="49"/>
-      <c r="I38" s="49"/>
+      <c r="B38" s="47"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="47"/>
+      <c r="F38" s="47"/>
+      <c r="G38" s="47"/>
+      <c r="H38" s="47"/>
+      <c r="I38" s="47"/>
       <c r="J38" s="26"/>
       <c r="K38" s="26"/>
       <c r="L38" s="26"/>
@@ -15107,15 +15147,15 @@
       <c r="B39" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="C39" s="33" t="s">
-        <v>205</v>
+      <c r="C39" s="29" t="s">
+        <v>213</v>
       </c>
       <c r="D39" s="13"/>
       <c r="E39" s="13"/>
       <c r="F39" s="13"/>
       <c r="G39" s="13"/>
       <c r="H39" s="13"/>
-      <c r="I39" s="36"/>
+      <c r="I39" s="33"/>
     </row>
     <row r="40" spans="1:26" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="27">
@@ -15125,13 +15165,13 @@
       <c r="B40" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="C40" s="33"/>
+      <c r="C40" s="30"/>
       <c r="D40" s="13"/>
       <c r="E40" s="13"/>
       <c r="F40" s="13"/>
       <c r="G40" s="13"/>
       <c r="H40" s="13"/>
-      <c r="I40" s="36"/>
+      <c r="I40" s="33"/>
     </row>
     <row r="41" spans="1:26" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="27">
@@ -15141,13 +15181,13 @@
       <c r="B41" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="C41" s="33"/>
+      <c r="C41" s="30"/>
       <c r="D41" s="13"/>
       <c r="E41" s="13"/>
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
       <c r="H41" s="13"/>
-      <c r="I41" s="36"/>
+      <c r="I41" s="33"/>
     </row>
     <row r="42" spans="1:26" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="27">
@@ -15157,13 +15197,13 @@
       <c r="B42" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="C42" s="33"/>
+      <c r="C42" s="30"/>
       <c r="D42" s="13"/>
       <c r="E42" s="13"/>
       <c r="F42" s="13"/>
       <c r="G42" s="13"/>
       <c r="H42" s="13"/>
-      <c r="I42" s="36"/>
+      <c r="I42" s="33"/>
     </row>
     <row r="43" spans="1:26" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="27">
@@ -15173,13 +15213,13 @@
       <c r="B43" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="C43" s="33"/>
+      <c r="C43" s="30"/>
       <c r="D43" s="13"/>
       <c r="E43" s="13"/>
       <c r="F43" s="13"/>
       <c r="G43" s="13"/>
       <c r="H43" s="13"/>
-      <c r="I43" s="36"/>
+      <c r="I43" s="33"/>
     </row>
     <row r="44" spans="1:26" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="27">
@@ -15189,13 +15229,13 @@
       <c r="B44" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="C44" s="33"/>
+      <c r="C44" s="30"/>
       <c r="D44" s="13"/>
       <c r="E44" s="13"/>
       <c r="F44" s="13"/>
       <c r="G44" s="13"/>
       <c r="H44" s="13"/>
-      <c r="I44" s="36"/>
+      <c r="I44" s="33"/>
     </row>
     <row r="45" spans="1:26" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="27">
@@ -15203,47 +15243,47 @@
         <v>39</v>
       </c>
       <c r="B45" s="29" t="s">
-        <v>129</v>
-      </c>
-      <c r="C45" s="33"/>
+        <v>126</v>
+      </c>
+      <c r="C45" s="30"/>
       <c r="D45" s="13"/>
       <c r="E45" s="13"/>
       <c r="F45" s="13"/>
       <c r="G45" s="13"/>
       <c r="H45" s="13"/>
-      <c r="I45" s="36"/>
-    </row>
-    <row r="46" spans="1:26" s="10" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I45" s="33"/>
+    </row>
+    <row r="46" spans="1:26" s="10" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>40</v>
       </c>
       <c r="B46" s="29" t="s">
-        <v>142</v>
-      </c>
-      <c r="C46" s="33"/>
+        <v>175</v>
+      </c>
+      <c r="C46" s="30"/>
       <c r="D46" s="13"/>
       <c r="E46" s="13"/>
       <c r="F46" s="13"/>
       <c r="G46" s="13"/>
       <c r="H46" s="13"/>
-      <c r="I46" s="36"/>
-    </row>
-    <row r="47" spans="1:26" s="10" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I46" s="33"/>
+    </row>
+    <row r="47" spans="1:26" s="10" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>41</v>
       </c>
       <c r="B47" s="29" t="s">
-        <v>143</v>
-      </c>
-      <c r="C47" s="33"/>
+        <v>176</v>
+      </c>
+      <c r="C47" s="30"/>
       <c r="D47" s="13"/>
       <c r="E47" s="13"/>
       <c r="F47" s="13"/>
       <c r="G47" s="13"/>
       <c r="H47" s="13"/>
-      <c r="I47" s="36"/>
+      <c r="I47" s="33"/>
     </row>
     <row r="48" spans="1:26" s="10" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="27">
@@ -15251,139 +15291,141 @@
         <v>42</v>
       </c>
       <c r="B48" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="C48" s="33"/>
+        <v>208</v>
+      </c>
+      <c r="C48" s="30"/>
       <c r="D48" s="13"/>
       <c r="E48" s="13"/>
       <c r="F48" s="13"/>
       <c r="G48" s="13"/>
       <c r="H48" s="13"/>
-      <c r="I48" s="36"/>
-    </row>
-    <row r="49" spans="1:9" s="10" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I48" s="33"/>
+    </row>
+    <row r="49" spans="1:9" s="10" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>43</v>
       </c>
       <c r="B49" s="29" t="s">
-        <v>175</v>
-      </c>
-      <c r="C49" s="33"/>
+        <v>209</v>
+      </c>
+      <c r="C49" s="30"/>
       <c r="D49" s="13"/>
       <c r="E49" s="13"/>
       <c r="F49" s="13"/>
       <c r="G49" s="13"/>
       <c r="H49" s="13"/>
-      <c r="I49" s="36"/>
-    </row>
-    <row r="50" spans="1:9" s="10" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I49" s="33"/>
+    </row>
+    <row r="50" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>44</v>
       </c>
       <c r="B50" s="29" t="s">
-        <v>176</v>
-      </c>
-      <c r="C50" s="33"/>
+        <v>210</v>
+      </c>
+      <c r="C50" s="30"/>
       <c r="D50" s="13"/>
       <c r="E50" s="13"/>
       <c r="F50" s="13"/>
       <c r="G50" s="13"/>
       <c r="H50" s="13"/>
-      <c r="I50" s="36"/>
-    </row>
-    <row r="51" spans="1:9" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I50" s="33"/>
+    </row>
+    <row r="51" spans="1:9" s="10" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>45</v>
       </c>
-      <c r="B51" s="30" t="s">
-        <v>144</v>
-      </c>
-      <c r="C51" s="33"/>
+      <c r="B51" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="C51" s="30"/>
       <c r="D51" s="13"/>
       <c r="E51" s="13"/>
       <c r="F51" s="13"/>
       <c r="G51" s="13"/>
       <c r="H51" s="13"/>
-      <c r="I51" s="36"/>
-    </row>
-    <row r="52" spans="1:9" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I51" s="33"/>
+    </row>
+    <row r="52" spans="1:9" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="27">
-        <f ca="1">IF(OFFSET(A52,-1,0) ="",OFFSET(A52,-2,0)+1,OFFSET(A52,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="0"/>
         <v>46</v>
       </c>
       <c r="B52" s="30" t="s">
-        <v>185</v>
-      </c>
-      <c r="C52" s="33"/>
+        <v>144</v>
+      </c>
+      <c r="C52" s="30"/>
       <c r="D52" s="13"/>
       <c r="E52" s="13"/>
       <c r="F52" s="13"/>
       <c r="G52" s="13"/>
       <c r="H52" s="13"/>
-      <c r="I52" s="36"/>
-    </row>
-    <row r="53" spans="1:9" s="10" customFormat="1" ht="24.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I52" s="33"/>
+    </row>
+    <row r="53" spans="1:9" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">IF(OFFSET(A53,-1,0) ="",OFFSET(A53,-2,0)+1,OFFSET(A53,-1,0)+1 )</f>
         <v>47</v>
       </c>
-      <c r="B53" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="C53" s="33"/>
+      <c r="B53" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="C53" s="29" t="s">
+        <v>214</v>
+      </c>
       <c r="D53" s="13"/>
       <c r="E53" s="13"/>
       <c r="F53" s="13"/>
       <c r="G53" s="13"/>
       <c r="H53" s="13"/>
-      <c r="I53" s="36"/>
-    </row>
-    <row r="54" spans="1:9" s="10" customFormat="1" ht="21.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="48" t="s">
+      <c r="I53" s="33"/>
+    </row>
+    <row r="54" spans="1:9" s="10" customFormat="1" ht="24.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B54" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="C54" s="30"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="13"/>
+      <c r="I54" s="33"/>
+    </row>
+    <row r="55" spans="1:9" s="10" customFormat="1" ht="21.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="B54" s="49"/>
-      <c r="C54" s="49"/>
-      <c r="D54" s="49"/>
-      <c r="E54" s="49"/>
-      <c r="F54" s="49"/>
-      <c r="G54" s="49"/>
-      <c r="H54" s="49"/>
-      <c r="I54" s="49"/>
-    </row>
-    <row r="55" spans="1:9" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="27">
-        <f ca="1">IF(OFFSET(A55,-2,0) ="",OFFSET(A55,-2,0)+1,OFFSET(A55,-2,0)+1 )</f>
-        <v>48</v>
-      </c>
-      <c r="B55" s="30" t="s">
+      <c r="B55" s="47"/>
+      <c r="C55" s="47"/>
+      <c r="D55" s="47"/>
+      <c r="E55" s="47"/>
+      <c r="F55" s="47"/>
+      <c r="G55" s="47"/>
+      <c r="H55" s="47"/>
+      <c r="I55" s="47"/>
+    </row>
+    <row r="56" spans="1:9" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="27">
+        <f ca="1">IF(OFFSET(A56,-2,0) ="",OFFSET(A56,-2,0)+1,OFFSET(A56,-2,0)+1 )</f>
+        <v>49</v>
+      </c>
+      <c r="B56" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="C55" s="34"/>
-      <c r="E55" s="13"/>
-      <c r="F55" s="13"/>
-      <c r="G55" s="13"/>
-      <c r="H55" s="13"/>
-      <c r="I55" s="36"/>
-    </row>
-    <row r="56" spans="1:9" s="10" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="27">
-        <f t="shared" ca="1" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="B56" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="C56" s="33"/>
-      <c r="D56" s="13"/>
+      <c r="C56" s="51"/>
       <c r="E56" s="13"/>
       <c r="F56" s="13"/>
       <c r="G56" s="13"/>
       <c r="H56" s="13"/>
-      <c r="I56" s="36"/>
+      <c r="I56" s="33"/>
     </row>
     <row r="57" spans="1:9" s="10" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="27">
@@ -15391,664 +15433,537 @@
         <v>50</v>
       </c>
       <c r="B57" s="30" t="s">
-        <v>204</v>
-      </c>
-      <c r="C57" s="33"/>
+        <v>148</v>
+      </c>
+      <c r="C57" s="30"/>
       <c r="D57" s="13"/>
       <c r="E57" s="13"/>
       <c r="F57" s="13"/>
       <c r="G57" s="13"/>
       <c r="H57" s="13"/>
-      <c r="I57" s="36"/>
-    </row>
-    <row r="58" spans="1:9" s="10" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I57" s="33"/>
+    </row>
+    <row r="58" spans="1:9" s="10" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>51</v>
       </c>
       <c r="B58" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="C58" s="33"/>
+        <v>202</v>
+      </c>
+      <c r="C58" s="30"/>
       <c r="D58" s="13"/>
       <c r="E58" s="13"/>
       <c r="F58" s="13"/>
       <c r="G58" s="13"/>
       <c r="H58" s="13"/>
-      <c r="I58" s="36"/>
-    </row>
-    <row r="59" spans="1:9" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I58" s="33"/>
+    </row>
+    <row r="59" spans="1:9" s="10" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>52</v>
       </c>
       <c r="B59" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="C59" s="33"/>
+        <v>149</v>
+      </c>
+      <c r="C59" s="30"/>
       <c r="D59" s="13"/>
       <c r="E59" s="13"/>
       <c r="F59" s="13"/>
       <c r="G59" s="13"/>
       <c r="H59" s="13"/>
-      <c r="I59" s="36"/>
-    </row>
-    <row r="60" spans="1:9" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I59" s="33"/>
+    </row>
+    <row r="60" spans="1:9" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>53</v>
       </c>
       <c r="B60" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="C60" s="33"/>
+        <v>150</v>
+      </c>
+      <c r="C60" s="30"/>
       <c r="D60" s="13"/>
       <c r="E60" s="13"/>
       <c r="F60" s="13"/>
       <c r="G60" s="13"/>
       <c r="H60" s="13"/>
-      <c r="I60" s="36"/>
-    </row>
-    <row r="61" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="48" t="s">
+      <c r="I60" s="33"/>
+    </row>
+    <row r="61" spans="1:9" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B61" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="C61" s="30"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="13"/>
+      <c r="I61" s="33"/>
+    </row>
+    <row r="62" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="46" t="s">
         <v>154</v>
       </c>
-      <c r="B61" s="49"/>
-      <c r="C61" s="49"/>
-      <c r="D61" s="49"/>
-      <c r="E61" s="49"/>
-      <c r="F61" s="49"/>
-      <c r="G61" s="49"/>
-      <c r="H61" s="49"/>
-      <c r="I61" s="49"/>
-    </row>
-    <row r="62" spans="1:9" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="27">
-        <f ca="1">IF(OFFSET(A62,-2,0) ="",OFFSET(A62,-2,0)+1,OFFSET(A62,-2,0)+1 )</f>
-        <v>54</v>
-      </c>
-      <c r="B62" s="30" t="s">
+      <c r="B62" s="47"/>
+      <c r="C62" s="47"/>
+      <c r="D62" s="47"/>
+      <c r="E62" s="47"/>
+      <c r="F62" s="47"/>
+      <c r="G62" s="47"/>
+      <c r="H62" s="47"/>
+      <c r="I62" s="47"/>
+    </row>
+    <row r="63" spans="1:9" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="27">
+        <f ca="1">IF(OFFSET(A63,-2,0) ="",OFFSET(A63,-2,0)+1,OFFSET(A63,-2,0)+1 )</f>
+        <v>55</v>
+      </c>
+      <c r="B63" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="C62" s="33"/>
-      <c r="D62" s="13"/>
-      <c r="E62" s="13"/>
-      <c r="F62" s="13"/>
-      <c r="G62" s="13"/>
-      <c r="H62" s="13"/>
-      <c r="I62" s="36"/>
-    </row>
-    <row r="63" spans="1:9" s="10" customFormat="1" ht="25" x14ac:dyDescent="0.25">
-      <c r="A63" s="27">
-        <f t="shared" ca="1" si="0"/>
-        <v>55</v>
-      </c>
-      <c r="B63" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="C63" s="33"/>
+      <c r="C63" s="30"/>
       <c r="D63" s="13"/>
       <c r="E63" s="13"/>
       <c r="F63" s="13"/>
       <c r="G63" s="13"/>
       <c r="H63" s="13"/>
-      <c r="I63" s="36"/>
-    </row>
-    <row r="64" spans="1:9" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I63" s="33"/>
+    </row>
+    <row r="64" spans="1:9" s="10" customFormat="1" ht="25" x14ac:dyDescent="0.25">
       <c r="A64" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>56</v>
       </c>
       <c r="B64" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="C64" s="33"/>
+        <v>148</v>
+      </c>
+      <c r="C64" s="30"/>
       <c r="D64" s="13"/>
       <c r="E64" s="13"/>
       <c r="F64" s="13"/>
       <c r="G64" s="13"/>
       <c r="H64" s="13"/>
-      <c r="I64" s="36"/>
-    </row>
-    <row r="65" spans="1:9" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I64" s="33"/>
+    </row>
+    <row r="65" spans="1:9" s="10" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>57</v>
       </c>
       <c r="B65" s="30" t="s">
-        <v>153</v>
-      </c>
-      <c r="C65" s="33"/>
+        <v>202</v>
+      </c>
+      <c r="C65" s="30"/>
       <c r="D65" s="13"/>
       <c r="E65" s="13"/>
       <c r="F65" s="13"/>
       <c r="G65" s="13"/>
       <c r="H65" s="13"/>
-      <c r="I65" s="36"/>
-    </row>
-    <row r="66" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="48" t="s">
-        <v>155</v>
-      </c>
-      <c r="B66" s="49"/>
-      <c r="C66" s="49"/>
-      <c r="D66" s="49"/>
-      <c r="E66" s="49"/>
-      <c r="F66" s="49"/>
-      <c r="G66" s="49"/>
-      <c r="H66" s="49"/>
-      <c r="I66" s="49"/>
-    </row>
-    <row r="67" spans="1:9" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I65" s="33"/>
+    </row>
+    <row r="66" spans="1:9" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B66" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="C66" s="30"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="13"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="13"/>
+      <c r="I66" s="33"/>
+    </row>
+    <row r="67" spans="1:9" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="27">
-        <f ca="1">IF(OFFSET(A67,-2,0) ="",OFFSET(A67,-2,0)+1,OFFSET(A67,-2,0)+1 )</f>
-        <v>58</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>59</v>
       </c>
       <c r="B67" s="30" t="s">
-        <v>146</v>
-      </c>
-      <c r="C67" s="33"/>
+        <v>153</v>
+      </c>
+      <c r="C67" s="30"/>
+      <c r="D67" s="13"/>
       <c r="E67" s="13"/>
       <c r="F67" s="13"/>
       <c r="G67" s="13"/>
       <c r="H67" s="13"/>
-      <c r="I67" s="36"/>
-    </row>
-    <row r="68" spans="1:9" s="10" customFormat="1" ht="25" x14ac:dyDescent="0.25">
-      <c r="A68" s="27">
-        <f t="shared" ca="1" si="0"/>
-        <v>59</v>
-      </c>
-      <c r="B68" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="C68" s="33"/>
-      <c r="E68" s="13"/>
-      <c r="F68" s="13"/>
-      <c r="G68" s="13"/>
-      <c r="H68" s="13"/>
-      <c r="I68" s="36"/>
-    </row>
-    <row r="69" spans="1:9" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I67" s="33"/>
+    </row>
+    <row r="68" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="46" t="s">
+        <v>155</v>
+      </c>
+      <c r="B68" s="47"/>
+      <c r="C68" s="47"/>
+      <c r="D68" s="47"/>
+      <c r="E68" s="47"/>
+      <c r="F68" s="47"/>
+      <c r="G68" s="47"/>
+      <c r="H68" s="47"/>
+      <c r="I68" s="47"/>
+    </row>
+    <row r="69" spans="1:9" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">IF(OFFSET(A69,-2,0) ="",OFFSET(A69,-2,0)+1,OFFSET(A69,-2,0)+1 )</f>
         <v>60</v>
       </c>
-      <c r="B69" s="29" t="s">
-        <v>156</v>
-      </c>
-      <c r="C69" s="33"/>
-      <c r="D69" s="30"/>
+      <c r="B69" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="C69" s="30"/>
       <c r="E69" s="13"/>
       <c r="F69" s="13"/>
       <c r="G69" s="13"/>
       <c r="H69" s="13"/>
-      <c r="I69" s="36"/>
-    </row>
-    <row r="70" spans="1:9" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I69" s="33"/>
+    </row>
+    <row r="70" spans="1:9" s="10" customFormat="1" ht="25" x14ac:dyDescent="0.25">
       <c r="A70" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>61</v>
       </c>
-      <c r="B70" s="29" t="s">
-        <v>158</v>
-      </c>
-      <c r="C70" s="33"/>
-      <c r="D70" s="13"/>
+      <c r="B70" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="C70" s="30"/>
       <c r="E70" s="13"/>
       <c r="F70" s="13"/>
       <c r="G70" s="13"/>
       <c r="H70" s="13"/>
-      <c r="I70" s="36"/>
-    </row>
-    <row r="71" spans="1:9" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I70" s="33"/>
+    </row>
+    <row r="71" spans="1:9" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>62</v>
       </c>
       <c r="B71" s="29" t="s">
-        <v>157</v>
-      </c>
-      <c r="C71" s="33"/>
-      <c r="D71" s="13"/>
+        <v>156</v>
+      </c>
+      <c r="C71" s="30"/>
+      <c r="D71" s="30"/>
       <c r="E71" s="13"/>
       <c r="F71" s="13"/>
       <c r="G71" s="13"/>
       <c r="H71" s="13"/>
-      <c r="I71" s="36"/>
-    </row>
-    <row r="72" spans="1:9" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I71" s="33"/>
+    </row>
+    <row r="72" spans="1:9" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>63</v>
       </c>
       <c r="B72" s="29" t="s">
-        <v>129</v>
-      </c>
-      <c r="C72" s="33"/>
+        <v>158</v>
+      </c>
+      <c r="C72" s="30"/>
       <c r="D72" s="13"/>
       <c r="E72" s="13"/>
       <c r="F72" s="13"/>
       <c r="G72" s="13"/>
       <c r="H72" s="13"/>
-      <c r="I72" s="36"/>
-    </row>
-    <row r="73" spans="1:9" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I72" s="33"/>
+    </row>
+    <row r="73" spans="1:9" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>64</v>
       </c>
       <c r="B73" s="29" t="s">
-        <v>142</v>
-      </c>
-      <c r="C73" s="33"/>
+        <v>157</v>
+      </c>
+      <c r="C73" s="30"/>
       <c r="D73" s="13"/>
       <c r="E73" s="13"/>
       <c r="F73" s="13"/>
       <c r="G73" s="13"/>
       <c r="H73" s="13"/>
-      <c r="I73" s="36"/>
-    </row>
-    <row r="74" spans="1:9" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I73" s="33"/>
+    </row>
+    <row r="74" spans="1:9" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>65</v>
       </c>
       <c r="B74" s="29" t="s">
-        <v>143</v>
-      </c>
-      <c r="C74" s="33"/>
+        <v>129</v>
+      </c>
+      <c r="C74" s="30"/>
       <c r="D74" s="13"/>
       <c r="E74" s="13"/>
       <c r="F74" s="13"/>
       <c r="G74" s="13"/>
       <c r="H74" s="13"/>
-      <c r="I74" s="36"/>
-    </row>
-    <row r="75" spans="1:9" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I74" s="33"/>
+    </row>
+    <row r="75" spans="1:9" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>66</v>
       </c>
       <c r="B75" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="C75" s="33"/>
+        <v>142</v>
+      </c>
+      <c r="C75" s="30"/>
       <c r="D75" s="13"/>
       <c r="E75" s="13"/>
       <c r="F75" s="13"/>
       <c r="G75" s="13"/>
       <c r="H75" s="13"/>
-      <c r="I75" s="36"/>
-    </row>
-    <row r="76" spans="1:9" s="10" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I75" s="33"/>
+    </row>
+    <row r="76" spans="1:9" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>67</v>
       </c>
-      <c r="B76" s="30" t="s">
-        <v>159</v>
-      </c>
-      <c r="C76" s="33"/>
+      <c r="B76" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="C76" s="30"/>
       <c r="D76" s="13"/>
       <c r="E76" s="13"/>
       <c r="F76" s="13"/>
       <c r="G76" s="13"/>
       <c r="H76" s="13"/>
-      <c r="I76" s="36"/>
-    </row>
-    <row r="77" spans="1:9" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I76" s="33"/>
+    </row>
+    <row r="77" spans="1:9" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>68</v>
       </c>
-      <c r="B77" s="30" t="s">
-        <v>160</v>
-      </c>
-      <c r="C77" s="33"/>
+      <c r="B77" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="C77" s="30"/>
       <c r="D77" s="13"/>
       <c r="E77" s="13"/>
       <c r="F77" s="13"/>
       <c r="G77" s="13"/>
       <c r="H77" s="13"/>
-      <c r="I77" s="36"/>
-    </row>
-    <row r="78" spans="1:9" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I77" s="33"/>
+    </row>
+    <row r="78" spans="1:9" s="10" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="27">
-        <f ca="1">IF(OFFSET(A78,-1,0) ="",OFFSET(A78,-2,0)+1,OFFSET(A78,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="0"/>
         <v>69</v>
       </c>
       <c r="B78" s="30" t="s">
-        <v>184</v>
-      </c>
-      <c r="C78" s="33"/>
-      <c r="D78" s="30"/>
+        <v>159</v>
+      </c>
+      <c r="C78" s="30"/>
+      <c r="D78" s="13"/>
       <c r="E78" s="13"/>
       <c r="F78" s="13"/>
       <c r="G78" s="13"/>
       <c r="H78" s="13"/>
-      <c r="I78" s="36"/>
-    </row>
-    <row r="79" spans="1:9" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I78" s="33"/>
+    </row>
+    <row r="79" spans="1:9" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>70</v>
       </c>
-      <c r="B79" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="C79" s="33"/>
+      <c r="B79" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="C79" s="30"/>
       <c r="D79" s="13"/>
       <c r="E79" s="13"/>
       <c r="F79" s="13"/>
       <c r="G79" s="13"/>
       <c r="H79" s="13"/>
-      <c r="I79" s="36"/>
-    </row>
-    <row r="80" spans="1:9" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="41" t="s">
+      <c r="I79" s="33"/>
+    </row>
+    <row r="80" spans="1:9" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="27">
+        <f ca="1">IF(OFFSET(A80,-1,0) ="",OFFSET(A80,-2,0)+1,OFFSET(A80,-1,0)+1 )</f>
+        <v>71</v>
+      </c>
+      <c r="B80" s="30" t="s">
+        <v>184</v>
+      </c>
+      <c r="C80" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="D80" s="30"/>
+      <c r="E80" s="13"/>
+      <c r="F80" s="13"/>
+      <c r="G80" s="13"/>
+      <c r="H80" s="13"/>
+      <c r="I80" s="33"/>
+    </row>
+    <row r="81" spans="1:9" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="B81" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="C81" s="30"/>
+      <c r="D81" s="13"/>
+      <c r="E81" s="13"/>
+      <c r="F81" s="13"/>
+      <c r="G81" s="13"/>
+      <c r="H81" s="13"/>
+      <c r="I81" s="33"/>
+    </row>
+    <row r="82" spans="1:9" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="38" t="s">
         <v>167</v>
       </c>
-      <c r="B80" s="50"/>
-      <c r="C80" s="50"/>
-      <c r="D80" s="50"/>
-      <c r="E80" s="50"/>
-      <c r="F80" s="50"/>
-      <c r="G80" s="50"/>
-      <c r="H80" s="50"/>
-      <c r="I80" s="50"/>
-    </row>
-    <row r="81" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="48" t="s">
+      <c r="B82" s="45"/>
+      <c r="C82" s="45"/>
+      <c r="D82" s="45"/>
+      <c r="E82" s="45"/>
+      <c r="F82" s="45"/>
+      <c r="G82" s="45"/>
+      <c r="H82" s="45"/>
+      <c r="I82" s="45"/>
+    </row>
+    <row r="83" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="46" t="s">
         <v>174</v>
       </c>
-      <c r="B81" s="49"/>
-      <c r="C81" s="49"/>
-      <c r="D81" s="49"/>
-      <c r="E81" s="49"/>
-      <c r="F81" s="49"/>
-      <c r="G81" s="49"/>
-      <c r="H81" s="49"/>
-      <c r="I81" s="49"/>
-    </row>
-    <row r="82" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="27">
-        <f ca="1">IF(OFFSET(A82,-3,0) ="",OFFSET(A82,-3,0)+1,OFFSET(A82,-3,0)+1 )</f>
-        <v>71</v>
-      </c>
-      <c r="B82" s="30" t="s">
+      <c r="B83" s="47"/>
+      <c r="C83" s="47"/>
+      <c r="D83" s="47"/>
+      <c r="E83" s="47"/>
+      <c r="F83" s="47"/>
+      <c r="G83" s="47"/>
+      <c r="H83" s="47"/>
+      <c r="I83" s="47"/>
+    </row>
+    <row r="84" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="27">
+        <f ca="1">IF(OFFSET(A84,-3,0) ="",OFFSET(A84,-3,0)+1,OFFSET(A84,-3,0)+1 )</f>
+        <v>73</v>
+      </c>
+      <c r="B84" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="C82" s="33"/>
-      <c r="D82" s="13"/>
-      <c r="E82" s="13"/>
-      <c r="F82" s="13"/>
-      <c r="G82" s="13"/>
-      <c r="H82" s="13"/>
-      <c r="I82" s="36"/>
-    </row>
-    <row r="83" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="27">
-        <f t="shared" ref="A83:A86" ca="1" si="2">IF(OFFSET(A83,-1,0) ="",OFFSET(A83,-2,0)+1,OFFSET(A83,-1,0)+1 )</f>
-        <v>72</v>
-      </c>
-      <c r="B83" s="30" t="s">
-        <v>182</v>
-      </c>
-      <c r="C83" s="33"/>
-      <c r="D83" s="13"/>
-      <c r="E83" s="13"/>
-      <c r="F83" s="13"/>
-      <c r="G83" s="13"/>
-      <c r="H83" s="13"/>
-      <c r="I83" s="36"/>
-    </row>
-    <row r="84" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="27">
-        <f t="shared" ca="1" si="2"/>
-        <v>73</v>
-      </c>
-      <c r="B84" s="30" t="s">
-        <v>179</v>
-      </c>
-      <c r="C84" s="33"/>
+      <c r="C84" s="30"/>
       <c r="D84" s="13"/>
       <c r="E84" s="13"/>
       <c r="F84" s="13"/>
       <c r="G84" s="13"/>
       <c r="H84" s="13"/>
-      <c r="I84" s="36"/>
-    </row>
-    <row r="85" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I84" s="33"/>
+    </row>
+    <row r="85" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="27">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ref="A85:A87" ca="1" si="2">IF(OFFSET(A85,-1,0) ="",OFFSET(A85,-2,0)+1,OFFSET(A85,-1,0)+1 )</f>
         <v>74</v>
       </c>
       <c r="B85" s="30" t="s">
-        <v>193</v>
-      </c>
-      <c r="C85" s="33" t="s">
-        <v>180</v>
-      </c>
-      <c r="D85" s="30"/>
+        <v>182</v>
+      </c>
+      <c r="C85" s="30"/>
+      <c r="D85" s="13"/>
       <c r="E85" s="13"/>
       <c r="F85" s="13"/>
       <c r="G85" s="13"/>
       <c r="H85" s="13"/>
-      <c r="I85" s="36"/>
-    </row>
-    <row r="86" spans="1:9" s="10" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I85" s="33"/>
+    </row>
+    <row r="86" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="27">
         <f t="shared" ca="1" si="2"/>
         <v>75</v>
       </c>
       <c r="B86" s="30" t="s">
-        <v>186</v>
-      </c>
-      <c r="C86" s="33"/>
+        <v>179</v>
+      </c>
+      <c r="C86" s="30"/>
       <c r="D86" s="13"/>
       <c r="E86" s="13"/>
       <c r="F86" s="13"/>
       <c r="G86" s="13"/>
       <c r="H86" s="13"/>
-      <c r="I86" s="36"/>
-    </row>
-    <row r="87" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="48" t="s">
-        <v>202</v>
-      </c>
-      <c r="B87" s="49"/>
-      <c r="C87" s="49"/>
-      <c r="D87" s="49"/>
-      <c r="E87" s="49"/>
-      <c r="F87" s="49"/>
-      <c r="G87" s="49"/>
-      <c r="H87" s="49"/>
-      <c r="I87" s="49"/>
-    </row>
-    <row r="88" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I86" s="33"/>
+    </row>
+    <row r="87" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>76</v>
+      </c>
+      <c r="B87" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="C87" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="D87" s="30"/>
+      <c r="E87" s="13"/>
+      <c r="F87" s="13"/>
+      <c r="G87" s="13"/>
+      <c r="H87" s="13"/>
+      <c r="I87" s="33"/>
+    </row>
+    <row r="88" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="27">
         <f ca="1">IF(OFFSET(A88,-2,0) ="",OFFSET(A88,-2,0)+1,OFFSET(A88,-2,0)+1 )</f>
         <v>76</v>
       </c>
       <c r="B88" s="30" t="s">
-        <v>188</v>
-      </c>
-      <c r="C88" s="33"/>
+        <v>193</v>
+      </c>
+      <c r="C88" s="30"/>
       <c r="D88" s="13"/>
       <c r="E88" s="13"/>
       <c r="F88" s="13"/>
       <c r="G88" s="13"/>
       <c r="H88" s="13"/>
-      <c r="I88" s="36"/>
-    </row>
-    <row r="89" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I88" s="33"/>
+    </row>
+    <row r="89" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="27">
-        <f t="shared" ref="A89:A93" ca="1" si="3">IF(OFFSET(A89,-1,0) ="",OFFSET(A89,-2,0)+1,OFFSET(A89,-1,0)+1 )</f>
+        <f ca="1">IF(OFFSET(A89,-2,0) ="",OFFSET(A89,-2,0)+1,OFFSET(A89,-2,0)+1 )</f>
         <v>77</v>
       </c>
       <c r="B89" s="30" t="s">
-        <v>189</v>
-      </c>
-      <c r="C89" s="33"/>
+        <v>194</v>
+      </c>
+      <c r="C89" s="30"/>
       <c r="D89" s="13"/>
       <c r="E89" s="13"/>
       <c r="F89" s="13"/>
       <c r="G89" s="13"/>
       <c r="H89" s="13"/>
-      <c r="I89" s="36"/>
-    </row>
-    <row r="90" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I89" s="33"/>
+    </row>
+    <row r="90" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="27">
-        <f t="shared" ca="1" si="3"/>
-        <v>78</v>
-      </c>
-      <c r="B90" s="30" t="s">
-        <v>190</v>
-      </c>
-      <c r="C90" s="33"/>
-      <c r="D90" s="13"/>
+        <f ca="1">IF(OFFSET(A90,-2,0) ="",OFFSET(A90,-2,0)+1,OFFSET(A90,-2,0)+1 )</f>
+        <v>77</v>
+      </c>
+      <c r="B90" s="29" t="s">
+        <v>212</v>
+      </c>
+      <c r="C90" s="30"/>
+      <c r="D90" s="30"/>
       <c r="E90" s="13"/>
       <c r="F90" s="13"/>
       <c r="G90" s="13"/>
       <c r="H90" s="13"/>
-      <c r="I90" s="36"/>
-    </row>
-    <row r="91" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="27">
-        <f t="shared" ca="1" si="3"/>
-        <v>79</v>
-      </c>
-      <c r="B91" s="30" t="s">
-        <v>193</v>
-      </c>
-      <c r="C91" s="33" t="s">
-        <v>180</v>
-      </c>
-      <c r="D91" s="30"/>
-      <c r="E91" s="13"/>
-      <c r="F91" s="13"/>
-      <c r="G91" s="13"/>
-      <c r="H91" s="13"/>
-      <c r="I91" s="36"/>
-    </row>
-    <row r="92" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="27">
-        <f t="shared" ca="1" si="3"/>
-        <v>80</v>
-      </c>
-      <c r="B92" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="C92" s="33"/>
-      <c r="D92" s="13"/>
-      <c r="E92" s="13"/>
-      <c r="F92" s="13"/>
-      <c r="G92" s="13"/>
-      <c r="H92" s="13"/>
-      <c r="I92" s="36"/>
-    </row>
-    <row r="93" spans="1:9" s="10" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="27">
-        <f t="shared" ca="1" si="3"/>
-        <v>81</v>
-      </c>
-      <c r="B93" s="30" t="s">
-        <v>187</v>
-      </c>
-      <c r="C93" s="33"/>
-      <c r="D93" s="13"/>
-      <c r="E93" s="13"/>
-      <c r="F93" s="13"/>
-      <c r="G93" s="13"/>
-      <c r="H93" s="13"/>
-      <c r="I93" s="36"/>
-    </row>
-    <row r="94" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="48" t="s">
-        <v>197</v>
-      </c>
-      <c r="B94" s="49"/>
-      <c r="C94" s="49"/>
-      <c r="D94" s="49"/>
-      <c r="E94" s="49"/>
-      <c r="F94" s="49"/>
-      <c r="G94" s="49"/>
-      <c r="H94" s="49"/>
-      <c r="I94" s="49"/>
-    </row>
-    <row r="95" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="27">
-        <f ca="1">IF(OFFSET(A95,-2,0) ="",OFFSET(A95,-2,0)+1,OFFSET(A95,-2,0)+1 )</f>
-        <v>82</v>
-      </c>
-      <c r="B95" s="30" t="s">
-        <v>194</v>
-      </c>
-      <c r="C95" s="33"/>
-      <c r="D95" s="13"/>
-      <c r="E95" s="13"/>
-      <c r="F95" s="13"/>
-      <c r="G95" s="13"/>
-      <c r="H95" s="13"/>
-      <c r="I95" s="36"/>
-    </row>
-    <row r="96" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="48" t="s">
-        <v>198</v>
-      </c>
-      <c r="B96" s="49"/>
-      <c r="C96" s="49"/>
-      <c r="D96" s="49"/>
-      <c r="E96" s="49"/>
-      <c r="F96" s="49"/>
-      <c r="G96" s="49"/>
-      <c r="H96" s="49"/>
-      <c r="I96" s="49"/>
-    </row>
-    <row r="97" spans="1:26" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="27">
-        <f ca="1">IF(OFFSET(A97,-2,0) ="",OFFSET(A97,-2,0)+1,OFFSET(A97,-2,0)+1 )</f>
-        <v>83</v>
-      </c>
-      <c r="B97" s="30" t="s">
-        <v>195</v>
-      </c>
-      <c r="C97" s="33"/>
-      <c r="D97" s="13"/>
-      <c r="E97" s="13"/>
-      <c r="F97" s="13"/>
-      <c r="G97" s="13"/>
-      <c r="H97" s="13"/>
-      <c r="I97" s="36"/>
-    </row>
-    <row r="98" spans="1:26" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="27"/>
-      <c r="B98" s="30"/>
-      <c r="C98" s="33"/>
-      <c r="D98" s="13"/>
-      <c r="E98" s="13"/>
-      <c r="F98" s="13"/>
-      <c r="G98" s="13"/>
-      <c r="H98" s="13"/>
-      <c r="I98" s="36"/>
-    </row>
-    <row r="99" spans="1:26" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="41" t="s">
+      <c r="I90" s="33"/>
+    </row>
+    <row r="100" spans="1:26" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="48" t="s">
         <v>207</v>
-      </c>
-      <c r="B99" s="50"/>
-      <c r="C99" s="50"/>
-      <c r="D99" s="50"/>
-      <c r="E99" s="50"/>
-      <c r="F99" s="50"/>
-      <c r="G99" s="50"/>
-      <c r="H99" s="50"/>
-      <c r="I99" s="50"/>
-    </row>
-    <row r="100" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="48" t="s">
-        <v>177</v>
       </c>
       <c r="B100" s="49"/>
       <c r="C100" s="49"/>
@@ -16057,1150 +15972,1227 @@
       <c r="F100" s="49"/>
       <c r="G100" s="49"/>
       <c r="H100" s="49"/>
-      <c r="I100" s="49"/>
-      <c r="J100" s="26"/>
-      <c r="K100" s="26"/>
-      <c r="L100" s="26"/>
-      <c r="M100" s="26"/>
-      <c r="N100" s="26"/>
-      <c r="O100" s="26"/>
-      <c r="P100" s="26"/>
-      <c r="Q100" s="26"/>
-      <c r="R100" s="26"/>
-      <c r="S100" s="26"/>
-      <c r="T100" s="26"/>
-      <c r="U100" s="26"/>
-      <c r="V100" s="26"/>
-      <c r="W100" s="26"/>
-      <c r="X100" s="26"/>
-      <c r="Y100" s="26"/>
-      <c r="Z100" s="26"/>
-    </row>
-    <row r="101" spans="1:26" s="10" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="27">
-        <f ca="1">IF(OFFSET(A101,-3,0) ="",OFFSET(A101,-3,0)+1,OFFSET(A101,-3,0)+1 )</f>
-        <v>1</v>
-      </c>
-      <c r="B101" s="30" t="s">
+      <c r="I100" s="50"/>
+    </row>
+    <row r="101" spans="1:26" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="38" t="s">
+        <v>204</v>
+      </c>
+      <c r="B101" s="45"/>
+      <c r="C101" s="45"/>
+      <c r="D101" s="45"/>
+      <c r="E101" s="45"/>
+      <c r="F101" s="45"/>
+      <c r="G101" s="45"/>
+      <c r="H101" s="45"/>
+      <c r="I101" s="45"/>
+    </row>
+    <row r="102" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A102" s="46" t="s">
+        <v>177</v>
+      </c>
+      <c r="B102" s="47"/>
+      <c r="C102" s="47"/>
+      <c r="D102" s="47"/>
+      <c r="E102" s="47"/>
+      <c r="F102" s="47"/>
+      <c r="G102" s="47"/>
+      <c r="H102" s="47"/>
+      <c r="I102" s="47"/>
+      <c r="J102" s="26"/>
+      <c r="K102" s="26"/>
+      <c r="L102" s="26"/>
+      <c r="M102" s="26"/>
+      <c r="N102" s="26"/>
+      <c r="O102" s="26"/>
+      <c r="P102" s="26"/>
+      <c r="Q102" s="26"/>
+      <c r="R102" s="26"/>
+      <c r="S102" s="26"/>
+      <c r="T102" s="26"/>
+      <c r="U102" s="26"/>
+      <c r="V102" s="26"/>
+      <c r="W102" s="26"/>
+      <c r="X102" s="26"/>
+      <c r="Y102" s="26"/>
+      <c r="Z102" s="26"/>
+    </row>
+    <row r="103" spans="1:26" s="10" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="27" t="e">
+        <f ca="1">IF(OFFSET(A103,-3,0) ="",OFFSET(A103,-3,0)+1,OFFSET(A103,-3,0)+1 )</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B103" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="C101" s="34"/>
-      <c r="D101" s="13"/>
-      <c r="E101" s="13"/>
-      <c r="F101" s="13"/>
-      <c r="G101" s="13"/>
-      <c r="H101" s="13"/>
-      <c r="I101" s="36"/>
-    </row>
-    <row r="102" spans="1:26" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="27">
-        <f ca="1">IF(OFFSET(A102,-1,0) ="",OFFSET(A102,-2,0)+1,OFFSET(A102,-1,0)+1 )</f>
-        <v>2</v>
-      </c>
-      <c r="B102" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="C102" s="33"/>
-      <c r="D102" s="13"/>
-      <c r="E102" s="13"/>
-      <c r="F102" s="13"/>
-      <c r="G102" s="13"/>
-      <c r="H102" s="13"/>
-      <c r="I102" s="36"/>
-    </row>
-    <row r="103" spans="1:26" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="27">
-        <f ca="1">IF(OFFSET(A103,-1,0) ="",OFFSET(A103,-2,0)+1,OFFSET(A103,-1,0)+1 )</f>
-        <v>3</v>
-      </c>
-      <c r="B103" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="C103" s="33"/>
-      <c r="D103" s="13"/>
+      <c r="C103" s="51"/>
+      <c r="D103" s="33" t="s">
+        <v>205</v>
+      </c>
       <c r="E103" s="13"/>
       <c r="F103" s="13"/>
       <c r="G103" s="13"/>
       <c r="H103" s="13"/>
-      <c r="I103" s="36"/>
-    </row>
-    <row r="104" spans="1:26" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="48" t="s">
-        <v>161</v>
-      </c>
-      <c r="B104" s="49"/>
-      <c r="C104" s="49"/>
-      <c r="D104" s="49"/>
-      <c r="E104" s="49"/>
-      <c r="F104" s="49"/>
-      <c r="G104" s="49"/>
-      <c r="H104" s="49"/>
-      <c r="I104" s="49"/>
-    </row>
-    <row r="105" spans="1:26" s="10" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="27">
-        <f ca="1">IF(OFFSET(A105,-2,0) ="",OFFSET(A105,-2,0)+1,OFFSET(A105,-2,0)+1 )</f>
-        <v>4</v>
-      </c>
-      <c r="B105" s="30" t="s">
-        <v>162</v>
-      </c>
-      <c r="C105" s="33"/>
+      <c r="I103" s="33"/>
+    </row>
+    <row r="104" spans="1:26" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="27" t="e">
+        <f ca="1">IF(OFFSET(A104,-1,0) ="",OFFSET(A104,-2,0)+1,OFFSET(A104,-1,0)+1 )</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B104" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="C104" s="30"/>
+      <c r="D104" s="13"/>
+      <c r="E104" s="13"/>
+      <c r="F104" s="13"/>
+      <c r="G104" s="13"/>
+      <c r="H104" s="13"/>
+      <c r="I104" s="33"/>
+    </row>
+    <row r="105" spans="1:26" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="27" t="e">
+        <f ca="1">IF(OFFSET(A105,-1,0) ="",OFFSET(A105,-2,0)+1,OFFSET(A105,-1,0)+1 )</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B105" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="C105" s="30"/>
       <c r="D105" s="13"/>
       <c r="E105" s="13"/>
       <c r="F105" s="13"/>
       <c r="G105" s="13"/>
       <c r="H105" s="13"/>
-      <c r="I105" s="36"/>
-    </row>
-    <row r="106" spans="1:26" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="27">
-        <f t="shared" ref="A106" ca="1" si="4">IF(OFFSET(A106,-1,0) ="",OFFSET(A106,-2,0)+1,OFFSET(A106,-1,0)+1 )</f>
-        <v>5</v>
-      </c>
-      <c r="B106" s="30" t="s">
+      <c r="I105" s="33"/>
+    </row>
+    <row r="106" spans="1:26" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="46" t="s">
+        <v>161</v>
+      </c>
+      <c r="B106" s="47"/>
+      <c r="C106" s="47"/>
+      <c r="D106" s="47"/>
+      <c r="E106" s="47"/>
+      <c r="F106" s="47"/>
+      <c r="G106" s="47"/>
+      <c r="H106" s="47"/>
+      <c r="I106" s="47"/>
+    </row>
+    <row r="107" spans="1:26" s="10" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="27" t="e">
+        <f ca="1">IF(OFFSET(A107,-2,0) ="",OFFSET(A107,-2,0)+1,OFFSET(A107,-2,0)+1 )</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B107" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="C107" s="30"/>
+      <c r="D107" s="13"/>
+      <c r="E107" s="13"/>
+      <c r="F107" s="13"/>
+      <c r="G107" s="13"/>
+      <c r="H107" s="13"/>
+      <c r="I107" s="33"/>
+    </row>
+    <row r="108" spans="1:26" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="27" t="e">
+        <f t="shared" ref="A108" ca="1" si="3">IF(OFFSET(A108,-1,0) ="",OFFSET(A108,-2,0)+1,OFFSET(A108,-1,0)+1 )</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B108" s="30" t="s">
         <v>163</v>
       </c>
-      <c r="C106" s="33"/>
-      <c r="D106" s="13"/>
-      <c r="E106" s="13"/>
-      <c r="F106" s="13"/>
-      <c r="G106" s="13"/>
-      <c r="H106" s="13"/>
-      <c r="I106" s="36"/>
-    </row>
-    <row r="107" spans="1:26" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="48" t="s">
-        <v>164</v>
-      </c>
-      <c r="B107" s="49"/>
-      <c r="C107" s="49"/>
-      <c r="D107" s="49"/>
-      <c r="E107" s="49"/>
-      <c r="F107" s="49"/>
-      <c r="G107" s="49"/>
-      <c r="H107" s="49"/>
-      <c r="I107" s="49"/>
-    </row>
-    <row r="108" spans="1:26" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="27">
-        <f ca="1">IF(OFFSET(A108,-2,0) ="",OFFSET(A108,-2,0)+1,OFFSET(A108,-2,0)+1 )</f>
-        <v>6</v>
-      </c>
-      <c r="B108" s="30" t="s">
-        <v>165</v>
-      </c>
-      <c r="C108" s="33"/>
+      <c r="C108" s="30"/>
       <c r="D108" s="13"/>
       <c r="E108" s="13"/>
       <c r="F108" s="13"/>
       <c r="G108" s="13"/>
       <c r="H108" s="13"/>
-      <c r="I108" s="36"/>
+      <c r="I108" s="33"/>
     </row>
     <row r="109" spans="1:26" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="48" t="s">
-        <v>192</v>
-      </c>
-      <c r="B109" s="49"/>
-      <c r="C109" s="49"/>
-      <c r="D109" s="49"/>
-      <c r="E109" s="49"/>
-      <c r="F109" s="49"/>
-      <c r="G109" s="49"/>
-      <c r="H109" s="49"/>
-      <c r="I109" s="49"/>
+      <c r="A109" s="46" t="s">
+        <v>164</v>
+      </c>
+      <c r="B109" s="47"/>
+      <c r="C109" s="47"/>
+      <c r="D109" s="47"/>
+      <c r="E109" s="47"/>
+      <c r="F109" s="47"/>
+      <c r="G109" s="47"/>
+      <c r="H109" s="47"/>
+      <c r="I109" s="47"/>
     </row>
     <row r="110" spans="1:26" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="27">
+      <c r="A110" s="27" t="e">
         <f ca="1">IF(OFFSET(A110,-2,0) ="",OFFSET(A110,-2,0)+1,OFFSET(A110,-2,0)+1 )</f>
-        <v>7</v>
+        <v>#VALUE!</v>
       </c>
       <c r="B110" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="C110" s="33"/>
+      <c r="C110" s="30"/>
       <c r="D110" s="13"/>
       <c r="E110" s="13"/>
       <c r="F110" s="13"/>
       <c r="G110" s="13"/>
       <c r="H110" s="13"/>
-      <c r="I110" s="36"/>
+      <c r="I110" s="33"/>
     </row>
     <row r="111" spans="1:26" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="48" t="s">
-        <v>196</v>
-      </c>
-      <c r="B111" s="49"/>
-      <c r="C111" s="49"/>
-      <c r="D111" s="49"/>
-      <c r="E111" s="49"/>
-      <c r="F111" s="49"/>
-      <c r="G111" s="49"/>
-      <c r="H111" s="49"/>
-      <c r="I111" s="49"/>
+      <c r="A111" s="46" t="s">
+        <v>192</v>
+      </c>
+      <c r="B111" s="47"/>
+      <c r="C111" s="47"/>
+      <c r="D111" s="47"/>
+      <c r="E111" s="47"/>
+      <c r="F111" s="47"/>
+      <c r="G111" s="47"/>
+      <c r="H111" s="47"/>
+      <c r="I111" s="47"/>
     </row>
     <row r="112" spans="1:26" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="27">
+      <c r="A112" s="27" t="e">
         <f ca="1">IF(OFFSET(A112,-2,0) ="",OFFSET(A112,-2,0)+1,OFFSET(A112,-2,0)+1 )</f>
-        <v>8</v>
+        <v>#VALUE!</v>
       </c>
       <c r="B112" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="C112" s="33"/>
+      <c r="C112" s="30"/>
       <c r="D112" s="13"/>
       <c r="E112" s="13"/>
       <c r="F112" s="13"/>
       <c r="G112" s="13"/>
       <c r="H112" s="13"/>
-      <c r="I112" s="36"/>
-    </row>
-    <row r="113" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="27"/>
-      <c r="B113" s="30"/>
-      <c r="C113" s="33"/>
-      <c r="D113" s="13"/>
-      <c r="E113" s="13"/>
-      <c r="F113" s="13"/>
-      <c r="G113" s="13"/>
-      <c r="H113" s="13"/>
-      <c r="I113" s="36"/>
+      <c r="I112" s="33"/>
+    </row>
+    <row r="113" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="B113" s="47"/>
+      <c r="C113" s="47"/>
+      <c r="D113" s="47"/>
+      <c r="E113" s="47"/>
+      <c r="F113" s="47"/>
+      <c r="G113" s="47"/>
+      <c r="H113" s="47"/>
+      <c r="I113" s="47"/>
     </row>
     <row r="114" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="27"/>
-      <c r="B114" s="30"/>
-      <c r="C114" s="33"/>
+      <c r="A114" s="27" t="e">
+        <f ca="1">IF(OFFSET(A114,-2,0) ="",OFFSET(A114,-2,0)+1,OFFSET(A114,-2,0)+1 )</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B114" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="C114" s="30"/>
       <c r="D114" s="13"/>
       <c r="E114" s="13"/>
       <c r="F114" s="13"/>
       <c r="G114" s="13"/>
       <c r="H114" s="13"/>
-      <c r="I114" s="36"/>
-    </row>
-    <row r="115" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="27"/>
-      <c r="B115" s="30"/>
-      <c r="C115" s="33"/>
+      <c r="I114" s="33"/>
+    </row>
+    <row r="115" spans="1:9" s="10" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="27" t="e">
+        <f ca="1">IF(OFFSET(A115,-1,0) ="",OFFSET(A115,-2,0)+1,OFFSET(A115,-1,0)+1 )</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B115" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="C115" s="30"/>
       <c r="D115" s="13"/>
       <c r="E115" s="13"/>
       <c r="F115" s="13"/>
       <c r="G115" s="13"/>
       <c r="H115" s="13"/>
-      <c r="I115" s="36"/>
-    </row>
-    <row r="116" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="27"/>
-      <c r="B116" s="30"/>
-      <c r="C116" s="33"/>
+      <c r="I115" s="33"/>
+    </row>
+    <row r="116" spans="1:9" s="10" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="27" t="e">
+        <f ca="1">IF(OFFSET(A116,-1,0) ="",OFFSET(A116,-2,0)+1,OFFSET(A116,-1,0)+1 )</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B116" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="C116" s="30"/>
       <c r="D116" s="13"/>
       <c r="E116" s="13"/>
       <c r="F116" s="13"/>
       <c r="G116" s="13"/>
       <c r="H116" s="13"/>
-      <c r="I116" s="36"/>
-    </row>
-    <row r="117" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="27"/>
-      <c r="B117" s="30"/>
-      <c r="C117" s="33"/>
-      <c r="D117" s="13"/>
-      <c r="E117" s="13"/>
-      <c r="F117" s="13"/>
-      <c r="G117" s="13"/>
-      <c r="H117" s="13"/>
-      <c r="I117" s="36"/>
-    </row>
-    <row r="118" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="27"/>
-      <c r="B118" s="30"/>
-      <c r="C118" s="33"/>
+      <c r="I116" s="33"/>
+    </row>
+    <row r="117" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="46" t="s">
+        <v>200</v>
+      </c>
+      <c r="B117" s="47"/>
+      <c r="C117" s="47"/>
+      <c r="D117" s="47"/>
+      <c r="E117" s="47"/>
+      <c r="F117" s="47"/>
+      <c r="G117" s="47"/>
+      <c r="H117" s="47"/>
+      <c r="I117" s="47"/>
+    </row>
+    <row r="118" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="27" t="e">
+        <f ca="1">IF(OFFSET(A118,-2,0) ="",OFFSET(A118,-2,0)+1,OFFSET(A118,-2,0)+1 )</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B118" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="C118" s="30"/>
       <c r="D118" s="13"/>
       <c r="E118" s="13"/>
       <c r="F118" s="13"/>
       <c r="G118" s="13"/>
       <c r="H118" s="13"/>
-      <c r="I118" s="36"/>
-    </row>
-    <row r="119" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="27"/>
-      <c r="B119" s="30"/>
-      <c r="C119" s="33"/>
+      <c r="I118" s="33"/>
+    </row>
+    <row r="119" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="27" t="e">
+        <f t="shared" ref="A119:A121" ca="1" si="4">IF(OFFSET(A119,-1,0) ="",OFFSET(A119,-2,0)+1,OFFSET(A119,-1,0)+1 )</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B119" s="30" t="s">
+        <v>189</v>
+      </c>
+      <c r="C119" s="30"/>
       <c r="D119" s="13"/>
       <c r="E119" s="13"/>
       <c r="F119" s="13"/>
       <c r="G119" s="13"/>
       <c r="H119" s="13"/>
-      <c r="I119" s="36"/>
+      <c r="I119" s="33"/>
     </row>
     <row r="120" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="27"/>
-      <c r="B120" s="30"/>
-      <c r="C120" s="33"/>
+      <c r="A120" s="27" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B120" s="30" t="s">
+        <v>190</v>
+      </c>
+      <c r="C120" s="30"/>
       <c r="D120" s="13"/>
       <c r="E120" s="13"/>
       <c r="F120" s="13"/>
       <c r="G120" s="13"/>
       <c r="H120" s="13"/>
-      <c r="I120" s="36"/>
-    </row>
-    <row r="121" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="27"/>
-      <c r="B121" s="30"/>
-      <c r="C121" s="33"/>
-      <c r="D121" s="13"/>
+      <c r="I120" s="33"/>
+    </row>
+    <row r="121" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="27" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B121" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="C121" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="D121" s="30"/>
       <c r="E121" s="13"/>
       <c r="F121" s="13"/>
       <c r="G121" s="13"/>
       <c r="H121" s="13"/>
-      <c r="I121" s="36"/>
-    </row>
-    <row r="122" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="27"/>
-      <c r="B122" s="30"/>
-      <c r="C122" s="33"/>
-      <c r="D122" s="13"/>
-      <c r="E122" s="13"/>
-      <c r="F122" s="13"/>
-      <c r="G122" s="13"/>
-      <c r="H122" s="13"/>
-      <c r="I122" s="36"/>
+      <c r="I121" s="33"/>
+    </row>
+    <row r="122" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="46" t="s">
+        <v>196</v>
+      </c>
+      <c r="B122" s="47"/>
+      <c r="C122" s="47"/>
+      <c r="D122" s="47"/>
+      <c r="E122" s="47"/>
+      <c r="F122" s="47"/>
+      <c r="G122" s="47"/>
+      <c r="H122" s="47"/>
+      <c r="I122" s="47"/>
     </row>
     <row r="123" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="27"/>
-      <c r="B123" s="30"/>
-      <c r="C123" s="33"/>
+      <c r="A123" s="27" t="e">
+        <f ca="1">IF(OFFSET(A123,-2,0) ="",OFFSET(A123,-2,0)+1,OFFSET(A123,-2,0)+1 )</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B123" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="C123" s="30"/>
       <c r="D123" s="13"/>
       <c r="E123" s="13"/>
       <c r="F123" s="13"/>
       <c r="G123" s="13"/>
       <c r="H123" s="13"/>
-      <c r="I123" s="36"/>
-    </row>
-    <row r="124" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="27"/>
-      <c r="B124" s="30"/>
-      <c r="C124" s="33"/>
-      <c r="D124" s="13"/>
-      <c r="E124" s="13"/>
-      <c r="F124" s="13"/>
-      <c r="G124" s="13"/>
-      <c r="H124" s="13"/>
-      <c r="I124" s="36"/>
+      <c r="I123" s="33"/>
+    </row>
+    <row r="124" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="46" t="s">
+        <v>197</v>
+      </c>
+      <c r="B124" s="47"/>
+      <c r="C124" s="47"/>
+      <c r="D124" s="47"/>
+      <c r="E124" s="47"/>
+      <c r="F124" s="47"/>
+      <c r="G124" s="47"/>
+      <c r="H124" s="47"/>
+      <c r="I124" s="47"/>
     </row>
     <row r="125" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="27"/>
-      <c r="B125" s="30"/>
-      <c r="C125" s="33"/>
+      <c r="A125" s="27" t="e">
+        <f ca="1">IF(OFFSET(A125,-2,0) ="",OFFSET(A125,-2,0)+1,OFFSET(A125,-2,0)+1 )</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B125" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="C125" s="30"/>
       <c r="D125" s="13"/>
       <c r="E125" s="13"/>
       <c r="F125" s="13"/>
       <c r="G125" s="13"/>
       <c r="H125" s="13"/>
-      <c r="I125" s="36"/>
+      <c r="I125" s="33"/>
     </row>
     <row r="126" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="27"/>
       <c r="B126" s="30"/>
-      <c r="C126" s="33"/>
+      <c r="C126" s="30"/>
       <c r="D126" s="13"/>
       <c r="E126" s="13"/>
       <c r="F126" s="13"/>
       <c r="G126" s="13"/>
       <c r="H126" s="13"/>
-      <c r="I126" s="36"/>
+      <c r="I126" s="33"/>
     </row>
     <row r="127" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="27"/>
       <c r="B127" s="30"/>
-      <c r="C127" s="33"/>
+      <c r="C127" s="30"/>
       <c r="D127" s="13"/>
       <c r="E127" s="13"/>
       <c r="F127" s="13"/>
       <c r="G127" s="13"/>
       <c r="H127" s="13"/>
-      <c r="I127" s="36"/>
+      <c r="I127" s="33"/>
     </row>
     <row r="128" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="27"/>
       <c r="B128" s="30"/>
-      <c r="C128" s="33"/>
+      <c r="C128" s="30"/>
       <c r="D128" s="13"/>
       <c r="E128" s="13"/>
       <c r="F128" s="13"/>
       <c r="G128" s="13"/>
       <c r="H128" s="13"/>
-      <c r="I128" s="36"/>
+      <c r="I128" s="33"/>
     </row>
     <row r="129" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="27"/>
       <c r="B129" s="30"/>
-      <c r="C129" s="33"/>
+      <c r="C129" s="30"/>
       <c r="D129" s="13"/>
       <c r="E129" s="13"/>
       <c r="F129" s="13"/>
       <c r="G129" s="13"/>
       <c r="H129" s="13"/>
-      <c r="I129" s="36"/>
+      <c r="I129" s="33"/>
     </row>
     <row r="130" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="27"/>
       <c r="B130" s="30"/>
-      <c r="C130" s="33"/>
+      <c r="C130" s="30"/>
       <c r="D130" s="13"/>
       <c r="E130" s="13"/>
       <c r="F130" s="13"/>
       <c r="G130" s="13"/>
       <c r="H130" s="13"/>
-      <c r="I130" s="36"/>
+      <c r="I130" s="33"/>
     </row>
     <row r="131" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="27"/>
       <c r="B131" s="30"/>
-      <c r="C131" s="33"/>
+      <c r="C131" s="30"/>
       <c r="D131" s="13"/>
       <c r="E131" s="13"/>
       <c r="F131" s="13"/>
       <c r="G131" s="13"/>
       <c r="H131" s="13"/>
-      <c r="I131" s="36"/>
+      <c r="I131" s="33"/>
     </row>
     <row r="132" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="27"/>
       <c r="B132" s="30"/>
-      <c r="C132" s="33"/>
+      <c r="C132" s="30"/>
       <c r="D132" s="13"/>
       <c r="E132" s="13"/>
       <c r="F132" s="13"/>
       <c r="G132" s="13"/>
       <c r="H132" s="13"/>
-      <c r="I132" s="36"/>
+      <c r="I132" s="33"/>
     </row>
     <row r="133" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="27"/>
       <c r="B133" s="30"/>
-      <c r="C133" s="33"/>
+      <c r="C133" s="30"/>
       <c r="D133" s="13"/>
       <c r="E133" s="13"/>
       <c r="F133" s="13"/>
       <c r="G133" s="13"/>
       <c r="H133" s="13"/>
-      <c r="I133" s="36"/>
+      <c r="I133" s="33"/>
     </row>
     <row r="134" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="27"/>
       <c r="B134" s="30"/>
-      <c r="C134" s="33"/>
+      <c r="C134" s="30"/>
       <c r="D134" s="13"/>
       <c r="E134" s="13"/>
       <c r="F134" s="13"/>
       <c r="G134" s="13"/>
       <c r="H134" s="13"/>
-      <c r="I134" s="36"/>
+      <c r="I134" s="33"/>
     </row>
     <row r="135" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="27"/>
       <c r="B135" s="30"/>
-      <c r="C135" s="33"/>
+      <c r="C135" s="30"/>
       <c r="D135" s="13"/>
       <c r="E135" s="13"/>
       <c r="F135" s="13"/>
       <c r="G135" s="13"/>
       <c r="H135" s="13"/>
-      <c r="I135" s="36"/>
+      <c r="I135" s="33"/>
     </row>
     <row r="136" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="27"/>
       <c r="B136" s="30"/>
-      <c r="C136" s="33"/>
+      <c r="C136" s="30"/>
       <c r="D136" s="13"/>
       <c r="E136" s="13"/>
       <c r="F136" s="13"/>
       <c r="G136" s="13"/>
       <c r="H136" s="13"/>
-      <c r="I136" s="36"/>
+      <c r="I136" s="33"/>
     </row>
     <row r="137" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="27"/>
       <c r="B137" s="30"/>
-      <c r="C137" s="33"/>
+      <c r="C137" s="30"/>
       <c r="D137" s="13"/>
       <c r="E137" s="13"/>
       <c r="F137" s="13"/>
       <c r="G137" s="13"/>
       <c r="H137" s="13"/>
-      <c r="I137" s="36"/>
+      <c r="I137" s="33"/>
     </row>
     <row r="138" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="27"/>
       <c r="B138" s="30"/>
-      <c r="C138" s="33"/>
+      <c r="C138" s="30"/>
       <c r="D138" s="13"/>
       <c r="E138" s="13"/>
       <c r="F138" s="13"/>
       <c r="G138" s="13"/>
       <c r="H138" s="13"/>
-      <c r="I138" s="36"/>
+      <c r="I138" s="33"/>
     </row>
     <row r="139" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="27"/>
       <c r="B139" s="30"/>
-      <c r="C139" s="33"/>
+      <c r="C139" s="30"/>
       <c r="D139" s="13"/>
       <c r="E139" s="13"/>
       <c r="F139" s="13"/>
       <c r="G139" s="13"/>
       <c r="H139" s="13"/>
-      <c r="I139" s="36"/>
+      <c r="I139" s="33"/>
     </row>
     <row r="140" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="27"/>
       <c r="B140" s="30"/>
-      <c r="C140" s="33"/>
+      <c r="C140" s="30"/>
       <c r="D140" s="13"/>
       <c r="E140" s="13"/>
       <c r="F140" s="13"/>
       <c r="G140" s="13"/>
       <c r="H140" s="13"/>
-      <c r="I140" s="36"/>
+      <c r="I140" s="33"/>
     </row>
     <row r="141" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="27"/>
       <c r="B141" s="30"/>
-      <c r="C141" s="33"/>
+      <c r="C141" s="30"/>
       <c r="D141" s="13"/>
       <c r="E141" s="13"/>
       <c r="F141" s="13"/>
       <c r="G141" s="13"/>
       <c r="H141" s="13"/>
-      <c r="I141" s="36"/>
+      <c r="I141" s="33"/>
     </row>
     <row r="142" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="27"/>
       <c r="B142" s="30"/>
-      <c r="C142" s="33"/>
+      <c r="C142" s="30"/>
       <c r="D142" s="13"/>
       <c r="E142" s="13"/>
       <c r="F142" s="13"/>
       <c r="G142" s="13"/>
       <c r="H142" s="13"/>
-      <c r="I142" s="36"/>
+      <c r="I142" s="33"/>
     </row>
     <row r="143" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="27"/>
       <c r="B143" s="30"/>
-      <c r="C143" s="33"/>
+      <c r="C143" s="30"/>
       <c r="D143" s="13"/>
       <c r="E143" s="13"/>
       <c r="F143" s="13"/>
       <c r="G143" s="13"/>
       <c r="H143" s="13"/>
-      <c r="I143" s="36"/>
+      <c r="I143" s="33"/>
     </row>
     <row r="144" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="27"/>
       <c r="B144" s="30"/>
-      <c r="C144" s="33"/>
+      <c r="C144" s="30"/>
       <c r="D144" s="13"/>
       <c r="E144" s="13"/>
       <c r="F144" s="13"/>
       <c r="G144" s="13"/>
       <c r="H144" s="13"/>
-      <c r="I144" s="36"/>
+      <c r="I144" s="33"/>
     </row>
     <row r="145" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="27"/>
       <c r="B145" s="30"/>
-      <c r="C145" s="33"/>
+      <c r="C145" s="30"/>
       <c r="D145" s="13"/>
       <c r="E145" s="13"/>
       <c r="F145" s="13"/>
       <c r="G145" s="13"/>
       <c r="H145" s="13"/>
-      <c r="I145" s="36"/>
+      <c r="I145" s="33"/>
     </row>
     <row r="146" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="27"/>
       <c r="B146" s="30"/>
-      <c r="C146" s="33"/>
+      <c r="C146" s="30"/>
       <c r="D146" s="13"/>
       <c r="E146" s="13"/>
       <c r="F146" s="13"/>
       <c r="G146" s="13"/>
       <c r="H146" s="13"/>
-      <c r="I146" s="36"/>
+      <c r="I146" s="33"/>
     </row>
     <row r="147" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="27"/>
       <c r="B147" s="30"/>
-      <c r="C147" s="33"/>
+      <c r="C147" s="30"/>
       <c r="D147" s="13"/>
       <c r="E147" s="13"/>
       <c r="F147" s="13"/>
       <c r="G147" s="13"/>
       <c r="H147" s="13"/>
-      <c r="I147" s="36"/>
+      <c r="I147" s="33"/>
     </row>
     <row r="148" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="27"/>
       <c r="B148" s="30"/>
-      <c r="C148" s="33"/>
+      <c r="C148" s="30"/>
       <c r="D148" s="13"/>
       <c r="E148" s="13"/>
       <c r="F148" s="13"/>
       <c r="G148" s="13"/>
       <c r="H148" s="13"/>
-      <c r="I148" s="36"/>
+      <c r="I148" s="33"/>
     </row>
     <row r="149" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="27"/>
       <c r="B149" s="30"/>
-      <c r="C149" s="33"/>
+      <c r="C149" s="30"/>
       <c r="D149" s="13"/>
       <c r="E149" s="13"/>
       <c r="F149" s="13"/>
       <c r="G149" s="13"/>
       <c r="H149" s="13"/>
-      <c r="I149" s="36"/>
+      <c r="I149" s="33"/>
     </row>
     <row r="150" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="27"/>
       <c r="B150" s="30"/>
-      <c r="C150" s="33"/>
+      <c r="C150" s="30"/>
       <c r="D150" s="13"/>
       <c r="E150" s="13"/>
       <c r="F150" s="13"/>
       <c r="G150" s="13"/>
       <c r="H150" s="13"/>
-      <c r="I150" s="36"/>
+      <c r="I150" s="33"/>
     </row>
     <row r="151" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="27"/>
       <c r="B151" s="30"/>
-      <c r="C151" s="33"/>
+      <c r="C151" s="30"/>
       <c r="D151" s="13"/>
       <c r="E151" s="13"/>
       <c r="F151" s="13"/>
       <c r="G151" s="13"/>
       <c r="H151" s="13"/>
-      <c r="I151" s="36"/>
+      <c r="I151" s="33"/>
     </row>
     <row r="152" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="27"/>
       <c r="B152" s="30"/>
-      <c r="C152" s="33"/>
+      <c r="C152" s="30"/>
       <c r="D152" s="13"/>
       <c r="E152" s="13"/>
       <c r="F152" s="13"/>
       <c r="G152" s="13"/>
       <c r="H152" s="13"/>
-      <c r="I152" s="36"/>
+      <c r="I152" s="33"/>
     </row>
     <row r="153" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="27"/>
       <c r="B153" s="30"/>
-      <c r="C153" s="33"/>
+      <c r="C153" s="30"/>
       <c r="D153" s="13"/>
       <c r="E153" s="13"/>
       <c r="F153" s="13"/>
       <c r="G153" s="13"/>
       <c r="H153" s="13"/>
-      <c r="I153" s="36"/>
+      <c r="I153" s="33"/>
     </row>
     <row r="154" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="27"/>
       <c r="B154" s="30"/>
-      <c r="C154" s="33"/>
+      <c r="C154" s="30"/>
       <c r="D154" s="13"/>
       <c r="E154" s="13"/>
       <c r="F154" s="13"/>
       <c r="G154" s="13"/>
       <c r="H154" s="13"/>
-      <c r="I154" s="36"/>
+      <c r="I154" s="33"/>
     </row>
     <row r="155" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="27"/>
       <c r="B155" s="30"/>
-      <c r="C155" s="33"/>
+      <c r="C155" s="30"/>
       <c r="D155" s="13"/>
       <c r="E155" s="13"/>
       <c r="F155" s="13"/>
       <c r="G155" s="13"/>
       <c r="H155" s="13"/>
-      <c r="I155" s="36"/>
+      <c r="I155" s="33"/>
     </row>
     <row r="156" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="27"/>
       <c r="B156" s="30"/>
-      <c r="C156" s="33"/>
+      <c r="C156" s="30"/>
       <c r="D156" s="13"/>
       <c r="E156" s="13"/>
       <c r="F156" s="13"/>
       <c r="G156" s="13"/>
       <c r="H156" s="13"/>
-      <c r="I156" s="36"/>
+      <c r="I156" s="33"/>
     </row>
     <row r="157" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="27"/>
       <c r="B157" s="30"/>
-      <c r="C157" s="33"/>
+      <c r="C157" s="30"/>
       <c r="D157" s="13"/>
       <c r="E157" s="13"/>
       <c r="F157" s="13"/>
       <c r="G157" s="13"/>
       <c r="H157" s="13"/>
-      <c r="I157" s="36"/>
+      <c r="I157" s="33"/>
     </row>
     <row r="158" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="27"/>
       <c r="B158" s="30"/>
-      <c r="C158" s="33"/>
+      <c r="C158" s="30"/>
       <c r="D158" s="13"/>
       <c r="E158" s="13"/>
       <c r="F158" s="13"/>
       <c r="G158" s="13"/>
       <c r="H158" s="13"/>
-      <c r="I158" s="36"/>
+      <c r="I158" s="33"/>
     </row>
     <row r="159" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="27"/>
       <c r="B159" s="30"/>
-      <c r="C159" s="33"/>
+      <c r="C159" s="30"/>
       <c r="D159" s="13"/>
       <c r="E159" s="13"/>
       <c r="F159" s="13"/>
       <c r="G159" s="13"/>
       <c r="H159" s="13"/>
-      <c r="I159" s="36"/>
+      <c r="I159" s="33"/>
     </row>
     <row r="160" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="27"/>
       <c r="B160" s="30"/>
-      <c r="C160" s="33"/>
+      <c r="C160" s="30"/>
       <c r="D160" s="13"/>
       <c r="E160" s="13"/>
       <c r="F160" s="13"/>
       <c r="G160" s="13"/>
       <c r="H160" s="13"/>
-      <c r="I160" s="36"/>
+      <c r="I160" s="33"/>
     </row>
     <row r="161" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="27"/>
       <c r="B161" s="30"/>
-      <c r="C161" s="33"/>
+      <c r="C161" s="30"/>
       <c r="D161" s="13"/>
       <c r="E161" s="13"/>
       <c r="F161" s="13"/>
       <c r="G161" s="13"/>
       <c r="H161" s="13"/>
-      <c r="I161" s="36"/>
+      <c r="I161" s="33"/>
     </row>
     <row r="162" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="27"/>
       <c r="B162" s="30"/>
-      <c r="C162" s="33"/>
+      <c r="C162" s="30"/>
       <c r="D162" s="13"/>
       <c r="E162" s="13"/>
       <c r="F162" s="13"/>
       <c r="G162" s="13"/>
       <c r="H162" s="13"/>
-      <c r="I162" s="36"/>
+      <c r="I162" s="33"/>
     </row>
     <row r="163" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="27"/>
       <c r="B163" s="30"/>
-      <c r="C163" s="33"/>
+      <c r="C163" s="30"/>
       <c r="D163" s="13"/>
       <c r="E163" s="13"/>
       <c r="F163" s="13"/>
       <c r="G163" s="13"/>
       <c r="H163" s="13"/>
-      <c r="I163" s="36"/>
+      <c r="I163" s="33"/>
     </row>
     <row r="164" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="27"/>
       <c r="B164" s="30"/>
-      <c r="C164" s="33"/>
+      <c r="C164" s="30"/>
       <c r="D164" s="13"/>
       <c r="E164" s="13"/>
       <c r="F164" s="13"/>
       <c r="G164" s="13"/>
       <c r="H164" s="13"/>
-      <c r="I164" s="36"/>
+      <c r="I164" s="33"/>
     </row>
     <row r="165" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="27"/>
       <c r="B165" s="30"/>
-      <c r="C165" s="33"/>
+      <c r="C165" s="30"/>
       <c r="D165" s="13"/>
       <c r="E165" s="13"/>
       <c r="F165" s="13"/>
       <c r="G165" s="13"/>
       <c r="H165" s="13"/>
-      <c r="I165" s="36"/>
+      <c r="I165" s="33"/>
     </row>
     <row r="166" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="27"/>
       <c r="B166" s="30"/>
-      <c r="C166" s="33"/>
+      <c r="C166" s="30"/>
       <c r="D166" s="13"/>
       <c r="E166" s="13"/>
       <c r="F166" s="13"/>
       <c r="G166" s="13"/>
       <c r="H166" s="13"/>
-      <c r="I166" s="36"/>
+      <c r="I166" s="33"/>
     </row>
     <row r="167" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="27"/>
       <c r="B167" s="30"/>
-      <c r="C167" s="33"/>
+      <c r="C167" s="30"/>
       <c r="D167" s="13"/>
       <c r="E167" s="13"/>
       <c r="F167" s="13"/>
       <c r="G167" s="13"/>
       <c r="H167" s="13"/>
-      <c r="I167" s="36"/>
+      <c r="I167" s="33"/>
     </row>
     <row r="168" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="27"/>
       <c r="B168" s="30"/>
-      <c r="C168" s="33"/>
+      <c r="C168" s="30"/>
       <c r="D168" s="13"/>
       <c r="E168" s="13"/>
       <c r="F168" s="13"/>
       <c r="G168" s="13"/>
       <c r="H168" s="13"/>
-      <c r="I168" s="36"/>
+      <c r="I168" s="33"/>
     </row>
     <row r="169" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="27"/>
       <c r="B169" s="30"/>
-      <c r="C169" s="33"/>
+      <c r="C169" s="30"/>
       <c r="D169" s="13"/>
       <c r="E169" s="13"/>
       <c r="F169" s="13"/>
       <c r="G169" s="13"/>
       <c r="H169" s="13"/>
-      <c r="I169" s="36"/>
+      <c r="I169" s="33"/>
     </row>
     <row r="170" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="27"/>
       <c r="B170" s="30"/>
-      <c r="C170" s="33"/>
+      <c r="C170" s="30"/>
       <c r="D170" s="13"/>
       <c r="E170" s="13"/>
       <c r="F170" s="13"/>
       <c r="G170" s="13"/>
       <c r="H170" s="13"/>
-      <c r="I170" s="36"/>
+      <c r="I170" s="33"/>
     </row>
     <row r="171" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="27"/>
       <c r="B171" s="30"/>
-      <c r="C171" s="33"/>
+      <c r="C171" s="30"/>
       <c r="D171" s="13"/>
       <c r="E171" s="13"/>
       <c r="F171" s="13"/>
       <c r="G171" s="13"/>
       <c r="H171" s="13"/>
-      <c r="I171" s="36"/>
+      <c r="I171" s="33"/>
     </row>
     <row r="172" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="27"/>
       <c r="B172" s="30"/>
-      <c r="C172" s="33"/>
+      <c r="C172" s="30"/>
       <c r="D172" s="13"/>
       <c r="E172" s="13"/>
       <c r="F172" s="13"/>
       <c r="G172" s="13"/>
       <c r="H172" s="13"/>
-      <c r="I172" s="36"/>
+      <c r="I172" s="33"/>
     </row>
     <row r="173" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="27"/>
       <c r="B173" s="30"/>
-      <c r="C173" s="33"/>
+      <c r="C173" s="30"/>
       <c r="D173" s="13"/>
       <c r="E173" s="13"/>
       <c r="F173" s="13"/>
       <c r="G173" s="13"/>
       <c r="H173" s="13"/>
-      <c r="I173" s="36"/>
+      <c r="I173" s="33"/>
     </row>
     <row r="174" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="27"/>
       <c r="B174" s="30"/>
-      <c r="C174" s="33"/>
+      <c r="C174" s="30"/>
       <c r="D174" s="13"/>
       <c r="E174" s="13"/>
       <c r="F174" s="13"/>
       <c r="G174" s="13"/>
       <c r="H174" s="13"/>
-      <c r="I174" s="36"/>
+      <c r="I174" s="33"/>
     </row>
     <row r="175" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="27"/>
       <c r="B175" s="30"/>
-      <c r="C175" s="33"/>
+      <c r="C175" s="30"/>
       <c r="D175" s="13"/>
       <c r="E175" s="13"/>
       <c r="F175" s="13"/>
       <c r="G175" s="13"/>
       <c r="H175" s="13"/>
-      <c r="I175" s="36"/>
+      <c r="I175" s="33"/>
     </row>
     <row r="176" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="27"/>
       <c r="B176" s="30"/>
-      <c r="C176" s="33"/>
+      <c r="C176" s="30"/>
       <c r="D176" s="13"/>
       <c r="E176" s="13"/>
       <c r="F176" s="13"/>
       <c r="G176" s="13"/>
       <c r="H176" s="13"/>
-      <c r="I176" s="36"/>
+      <c r="I176" s="33"/>
     </row>
     <row r="177" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="27"/>
       <c r="B177" s="30"/>
-      <c r="C177" s="33"/>
+      <c r="C177" s="30"/>
       <c r="D177" s="13"/>
       <c r="E177" s="13"/>
       <c r="F177" s="13"/>
       <c r="G177" s="13"/>
       <c r="H177" s="13"/>
-      <c r="I177" s="36"/>
+      <c r="I177" s="33"/>
     </row>
     <row r="178" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="27"/>
       <c r="B178" s="30"/>
-      <c r="C178" s="33"/>
+      <c r="C178" s="30"/>
       <c r="D178" s="13"/>
       <c r="E178" s="13"/>
       <c r="F178" s="13"/>
       <c r="G178" s="13"/>
       <c r="H178" s="13"/>
-      <c r="I178" s="36"/>
+      <c r="I178" s="33"/>
     </row>
     <row r="179" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="27"/>
       <c r="B179" s="30"/>
-      <c r="C179" s="33"/>
+      <c r="C179" s="30"/>
       <c r="D179" s="13"/>
       <c r="E179" s="13"/>
       <c r="F179" s="13"/>
       <c r="G179" s="13"/>
       <c r="H179" s="13"/>
-      <c r="I179" s="36"/>
+      <c r="I179" s="33"/>
     </row>
     <row r="180" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="27"/>
       <c r="B180" s="30"/>
-      <c r="C180" s="33"/>
+      <c r="C180" s="30"/>
       <c r="D180" s="13"/>
       <c r="E180" s="13"/>
       <c r="F180" s="13"/>
       <c r="G180" s="13"/>
       <c r="H180" s="13"/>
-      <c r="I180" s="36"/>
+      <c r="I180" s="33"/>
     </row>
     <row r="181" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="27"/>
       <c r="B181" s="30"/>
-      <c r="C181" s="33"/>
+      <c r="C181" s="30"/>
       <c r="D181" s="13"/>
       <c r="E181" s="13"/>
       <c r="F181" s="13"/>
       <c r="G181" s="13"/>
       <c r="H181" s="13"/>
-      <c r="I181" s="36"/>
+      <c r="I181" s="33"/>
     </row>
     <row r="182" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="27"/>
       <c r="B182" s="30"/>
-      <c r="C182" s="33"/>
+      <c r="C182" s="30"/>
       <c r="D182" s="13"/>
       <c r="E182" s="13"/>
       <c r="F182" s="13"/>
       <c r="G182" s="13"/>
       <c r="H182" s="13"/>
-      <c r="I182" s="36"/>
+      <c r="I182" s="33"/>
     </row>
     <row r="183" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="27"/>
       <c r="B183" s="30"/>
-      <c r="C183" s="33"/>
+      <c r="C183" s="30"/>
       <c r="D183" s="13"/>
       <c r="E183" s="13"/>
       <c r="F183" s="13"/>
       <c r="G183" s="13"/>
       <c r="H183" s="13"/>
-      <c r="I183" s="36"/>
+      <c r="I183" s="33"/>
     </row>
     <row r="184" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="27"/>
       <c r="B184" s="30"/>
-      <c r="C184" s="33"/>
+      <c r="C184" s="30"/>
       <c r="D184" s="13"/>
       <c r="E184" s="13"/>
       <c r="F184" s="13"/>
       <c r="G184" s="13"/>
       <c r="H184" s="13"/>
-      <c r="I184" s="36"/>
+      <c r="I184" s="33"/>
     </row>
     <row r="185" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="27"/>
       <c r="B185" s="30"/>
-      <c r="C185" s="33"/>
+      <c r="C185" s="30"/>
       <c r="D185" s="13"/>
       <c r="E185" s="13"/>
       <c r="F185" s="13"/>
       <c r="G185" s="13"/>
       <c r="H185" s="13"/>
-      <c r="I185" s="36"/>
+      <c r="I185" s="33"/>
     </row>
     <row r="186" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="27"/>
       <c r="B186" s="30"/>
-      <c r="C186" s="33"/>
+      <c r="C186" s="30"/>
       <c r="D186" s="13"/>
       <c r="E186" s="13"/>
       <c r="F186" s="13"/>
       <c r="G186" s="13"/>
       <c r="H186" s="13"/>
-      <c r="I186" s="36"/>
+      <c r="I186" s="33"/>
     </row>
     <row r="187" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="27"/>
       <c r="B187" s="30"/>
-      <c r="C187" s="33"/>
+      <c r="C187" s="30"/>
       <c r="D187" s="13"/>
       <c r="E187" s="13"/>
       <c r="F187" s="13"/>
       <c r="G187" s="13"/>
       <c r="H187" s="13"/>
-      <c r="I187" s="36"/>
+      <c r="I187" s="33"/>
     </row>
     <row r="188" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="27"/>
       <c r="B188" s="30"/>
-      <c r="C188" s="33"/>
+      <c r="C188" s="30"/>
       <c r="D188" s="13"/>
       <c r="E188" s="13"/>
       <c r="F188" s="13"/>
       <c r="G188" s="13"/>
       <c r="H188" s="13"/>
-      <c r="I188" s="36"/>
+      <c r="I188" s="33"/>
     </row>
     <row r="189" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="27"/>
       <c r="B189" s="30"/>
-      <c r="C189" s="33"/>
+      <c r="C189" s="30"/>
       <c r="D189" s="13"/>
       <c r="E189" s="13"/>
       <c r="F189" s="13"/>
       <c r="G189" s="13"/>
       <c r="H189" s="13"/>
-      <c r="I189" s="36"/>
+      <c r="I189" s="33"/>
     </row>
     <row r="190" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="27"/>
       <c r="B190" s="30"/>
-      <c r="C190" s="33"/>
+      <c r="C190" s="30"/>
       <c r="D190" s="13"/>
       <c r="E190" s="13"/>
       <c r="F190" s="13"/>
       <c r="G190" s="13"/>
       <c r="H190" s="13"/>
-      <c r="I190" s="36"/>
+      <c r="I190" s="33"/>
     </row>
     <row r="191" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="27"/>
       <c r="B191" s="30"/>
-      <c r="C191" s="33"/>
+      <c r="C191" s="30"/>
       <c r="D191" s="13"/>
       <c r="E191" s="13"/>
       <c r="F191" s="13"/>
       <c r="G191" s="13"/>
       <c r="H191" s="13"/>
-      <c r="I191" s="36"/>
+      <c r="I191" s="33"/>
     </row>
     <row r="192" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="27"/>
       <c r="B192" s="30"/>
-      <c r="C192" s="33"/>
+      <c r="C192" s="30"/>
       <c r="D192" s="13"/>
       <c r="E192" s="13"/>
       <c r="F192" s="13"/>
       <c r="G192" s="13"/>
       <c r="H192" s="13"/>
-      <c r="I192" s="36"/>
+      <c r="I192" s="33"/>
     </row>
     <row r="193" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="27"/>
       <c r="B193" s="30"/>
-      <c r="C193" s="33"/>
+      <c r="C193" s="30"/>
       <c r="D193" s="13"/>
       <c r="E193" s="13"/>
       <c r="F193" s="13"/>
       <c r="G193" s="13"/>
       <c r="H193" s="13"/>
-      <c r="I193" s="36"/>
+      <c r="I193" s="33"/>
     </row>
     <row r="194" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="27"/>
       <c r="B194" s="30"/>
-      <c r="C194" s="33"/>
+      <c r="C194" s="30"/>
       <c r="D194" s="13"/>
       <c r="E194" s="13"/>
       <c r="F194" s="13"/>
       <c r="G194" s="13"/>
       <c r="H194" s="13"/>
-      <c r="I194" s="36"/>
+      <c r="I194" s="33"/>
     </row>
     <row r="195" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="27"/>
       <c r="B195" s="30"/>
-      <c r="C195" s="33"/>
+      <c r="C195" s="30"/>
       <c r="D195" s="13"/>
       <c r="E195" s="13"/>
       <c r="F195" s="13"/>
       <c r="G195" s="13"/>
       <c r="H195" s="13"/>
-      <c r="I195" s="36"/>
+      <c r="I195" s="33"/>
     </row>
     <row r="196" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="27"/>
       <c r="B196" s="30"/>
-      <c r="C196" s="33"/>
+      <c r="C196" s="30"/>
       <c r="D196" s="13"/>
       <c r="E196" s="13"/>
       <c r="F196" s="13"/>
       <c r="G196" s="13"/>
       <c r="H196" s="13"/>
-      <c r="I196" s="36"/>
+      <c r="I196" s="33"/>
+    </row>
+    <row r="197" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A197" s="27"/>
+      <c r="B197" s="30"/>
+      <c r="C197" s="30"/>
+      <c r="D197" s="13"/>
+      <c r="E197" s="13"/>
+      <c r="F197" s="13"/>
+      <c r="G197" s="13"/>
+      <c r="H197" s="13"/>
+      <c r="I197" s="33"/>
+    </row>
+    <row r="198" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A198" s="27"/>
+      <c r="B198" s="30"/>
+      <c r="C198" s="30"/>
+      <c r="D198" s="13"/>
+      <c r="E198" s="13"/>
+      <c r="F198" s="13"/>
+      <c r="G198" s="13"/>
+      <c r="H198" s="13"/>
+      <c r="I198" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="A107:I107"/>
-    <mergeCell ref="A109:I109"/>
-    <mergeCell ref="A111:I111"/>
-    <mergeCell ref="A104:I104"/>
+  <mergeCells count="20">
+    <mergeCell ref="A113:I113"/>
+    <mergeCell ref="A106:I106"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A17:I17"/>
     <mergeCell ref="A29:I29"/>
     <mergeCell ref="A38:I38"/>
-    <mergeCell ref="A80:I80"/>
-    <mergeCell ref="A54:I54"/>
-    <mergeCell ref="A61:I61"/>
-    <mergeCell ref="A66:I66"/>
-    <mergeCell ref="A94:I94"/>
-    <mergeCell ref="A96:I96"/>
-    <mergeCell ref="A81:I81"/>
-    <mergeCell ref="A99:I99"/>
+    <mergeCell ref="A82:I82"/>
+    <mergeCell ref="A55:I55"/>
+    <mergeCell ref="A62:I62"/>
+    <mergeCell ref="A68:I68"/>
+    <mergeCell ref="A122:I122"/>
+    <mergeCell ref="A124:I124"/>
+    <mergeCell ref="A83:I83"/>
     <mergeCell ref="A100:I100"/>
-    <mergeCell ref="A87:I87"/>
+    <mergeCell ref="A101:I101"/>
+    <mergeCell ref="A102:I102"/>
+    <mergeCell ref="A117:I117"/>
+    <mergeCell ref="A109:I109"/>
+    <mergeCell ref="A111:I111"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Done checklist, ready for 6pm
</commit_message>
<xml_diff>
--- a/Middle Assignment/TestDesignTechique1_PhamHongAnh.xlsx
+++ b/Middle Assignment/TestDesignTechique1_PhamHongAnh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NashTech\Rookies\NashTech_Homework\Middle Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F211A0-F8CC-4C66-9A19-982B7E54F47B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE65E6A9-0CE3-4A13-A575-6A34BED6C8E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -851,7 +851,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="223">
   <si>
     <t>ID</t>
   </si>
@@ -1483,9 +1483,6 @@
     <t>Check all drop down values</t>
   </si>
   <si>
-    <t>Check boundary value của phone number (Done)</t>
-  </si>
-  <si>
     <t>3.  Test flow</t>
   </si>
   <si>
@@ -1513,10 +1510,37 @@
     <t>When clicking on the "Sign up with email" button</t>
   </si>
   <si>
-    <t>Thêm decision table (Done)</t>
-  </si>
-  <si>
-    <t>Chuyển vào từng field tương ứng (Done)</t>
+    <t>Check drop down values of the Month field</t>
+  </si>
+  <si>
+    <t>Check drop down values of the Day field</t>
+  </si>
+  <si>
+    <t>Check drop down values of the Year field</t>
+  </si>
+  <si>
+    <t>When selecting a month only</t>
+  </si>
+  <si>
+    <t>When selecting a day only</t>
+  </si>
+  <si>
+    <t>When selecting a year only</t>
+  </si>
+  <si>
+    <t>When selecting a month and a day only</t>
+  </si>
+  <si>
+    <t>When selecting a month and a year only</t>
+  </si>
+  <si>
+    <t>When selecting a day and a year only</t>
+  </si>
+  <si>
+    <t>Check default - The checkbox is unchecked</t>
+  </si>
+  <si>
+    <t>When clicking on the checkbox</t>
   </si>
 </sst>
 </file>
@@ -1846,6 +1870,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1872,13 +1899,13 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1889,9 +1916,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2173,17 +2197,17 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -2203,17 +2227,17 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -2602,17 +2626,17 @@
       <c r="Z13" s="2"/>
     </row>
     <row r="14" spans="1:26" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="40" t="s">
+      <c r="A14" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="41"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -3000,17 +3024,17 @@
       <c r="Z24" s="2"/>
     </row>
     <row r="25" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="42" t="s">
+      <c r="A25" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="44"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="45"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
@@ -3102,17 +3126,17 @@
       <c r="Z27" s="2"/>
     </row>
     <row r="28" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="44"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="45"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
@@ -3205,17 +3229,17 @@
       <c r="Z30" s="2"/>
     </row>
     <row r="31" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="38" t="s">
+      <c r="A31" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="39"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="39"/>
-      <c r="I31" s="39"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -3235,17 +3259,17 @@
       <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="37"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="38"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
@@ -3439,17 +3463,17 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="35" t="s">
+      <c r="A42" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="37"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="37"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="37"/>
+      <c r="G42" s="37"/>
+      <c r="H42" s="37"/>
+      <c r="I42" s="38"/>
     </row>
     <row r="43" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
@@ -14416,10 +14440,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{861DB058-9ABC-4928-81FB-0309C7B8DB85}">
-  <dimension ref="A1:Z198"/>
+  <dimension ref="A1:Z206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -14482,17 +14506,17 @@
       <c r="Z1" s="26"/>
     </row>
     <row r="2" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="39" t="s">
         <v>166</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
       <c r="J2" s="26"/>
       <c r="K2" s="26"/>
       <c r="L2" s="26"/>
@@ -14512,7 +14536,7 @@
       <c r="Z2" s="26"/>
     </row>
     <row r="3" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="41" t="s">
         <v>198</v>
       </c>
       <c r="B3" s="47"/>
@@ -14548,9 +14572,7 @@
       <c r="B4" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="C4" s="33" t="s">
-        <v>203</v>
-      </c>
+      <c r="C4" s="33"/>
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
@@ -14624,7 +14646,7 @@
     </row>
     <row r="9" spans="1:26" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27">
-        <f t="shared" ref="A9:A81" ca="1" si="0">IF(OFFSET(A9,-1,0) ="",OFFSET(A9,-2,0)+1,OFFSET(A9,-1,0)+1 )</f>
+        <f t="shared" ref="A9:A89" ca="1" si="0">IF(OFFSET(A9,-1,0) ="",OFFSET(A9,-2,0)+1,OFFSET(A9,-1,0)+1 )</f>
         <v>6</v>
       </c>
       <c r="B9" s="30" t="s">
@@ -14918,7 +14940,7 @@
       <c r="B26" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="C26" s="51"/>
+      <c r="C26" s="35"/>
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
@@ -14934,9 +14956,7 @@
       <c r="B27" s="30" t="s">
         <v>183</v>
       </c>
-      <c r="C27" s="29" t="s">
-        <v>214</v>
-      </c>
+      <c r="C27" s="29"/>
       <c r="D27" s="30"/>
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
@@ -14952,7 +14972,7 @@
       <c r="B28" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="C28" s="51"/>
+      <c r="C28" s="35"/>
       <c r="E28" s="13"/>
       <c r="F28" s="13"/>
       <c r="G28" s="13"/>
@@ -14997,7 +15017,7 @@
       <c r="B30" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="C30" s="51"/>
+      <c r="C30" s="35"/>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
       <c r="G30" s="13"/>
@@ -15012,7 +15032,7 @@
       <c r="B31" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="C31" s="51"/>
+      <c r="C31" s="35"/>
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
       <c r="G31" s="13"/>
@@ -15027,7 +15047,7 @@
       <c r="B32" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="C32" s="51"/>
+      <c r="C32" s="35"/>
       <c r="E32" s="13"/>
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
@@ -15042,7 +15062,7 @@
       <c r="B33" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="C33" s="51"/>
+      <c r="C33" s="35"/>
       <c r="E33" s="13"/>
       <c r="F33" s="13"/>
       <c r="G33" s="13"/>
@@ -15057,7 +15077,7 @@
       <c r="B34" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C34" s="51"/>
+      <c r="C34" s="35"/>
       <c r="E34" s="13"/>
       <c r="F34" s="13"/>
       <c r="G34" s="13"/>
@@ -15072,7 +15092,7 @@
       <c r="B35" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="C35" s="51"/>
+      <c r="C35" s="35"/>
       <c r="E35" s="13"/>
       <c r="F35" s="13"/>
       <c r="G35" s="13"/>
@@ -15087,7 +15107,7 @@
       <c r="B36" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="C36" s="51"/>
+      <c r="C36" s="35"/>
       <c r="E36" s="13"/>
       <c r="F36" s="13"/>
       <c r="G36" s="13"/>
@@ -15102,7 +15122,7 @@
       <c r="B37" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="C37" s="51"/>
+      <c r="C37" s="35"/>
       <c r="E37" s="13"/>
       <c r="F37" s="13"/>
       <c r="G37" s="13"/>
@@ -15147,9 +15167,7 @@
       <c r="B39" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="C39" s="29" t="s">
-        <v>213</v>
-      </c>
+      <c r="C39" s="29"/>
       <c r="D39" s="13"/>
       <c r="E39" s="13"/>
       <c r="F39" s="13"/>
@@ -15291,7 +15309,7 @@
         <v>42</v>
       </c>
       <c r="B48" s="29" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C48" s="30"/>
       <c r="D48" s="13"/>
@@ -15307,7 +15325,7 @@
         <v>43</v>
       </c>
       <c r="B49" s="29" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C49" s="30"/>
       <c r="D49" s="13"/>
@@ -15323,7 +15341,7 @@
         <v>44</v>
       </c>
       <c r="B50" s="29" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C50" s="30"/>
       <c r="D50" s="13"/>
@@ -15339,7 +15357,7 @@
         <v>45</v>
       </c>
       <c r="B51" s="29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C51" s="30"/>
       <c r="D51" s="13"/>
@@ -15373,9 +15391,7 @@
       <c r="B53" s="30" t="s">
         <v>185</v>
       </c>
-      <c r="C53" s="29" t="s">
-        <v>214</v>
-      </c>
+      <c r="C53" s="29"/>
       <c r="D53" s="13"/>
       <c r="E53" s="13"/>
       <c r="F53" s="13"/>
@@ -15420,14 +15436,14 @@
       <c r="B56" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="C56" s="51"/>
+      <c r="C56" s="35"/>
       <c r="E56" s="13"/>
       <c r="F56" s="13"/>
       <c r="G56" s="13"/>
       <c r="H56" s="13"/>
       <c r="I56" s="33"/>
     </row>
-    <row r="57" spans="1:9" s="10" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>50</v>
@@ -15443,13 +15459,13 @@
       <c r="H57" s="13"/>
       <c r="I57" s="33"/>
     </row>
-    <row r="58" spans="1:9" s="10" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>51</v>
       </c>
       <c r="B58" s="30" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="C58" s="30"/>
       <c r="D58" s="13"/>
@@ -15459,13 +15475,13 @@
       <c r="H58" s="13"/>
       <c r="I58" s="33"/>
     </row>
-    <row r="59" spans="1:9" s="10" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" s="10" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>52</v>
       </c>
       <c r="B59" s="30" t="s">
-        <v>149</v>
+        <v>213</v>
       </c>
       <c r="C59" s="30"/>
       <c r="D59" s="13"/>
@@ -15475,13 +15491,13 @@
       <c r="H59" s="13"/>
       <c r="I59" s="33"/>
     </row>
-    <row r="60" spans="1:9" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" s="10" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>53</v>
       </c>
       <c r="B60" s="30" t="s">
-        <v>150</v>
+        <v>214</v>
       </c>
       <c r="C60" s="30"/>
       <c r="D60" s="13"/>
@@ -15491,13 +15507,13 @@
       <c r="H60" s="13"/>
       <c r="I60" s="33"/>
     </row>
-    <row r="61" spans="1:9" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" s="10" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>54</v>
       </c>
       <c r="B61" s="30" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C61" s="30"/>
       <c r="D61" s="13"/>
@@ -15507,26 +15523,29 @@
       <c r="H61" s="13"/>
       <c r="I61" s="33"/>
     </row>
-    <row r="62" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="46" t="s">
-        <v>154</v>
-      </c>
-      <c r="B62" s="47"/>
-      <c r="C62" s="47"/>
-      <c r="D62" s="47"/>
-      <c r="E62" s="47"/>
-      <c r="F62" s="47"/>
-      <c r="G62" s="47"/>
-      <c r="H62" s="47"/>
-      <c r="I62" s="47"/>
-    </row>
-    <row r="63" spans="1:9" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B62" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="C62" s="30"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="13"/>
+      <c r="F62" s="13"/>
+      <c r="G62" s="13"/>
+      <c r="H62" s="13"/>
+      <c r="I62" s="33"/>
+    </row>
+    <row r="63" spans="1:9" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="27">
-        <f ca="1">IF(OFFSET(A63,-2,0) ="",OFFSET(A63,-2,0)+1,OFFSET(A63,-2,0)+1 )</f>
-        <v>55</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>56</v>
       </c>
       <c r="B63" s="30" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="C63" s="30"/>
       <c r="D63" s="13"/>
@@ -15536,13 +15555,13 @@
       <c r="H63" s="13"/>
       <c r="I63" s="33"/>
     </row>
-    <row r="64" spans="1:9" s="10" customFormat="1" ht="25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B64" s="30" t="s">
-        <v>148</v>
+        <v>215</v>
       </c>
       <c r="C64" s="30"/>
       <c r="D64" s="13"/>
@@ -15552,13 +15571,13 @@
       <c r="H64" s="13"/>
       <c r="I64" s="33"/>
     </row>
-    <row r="65" spans="1:9" s="10" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B65" s="30" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="C65" s="30"/>
       <c r="D65" s="13"/>
@@ -15568,13 +15587,13 @@
       <c r="H65" s="13"/>
       <c r="I65" s="33"/>
     </row>
-    <row r="66" spans="1:9" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B66" s="30" t="s">
-        <v>152</v>
+        <v>217</v>
       </c>
       <c r="C66" s="30"/>
       <c r="D66" s="13"/>
@@ -15584,13 +15603,13 @@
       <c r="H66" s="13"/>
       <c r="I66" s="33"/>
     </row>
-    <row r="67" spans="1:9" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B67" s="30" t="s">
-        <v>153</v>
+        <v>218</v>
       </c>
       <c r="C67" s="30"/>
       <c r="D67" s="13"/>
@@ -15600,72 +15619,74 @@
       <c r="H67" s="13"/>
       <c r="I67" s="33"/>
     </row>
-    <row r="68" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="46" t="s">
-        <v>155</v>
-      </c>
-      <c r="B68" s="47"/>
-      <c r="C68" s="47"/>
-      <c r="D68" s="47"/>
-      <c r="E68" s="47"/>
-      <c r="F68" s="47"/>
-      <c r="G68" s="47"/>
-      <c r="H68" s="47"/>
-      <c r="I68" s="47"/>
-    </row>
-    <row r="69" spans="1:9" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="B68" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="C68" s="30"/>
+      <c r="D68" s="13"/>
+      <c r="E68" s="13"/>
+      <c r="F68" s="13"/>
+      <c r="G68" s="13"/>
+      <c r="H68" s="13"/>
+      <c r="I68" s="33"/>
+    </row>
+    <row r="69" spans="1:9" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="27">
-        <f ca="1">IF(OFFSET(A69,-2,0) ="",OFFSET(A69,-2,0)+1,OFFSET(A69,-2,0)+1 )</f>
-        <v>60</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>62</v>
       </c>
       <c r="B69" s="30" t="s">
-        <v>146</v>
+        <v>220</v>
       </c>
       <c r="C69" s="30"/>
+      <c r="D69" s="13"/>
       <c r="E69" s="13"/>
       <c r="F69" s="13"/>
       <c r="G69" s="13"/>
       <c r="H69" s="13"/>
       <c r="I69" s="33"/>
     </row>
-    <row r="70" spans="1:9" s="10" customFormat="1" ht="25" x14ac:dyDescent="0.25">
-      <c r="A70" s="27">
-        <f t="shared" ca="1" si="0"/>
-        <v>61</v>
-      </c>
-      <c r="B70" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="C70" s="30"/>
-      <c r="E70" s="13"/>
-      <c r="F70" s="13"/>
-      <c r="G70" s="13"/>
-      <c r="H70" s="13"/>
-      <c r="I70" s="33"/>
-    </row>
-    <row r="71" spans="1:9" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="46" t="s">
+        <v>154</v>
+      </c>
+      <c r="B70" s="47"/>
+      <c r="C70" s="47"/>
+      <c r="D70" s="47"/>
+      <c r="E70" s="47"/>
+      <c r="F70" s="47"/>
+      <c r="G70" s="47"/>
+      <c r="H70" s="47"/>
+      <c r="I70" s="47"/>
+    </row>
+    <row r="71" spans="1:9" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="27">
-        <f t="shared" ca="1" si="0"/>
-        <v>62</v>
-      </c>
-      <c r="B71" s="29" t="s">
-        <v>156</v>
+        <f ca="1">IF(OFFSET(A71,-2,0) ="",OFFSET(A71,-2,0)+1,OFFSET(A71,-2,0)+1 )</f>
+        <v>63</v>
+      </c>
+      <c r="B71" s="30" t="s">
+        <v>146</v>
       </c>
       <c r="C71" s="30"/>
-      <c r="D71" s="30"/>
+      <c r="D71" s="13"/>
       <c r="E71" s="13"/>
       <c r="F71" s="13"/>
       <c r="G71" s="13"/>
       <c r="H71" s="13"/>
       <c r="I71" s="33"/>
     </row>
-    <row r="72" spans="1:9" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
-      </c>
-      <c r="B72" s="29" t="s">
-        <v>158</v>
+        <v>64</v>
+      </c>
+      <c r="B72" s="30" t="s">
+        <v>148</v>
       </c>
       <c r="C72" s="30"/>
       <c r="D72" s="13"/>
@@ -15675,13 +15696,13 @@
       <c r="H72" s="13"/>
       <c r="I72" s="33"/>
     </row>
-    <row r="73" spans="1:9" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" s="10" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="B73" s="29" t="s">
-        <v>157</v>
+        <v>65</v>
+      </c>
+      <c r="B73" s="30" t="s">
+        <v>202</v>
       </c>
       <c r="C73" s="30"/>
       <c r="D73" s="13"/>
@@ -15691,13 +15712,13 @@
       <c r="H73" s="13"/>
       <c r="I73" s="33"/>
     </row>
-    <row r="74" spans="1:9" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>65</v>
-      </c>
-      <c r="B74" s="29" t="s">
-        <v>129</v>
+        <v>66</v>
+      </c>
+      <c r="B74" s="30" t="s">
+        <v>152</v>
       </c>
       <c r="C74" s="30"/>
       <c r="D74" s="13"/>
@@ -15707,13 +15728,13 @@
       <c r="H74" s="13"/>
       <c r="I74" s="33"/>
     </row>
-    <row r="75" spans="1:9" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="27">
         <f t="shared" ca="1" si="0"/>
-        <v>66</v>
-      </c>
-      <c r="B75" s="29" t="s">
-        <v>142</v>
+        <v>67</v>
+      </c>
+      <c r="B75" s="30" t="s">
+        <v>153</v>
       </c>
       <c r="C75" s="30"/>
       <c r="D75" s="13"/>
@@ -15723,95 +15744,88 @@
       <c r="H75" s="13"/>
       <c r="I75" s="33"/>
     </row>
-    <row r="76" spans="1:9" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="27">
-        <f t="shared" ca="1" si="0"/>
-        <v>67</v>
-      </c>
-      <c r="B76" s="29" t="s">
-        <v>143</v>
-      </c>
-      <c r="C76" s="30"/>
-      <c r="D76" s="13"/>
-      <c r="E76" s="13"/>
-      <c r="F76" s="13"/>
-      <c r="G76" s="13"/>
-      <c r="H76" s="13"/>
-      <c r="I76" s="33"/>
-    </row>
-    <row r="77" spans="1:9" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="46" t="s">
+        <v>155</v>
+      </c>
+      <c r="B76" s="47"/>
+      <c r="C76" s="47"/>
+      <c r="D76" s="47"/>
+      <c r="E76" s="47"/>
+      <c r="F76" s="47"/>
+      <c r="G76" s="47"/>
+      <c r="H76" s="47"/>
+      <c r="I76" s="47"/>
+    </row>
+    <row r="77" spans="1:9" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">IF(OFFSET(A77,-2,0) ="",OFFSET(A77,-2,0)+1,OFFSET(A77,-2,0)+1 )</f>
         <v>68</v>
       </c>
-      <c r="B77" s="29" t="s">
-        <v>126</v>
+      <c r="B77" s="30" t="s">
+        <v>146</v>
       </c>
       <c r="C77" s="30"/>
-      <c r="D77" s="13"/>
       <c r="E77" s="13"/>
       <c r="F77" s="13"/>
       <c r="G77" s="13"/>
       <c r="H77" s="13"/>
       <c r="I77" s="33"/>
     </row>
-    <row r="78" spans="1:9" s="10" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" s="10" customFormat="1" ht="25" x14ac:dyDescent="0.25">
       <c r="A78" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>69</v>
       </c>
       <c r="B78" s="30" t="s">
-        <v>159</v>
+        <v>134</v>
       </c>
       <c r="C78" s="30"/>
-      <c r="D78" s="13"/>
       <c r="E78" s="13"/>
       <c r="F78" s="13"/>
       <c r="G78" s="13"/>
       <c r="H78" s="13"/>
       <c r="I78" s="33"/>
     </row>
-    <row r="79" spans="1:9" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>70</v>
       </c>
-      <c r="B79" s="30" t="s">
-        <v>160</v>
+      <c r="B79" s="29" t="s">
+        <v>156</v>
       </c>
       <c r="C79" s="30"/>
-      <c r="D79" s="13"/>
+      <c r="D79" s="30"/>
       <c r="E79" s="13"/>
       <c r="F79" s="13"/>
       <c r="G79" s="13"/>
       <c r="H79" s="13"/>
       <c r="I79" s="33"/>
     </row>
-    <row r="80" spans="1:9" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="27">
-        <f ca="1">IF(OFFSET(A80,-1,0) ="",OFFSET(A80,-2,0)+1,OFFSET(A80,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="0"/>
         <v>71</v>
       </c>
-      <c r="B80" s="30" t="s">
-        <v>184</v>
-      </c>
-      <c r="C80" s="29" t="s">
-        <v>214</v>
-      </c>
-      <c r="D80" s="30"/>
+      <c r="B80" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="C80" s="30"/>
+      <c r="D80" s="13"/>
       <c r="E80" s="13"/>
       <c r="F80" s="13"/>
       <c r="G80" s="13"/>
       <c r="H80" s="13"/>
       <c r="I80" s="33"/>
     </row>
-    <row r="81" spans="1:9" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>72</v>
       </c>
-      <c r="B81" s="15" t="s">
-        <v>145</v>
+      <c r="B81" s="29" t="s">
+        <v>157</v>
       </c>
       <c r="C81" s="30"/>
       <c r="D81" s="13"/>
@@ -15821,39 +15835,45 @@
       <c r="H81" s="13"/>
       <c r="I81" s="33"/>
     </row>
-    <row r="82" spans="1:9" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="38" t="s">
-        <v>167</v>
-      </c>
-      <c r="B82" s="45"/>
-      <c r="C82" s="45"/>
-      <c r="D82" s="45"/>
-      <c r="E82" s="45"/>
-      <c r="F82" s="45"/>
-      <c r="G82" s="45"/>
-      <c r="H82" s="45"/>
-      <c r="I82" s="45"/>
-    </row>
-    <row r="83" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="46" t="s">
-        <v>174</v>
-      </c>
-      <c r="B83" s="47"/>
-      <c r="C83" s="47"/>
-      <c r="D83" s="47"/>
-      <c r="E83" s="47"/>
-      <c r="F83" s="47"/>
-      <c r="G83" s="47"/>
-      <c r="H83" s="47"/>
-      <c r="I83" s="47"/>
-    </row>
-    <row r="84" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="B82" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="C82" s="30"/>
+      <c r="D82" s="13"/>
+      <c r="E82" s="13"/>
+      <c r="F82" s="13"/>
+      <c r="G82" s="13"/>
+      <c r="H82" s="13"/>
+      <c r="I82" s="33"/>
+    </row>
+    <row r="83" spans="1:9" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="B83" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="C83" s="30"/>
+      <c r="D83" s="13"/>
+      <c r="E83" s="13"/>
+      <c r="F83" s="13"/>
+      <c r="G83" s="13"/>
+      <c r="H83" s="13"/>
+      <c r="I83" s="33"/>
+    </row>
+    <row r="84" spans="1:9" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="27">
-        <f ca="1">IF(OFFSET(A84,-3,0) ="",OFFSET(A84,-3,0)+1,OFFSET(A84,-3,0)+1 )</f>
-        <v>73</v>
-      </c>
-      <c r="B84" s="30" t="s">
-        <v>178</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="B84" s="29" t="s">
+        <v>143</v>
       </c>
       <c r="C84" s="30"/>
       <c r="D84" s="13"/>
@@ -15863,13 +15883,13 @@
       <c r="H84" s="13"/>
       <c r="I84" s="33"/>
     </row>
-    <row r="85" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="27">
-        <f t="shared" ref="A85:A87" ca="1" si="2">IF(OFFSET(A85,-1,0) ="",OFFSET(A85,-2,0)+1,OFFSET(A85,-1,0)+1 )</f>
-        <v>74</v>
-      </c>
-      <c r="B85" s="30" t="s">
-        <v>182</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="B85" s="29" t="s">
+        <v>126</v>
       </c>
       <c r="C85" s="30"/>
       <c r="D85" s="13"/>
@@ -15879,13 +15899,13 @@
       <c r="H85" s="13"/>
       <c r="I85" s="33"/>
     </row>
-    <row r="86" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" s="10" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="27">
-        <f t="shared" ca="1" si="2"/>
-        <v>75</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>77</v>
       </c>
       <c r="B86" s="30" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="C86" s="30"/>
       <c r="D86" s="13"/>
@@ -15895,47 +15915,45 @@
       <c r="H86" s="13"/>
       <c r="I86" s="33"/>
     </row>
-    <row r="87" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="27">
-        <f t="shared" ca="1" si="2"/>
-        <v>76</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>78</v>
       </c>
       <c r="B87" s="30" t="s">
-        <v>206</v>
-      </c>
-      <c r="C87" s="30" t="s">
-        <v>180</v>
-      </c>
-      <c r="D87" s="30"/>
+        <v>160</v>
+      </c>
+      <c r="C87" s="30"/>
+      <c r="D87" s="13"/>
       <c r="E87" s="13"/>
       <c r="F87" s="13"/>
       <c r="G87" s="13"/>
       <c r="H87" s="13"/>
       <c r="I87" s="33"/>
     </row>
-    <row r="88" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="27">
-        <f ca="1">IF(OFFSET(A88,-2,0) ="",OFFSET(A88,-2,0)+1,OFFSET(A88,-2,0)+1 )</f>
-        <v>76</v>
+        <f ca="1">IF(OFFSET(A88,-1,0) ="",OFFSET(A88,-2,0)+1,OFFSET(A88,-1,0)+1 )</f>
+        <v>79</v>
       </c>
       <c r="B88" s="30" t="s">
-        <v>193</v>
-      </c>
-      <c r="C88" s="30"/>
-      <c r="D88" s="13"/>
+        <v>184</v>
+      </c>
+      <c r="C88" s="29"/>
+      <c r="D88" s="30"/>
       <c r="E88" s="13"/>
       <c r="F88" s="13"/>
       <c r="G88" s="13"/>
       <c r="H88" s="13"/>
       <c r="I88" s="33"/>
     </row>
-    <row r="89" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="27">
-        <f ca="1">IF(OFFSET(A89,-2,0) ="",OFFSET(A89,-2,0)+1,OFFSET(A89,-2,0)+1 )</f>
-        <v>77</v>
-      </c>
-      <c r="B89" s="30" t="s">
-        <v>194</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="B89" s="15" t="s">
+        <v>145</v>
       </c>
       <c r="C89" s="30"/>
       <c r="D89" s="13"/>
@@ -15945,222 +15963,259 @@
       <c r="H89" s="13"/>
       <c r="I89" s="33"/>
     </row>
-    <row r="90" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="27">
-        <f ca="1">IF(OFFSET(A90,-2,0) ="",OFFSET(A90,-2,0)+1,OFFSET(A90,-2,0)+1 )</f>
-        <v>77</v>
-      </c>
-      <c r="B90" s="29" t="s">
-        <v>212</v>
-      </c>
-      <c r="C90" s="30"/>
-      <c r="D90" s="30"/>
-      <c r="E90" s="13"/>
-      <c r="F90" s="13"/>
-      <c r="G90" s="13"/>
-      <c r="H90" s="13"/>
-      <c r="I90" s="33"/>
-    </row>
-    <row r="100" spans="1:26" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="48" t="s">
-        <v>207</v>
-      </c>
-      <c r="B100" s="49"/>
-      <c r="C100" s="49"/>
-      <c r="D100" s="49"/>
-      <c r="E100" s="49"/>
-      <c r="F100" s="49"/>
-      <c r="G100" s="49"/>
-      <c r="H100" s="49"/>
-      <c r="I100" s="50"/>
-    </row>
-    <row r="101" spans="1:26" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="38" t="s">
+    <row r="90" spans="1:9" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="B90" s="48"/>
+      <c r="C90" s="48"/>
+      <c r="D90" s="48"/>
+      <c r="E90" s="48"/>
+      <c r="F90" s="48"/>
+      <c r="G90" s="48"/>
+      <c r="H90" s="48"/>
+      <c r="I90" s="48"/>
+    </row>
+    <row r="91" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="46" t="s">
+        <v>174</v>
+      </c>
+      <c r="B91" s="47"/>
+      <c r="C91" s="47"/>
+      <c r="D91" s="47"/>
+      <c r="E91" s="47"/>
+      <c r="F91" s="47"/>
+      <c r="G91" s="47"/>
+      <c r="H91" s="47"/>
+      <c r="I91" s="47"/>
+    </row>
+    <row r="92" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="27">
+        <f ca="1">IF(OFFSET(A92,-3,0) ="",OFFSET(A92,-3,0)+1,OFFSET(A92,-3,0)+1 )</f>
+        <v>81</v>
+      </c>
+      <c r="B92" s="30" t="s">
+        <v>178</v>
+      </c>
+      <c r="C92" s="30"/>
+      <c r="D92" s="13"/>
+      <c r="E92" s="13"/>
+      <c r="F92" s="13"/>
+      <c r="G92" s="13"/>
+      <c r="H92" s="13"/>
+      <c r="I92" s="33"/>
+    </row>
+    <row r="93" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="27">
+        <f t="shared" ref="A93:A95" ca="1" si="2">IF(OFFSET(A93,-1,0) ="",OFFSET(A93,-2,0)+1,OFFSET(A93,-1,0)+1 )</f>
+        <v>82</v>
+      </c>
+      <c r="B93" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="C93" s="30"/>
+      <c r="D93" s="13"/>
+      <c r="E93" s="13"/>
+      <c r="F93" s="13"/>
+      <c r="G93" s="13"/>
+      <c r="H93" s="13"/>
+      <c r="I93" s="33"/>
+    </row>
+    <row r="94" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>83</v>
+      </c>
+      <c r="B94" s="30" t="s">
+        <v>179</v>
+      </c>
+      <c r="C94" s="30"/>
+      <c r="D94" s="13"/>
+      <c r="E94" s="13"/>
+      <c r="F94" s="13"/>
+      <c r="G94" s="13"/>
+      <c r="H94" s="13"/>
+      <c r="I94" s="33"/>
+    </row>
+    <row r="95" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>84</v>
+      </c>
+      <c r="B95" s="30" t="s">
+        <v>205</v>
+      </c>
+      <c r="C95" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="D95" s="30"/>
+      <c r="E95" s="13"/>
+      <c r="F95" s="13"/>
+      <c r="G95" s="13"/>
+      <c r="H95" s="13"/>
+      <c r="I95" s="33"/>
+    </row>
+    <row r="96" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="27">
+        <f ca="1">IF(OFFSET(A96,-2,0) ="",OFFSET(A96,-2,0)+1,OFFSET(A96,-2,0)+1 )</f>
+        <v>84</v>
+      </c>
+      <c r="B96" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="C96" s="30"/>
+      <c r="D96" s="13"/>
+      <c r="E96" s="13"/>
+      <c r="F96" s="13"/>
+      <c r="G96" s="13"/>
+      <c r="H96" s="13"/>
+      <c r="I96" s="33"/>
+    </row>
+    <row r="97" spans="1:26" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="27">
+        <f ca="1">IF(OFFSET(A97,-2,0) ="",OFFSET(A97,-2,0)+1,OFFSET(A97,-2,0)+1 )</f>
+        <v>85</v>
+      </c>
+      <c r="B97" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="C97" s="30"/>
+      <c r="D97" s="13"/>
+      <c r="E97" s="13"/>
+      <c r="F97" s="13"/>
+      <c r="G97" s="13"/>
+      <c r="H97" s="13"/>
+      <c r="I97" s="33"/>
+    </row>
+    <row r="98" spans="1:26" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="27">
+        <f ca="1">IF(OFFSET(A98,-2,0) ="",OFFSET(A98,-2,0)+1,OFFSET(A98,-2,0)+1 )</f>
+        <v>85</v>
+      </c>
+      <c r="B98" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="C98" s="30"/>
+      <c r="D98" s="30"/>
+      <c r="E98" s="13"/>
+      <c r="F98" s="13"/>
+      <c r="G98" s="13"/>
+      <c r="H98" s="13"/>
+      <c r="I98" s="33"/>
+    </row>
+    <row r="99" spans="1:26" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="27">
+        <f ca="1">IF(OFFSET(A99,-2,0) ="",OFFSET(A99,-2,0)+1,OFFSET(A99,-2,0)+1 )</f>
+        <v>86</v>
+      </c>
+      <c r="B99" s="29" t="s">
+        <v>221</v>
+      </c>
+      <c r="C99" s="30"/>
+      <c r="D99" s="30"/>
+      <c r="E99" s="13"/>
+      <c r="F99" s="13"/>
+      <c r="G99" s="13"/>
+      <c r="H99" s="13"/>
+      <c r="I99" s="33"/>
+    </row>
+    <row r="100" spans="1:26" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="27">
+        <f ca="1">IF(OFFSET(A100,-2,0) ="",OFFSET(A100,-2,0)+1,OFFSET(A100,-2,0)+1 )</f>
+        <v>86</v>
+      </c>
+      <c r="B100" s="29" t="s">
+        <v>222</v>
+      </c>
+      <c r="C100" s="30"/>
+      <c r="D100" s="30"/>
+      <c r="E100" s="13"/>
+      <c r="F100" s="13"/>
+      <c r="G100" s="13"/>
+      <c r="H100" s="13"/>
+      <c r="I100" s="33"/>
+    </row>
+    <row r="108" spans="1:26" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="49" t="s">
+        <v>206</v>
+      </c>
+      <c r="B108" s="50"/>
+      <c r="C108" s="50"/>
+      <c r="D108" s="50"/>
+      <c r="E108" s="50"/>
+      <c r="F108" s="50"/>
+      <c r="G108" s="50"/>
+      <c r="H108" s="50"/>
+      <c r="I108" s="51"/>
+    </row>
+    <row r="109" spans="1:26" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="39" t="s">
+        <v>203</v>
+      </c>
+      <c r="B109" s="48"/>
+      <c r="C109" s="48"/>
+      <c r="D109" s="48"/>
+      <c r="E109" s="48"/>
+      <c r="F109" s="48"/>
+      <c r="G109" s="48"/>
+      <c r="H109" s="48"/>
+      <c r="I109" s="48"/>
+    </row>
+    <row r="110" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A110" s="46" t="s">
+        <v>177</v>
+      </c>
+      <c r="B110" s="47"/>
+      <c r="C110" s="47"/>
+      <c r="D110" s="47"/>
+      <c r="E110" s="47"/>
+      <c r="F110" s="47"/>
+      <c r="G110" s="47"/>
+      <c r="H110" s="47"/>
+      <c r="I110" s="47"/>
+      <c r="J110" s="26"/>
+      <c r="K110" s="26"/>
+      <c r="L110" s="26"/>
+      <c r="M110" s="26"/>
+      <c r="N110" s="26"/>
+      <c r="O110" s="26"/>
+      <c r="P110" s="26"/>
+      <c r="Q110" s="26"/>
+      <c r="R110" s="26"/>
+      <c r="S110" s="26"/>
+      <c r="T110" s="26"/>
+      <c r="U110" s="26"/>
+      <c r="V110" s="26"/>
+      <c r="W110" s="26"/>
+      <c r="X110" s="26"/>
+      <c r="Y110" s="26"/>
+      <c r="Z110" s="26"/>
+    </row>
+    <row r="111" spans="1:26" s="10" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="27" t="e">
+        <f ca="1">IF(OFFSET(A111,-3,0) ="",OFFSET(A111,-3,0)+1,OFFSET(A111,-3,0)+1 )</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B111" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="C111" s="35"/>
+      <c r="D111" s="33" t="s">
         <v>204</v>
       </c>
-      <c r="B101" s="45"/>
-      <c r="C101" s="45"/>
-      <c r="D101" s="45"/>
-      <c r="E101" s="45"/>
-      <c r="F101" s="45"/>
-      <c r="G101" s="45"/>
-      <c r="H101" s="45"/>
-      <c r="I101" s="45"/>
-    </row>
-    <row r="102" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="46" t="s">
-        <v>177</v>
-      </c>
-      <c r="B102" s="47"/>
-      <c r="C102" s="47"/>
-      <c r="D102" s="47"/>
-      <c r="E102" s="47"/>
-      <c r="F102" s="47"/>
-      <c r="G102" s="47"/>
-      <c r="H102" s="47"/>
-      <c r="I102" s="47"/>
-      <c r="J102" s="26"/>
-      <c r="K102" s="26"/>
-      <c r="L102" s="26"/>
-      <c r="M102" s="26"/>
-      <c r="N102" s="26"/>
-      <c r="O102" s="26"/>
-      <c r="P102" s="26"/>
-      <c r="Q102" s="26"/>
-      <c r="R102" s="26"/>
-      <c r="S102" s="26"/>
-      <c r="T102" s="26"/>
-      <c r="U102" s="26"/>
-      <c r="V102" s="26"/>
-      <c r="W102" s="26"/>
-      <c r="X102" s="26"/>
-      <c r="Y102" s="26"/>
-      <c r="Z102" s="26"/>
-    </row>
-    <row r="103" spans="1:26" s="10" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="27" t="e">
-        <f ca="1">IF(OFFSET(A103,-3,0) ="",OFFSET(A103,-3,0)+1,OFFSET(A103,-3,0)+1 )</f>
+      <c r="E111" s="13"/>
+      <c r="F111" s="13"/>
+      <c r="G111" s="13"/>
+      <c r="H111" s="13"/>
+      <c r="I111" s="33"/>
+    </row>
+    <row r="112" spans="1:26" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="27" t="e">
+        <f ca="1">IF(OFFSET(A112,-1,0) ="",OFFSET(A112,-2,0)+1,OFFSET(A112,-1,0)+1 )</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B103" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="C103" s="51"/>
-      <c r="D103" s="33" t="s">
-        <v>205</v>
-      </c>
-      <c r="E103" s="13"/>
-      <c r="F103" s="13"/>
-      <c r="G103" s="13"/>
-      <c r="H103" s="13"/>
-      <c r="I103" s="33"/>
-    </row>
-    <row r="104" spans="1:26" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="27" t="e">
-        <f ca="1">IF(OFFSET(A104,-1,0) ="",OFFSET(A104,-2,0)+1,OFFSET(A104,-1,0)+1 )</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="B104" s="12" t="s">
+      <c r="B112" s="12" t="s">
         <v>181</v>
-      </c>
-      <c r="C104" s="30"/>
-      <c r="D104" s="13"/>
-      <c r="E104" s="13"/>
-      <c r="F104" s="13"/>
-      <c r="G104" s="13"/>
-      <c r="H104" s="13"/>
-      <c r="I104" s="33"/>
-    </row>
-    <row r="105" spans="1:26" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="27" t="e">
-        <f ca="1">IF(OFFSET(A105,-1,0) ="",OFFSET(A105,-2,0)+1,OFFSET(A105,-1,0)+1 )</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="B105" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="C105" s="30"/>
-      <c r="D105" s="13"/>
-      <c r="E105" s="13"/>
-      <c r="F105" s="13"/>
-      <c r="G105" s="13"/>
-      <c r="H105" s="13"/>
-      <c r="I105" s="33"/>
-    </row>
-    <row r="106" spans="1:26" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="46" t="s">
-        <v>161</v>
-      </c>
-      <c r="B106" s="47"/>
-      <c r="C106" s="47"/>
-      <c r="D106" s="47"/>
-      <c r="E106" s="47"/>
-      <c r="F106" s="47"/>
-      <c r="G106" s="47"/>
-      <c r="H106" s="47"/>
-      <c r="I106" s="47"/>
-    </row>
-    <row r="107" spans="1:26" s="10" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="27" t="e">
-        <f ca="1">IF(OFFSET(A107,-2,0) ="",OFFSET(A107,-2,0)+1,OFFSET(A107,-2,0)+1 )</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="B107" s="30" t="s">
-        <v>162</v>
-      </c>
-      <c r="C107" s="30"/>
-      <c r="D107" s="13"/>
-      <c r="E107" s="13"/>
-      <c r="F107" s="13"/>
-      <c r="G107" s="13"/>
-      <c r="H107" s="13"/>
-      <c r="I107" s="33"/>
-    </row>
-    <row r="108" spans="1:26" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="27" t="e">
-        <f t="shared" ref="A108" ca="1" si="3">IF(OFFSET(A108,-1,0) ="",OFFSET(A108,-2,0)+1,OFFSET(A108,-1,0)+1 )</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="B108" s="30" t="s">
-        <v>163</v>
-      </c>
-      <c r="C108" s="30"/>
-      <c r="D108" s="13"/>
-      <c r="E108" s="13"/>
-      <c r="F108" s="13"/>
-      <c r="G108" s="13"/>
-      <c r="H108" s="13"/>
-      <c r="I108" s="33"/>
-    </row>
-    <row r="109" spans="1:26" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="46" t="s">
-        <v>164</v>
-      </c>
-      <c r="B109" s="47"/>
-      <c r="C109" s="47"/>
-      <c r="D109" s="47"/>
-      <c r="E109" s="47"/>
-      <c r="F109" s="47"/>
-      <c r="G109" s="47"/>
-      <c r="H109" s="47"/>
-      <c r="I109" s="47"/>
-    </row>
-    <row r="110" spans="1:26" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="27" t="e">
-        <f ca="1">IF(OFFSET(A110,-2,0) ="",OFFSET(A110,-2,0)+1,OFFSET(A110,-2,0)+1 )</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="B110" s="30" t="s">
-        <v>165</v>
-      </c>
-      <c r="C110" s="30"/>
-      <c r="D110" s="13"/>
-      <c r="E110" s="13"/>
-      <c r="F110" s="13"/>
-      <c r="G110" s="13"/>
-      <c r="H110" s="13"/>
-      <c r="I110" s="33"/>
-    </row>
-    <row r="111" spans="1:26" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="46" t="s">
-        <v>192</v>
-      </c>
-      <c r="B111" s="47"/>
-      <c r="C111" s="47"/>
-      <c r="D111" s="47"/>
-      <c r="E111" s="47"/>
-      <c r="F111" s="47"/>
-      <c r="G111" s="47"/>
-      <c r="H111" s="47"/>
-      <c r="I111" s="47"/>
-    </row>
-    <row r="112" spans="1:26" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="27" t="e">
-        <f ca="1">IF(OFFSET(A112,-2,0) ="",OFFSET(A112,-2,0)+1,OFFSET(A112,-2,0)+1 )</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="B112" s="30" t="s">
-        <v>165</v>
       </c>
       <c r="C112" s="30"/>
       <c r="D112" s="13"/>
@@ -16170,42 +16225,42 @@
       <c r="H112" s="13"/>
       <c r="I112" s="33"/>
     </row>
-    <row r="113" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="B113" s="47"/>
-      <c r="C113" s="47"/>
-      <c r="D113" s="47"/>
-      <c r="E113" s="47"/>
-      <c r="F113" s="47"/>
-      <c r="G113" s="47"/>
-      <c r="H113" s="47"/>
-      <c r="I113" s="47"/>
-    </row>
-    <row r="114" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="27" t="e">
-        <f ca="1">IF(OFFSET(A114,-2,0) ="",OFFSET(A114,-2,0)+1,OFFSET(A114,-2,0)+1 )</f>
+    <row r="113" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="27" t="e">
+        <f ca="1">IF(OFFSET(A113,-1,0) ="",OFFSET(A113,-2,0)+1,OFFSET(A113,-1,0)+1 )</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B114" s="30" t="s">
-        <v>165</v>
-      </c>
-      <c r="C114" s="30"/>
-      <c r="D114" s="13"/>
-      <c r="E114" s="13"/>
-      <c r="F114" s="13"/>
-      <c r="G114" s="13"/>
-      <c r="H114" s="13"/>
-      <c r="I114" s="33"/>
-    </row>
-    <row r="115" spans="1:9" s="10" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B113" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="C113" s="30"/>
+      <c r="D113" s="13"/>
+      <c r="E113" s="13"/>
+      <c r="F113" s="13"/>
+      <c r="G113" s="13"/>
+      <c r="H113" s="13"/>
+      <c r="I113" s="33"/>
+    </row>
+    <row r="114" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="46" t="s">
+        <v>161</v>
+      </c>
+      <c r="B114" s="47"/>
+      <c r="C114" s="47"/>
+      <c r="D114" s="47"/>
+      <c r="E114" s="47"/>
+      <c r="F114" s="47"/>
+      <c r="G114" s="47"/>
+      <c r="H114" s="47"/>
+      <c r="I114" s="47"/>
+    </row>
+    <row r="115" spans="1:9" s="10" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="27" t="e">
-        <f ca="1">IF(OFFSET(A115,-1,0) ="",OFFSET(A115,-2,0)+1,OFFSET(A115,-1,0)+1 )</f>
+        <f ca="1">IF(OFFSET(A115,-2,0) ="",OFFSET(A115,-2,0)+1,OFFSET(A115,-2,0)+1 )</f>
         <v>#VALUE!</v>
       </c>
       <c r="B115" s="30" t="s">
-        <v>187</v>
+        <v>162</v>
       </c>
       <c r="C115" s="30"/>
       <c r="D115" s="13"/>
@@ -16215,13 +16270,13 @@
       <c r="H115" s="13"/>
       <c r="I115" s="33"/>
     </row>
-    <row r="116" spans="1:9" s="10" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="27" t="e">
-        <f ca="1">IF(OFFSET(A116,-1,0) ="",OFFSET(A116,-2,0)+1,OFFSET(A116,-1,0)+1 )</f>
+        <f t="shared" ref="A116" ca="1" si="3">IF(OFFSET(A116,-1,0) ="",OFFSET(A116,-2,0)+1,OFFSET(A116,-1,0)+1 )</f>
         <v>#VALUE!</v>
       </c>
       <c r="B116" s="30" t="s">
-        <v>186</v>
+        <v>163</v>
       </c>
       <c r="C116" s="30"/>
       <c r="D116" s="13"/>
@@ -16231,9 +16286,9 @@
       <c r="H116" s="13"/>
       <c r="I116" s="33"/>
     </row>
-    <row r="117" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="46" t="s">
-        <v>200</v>
+        <v>164</v>
       </c>
       <c r="B117" s="47"/>
       <c r="C117" s="47"/>
@@ -16244,13 +16299,13 @@
       <c r="H117" s="47"/>
       <c r="I117" s="47"/>
     </row>
-    <row r="118" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="27" t="e">
         <f ca="1">IF(OFFSET(A118,-2,0) ="",OFFSET(A118,-2,0)+1,OFFSET(A118,-2,0)+1 )</f>
         <v>#VALUE!</v>
       </c>
       <c r="B118" s="30" t="s">
-        <v>188</v>
+        <v>165</v>
       </c>
       <c r="C118" s="30"/>
       <c r="D118" s="13"/>
@@ -16260,29 +16315,26 @@
       <c r="H118" s="13"/>
       <c r="I118" s="33"/>
     </row>
-    <row r="119" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="27" t="e">
-        <f t="shared" ref="A119:A121" ca="1" si="4">IF(OFFSET(A119,-1,0) ="",OFFSET(A119,-2,0)+1,OFFSET(A119,-1,0)+1 )</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="B119" s="30" t="s">
-        <v>189</v>
-      </c>
-      <c r="C119" s="30"/>
-      <c r="D119" s="13"/>
-      <c r="E119" s="13"/>
-      <c r="F119" s="13"/>
-      <c r="G119" s="13"/>
-      <c r="H119" s="13"/>
-      <c r="I119" s="33"/>
+    <row r="119" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="46" t="s">
+        <v>192</v>
+      </c>
+      <c r="B119" s="47"/>
+      <c r="C119" s="47"/>
+      <c r="D119" s="47"/>
+      <c r="E119" s="47"/>
+      <c r="F119" s="47"/>
+      <c r="G119" s="47"/>
+      <c r="H119" s="47"/>
+      <c r="I119" s="47"/>
     </row>
     <row r="120" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="27" t="e">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">IF(OFFSET(A120,-2,0) ="",OFFSET(A120,-2,0)+1,OFFSET(A120,-2,0)+1 )</f>
         <v>#VALUE!</v>
       </c>
       <c r="B120" s="30" t="s">
-        <v>190</v>
+        <v>165</v>
       </c>
       <c r="C120" s="30"/>
       <c r="D120" s="13"/>
@@ -16292,44 +16344,42 @@
       <c r="H120" s="13"/>
       <c r="I120" s="33"/>
     </row>
-    <row r="121" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="27" t="e">
-        <f t="shared" ca="1" si="4"/>
+    <row r="121" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="B121" s="47"/>
+      <c r="C121" s="47"/>
+      <c r="D121" s="47"/>
+      <c r="E121" s="47"/>
+      <c r="F121" s="47"/>
+      <c r="G121" s="47"/>
+      <c r="H121" s="47"/>
+      <c r="I121" s="47"/>
+    </row>
+    <row r="122" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="27" t="e">
+        <f ca="1">IF(OFFSET(A122,-2,0) ="",OFFSET(A122,-2,0)+1,OFFSET(A122,-2,0)+1 )</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B121" s="30" t="s">
-        <v>206</v>
-      </c>
-      <c r="C121" s="30" t="s">
-        <v>180</v>
-      </c>
-      <c r="D121" s="30"/>
-      <c r="E121" s="13"/>
-      <c r="F121" s="13"/>
-      <c r="G121" s="13"/>
-      <c r="H121" s="13"/>
-      <c r="I121" s="33"/>
-    </row>
-    <row r="122" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="46" t="s">
-        <v>196</v>
-      </c>
-      <c r="B122" s="47"/>
-      <c r="C122" s="47"/>
-      <c r="D122" s="47"/>
-      <c r="E122" s="47"/>
-      <c r="F122" s="47"/>
-      <c r="G122" s="47"/>
-      <c r="H122" s="47"/>
-      <c r="I122" s="47"/>
-    </row>
-    <row r="123" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B122" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="C122" s="30"/>
+      <c r="D122" s="13"/>
+      <c r="E122" s="13"/>
+      <c r="F122" s="13"/>
+      <c r="G122" s="13"/>
+      <c r="H122" s="13"/>
+      <c r="I122" s="33"/>
+    </row>
+    <row r="123" spans="1:9" s="10" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="27" t="e">
-        <f ca="1">IF(OFFSET(A123,-2,0) ="",OFFSET(A123,-2,0)+1,OFFSET(A123,-2,0)+1 )</f>
+        <f ca="1">IF(OFFSET(A123,-1,0) ="",OFFSET(A123,-2,0)+1,OFFSET(A123,-1,0)+1 )</f>
         <v>#VALUE!</v>
       </c>
       <c r="B123" s="30" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C123" s="30"/>
       <c r="D123" s="13"/>
@@ -16339,38 +16389,43 @@
       <c r="H123" s="13"/>
       <c r="I123" s="33"/>
     </row>
-    <row r="124" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="46" t="s">
-        <v>197</v>
-      </c>
-      <c r="B124" s="47"/>
-      <c r="C124" s="47"/>
-      <c r="D124" s="47"/>
-      <c r="E124" s="47"/>
-      <c r="F124" s="47"/>
-      <c r="G124" s="47"/>
-      <c r="H124" s="47"/>
-      <c r="I124" s="47"/>
-    </row>
-    <row r="125" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="27" t="e">
-        <f ca="1">IF(OFFSET(A125,-2,0) ="",OFFSET(A125,-2,0)+1,OFFSET(A125,-2,0)+1 )</f>
+    <row r="124" spans="1:9" s="10" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="27" t="e">
+        <f ca="1">IF(OFFSET(A124,-1,0) ="",OFFSET(A124,-2,0)+1,OFFSET(A124,-1,0)+1 )</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B125" s="30" t="s">
-        <v>194</v>
-      </c>
-      <c r="C125" s="30"/>
-      <c r="D125" s="13"/>
-      <c r="E125" s="13"/>
-      <c r="F125" s="13"/>
-      <c r="G125" s="13"/>
-      <c r="H125" s="13"/>
-      <c r="I125" s="33"/>
-    </row>
-    <row r="126" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="27"/>
-      <c r="B126" s="30"/>
+      <c r="B124" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="C124" s="30"/>
+      <c r="D124" s="13"/>
+      <c r="E124" s="13"/>
+      <c r="F124" s="13"/>
+      <c r="G124" s="13"/>
+      <c r="H124" s="13"/>
+      <c r="I124" s="33"/>
+    </row>
+    <row r="125" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="46" t="s">
+        <v>200</v>
+      </c>
+      <c r="B125" s="47"/>
+      <c r="C125" s="47"/>
+      <c r="D125" s="47"/>
+      <c r="E125" s="47"/>
+      <c r="F125" s="47"/>
+      <c r="G125" s="47"/>
+      <c r="H125" s="47"/>
+      <c r="I125" s="47"/>
+    </row>
+    <row r="126" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="27" t="e">
+        <f ca="1">IF(OFFSET(A126,-2,0) ="",OFFSET(A126,-2,0)+1,OFFSET(A126,-2,0)+1 )</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B126" s="30" t="s">
+        <v>188</v>
+      </c>
       <c r="C126" s="30"/>
       <c r="D126" s="13"/>
       <c r="E126" s="13"/>
@@ -16379,9 +16434,14 @@
       <c r="H126" s="13"/>
       <c r="I126" s="33"/>
     </row>
-    <row r="127" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="27"/>
-      <c r="B127" s="30"/>
+    <row r="127" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="27" t="e">
+        <f t="shared" ref="A127:A129" ca="1" si="4">IF(OFFSET(A127,-1,0) ="",OFFSET(A127,-2,0)+1,OFFSET(A127,-1,0)+1 )</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B127" s="30" t="s">
+        <v>189</v>
+      </c>
       <c r="C127" s="30"/>
       <c r="D127" s="13"/>
       <c r="E127" s="13"/>
@@ -16391,8 +16451,13 @@
       <c r="I127" s="33"/>
     </row>
     <row r="128" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="27"/>
-      <c r="B128" s="30"/>
+      <c r="A128" s="27" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B128" s="30" t="s">
+        <v>190</v>
+      </c>
       <c r="C128" s="30"/>
       <c r="D128" s="13"/>
       <c r="E128" s="13"/>
@@ -16401,31 +16466,45 @@
       <c r="H128" s="13"/>
       <c r="I128" s="33"/>
     </row>
-    <row r="129" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="27"/>
-      <c r="B129" s="30"/>
-      <c r="C129" s="30"/>
-      <c r="D129" s="13"/>
+    <row r="129" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="27" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B129" s="30" t="s">
+        <v>205</v>
+      </c>
+      <c r="C129" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="D129" s="30"/>
       <c r="E129" s="13"/>
       <c r="F129" s="13"/>
       <c r="G129" s="13"/>
       <c r="H129" s="13"/>
       <c r="I129" s="33"/>
     </row>
-    <row r="130" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="27"/>
-      <c r="B130" s="30"/>
-      <c r="C130" s="30"/>
-      <c r="D130" s="13"/>
-      <c r="E130" s="13"/>
-      <c r="F130" s="13"/>
-      <c r="G130" s="13"/>
-      <c r="H130" s="13"/>
-      <c r="I130" s="33"/>
+    <row r="130" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="46" t="s">
+        <v>196</v>
+      </c>
+      <c r="B130" s="47"/>
+      <c r="C130" s="47"/>
+      <c r="D130" s="47"/>
+      <c r="E130" s="47"/>
+      <c r="F130" s="47"/>
+      <c r="G130" s="47"/>
+      <c r="H130" s="47"/>
+      <c r="I130" s="47"/>
     </row>
     <row r="131" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="27"/>
-      <c r="B131" s="30"/>
+      <c r="A131" s="27" t="e">
+        <f ca="1">IF(OFFSET(A131,-2,0) ="",OFFSET(A131,-2,0)+1,OFFSET(A131,-2,0)+1 )</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B131" s="30" t="s">
+        <v>193</v>
+      </c>
       <c r="C131" s="30"/>
       <c r="D131" s="13"/>
       <c r="E131" s="13"/>
@@ -16434,20 +16513,27 @@
       <c r="H131" s="13"/>
       <c r="I131" s="33"/>
     </row>
-    <row r="132" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="27"/>
-      <c r="B132" s="30"/>
-      <c r="C132" s="30"/>
-      <c r="D132" s="13"/>
-      <c r="E132" s="13"/>
-      <c r="F132" s="13"/>
-      <c r="G132" s="13"/>
-      <c r="H132" s="13"/>
-      <c r="I132" s="33"/>
+    <row r="132" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="46" t="s">
+        <v>197</v>
+      </c>
+      <c r="B132" s="47"/>
+      <c r="C132" s="47"/>
+      <c r="D132" s="47"/>
+      <c r="E132" s="47"/>
+      <c r="F132" s="47"/>
+      <c r="G132" s="47"/>
+      <c r="H132" s="47"/>
+      <c r="I132" s="47"/>
     </row>
     <row r="133" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="27"/>
-      <c r="B133" s="30"/>
+      <c r="A133" s="27" t="e">
+        <f ca="1">IF(OFFSET(A133,-2,0) ="",OFFSET(A133,-2,0)+1,OFFSET(A133,-2,0)+1 )</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B133" s="30" t="s">
+        <v>194</v>
+      </c>
       <c r="C133" s="30"/>
       <c r="D133" s="13"/>
       <c r="E133" s="13"/>
@@ -17171,28 +17257,116 @@
       <c r="H198" s="13"/>
       <c r="I198" s="33"/>
     </row>
+    <row r="199" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A199" s="27"/>
+      <c r="B199" s="30"/>
+      <c r="C199" s="30"/>
+      <c r="D199" s="13"/>
+      <c r="E199" s="13"/>
+      <c r="F199" s="13"/>
+      <c r="G199" s="13"/>
+      <c r="H199" s="13"/>
+      <c r="I199" s="33"/>
+    </row>
+    <row r="200" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A200" s="27"/>
+      <c r="B200" s="30"/>
+      <c r="C200" s="30"/>
+      <c r="D200" s="13"/>
+      <c r="E200" s="13"/>
+      <c r="F200" s="13"/>
+      <c r="G200" s="13"/>
+      <c r="H200" s="13"/>
+      <c r="I200" s="33"/>
+    </row>
+    <row r="201" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A201" s="27"/>
+      <c r="B201" s="30"/>
+      <c r="C201" s="30"/>
+      <c r="D201" s="13"/>
+      <c r="E201" s="13"/>
+      <c r="F201" s="13"/>
+      <c r="G201" s="13"/>
+      <c r="H201" s="13"/>
+      <c r="I201" s="33"/>
+    </row>
+    <row r="202" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A202" s="27"/>
+      <c r="B202" s="30"/>
+      <c r="C202" s="30"/>
+      <c r="D202" s="13"/>
+      <c r="E202" s="13"/>
+      <c r="F202" s="13"/>
+      <c r="G202" s="13"/>
+      <c r="H202" s="13"/>
+      <c r="I202" s="33"/>
+    </row>
+    <row r="203" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A203" s="27"/>
+      <c r="B203" s="30"/>
+      <c r="C203" s="30"/>
+      <c r="D203" s="13"/>
+      <c r="E203" s="13"/>
+      <c r="F203" s="13"/>
+      <c r="G203" s="13"/>
+      <c r="H203" s="13"/>
+      <c r="I203" s="33"/>
+    </row>
+    <row r="204" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A204" s="27"/>
+      <c r="B204" s="30"/>
+      <c r="C204" s="30"/>
+      <c r="D204" s="13"/>
+      <c r="E204" s="13"/>
+      <c r="F204" s="13"/>
+      <c r="G204" s="13"/>
+      <c r="H204" s="13"/>
+      <c r="I204" s="33"/>
+    </row>
+    <row r="205" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A205" s="27"/>
+      <c r="B205" s="30"/>
+      <c r="C205" s="30"/>
+      <c r="D205" s="13"/>
+      <c r="E205" s="13"/>
+      <c r="F205" s="13"/>
+      <c r="G205" s="13"/>
+      <c r="H205" s="13"/>
+      <c r="I205" s="33"/>
+    </row>
+    <row r="206" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A206" s="27"/>
+      <c r="B206" s="30"/>
+      <c r="C206" s="30"/>
+      <c r="D206" s="13"/>
+      <c r="E206" s="13"/>
+      <c r="F206" s="13"/>
+      <c r="G206" s="13"/>
+      <c r="H206" s="13"/>
+      <c r="I206" s="33"/>
+    </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A113:I113"/>
-    <mergeCell ref="A106:I106"/>
+    <mergeCell ref="A130:I130"/>
+    <mergeCell ref="A132:I132"/>
+    <mergeCell ref="A91:I91"/>
+    <mergeCell ref="A108:I108"/>
+    <mergeCell ref="A109:I109"/>
+    <mergeCell ref="A110:I110"/>
+    <mergeCell ref="A125:I125"/>
+    <mergeCell ref="A117:I117"/>
+    <mergeCell ref="A119:I119"/>
+    <mergeCell ref="A121:I121"/>
+    <mergeCell ref="A114:I114"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A17:I17"/>
     <mergeCell ref="A29:I29"/>
     <mergeCell ref="A38:I38"/>
-    <mergeCell ref="A82:I82"/>
+    <mergeCell ref="A90:I90"/>
     <mergeCell ref="A55:I55"/>
-    <mergeCell ref="A62:I62"/>
-    <mergeCell ref="A68:I68"/>
-    <mergeCell ref="A122:I122"/>
-    <mergeCell ref="A124:I124"/>
-    <mergeCell ref="A83:I83"/>
-    <mergeCell ref="A100:I100"/>
-    <mergeCell ref="A101:I101"/>
-    <mergeCell ref="A102:I102"/>
-    <mergeCell ref="A117:I117"/>
-    <mergeCell ref="A109:I109"/>
-    <mergeCell ref="A111:I111"/>
+    <mergeCell ref="A70:I70"/>
+    <mergeCell ref="A76:I76"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>